<commit_message>
Update on the codebase and remove redundant codes
</commit_message>
<xml_diff>
--- a/model_coefficients.xlsx
+++ b/model_coefficients.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -490,13 +490,13 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>-1.543622004151653</v>
+        <v>-1.544227736756907</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1373834749768942</v>
+        <v>0.1374803463640217</v>
       </c>
       <c r="G2" t="n">
-        <v>-11.2358637339755</v>
+        <v>-11.23235267866474</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -522,16 +522,16 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>-0.6259535499863195</v>
+        <v>-0.6211846332349278</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1969462641680273</v>
+        <v>0.1947782623656088</v>
       </c>
       <c r="G3" t="n">
-        <v>-3.178296133858628</v>
+        <v>-3.189188699433734</v>
       </c>
       <c r="H3" t="n">
-        <v>0.001481433580337255</v>
+        <v>0.001426727125682481</v>
       </c>
     </row>
     <row r="4">
@@ -554,16 +554,16 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.3736949891941211</v>
+        <v>0.3738033665669097</v>
       </c>
       <c r="F4" t="n">
-        <v>0.065162034854666</v>
+        <v>0.06517887158621102</v>
       </c>
       <c r="G4" t="n">
-        <v>5.734857574995257</v>
+        <v>5.735038939217459</v>
       </c>
       <c r="H4" t="n">
-        <v>9.759432151312808e-09</v>
+        <v>9.748994500569097e-09</v>
       </c>
     </row>
     <row r="5">
@@ -586,16 +586,16 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>2.781780629664026</v>
+        <v>2.763399168412315</v>
       </c>
       <c r="F5" t="n">
-        <v>0.694567185188624</v>
+        <v>0.6857906494631487</v>
       </c>
       <c r="G5" t="n">
-        <v>4.005056226352776</v>
+        <v>4.029508379228461</v>
       </c>
       <c r="H5" t="n">
-        <v>6.200273142420443e-05</v>
+        <v>5.589362359414984e-05</v>
       </c>
     </row>
     <row r="6">
@@ -618,16 +618,16 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.07554290494455752</v>
+        <v>0.07555048553970903</v>
       </c>
       <c r="F6" t="n">
-        <v>0.01841278783221918</v>
+        <v>0.01841369181064835</v>
       </c>
       <c r="G6" t="n">
-        <v>4.102741292020313</v>
+        <v>4.102951559769043</v>
       </c>
       <c r="H6" t="n">
-        <v>4.08283697905798e-05</v>
+        <v>4.079126777578601e-05</v>
       </c>
     </row>
     <row r="7">
@@ -650,13 +650,13 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>-0.2884833888957783</v>
+        <v>-0.2885063181629864</v>
       </c>
       <c r="F7" t="n">
-        <v>0.02305108514786198</v>
+        <v>0.02305677571274468</v>
       </c>
       <c r="G7" t="n">
-        <v>-12.51495914542751</v>
+        <v>-12.51286484046427</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -682,16 +682,16 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>-0.01870870766980713</v>
+        <v>-0.01876471678302588</v>
       </c>
       <c r="F8" t="n">
-        <v>0.01972698796972728</v>
+        <v>0.01977713744507669</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.9483813594639402</v>
+        <v>-0.9488085338026686</v>
       </c>
       <c r="H8" t="n">
-        <v>0.3429353455086781</v>
+        <v>0.3427180007858519</v>
       </c>
     </row>
     <row r="9">
@@ -714,16 +714,16 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.1757600458590779</v>
+        <v>0.1762214357850047</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0265955893156254</v>
+        <v>0.02662269387679186</v>
       </c>
       <c r="G9" t="n">
-        <v>6.608616329821541</v>
+        <v>6.619218798590674</v>
       </c>
       <c r="H9" t="n">
-        <v>3.879296883724237e-11</v>
+        <v>3.611022592053814e-11</v>
       </c>
     </row>
     <row r="10">
@@ -784,13 +784,13 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1.150786793544271</v>
+        <v>1.151134010684105</v>
       </c>
       <c r="F11" t="n">
-        <v>0.04488042872743582</v>
+        <v>0.04490641449745921</v>
       </c>
       <c r="G11" t="n">
-        <v>25.64117202416883</v>
+        <v>25.63406639208753</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -816,13 +816,13 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1.076403382530374</v>
+        <v>1.076733639619282</v>
       </c>
       <c r="F12" t="n">
-        <v>0.04762078347985448</v>
+        <v>0.04764652517939417</v>
       </c>
       <c r="G12" t="n">
-        <v>22.60364706017767</v>
+        <v>22.59836652395255</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -848,13 +848,13 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>1.24725043532273</v>
+        <v>1.24767138880253</v>
       </c>
       <c r="F13" t="n">
-        <v>0.05131774946368497</v>
+        <v>0.05134720020999142</v>
       </c>
       <c r="G13" t="n">
-        <v>24.3044647969421</v>
+        <v>24.29872288412431</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -880,13 +880,13 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>1.020354467155238</v>
+        <v>1.020711421314317</v>
       </c>
       <c r="F14" t="n">
-        <v>0.04904290358569496</v>
+        <v>0.04906821036273966</v>
       </c>
       <c r="G14" t="n">
-        <v>20.8053437405377</v>
+        <v>20.80188810123388</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -912,13 +912,13 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0.8323978639677</v>
+        <v>0.8327749059505605</v>
       </c>
       <c r="F15" t="n">
-        <v>0.05286351694964178</v>
+        <v>0.05288889471981514</v>
       </c>
       <c r="G15" t="n">
-        <v>15.74616885109825</v>
+        <v>15.74574228382978</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -944,13 +944,13 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.6915387136403275</v>
+        <v>0.691845028555817</v>
       </c>
       <c r="F16" t="n">
-        <v>0.04925067769026637</v>
+        <v>0.04927248592272354</v>
       </c>
       <c r="G16" t="n">
-        <v>14.04120199066739</v>
+        <v>14.0412040428979</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -976,13 +976,13 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0.8091169030949918</v>
+        <v>0.8094060238267657</v>
       </c>
       <c r="F17" t="n">
-        <v>0.04713489122425082</v>
+        <v>0.04715725904067446</v>
       </c>
       <c r="G17" t="n">
-        <v>17.16598642878668</v>
+        <v>17.1639751816675</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1008,13 +1008,13 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>1.154955526171788</v>
+        <v>1.155311956182193</v>
       </c>
       <c r="F18" t="n">
-        <v>0.04692638540118947</v>
+        <v>0.04695333577071551</v>
       </c>
       <c r="G18" t="n">
-        <v>24.61207093350728</v>
+        <v>24.60553520199831</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -1040,13 +1040,13 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>1.223830564028048</v>
+        <v>1.22419995216538</v>
       </c>
       <c r="F19" t="n">
-        <v>0.04594332398076227</v>
+        <v>0.04597095371446545</v>
       </c>
       <c r="G19" t="n">
-        <v>26.63783239788792</v>
+        <v>26.62985762145582</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -1072,13 +1072,13 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>0.5114064000794257</v>
+        <v>0.5115842640386148</v>
       </c>
       <c r="F20" t="n">
-        <v>0.04757333998215175</v>
+        <v>0.0475928109055167</v>
       </c>
       <c r="G20" t="n">
-        <v>10.74985275914077</v>
+        <v>10.74919203750089</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
@@ -1104,16 +1104,16 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0.320354211969791</v>
+        <v>0.3204552152093691</v>
       </c>
       <c r="F21" t="n">
-        <v>0.04552955217584625</v>
+        <v>0.04554682398534928</v>
       </c>
       <c r="G21" t="n">
-        <v>7.036181922577859</v>
+        <v>7.0357313016032</v>
       </c>
       <c r="H21" t="n">
-        <v>1.975752894622929e-12</v>
+        <v>1.982192188165754e-12</v>
       </c>
     </row>
     <row r="22">
@@ -1174,16 +1174,16 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>1.062386314529807</v>
+        <v>1.054028003124819</v>
       </c>
       <c r="F23" t="n">
-        <v>0.3855063050030931</v>
+        <v>0.3817203198279964</v>
       </c>
       <c r="G23" t="n">
-        <v>2.755820853613607</v>
+        <v>2.761257256613963</v>
       </c>
       <c r="H23" t="n">
-        <v>0.005854505271153165</v>
+        <v>0.005757930181657933</v>
       </c>
     </row>
     <row r="24">
@@ -1206,16 +1206,16 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0.1125417089590994</v>
+        <v>0.1109164934599245</v>
       </c>
       <c r="F24" t="n">
-        <v>0.2912408532693559</v>
+        <v>0.2893921469828211</v>
       </c>
       <c r="G24" t="n">
-        <v>0.386421436743382</v>
+        <v>0.3832740266657113</v>
       </c>
       <c r="H24" t="n">
-        <v>0.6991845765065512</v>
+        <v>0.7015165952932785</v>
       </c>
     </row>
     <row r="25">
@@ -1238,16 +1238,16 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0.9367084238393153</v>
+        <v>0.9304454824590691</v>
       </c>
       <c r="F25" t="n">
-        <v>0.3471760113151371</v>
+        <v>0.3439920150237046</v>
       </c>
       <c r="G25" t="n">
-        <v>2.698079341047422</v>
+        <v>2.704846164502531</v>
       </c>
       <c r="H25" t="n">
-        <v>0.006974081678205346</v>
+        <v>0.006833602791120441</v>
       </c>
     </row>
     <row r="26">
@@ -1270,16 +1270,16 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0.486889109543455</v>
+        <v>0.4846769104861006</v>
       </c>
       <c r="F26" t="n">
-        <v>0.2142934025332451</v>
+        <v>0.2126499729358546</v>
       </c>
       <c r="G26" t="n">
-        <v>2.272067659505513</v>
+        <v>2.279223946245331</v>
       </c>
       <c r="H26" t="n">
-        <v>0.02308242408086314</v>
+        <v>0.02265375632057243</v>
       </c>
     </row>
     <row r="27">
@@ -1302,16 +1302,16 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>0.02774440728088904</v>
+        <v>0.02686528984863582</v>
       </c>
       <c r="F27" t="n">
-        <v>0.2614196626756607</v>
+        <v>0.2597819392295881</v>
       </c>
       <c r="G27" t="n">
-        <v>0.106129764673459</v>
+        <v>0.1034147713586417</v>
       </c>
       <c r="H27" t="n">
-        <v>0.9154793957073766</v>
+        <v>0.9176337891538631</v>
       </c>
     </row>
     <row r="28">
@@ -1334,16 +1334,16 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>0.1930687176169492</v>
+        <v>0.1922763257028656</v>
       </c>
       <c r="F28" t="n">
-        <v>0.1806110264078497</v>
+        <v>0.1794275387836337</v>
       </c>
       <c r="G28" t="n">
-        <v>1.068975252817062</v>
+        <v>1.071609893360095</v>
       </c>
       <c r="H28" t="n">
-        <v>0.2850808206734401</v>
+        <v>0.283895287807014</v>
       </c>
     </row>
     <row r="29">
@@ -1366,16 +1366,16 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>1.49515702104668</v>
+        <v>1.486097864801565</v>
       </c>
       <c r="F29" t="n">
-        <v>0.4042793496243877</v>
+        <v>0.3997342276056048</v>
       </c>
       <c r="G29" t="n">
-        <v>3.698326472603954</v>
+        <v>3.717714826922694</v>
       </c>
       <c r="H29" t="n">
-        <v>0.0002170256400420012</v>
+        <v>0.0002010330158164209</v>
       </c>
     </row>
     <row r="30">
@@ -1398,16 +1398,16 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>1.944383595068592</v>
+        <v>1.930446279682593</v>
       </c>
       <c r="F30" t="n">
-        <v>0.509706451483417</v>
+        <v>0.5033237544512432</v>
       </c>
       <c r="G30" t="n">
-        <v>3.814712545634782</v>
+        <v>3.835396725480317</v>
       </c>
       <c r="H30" t="n">
-        <v>0.0001363415460091666</v>
+        <v>0.0001253617751226788</v>
       </c>
     </row>
     <row r="31">
@@ -1430,16 +1430,16 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>-1.596695061151823</v>
+        <v>-1.588861919258735</v>
       </c>
       <c r="F31" t="n">
-        <v>0.4409767734737947</v>
+        <v>0.4365093914148158</v>
       </c>
       <c r="G31" t="n">
-        <v>-3.620814421971109</v>
+        <v>-3.639926082930932</v>
       </c>
       <c r="H31" t="n">
-        <v>0.0002936771135366723</v>
+        <v>0.000272716316984889</v>
       </c>
     </row>
     <row r="32">
@@ -1462,16 +1462,16 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>1.499093711313277</v>
+        <v>1.489315916307896</v>
       </c>
       <c r="F32" t="n">
-        <v>0.4023199477207487</v>
+        <v>0.3976130482060837</v>
       </c>
       <c r="G32" t="n">
-        <v>3.726123250418782</v>
+        <v>3.745641454734741</v>
       </c>
       <c r="H32" t="n">
-        <v>0.0001944473520891776</v>
+        <v>0.0001799334248100415</v>
       </c>
     </row>
     <row r="33">
@@ -1494,16 +1494,16 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>2.835433495490076</v>
+        <v>2.818817076729233</v>
       </c>
       <c r="F33" t="n">
-        <v>0.7143209451084808</v>
+        <v>0.7058822514330997</v>
       </c>
       <c r="G33" t="n">
-        <v>3.969411109813533</v>
+        <v>3.993324766279939</v>
       </c>
       <c r="H33" t="n">
-        <v>7.205047865244119e-05</v>
+        <v>6.515323315414712e-05</v>
       </c>
     </row>
     <row r="34">
@@ -1526,16 +1526,16 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>2.822848242641388</v>
+        <v>2.804638815962098</v>
       </c>
       <c r="F34" t="n">
-        <v>0.720996683243408</v>
+        <v>0.7121987440201824</v>
       </c>
       <c r="G34" t="n">
-        <v>3.915202813331779</v>
+        <v>3.938000227473978</v>
       </c>
       <c r="H34" t="n">
-        <v>9.032824531529648e-05</v>
+        <v>8.216351668188793e-05</v>
       </c>
     </row>
     <row r="35">
@@ -1558,16 +1558,16 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>4.208926716955204</v>
+        <v>4.182177777896281</v>
       </c>
       <c r="F35" t="n">
-        <v>1.048156814568538</v>
+        <v>1.035139447926546</v>
       </c>
       <c r="G35" t="n">
-        <v>4.015550591715368</v>
+        <v>4.040207129840743</v>
       </c>
       <c r="H35" t="n">
-        <v>5.930717431978927e-05</v>
+        <v>5.340401571474196e-05</v>
       </c>
     </row>
     <row r="36">
@@ -1590,16 +1590,16 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>2.188957418924717</v>
+        <v>2.17546380209388</v>
       </c>
       <c r="F36" t="n">
-        <v>0.5624839012112759</v>
+        <v>0.5558061096143577</v>
       </c>
       <c r="G36" t="n">
-        <v>3.891591233468255</v>
+        <v>3.914069608913434</v>
       </c>
       <c r="H36" t="n">
-        <v>9.958892738737291e-05</v>
+        <v>9.075345440634486e-05</v>
       </c>
     </row>
     <row r="37">
@@ -1622,16 +1622,16 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>4.22871128303236</v>
+        <v>4.201474336152049</v>
       </c>
       <c r="F37" t="n">
-        <v>1.0514857107364</v>
+        <v>1.03831978500017</v>
       </c>
       <c r="G37" t="n">
-        <v>4.021653589630612</v>
+        <v>4.046416524892966</v>
       </c>
       <c r="H37" t="n">
-        <v>5.779100621650102e-05</v>
+        <v>5.2007658587927e-05</v>
       </c>
     </row>
     <row r="38">
@@ -1654,16 +1654,16 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>2.131778152715139</v>
+        <v>2.119233693159326</v>
       </c>
       <c r="F38" t="n">
-        <v>0.551762799888192</v>
+        <v>0.545394882115033</v>
       </c>
       <c r="G38" t="n">
-        <v>3.863577162402493</v>
+        <v>3.885686798044538</v>
       </c>
       <c r="H38" t="n">
-        <v>0.0001117385746889354</v>
+        <v>0.0001020409949625822</v>
       </c>
     </row>
     <row r="39">
@@ -1686,16 +1686,16 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>1.558140423386612</v>
+        <v>1.547754139893357</v>
       </c>
       <c r="F39" t="n">
-        <v>0.4395921989170747</v>
+        <v>0.4346313234732209</v>
       </c>
       <c r="G39" t="n">
-        <v>3.544513363115885</v>
+        <v>3.561073618719886</v>
       </c>
       <c r="H39" t="n">
-        <v>0.0003933385652643562</v>
+        <v>0.000369341500632947</v>
       </c>
     </row>
     <row r="40">
@@ -1718,16 +1718,16 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>4.58906980269172</v>
+        <v>4.560223163024439</v>
       </c>
       <c r="F40" t="n">
-        <v>1.135286958138384</v>
+        <v>1.121170561973547</v>
       </c>
       <c r="G40" t="n">
-        <v>4.042211327973611</v>
+        <v>4.067376827120053</v>
       </c>
       <c r="H40" t="n">
-        <v>5.294947849487919e-05</v>
+        <v>4.7545325076781e-05</v>
       </c>
     </row>
     <row r="41">
@@ -1750,16 +1750,16 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>4.427114118942246</v>
+        <v>4.397924301908432</v>
       </c>
       <c r="F41" t="n">
-        <v>1.094546643219245</v>
+        <v>1.080601106154477</v>
       </c>
       <c r="G41" t="n">
-        <v>4.044701197856053</v>
+        <v>4.069886914659198</v>
       </c>
       <c r="H41" t="n">
-        <v>5.238989970024477e-05</v>
+        <v>4.703596343103023e-05</v>
       </c>
     </row>
     <row r="42">
@@ -1782,16 +1782,16 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>3.734514661486078</v>
+        <v>3.708951473101627</v>
       </c>
       <c r="F42" t="n">
-        <v>0.9251309187444091</v>
+        <v>0.9131414882975555</v>
       </c>
       <c r="G42" t="n">
-        <v>4.036741812229709</v>
+        <v>4.061748941023879</v>
       </c>
       <c r="H42" t="n">
-        <v>5.419865885203379e-05</v>
+        <v>4.870644221299791e-05</v>
       </c>
     </row>
     <row r="43">
@@ -1814,16 +1814,16 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>4.362103487775443</v>
+        <v>4.334633671234213</v>
       </c>
       <c r="F43" t="n">
-        <v>1.077722306571052</v>
+        <v>1.064293136420555</v>
       </c>
       <c r="G43" t="n">
-        <v>4.047520832755269</v>
+        <v>4.072781758048762</v>
       </c>
       <c r="H43" t="n">
-        <v>5.176297619535752e-05</v>
+        <v>4.645494991639687e-05</v>
       </c>
     </row>
     <row r="44">
@@ -1846,16 +1846,16 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>3.106277704777547</v>
+        <v>3.086266759024388</v>
       </c>
       <c r="F44" t="n">
-        <v>0.7782842203005975</v>
+        <v>0.7686137438040733</v>
       </c>
       <c r="G44" t="n">
-        <v>3.991186797509289</v>
+        <v>4.015367645842007</v>
       </c>
       <c r="H44" t="n">
-        <v>6.574347073895481e-05</v>
+        <v>5.935319994532229e-05</v>
       </c>
     </row>
     <row r="45">
@@ -1878,16 +1878,16 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>3.502117437262926</v>
+        <v>3.480490249293395</v>
       </c>
       <c r="F45" t="n">
-        <v>0.8776630895444631</v>
+        <v>0.8669824355196666</v>
       </c>
       <c r="G45" t="n">
-        <v>3.990275401779347</v>
+        <v>4.01448761439231</v>
       </c>
       <c r="H45" t="n">
-        <v>6.599661873485374e-05</v>
+        <v>5.957507183063093e-05</v>
       </c>
     </row>
     <row r="46">
@@ -1910,16 +1910,16 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>3.65873327736255</v>
+        <v>3.634627728524323</v>
       </c>
       <c r="F46" t="n">
-        <v>0.917564354632736</v>
+        <v>0.9060460537538362</v>
       </c>
       <c r="G46" t="n">
-        <v>3.987440509088876</v>
+        <v>4.011526470935665</v>
       </c>
       <c r="H46" t="n">
-        <v>6.678994485764811e-05</v>
+        <v>6.032741115991058e-05</v>
       </c>
     </row>
     <row r="47">
@@ -1942,16 +1942,16 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>-2.524492103467064</v>
+        <v>-2.501813430712308</v>
       </c>
       <c r="F47" t="n">
-        <v>0.6919826723318739</v>
+        <v>0.682691817743867</v>
       </c>
       <c r="G47" t="n">
-        <v>-3.648201327001832</v>
+        <v>-3.664630753853968</v>
       </c>
       <c r="H47" t="n">
-        <v>0.0002640826680517794</v>
+        <v>0.0002476956743244774</v>
       </c>
     </row>
     <row r="48">
@@ -1974,16 +1974,16 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>-0.7126661458372235</v>
+        <v>-0.7038205870955599</v>
       </c>
       <c r="F48" t="n">
-        <v>0.2879619243803098</v>
+        <v>0.2848576580413573</v>
       </c>
       <c r="G48" t="n">
-        <v>-2.474862422760914</v>
+        <v>-2.470779939470346</v>
       </c>
       <c r="H48" t="n">
-        <v>0.01332875090024732</v>
+        <v>0.01348187529586964</v>
       </c>
     </row>
     <row r="49">
@@ -2006,16 +2006,16 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>-1.704071083053957</v>
+        <v>-1.69338363239048</v>
       </c>
       <c r="F49" t="n">
-        <v>0.510547938315727</v>
+        <v>0.5052085493492804</v>
       </c>
       <c r="G49" t="n">
-        <v>-3.337729829391277</v>
+        <v>-3.351850705155808</v>
       </c>
       <c r="H49" t="n">
-        <v>0.000844658348849503</v>
+        <v>0.0008027329486648416</v>
       </c>
     </row>
     <row r="50">
@@ -2038,16 +2038,16 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>2.97040848180984</v>
+        <v>2.950539665858639</v>
       </c>
       <c r="F50" t="n">
-        <v>0.762276938584051</v>
+        <v>0.7528535644503864</v>
       </c>
       <c r="G50" t="n">
-        <v>3.896757636828885</v>
+        <v>3.919141523901442</v>
       </c>
       <c r="H50" t="n">
-        <v>9.748909151574559e-05</v>
+        <v>8.886492549753378e-05</v>
       </c>
     </row>
     <row r="51">
@@ -2070,16 +2070,16 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>2.765565181369542</v>
+        <v>2.750036442356047</v>
       </c>
       <c r="F51" t="n">
-        <v>0.7268781868280334</v>
+        <v>0.7187719483704249</v>
       </c>
       <c r="G51" t="n">
-        <v>3.804716156683928</v>
+        <v>3.826020824250319</v>
       </c>
       <c r="H51" t="n">
-        <v>0.0001419668916695649</v>
+        <v>0.0001302312779918324</v>
       </c>
     </row>
     <row r="52">
@@ -2102,16 +2102,16 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>1.989529473326369</v>
+        <v>1.980354700656758</v>
       </c>
       <c r="F52" t="n">
-        <v>0.5465996114603479</v>
+        <v>0.5411670651039523</v>
       </c>
       <c r="G52" t="n">
-        <v>3.639829651556671</v>
+        <v>3.659414676820169</v>
       </c>
       <c r="H52" t="n">
-        <v>0.0002728184667573075</v>
+        <v>0.0002527919927652889</v>
       </c>
     </row>
     <row r="53">
@@ -2134,16 +2134,16 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>2.208301437687047</v>
+        <v>2.196162308526721</v>
       </c>
       <c r="F53" t="n">
-        <v>0.593343588226616</v>
+        <v>0.5869112838547597</v>
       </c>
       <c r="G53" t="n">
-        <v>3.721792029949277</v>
+        <v>3.741898254364545</v>
       </c>
       <c r="H53" t="n">
-        <v>0.0001978139176299631</v>
+        <v>0.0001826354623226667</v>
       </c>
     </row>
     <row r="54">
@@ -2166,16 +2166,16 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>1.497535717145966</v>
+        <v>1.489484049252733</v>
       </c>
       <c r="F54" t="n">
-        <v>0.4483772350089874</v>
+        <v>0.4439579938148496</v>
       </c>
       <c r="G54" t="n">
-        <v>3.339901315713786</v>
+        <v>3.355011217278722</v>
       </c>
       <c r="H54" t="n">
-        <v>0.0008380816489752529</v>
+        <v>0.0007936176637688419</v>
       </c>
     </row>
     <row r="55">
@@ -2236,13 +2236,13 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>1.639330877721786</v>
+        <v>1.640574416658157</v>
       </c>
       <c r="F56" t="n">
-        <v>0.1662004060243831</v>
+        <v>0.1662783708637904</v>
       </c>
       <c r="G56" t="n">
-        <v>9.863579259074839</v>
+        <v>9.866433067185831</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -2306,16 +2306,16 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>-1.94369498875309</v>
+        <v>-1.93473093434308</v>
       </c>
       <c r="F58" t="n">
-        <v>0.8441056805412356</v>
+        <v>0.8419343491383622</v>
       </c>
       <c r="G58" t="n">
-        <v>-2.302667821764333</v>
+        <v>-2.297959379280333</v>
       </c>
       <c r="H58" t="n">
-        <v>0.02129754000512318</v>
+        <v>0.02156410117042817</v>
       </c>
     </row>
     <row r="59">
@@ -2338,16 +2338,16 @@
         </is>
       </c>
       <c r="E59" t="n">
-        <v>0.2673922278668395</v>
+        <v>0.265832672338759</v>
       </c>
       <c r="F59" t="n">
-        <v>0.05472609466016464</v>
+        <v>0.0544804011140976</v>
       </c>
       <c r="G59" t="n">
-        <v>4.886009672760177</v>
+        <v>4.879418412818762</v>
       </c>
       <c r="H59" t="n">
-        <v>1.029001449825984e-06</v>
+        <v>1.063991259098174e-06</v>
       </c>
     </row>
     <row r="60">
@@ -2408,16 +2408,16 @@
         </is>
       </c>
       <c r="E61" t="n">
-        <v>0.3733717181608778</v>
+        <v>0.3736337054327856</v>
       </c>
       <c r="F61" t="n">
-        <v>0.09501016037205096</v>
+        <v>0.09506487230165046</v>
       </c>
       <c r="G61" t="n">
-        <v>3.929808314130394</v>
+        <v>3.930302501677778</v>
       </c>
       <c r="H61" t="n">
-        <v>8.501360643431433e-05</v>
+        <v>8.483905640277456e-05</v>
       </c>
     </row>
     <row r="62">
@@ -2440,16 +2440,16 @@
         </is>
       </c>
       <c r="E62" t="n">
-        <v>0.1139296067234791</v>
+        <v>0.1138770845241973</v>
       </c>
       <c r="F62" t="n">
-        <v>0.06147169039748996</v>
+        <v>0.06150223058059603</v>
       </c>
       <c r="G62" t="n">
-        <v>1.853367070027373</v>
+        <v>1.851592754397984</v>
       </c>
       <c r="H62" t="n">
-        <v>0.063829763884093</v>
+        <v>0.06408432428014277</v>
       </c>
     </row>
     <row r="63">
@@ -2472,13 +2472,13 @@
         </is>
       </c>
       <c r="E63" t="n">
-        <v>-2.694261553652603</v>
+        <v>-2.696439807135325</v>
       </c>
       <c r="F63" t="n">
-        <v>0.2270300725544502</v>
+        <v>0.2272762662466292</v>
       </c>
       <c r="G63" t="n">
-        <v>-11.86742145358101</v>
+        <v>-11.8641504089011</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
@@ -2504,13 +2504,13 @@
         </is>
       </c>
       <c r="E64" t="n">
-        <v>-3.091722457097386</v>
+        <v>-3.092861130431471</v>
       </c>
       <c r="F64" t="n">
-        <v>0.2456419183040371</v>
+        <v>0.2458397665694307</v>
       </c>
       <c r="G64" t="n">
-        <v>-12.58629829318503</v>
+        <v>-12.58080079385935</v>
       </c>
       <c r="H64" t="n">
         <v>0</v>
@@ -2536,13 +2536,13 @@
         </is>
       </c>
       <c r="E65" t="n">
-        <v>-2.979227682358041</v>
+        <v>-2.979601123185316</v>
       </c>
       <c r="F65" t="n">
-        <v>0.2397439374820822</v>
+        <v>0.2398900944958562</v>
       </c>
       <c r="G65" t="n">
-        <v>-12.42670706769498</v>
+        <v>-12.42069260689863</v>
       </c>
       <c r="H65" t="n">
         <v>0</v>
@@ -2568,13 +2568,13 @@
         </is>
       </c>
       <c r="E66" t="n">
-        <v>-3.606334119257016</v>
+        <v>-3.607892330061275</v>
       </c>
       <c r="F66" t="n">
-        <v>0.2766795248998795</v>
+        <v>0.2769224797453921</v>
       </c>
       <c r="G66" t="n">
-        <v>-13.03433682181212</v>
+        <v>-13.02852817642473</v>
       </c>
       <c r="H66" t="n">
         <v>0</v>
@@ -2600,13 +2600,13 @@
         </is>
       </c>
       <c r="E67" t="n">
-        <v>-3.440051779228314</v>
+        <v>-3.441654915979364</v>
       </c>
       <c r="F67" t="n">
-        <v>0.2658395620352256</v>
+        <v>0.2660800449841673</v>
       </c>
       <c r="G67" t="n">
-        <v>-12.94033044923368</v>
+        <v>-12.93466000492904</v>
       </c>
       <c r="H67" t="n">
         <v>0</v>
@@ -2632,13 +2632,13 @@
         </is>
       </c>
       <c r="E68" t="n">
-        <v>-3.362822128788456</v>
+        <v>-3.364559307110065</v>
       </c>
       <c r="F68" t="n">
-        <v>0.2606626214575626</v>
+        <v>0.2609077073096849</v>
       </c>
       <c r="G68" t="n">
-        <v>-12.90105236405383</v>
+        <v>-12.8955918619284</v>
       </c>
       <c r="H68" t="n">
         <v>0</v>
@@ -2664,13 +2664,13 @@
         </is>
       </c>
       <c r="E69" t="n">
-        <v>-2.90333652365716</v>
+        <v>-2.904678044340603</v>
       </c>
       <c r="F69" t="n">
-        <v>0.2494335750552143</v>
+        <v>0.249643205786847</v>
       </c>
       <c r="G69" t="n">
-        <v>-11.63971820154059</v>
+        <v>-11.63531783360077</v>
       </c>
       <c r="H69" t="n">
         <v>0</v>
@@ -2696,13 +2696,13 @@
         </is>
       </c>
       <c r="E70" t="n">
-        <v>-2.921211204167461</v>
+        <v>-2.923354494201891</v>
       </c>
       <c r="F70" t="n">
-        <v>0.2389982030305541</v>
+        <v>0.239251241287325</v>
       </c>
       <c r="G70" t="n">
-        <v>-12.2227329206395</v>
+        <v>-12.21876416799408</v>
       </c>
       <c r="H70" t="n">
         <v>0</v>
@@ -2728,13 +2728,13 @@
         </is>
       </c>
       <c r="E71" t="n">
-        <v>-3.376544661573007</v>
+        <v>-3.378314231896166</v>
       </c>
       <c r="F71" t="n">
-        <v>0.2643879578341175</v>
+        <v>0.2646358926866988</v>
       </c>
       <c r="G71" t="n">
-        <v>-12.77117418365457</v>
+        <v>-12.76589580341988</v>
       </c>
       <c r="H71" t="n">
         <v>0</v>
@@ -2760,13 +2760,13 @@
         </is>
       </c>
       <c r="E72" t="n">
-        <v>-2.115910372998708</v>
+        <v>-2.116846368118191</v>
       </c>
       <c r="F72" t="n">
-        <v>0.2098320298798729</v>
+        <v>0.2099888494080342</v>
       </c>
       <c r="G72" t="n">
-        <v>-10.08382930956711</v>
+        <v>-10.08075606907497</v>
       </c>
       <c r="H72" t="n">
         <v>0</v>
@@ -2792,13 +2792,13 @@
         </is>
       </c>
       <c r="E73" t="n">
-        <v>-1.102626676026867</v>
+        <v>-1.1039803472652</v>
       </c>
       <c r="F73" t="n">
-        <v>0.127608811274748</v>
+        <v>0.1277319044760435</v>
       </c>
       <c r="G73" t="n">
-        <v>-8.640678218091207</v>
+        <v>-8.642949087662055</v>
       </c>
       <c r="H73" t="n">
         <v>0</v>
@@ -2824,13 +2824,13 @@
         </is>
       </c>
       <c r="E74" t="n">
-        <v>-1.640561519863819</v>
+        <v>-1.64151213650257</v>
       </c>
       <c r="F74" t="n">
-        <v>0.1570740525435081</v>
+        <v>0.1572051537165383</v>
       </c>
       <c r="G74" t="n">
-        <v>-10.44451004661609</v>
+        <v>-10.44184683316421</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -2856,13 +2856,13 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>-1.384249198602611</v>
+        <v>-1.384652555432732</v>
       </c>
       <c r="F75" t="n">
-        <v>0.1582458821945364</v>
+        <v>0.1583453137443888</v>
       </c>
       <c r="G75" t="n">
-        <v>-8.747457939487896</v>
+        <v>-8.74451237413431</v>
       </c>
       <c r="H75" t="n">
         <v>0</v>
@@ -2888,13 +2888,13 @@
         </is>
       </c>
       <c r="E76" t="n">
-        <v>-2.334800861789402</v>
+        <v>-2.335696184774006</v>
       </c>
       <c r="F76" t="n">
-        <v>0.2092444005897471</v>
+        <v>0.2094016817049277</v>
       </c>
       <c r="G76" t="n">
-        <v>-11.1582477485548</v>
+        <v>-11.15414243928628</v>
       </c>
       <c r="H76" t="n">
         <v>0</v>
@@ -2920,13 +2920,13 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>-1.924877212734209</v>
+        <v>-1.926647181222542</v>
       </c>
       <c r="F77" t="n">
-        <v>0.1822912215466329</v>
+        <v>0.1824774295040445</v>
       </c>
       <c r="G77" t="n">
-        <v>-10.55935220792426</v>
+        <v>-10.55827663973796</v>
       </c>
       <c r="H77" t="n">
         <v>0</v>
@@ -2952,13 +2952,13 @@
         </is>
       </c>
       <c r="E78" t="n">
-        <v>-2.078384850757647</v>
+        <v>-2.079398264587354</v>
       </c>
       <c r="F78" t="n">
-        <v>0.1829459773350342</v>
+        <v>0.1830968926179961</v>
       </c>
       <c r="G78" t="n">
-        <v>-11.36064799577463</v>
+        <v>-11.35681897624743</v>
       </c>
       <c r="H78" t="n">
         <v>0</v>
@@ -2984,13 +2984,13 @@
         </is>
       </c>
       <c r="E79" t="n">
-        <v>-1.997288779949946</v>
+        <v>-1.998889277742667</v>
       </c>
       <c r="F79" t="n">
-        <v>0.1963989493852614</v>
+        <v>0.1965813390608637</v>
       </c>
       <c r="G79" t="n">
-        <v>-10.16954920681293</v>
+        <v>-10.16825547776751</v>
       </c>
       <c r="H79" t="n">
         <v>0</v>
@@ -3016,13 +3016,13 @@
         </is>
       </c>
       <c r="E80" t="n">
-        <v>-1.554840585481027</v>
+        <v>-1.555553502061829</v>
       </c>
       <c r="F80" t="n">
-        <v>0.1957896409051346</v>
+        <v>0.1959208724594057</v>
       </c>
       <c r="G80" t="n">
-        <v>-7.941383304474458</v>
+        <v>-7.939702812298349</v>
       </c>
       <c r="H80" t="n">
         <v>1.998401444325282e-15</v>
@@ -3048,13 +3048,13 @@
         </is>
       </c>
       <c r="E81" t="n">
-        <v>-1.688753162342394</v>
+        <v>-1.689861259701232</v>
       </c>
       <c r="F81" t="n">
-        <v>0.1795317971656285</v>
+        <v>0.1796807560718206</v>
       </c>
       <c r="G81" t="n">
-        <v>-9.406429328922805</v>
+        <v>-9.404798246821541</v>
       </c>
       <c r="H81" t="n">
         <v>0</v>
@@ -3080,16 +3080,16 @@
         </is>
       </c>
       <c r="E82" t="n">
-        <v>-0.002692990479857126</v>
+        <v>-0.00277868430123764</v>
       </c>
       <c r="F82" t="n">
-        <v>0.1010716409445606</v>
+        <v>0.1011240315037278</v>
       </c>
       <c r="G82" t="n">
-        <v>-0.02664437279006512</v>
+        <v>-0.02747798183963551</v>
       </c>
       <c r="H82" t="n">
-        <v>0.9787433814406084</v>
+        <v>0.9780785011623763</v>
       </c>
     </row>
     <row r="83">
@@ -3150,13 +3150,13 @@
         </is>
       </c>
       <c r="E84" t="n">
-        <v>1.089787062174687</v>
+        <v>1.090063497198842</v>
       </c>
       <c r="F84" t="n">
-        <v>0.05207707624140506</v>
+        <v>0.05209942640687746</v>
       </c>
       <c r="G84" t="n">
-        <v>20.92642561387308</v>
+        <v>20.92275428648528</v>
       </c>
       <c r="H84" t="n">
         <v>0</v>
@@ -3182,13 +3182,13 @@
         </is>
       </c>
       <c r="E85" t="n">
-        <v>0.9477446824829582</v>
+        <v>0.9479740397710711</v>
       </c>
       <c r="F85" t="n">
-        <v>0.05181609824245388</v>
+        <v>0.05183638206095197</v>
       </c>
       <c r="G85" t="n">
-        <v>18.29054511264152</v>
+        <v>18.28781257608035</v>
       </c>
       <c r="H85" t="n">
         <v>0</v>
@@ -3214,13 +3214,13 @@
         </is>
       </c>
       <c r="E86" t="n">
-        <v>0.9655770741187069</v>
+        <v>0.9658099081045293</v>
       </c>
       <c r="F86" t="n">
-        <v>0.05069511947084018</v>
+        <v>0.05071548820406841</v>
       </c>
       <c r="G86" t="n">
-        <v>19.04674619920878</v>
+        <v>19.04368748653805</v>
       </c>
       <c r="H86" t="n">
         <v>0</v>
@@ -3246,13 +3246,13 @@
         </is>
       </c>
       <c r="E87" t="n">
-        <v>1.23378853010534</v>
+        <v>1.234150009022377</v>
       </c>
       <c r="F87" t="n">
-        <v>0.05335357875001427</v>
+        <v>0.05337863194324964</v>
       </c>
       <c r="G87" t="n">
-        <v>23.12475674524242</v>
+        <v>23.12067514790119</v>
       </c>
       <c r="H87" t="n">
         <v>0</v>
@@ -3278,13 +3278,13 @@
         </is>
       </c>
       <c r="E88" t="n">
-        <v>1.380388051013261</v>
+        <v>1.38078478946746</v>
       </c>
       <c r="F88" t="n">
-        <v>0.05832003994283823</v>
+        <v>0.05834771289508298</v>
       </c>
       <c r="G88" t="n">
-        <v>23.66918905306931</v>
+        <v>23.66476286614064</v>
       </c>
       <c r="H88" t="n">
         <v>0</v>
@@ -3310,13 +3310,13 @@
         </is>
       </c>
       <c r="E89" t="n">
-        <v>0.928637620655411</v>
+        <v>0.9289124831245198</v>
       </c>
       <c r="F89" t="n">
-        <v>0.05742541233351071</v>
+        <v>0.05744915565337803</v>
       </c>
       <c r="G89" t="n">
-        <v>16.17119639030143</v>
+        <v>16.16929739947762</v>
       </c>
       <c r="H89" t="n">
         <v>0</v>
@@ -3342,13 +3342,13 @@
         </is>
       </c>
       <c r="E90" t="n">
-        <v>-0.9470882174569597</v>
+        <v>-0.9473613349302976</v>
       </c>
       <c r="F90" t="n">
-        <v>0.04686577399852834</v>
+        <v>0.04688550490025854</v>
       </c>
       <c r="G90" t="n">
-        <v>-20.20852610833849</v>
+        <v>-20.20584692274195</v>
       </c>
       <c r="H90" t="n">
         <v>0</v>
@@ -3374,13 +3374,13 @@
         </is>
       </c>
       <c r="E91" t="n">
-        <v>0.9474539364468894</v>
+        <v>0.9477558870595876</v>
       </c>
       <c r="F91" t="n">
-        <v>0.05127621425367996</v>
+        <v>0.05129759028586361</v>
       </c>
       <c r="G91" t="n">
-        <v>18.47745490220967</v>
+        <v>18.47564148256474</v>
       </c>
       <c r="H91" t="n">
         <v>0</v>
@@ -3406,13 +3406,13 @@
         </is>
       </c>
       <c r="E92" t="n">
-        <v>-0.9498616302455668</v>
+        <v>-0.9501319190949333</v>
       </c>
       <c r="F92" t="n">
-        <v>0.04815461587553418</v>
+        <v>0.04817464045982492</v>
       </c>
       <c r="G92" t="n">
-        <v>-19.72524571021313</v>
+        <v>-19.7226571907178</v>
       </c>
       <c r="H92" t="n">
         <v>0</v>
@@ -3438,13 +3438,13 @@
         </is>
       </c>
       <c r="E93" t="n">
-        <v>1.005586992841631</v>
+        <v>1.005897143401007</v>
       </c>
       <c r="F93" t="n">
-        <v>0.04750249381957659</v>
+        <v>0.04752370655154801</v>
       </c>
       <c r="G93" t="n">
-        <v>21.16914106951669</v>
+        <v>21.16621821761239</v>
       </c>
       <c r="H93" t="n">
         <v>0</v>
@@ -3470,13 +3470,13 @@
         </is>
       </c>
       <c r="E94" t="n">
-        <v>1.094109737718499</v>
+        <v>1.094411829823669</v>
       </c>
       <c r="F94" t="n">
-        <v>0.0543863198494464</v>
+        <v>0.05440942659711717</v>
       </c>
       <c r="G94" t="n">
-        <v>20.11737033737757</v>
+        <v>20.11437903779602</v>
       </c>
       <c r="H94" t="n">
         <v>0</v>
@@ -3502,13 +3502,13 @@
         </is>
       </c>
       <c r="E95" t="n">
-        <v>1.019441737615381</v>
+        <v>1.019779347088995</v>
       </c>
       <c r="F95" t="n">
-        <v>0.04974759807300198</v>
+        <v>0.0497691811647229</v>
       </c>
       <c r="G95" t="n">
-        <v>20.49228057400705</v>
+        <v>20.49017731863627</v>
       </c>
       <c r="H95" t="n">
         <v>0</v>
@@ -3534,13 +3534,13 @@
         </is>
       </c>
       <c r="E96" t="n">
-        <v>1.197907310374674</v>
+        <v>1.198288140065035</v>
       </c>
       <c r="F96" t="n">
-        <v>0.05170320759980154</v>
+        <v>0.05172767554160178</v>
       </c>
       <c r="G96" t="n">
-        <v>23.16891670674806</v>
+        <v>23.16531967646896</v>
       </c>
       <c r="H96" t="n">
         <v>0</v>
@@ -3566,13 +3566,13 @@
         </is>
       </c>
       <c r="E97" t="n">
-        <v>0.9404105427116408</v>
+        <v>0.9407509020578114</v>
       </c>
       <c r="F97" t="n">
-        <v>0.05073281445721003</v>
+        <v>0.05075449174494279</v>
       </c>
       <c r="G97" t="n">
-        <v>18.53653405107816</v>
+        <v>18.53532307577512</v>
       </c>
       <c r="H97" t="n">
         <v>0</v>
@@ -3598,13 +3598,13 @@
         </is>
       </c>
       <c r="E98" t="n">
-        <v>0.9532753125288226</v>
+        <v>0.9535841793225448</v>
       </c>
       <c r="F98" t="n">
-        <v>0.04613637398941792</v>
+        <v>0.04615658121434531</v>
       </c>
       <c r="G98" t="n">
-        <v>20.66212036357276</v>
+        <v>20.65976626114402</v>
       </c>
       <c r="H98" t="n">
         <v>0</v>
@@ -3630,13 +3630,13 @@
         </is>
       </c>
       <c r="E99" t="n">
-        <v>0.8144291359294661</v>
+        <v>0.8146394215022433</v>
       </c>
       <c r="F99" t="n">
-        <v>0.04217008688314577</v>
+        <v>0.04218753846877193</v>
       </c>
       <c r="G99" t="n">
-        <v>19.31295845244412</v>
+        <v>19.30995386436082</v>
       </c>
       <c r="H99" t="n">
         <v>0</v>
@@ -3662,16 +3662,16 @@
         </is>
       </c>
       <c r="E100" t="n">
-        <v>0.01002652522661394</v>
+        <v>0.01008238770382181</v>
       </c>
       <c r="F100" t="n">
-        <v>0.002712599916812423</v>
+        <v>0.002713778206096709</v>
       </c>
       <c r="G100" t="n">
-        <v>3.69627867374553</v>
+        <v>3.715258556301948</v>
       </c>
       <c r="H100" t="n">
-        <v>0.000218782816912011</v>
+        <v>0.000202996017306889</v>
       </c>
     </row>
     <row r="101">
@@ -3694,16 +3694,16 @@
         </is>
       </c>
       <c r="E101" t="n">
-        <v>0.05217338187963556</v>
+        <v>0.05212081046978243</v>
       </c>
       <c r="F101" t="n">
-        <v>0.007645494163199063</v>
+        <v>0.007641412337464813</v>
       </c>
       <c r="G101" t="n">
-        <v>6.824069283048261</v>
+        <v>6.820834704524489</v>
       </c>
       <c r="H101" t="n">
-        <v>8.849809773892048e-12</v>
+        <v>9.051204230559051e-12</v>
       </c>
     </row>
     <row r="102">
@@ -3726,13 +3726,13 @@
         </is>
       </c>
       <c r="E102" t="n">
-        <v>-0.06421116759788674</v>
+        <v>-0.06416690975037607</v>
       </c>
       <c r="F102" t="n">
-        <v>0.006983793051517376</v>
+        <v>0.006979736388850911</v>
       </c>
       <c r="G102" t="n">
-        <v>-9.194311331253036</v>
+        <v>-9.193314212221516</v>
       </c>
       <c r="H102" t="n">
         <v>0</v>
@@ -3758,13 +3758,13 @@
         </is>
       </c>
       <c r="E103" t="n">
-        <v>0.2208076874374098</v>
+        <v>0.2206752255185965</v>
       </c>
       <c r="F103" t="n">
-        <v>0.0172747208944877</v>
+        <v>0.01726834997544978</v>
       </c>
       <c r="G103" t="n">
-        <v>12.78212764034217</v>
+        <v>12.77917263777656</v>
       </c>
       <c r="H103" t="n">
         <v>0</v>
@@ -3790,16 +3790,16 @@
         </is>
       </c>
       <c r="E104" t="n">
-        <v>0.01674755367294831</v>
+        <v>0.01695994089301799</v>
       </c>
       <c r="F104" t="n">
-        <v>0.008232116737245151</v>
+        <v>0.008284249348133486</v>
       </c>
       <c r="G104" t="n">
-        <v>2.034416445425482</v>
+        <v>2.04725137767515</v>
       </c>
       <c r="H104" t="n">
-        <v>0.04190962513894836</v>
+        <v>0.04063340922770342</v>
       </c>
     </row>
     <row r="105">
@@ -3822,16 +3822,16 @@
         </is>
       </c>
       <c r="E105" t="n">
-        <v>0.02615480399155708</v>
+        <v>0.02613503407073218</v>
       </c>
       <c r="F105" t="n">
-        <v>0.006946478365798096</v>
+        <v>0.006940900472525304</v>
       </c>
       <c r="G105" t="n">
-        <v>3.765189008083366</v>
+        <v>3.765366492491732</v>
       </c>
       <c r="H105" t="n">
-        <v>0.0001664231447682241</v>
+        <v>0.0001663049671845052</v>
       </c>
     </row>
     <row r="106">
@@ -3854,16 +3854,16 @@
         </is>
       </c>
       <c r="E106" t="n">
-        <v>3.314377376839963e-17</v>
+        <v>0</v>
       </c>
       <c r="F106" t="n">
-        <v>0.006972816388456252</v>
+        <v>0.007015256165930648</v>
       </c>
       <c r="G106" t="n">
-        <v>4.753283596928933e-15</v>
+        <v>0</v>
       </c>
       <c r="H106" t="n">
-        <v>0.9999999999999962</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -3886,13 +3886,13 @@
         </is>
       </c>
       <c r="E107" t="n">
-        <v>0.1466722006753863</v>
+        <v>0.1465629875818042</v>
       </c>
       <c r="F107" t="n">
-        <v>0.01169675191259976</v>
+        <v>0.01169123509790504</v>
       </c>
       <c r="G107" t="n">
-        <v>12.53956668986466</v>
+        <v>12.53614236151412</v>
       </c>
       <c r="H107" t="n">
         <v>0</v>
@@ -3918,13 +3918,13 @@
         </is>
       </c>
       <c r="E108" t="n">
-        <v>1.326261134820139</v>
+        <v>1.326154372395091</v>
       </c>
       <c r="F108" t="n">
-        <v>0.04830957613120607</v>
+        <v>0.04830685757628697</v>
       </c>
       <c r="G108" t="n">
-        <v>27.45337966101453</v>
+        <v>27.45271456072989</v>
       </c>
       <c r="H108" t="n">
         <v>0</v>
@@ -3950,13 +3950,13 @@
         </is>
       </c>
       <c r="E109" t="n">
-        <v>1.783935049385091</v>
+        <v>1.784080286875853</v>
       </c>
       <c r="F109" t="n">
-        <v>0.064961044849039</v>
+        <v>0.06496602478507055</v>
       </c>
       <c r="G109" t="n">
-        <v>27.46161262497026</v>
+        <v>27.46174316114814</v>
       </c>
       <c r="H109" t="n">
         <v>0</v>
@@ -3982,13 +3982,13 @@
         </is>
       </c>
       <c r="E110" t="n">
-        <v>1.856525327800934</v>
+        <v>1.856702000554365</v>
       </c>
       <c r="F110" t="n">
-        <v>0.06749999205134055</v>
+        <v>0.06750639713166819</v>
       </c>
       <c r="G110" t="n">
-        <v>27.50408216880018</v>
+        <v>27.50408967768562</v>
       </c>
       <c r="H110" t="n">
         <v>0</v>
@@ -4014,13 +4014,13 @@
         </is>
       </c>
       <c r="E111" t="n">
-        <v>1.49721288477156</v>
+        <v>1.497275057246745</v>
       </c>
       <c r="F111" t="n">
-        <v>0.05451392619321982</v>
+        <v>0.05451614058958663</v>
       </c>
       <c r="G111" t="n">
-        <v>27.46477807225545</v>
+        <v>27.46480291939964</v>
       </c>
       <c r="H111" t="n">
         <v>0</v>
@@ -4046,13 +4046,13 @@
         </is>
       </c>
       <c r="E112" t="n">
-        <v>0.6995077301493985</v>
+        <v>0.6995209815129506</v>
       </c>
       <c r="F112" t="n">
-        <v>0.0254537227779645</v>
+        <v>0.02545428407591872</v>
       </c>
       <c r="G112" t="n">
-        <v>27.4815490144132</v>
+        <v>27.48146360742701</v>
       </c>
       <c r="H112" t="n">
         <v>0</v>
@@ -4078,13 +4078,13 @@
         </is>
       </c>
       <c r="E113" t="n">
-        <v>1.508322590710204</v>
+        <v>1.508391397954608</v>
       </c>
       <c r="F113" t="n">
-        <v>0.05483909969589635</v>
+        <v>0.05484159789415468</v>
       </c>
       <c r="G113" t="n">
-        <v>27.50451045051654</v>
+        <v>27.50451219233852</v>
       </c>
       <c r="H113" t="n">
         <v>0</v>
@@ -4110,13 +4110,13 @@
         </is>
       </c>
       <c r="E114" t="n">
-        <v>0.6709598544811164</v>
+        <v>0.6709534574515967</v>
       </c>
       <c r="F114" t="n">
-        <v>0.02439785219693193</v>
+        <v>0.02439763506374823</v>
       </c>
       <c r="G114" t="n">
-        <v>27.50077543866709</v>
+        <v>27.50075799031223</v>
       </c>
       <c r="H114" t="n">
         <v>0</v>
@@ -4142,13 +4142,13 @@
         </is>
       </c>
       <c r="E115" t="n">
-        <v>1.463015446025288</v>
+        <v>1.463122212020547</v>
       </c>
       <c r="F115" t="n">
-        <v>0.05339371565580293</v>
+        <v>0.05339801370686854</v>
       </c>
       <c r="G115" t="n">
-        <v>27.40051760827183</v>
+        <v>27.40031155512713</v>
       </c>
       <c r="H115" t="n">
         <v>0</v>
@@ -4174,13 +4174,13 @@
         </is>
       </c>
       <c r="E116" t="n">
-        <v>0.4292886057093184</v>
+        <v>0.4293155643818575</v>
       </c>
       <c r="F116" t="n">
-        <v>0.01677034960897796</v>
+        <v>0.01677057996700266</v>
       </c>
       <c r="G116" t="n">
-        <v>25.59807133978303</v>
+        <v>25.59932722666527</v>
       </c>
       <c r="H116" t="n">
         <v>0</v>
@@ -4206,13 +4206,13 @@
         </is>
       </c>
       <c r="E117" t="n">
-        <v>0.2590392178738499</v>
+        <v>0.2590356807181278</v>
       </c>
       <c r="F117" t="n">
-        <v>0.01111870140864099</v>
+        <v>0.01111859860640905</v>
       </c>
       <c r="G117" t="n">
-        <v>23.29761438230887</v>
+        <v>23.29751166172285</v>
       </c>
       <c r="H117" t="n">
         <v>0</v>
@@ -4238,13 +4238,13 @@
         </is>
       </c>
       <c r="E118" t="n">
-        <v>0.4402170116097489</v>
+        <v>0.4402301625046139</v>
       </c>
       <c r="F118" t="n">
-        <v>0.01736624777468091</v>
+        <v>0.01736675308100399</v>
       </c>
       <c r="G118" t="n">
-        <v>25.34899981251064</v>
+        <v>25.34901949868771</v>
       </c>
       <c r="H118" t="n">
         <v>0</v>
@@ -4270,13 +4270,13 @@
         </is>
       </c>
       <c r="E119" t="n">
-        <v>0.5501920397785477</v>
+        <v>0.5502285578674604</v>
       </c>
       <c r="F119" t="n">
-        <v>0.02135494847914821</v>
+        <v>0.02135547524730159</v>
       </c>
       <c r="G119" t="n">
-        <v>25.76414737268096</v>
+        <v>25.7652218679245</v>
       </c>
       <c r="H119" t="n">
         <v>0</v>
@@ -4302,13 +4302,13 @@
         </is>
       </c>
       <c r="E120" t="n">
-        <v>0.722746764864478</v>
+        <v>0.722774580284951</v>
       </c>
       <c r="F120" t="n">
-        <v>0.02787151626282019</v>
+        <v>0.02787245135258055</v>
       </c>
       <c r="G120" t="n">
-        <v>25.93137589011152</v>
+        <v>25.93150387513734</v>
       </c>
       <c r="H120" t="n">
         <v>0</v>
@@ -4334,13 +4334,13 @@
         </is>
       </c>
       <c r="E121" t="n">
-        <v>0.8722576988109796</v>
+        <v>0.8722803744906523</v>
       </c>
       <c r="F121" t="n">
-        <v>0.03289131827899488</v>
+        <v>0.03289206074173816</v>
       </c>
       <c r="G121" t="n">
-        <v>26.51939005258732</v>
+        <v>26.51948083499853</v>
       </c>
       <c r="H121" t="n">
         <v>0</v>
@@ -4366,13 +4366,13 @@
         </is>
       </c>
       <c r="E122" t="n">
-        <v>0.79397657182366</v>
+        <v>0.7940045812891783</v>
       </c>
       <c r="F122" t="n">
-        <v>0.03009658120390395</v>
+        <v>0.03009751065256093</v>
       </c>
       <c r="G122" t="n">
-        <v>26.38095557824652</v>
+        <v>26.38107152543651</v>
       </c>
       <c r="H122" t="n">
         <v>0</v>
@@ -4398,13 +4398,13 @@
         </is>
       </c>
       <c r="E123" t="n">
-        <v>0.3516515670638951</v>
+        <v>0.3516518322004149</v>
       </c>
       <c r="F123" t="n">
-        <v>0.01303121443819155</v>
+        <v>0.0130309816789462</v>
       </c>
       <c r="G123" t="n">
-        <v>26.98532578869229</v>
+        <v>26.98582814689881</v>
       </c>
       <c r="H123" t="n">
         <v>0</v>
@@ -4430,13 +4430,13 @@
         </is>
       </c>
       <c r="E124" t="n">
-        <v>0.2363739064133579</v>
+        <v>0.2363663017634986</v>
       </c>
       <c r="F124" t="n">
-        <v>0.01106841863358573</v>
+        <v>0.01109497654228807</v>
       </c>
       <c r="G124" t="n">
-        <v>21.35570709936423</v>
+        <v>21.30390279252</v>
       </c>
       <c r="H124" t="n">
         <v>0</v>
@@ -4462,13 +4462,13 @@
         </is>
       </c>
       <c r="E125" t="n">
-        <v>0.6420204403183132</v>
+        <v>0.6420116558450213</v>
       </c>
       <c r="F125" t="n">
-        <v>0.02354466442001833</v>
+        <v>0.02354448368911488</v>
       </c>
       <c r="G125" t="n">
-        <v>27.26819243790883</v>
+        <v>27.2680286514233</v>
       </c>
       <c r="H125" t="n">
         <v>0</v>
@@ -4494,13 +4494,13 @@
         </is>
       </c>
       <c r="E126" t="n">
-        <v>0.7189270485495847</v>
+        <v>0.7189389646863935</v>
       </c>
       <c r="F126" t="n">
-        <v>0.02648223785700905</v>
+        <v>0.02648212992206924</v>
       </c>
       <c r="G126" t="n">
-        <v>27.14751874083628</v>
+        <v>27.14807935671775</v>
       </c>
       <c r="H126" t="n">
         <v>0</v>
@@ -4526,13 +4526,13 @@
         </is>
       </c>
       <c r="E127" t="n">
-        <v>0.9103281273221108</v>
+        <v>0.9103441918181352</v>
       </c>
       <c r="F127" t="n">
-        <v>0.03332770050926376</v>
+        <v>0.03332898111088946</v>
       </c>
       <c r="G127" t="n">
-        <v>27.31445954519909</v>
+        <v>27.31389203774333</v>
       </c>
       <c r="H127" t="n">
         <v>0</v>
@@ -4558,13 +4558,13 @@
         </is>
       </c>
       <c r="E128" t="n">
-        <v>0.5914643809627651</v>
+        <v>0.5914724311757752</v>
       </c>
       <c r="F128" t="n">
-        <v>0.02170780099900126</v>
+        <v>0.02170804144371578</v>
       </c>
       <c r="G128" t="n">
-        <v>27.24662811137484</v>
+        <v>27.24669715976394</v>
       </c>
       <c r="H128" t="n">
         <v>0</v>
@@ -4590,13 +4590,13 @@
         </is>
       </c>
       <c r="E129" t="n">
-        <v>0.4176628749579965</v>
+        <v>0.4176480039797151</v>
       </c>
       <c r="F129" t="n">
-        <v>0.01708441341961174</v>
+        <v>0.01708405863462072</v>
       </c>
       <c r="G129" t="n">
-        <v>24.44701288099836</v>
+        <v>24.44665011327624</v>
       </c>
       <c r="H129" t="n">
         <v>0</v>
@@ -4622,13 +4622,13 @@
         </is>
       </c>
       <c r="E130" t="n">
-        <v>0.5501335482016469</v>
+        <v>0.5501129941773252</v>
       </c>
       <c r="F130" t="n">
-        <v>0.0211938688711211</v>
+        <v>0.02119325995651558</v>
       </c>
       <c r="G130" t="n">
-        <v>25.95720260047967</v>
+        <v>25.95697855261967</v>
       </c>
       <c r="H130" t="n">
         <v>0</v>
@@ -4654,13 +4654,13 @@
         </is>
       </c>
       <c r="E131" t="n">
-        <v>0.5960619876026261</v>
+        <v>0.5960387390975855</v>
       </c>
       <c r="F131" t="n">
-        <v>0.02241848583224864</v>
+        <v>0.02241847685640763</v>
       </c>
       <c r="G131" t="n">
-        <v>26.58796816324733</v>
+        <v>26.58694178416673</v>
       </c>
       <c r="H131" t="n">
         <v>0</v>
@@ -4686,13 +4686,13 @@
         </is>
       </c>
       <c r="E132" t="n">
-        <v>0.8675156891678142</v>
+        <v>0.8675147121166908</v>
       </c>
       <c r="F132" t="n">
-        <v>0.0323059648113876</v>
+        <v>0.03230617507217885</v>
       </c>
       <c r="G132" t="n">
-        <v>26.8531119316755</v>
+        <v>26.85290691800023</v>
       </c>
       <c r="H132" t="n">
         <v>0</v>
@@ -4718,13 +4718,13 @@
         </is>
       </c>
       <c r="E133" t="n">
-        <v>0.8073361000617254</v>
+        <v>0.8073154128436526</v>
       </c>
       <c r="F133" t="n">
-        <v>0.02987739595527674</v>
+        <v>0.02987680073071458</v>
       </c>
       <c r="G133" t="n">
-        <v>27.02163539430275</v>
+        <v>27.02148131900474</v>
       </c>
       <c r="H133" t="n">
         <v>0</v>
@@ -4750,13 +4750,13 @@
         </is>
       </c>
       <c r="E134" t="n">
-        <v>0.9023476873854538</v>
+        <v>0.9023387449227733</v>
       </c>
       <c r="F134" t="n">
-        <v>0.03353858865523695</v>
+        <v>0.03353818161606752</v>
       </c>
       <c r="G134" t="n">
-        <v>26.90476026389531</v>
+        <v>26.90482016066056</v>
       </c>
       <c r="H134" t="n">
         <v>0</v>
@@ -4782,13 +4782,13 @@
         </is>
       </c>
       <c r="E135" t="n">
-        <v>0.745376090665137</v>
+        <v>0.7453767307490058</v>
       </c>
       <c r="F135" t="n">
-        <v>0.02879274190699191</v>
+        <v>0.02879291329635829</v>
       </c>
       <c r="G135" t="n">
-        <v>25.88763838633394</v>
+        <v>25.88750652117558</v>
       </c>
       <c r="H135" t="n">
         <v>0</v>
@@ -4814,13 +4814,13 @@
         </is>
       </c>
       <c r="E136" t="n">
-        <v>0.6266385165927064</v>
+        <v>0.6266337395802929</v>
       </c>
       <c r="F136" t="n">
-        <v>0.02322149928985094</v>
+        <v>0.02322153441301407</v>
       </c>
       <c r="G136" t="n">
-        <v>26.98527380786289</v>
+        <v>26.98502727718643</v>
       </c>
       <c r="H136" t="n">
         <v>0</v>
@@ -4846,13 +4846,13 @@
         </is>
       </c>
       <c r="E137" t="n">
-        <v>0.6779411184052242</v>
+        <v>0.6779204703702607</v>
       </c>
       <c r="F137" t="n">
-        <v>0.02636923694138995</v>
+        <v>0.02636832336264643</v>
       </c>
       <c r="G137" t="n">
-        <v>25.70954631286269</v>
+        <v>25.7096540049603</v>
       </c>
       <c r="H137" t="n">
         <v>0</v>
@@ -4878,13 +4878,13 @@
         </is>
       </c>
       <c r="E138" t="n">
-        <v>0.64386214652342</v>
+        <v>0.6438627090183818</v>
       </c>
       <c r="F138" t="n">
-        <v>0.0241374358238425</v>
+        <v>0.02413754790938498</v>
       </c>
       <c r="G138" t="n">
-        <v>26.67483618374867</v>
+        <v>26.67473561974228</v>
       </c>
       <c r="H138" t="n">
         <v>0</v>
@@ -4910,13 +4910,13 @@
         </is>
       </c>
       <c r="E139" t="n">
-        <v>0.6908005396544534</v>
+        <v>0.6908078817434892</v>
       </c>
       <c r="F139" t="n">
-        <v>0.02553050870995842</v>
+        <v>0.02553121018156579</v>
       </c>
       <c r="G139" t="n">
-        <v>27.05784469378561</v>
+        <v>27.05738885089017</v>
       </c>
       <c r="H139" t="n">
         <v>0</v>
@@ -4942,13 +4942,13 @@
         </is>
       </c>
       <c r="E140" t="n">
-        <v>1.044877906192007</v>
+        <v>1.044917619041998</v>
       </c>
       <c r="F140" t="n">
-        <v>0.03820835093124832</v>
+        <v>0.0382096751940762</v>
       </c>
       <c r="G140" t="n">
-        <v>27.34684645366669</v>
+        <v>27.34693801261752</v>
       </c>
       <c r="H140" t="n">
         <v>0</v>
@@ -4974,13 +4974,13 @@
         </is>
       </c>
       <c r="E141" t="n">
-        <v>0.5053200420080647</v>
+        <v>0.5052990567705691</v>
       </c>
       <c r="F141" t="n">
-        <v>0.02048796661127851</v>
+        <v>0.02048773845721157</v>
       </c>
       <c r="G141" t="n">
-        <v>24.66423591813277</v>
+        <v>24.66348629943795</v>
       </c>
       <c r="H141" t="n">
         <v>0</v>
@@ -5006,13 +5006,13 @@
         </is>
       </c>
       <c r="E142" t="n">
-        <v>0.4374036693289233</v>
+        <v>0.4374591178611263</v>
       </c>
       <c r="F142" t="n">
-        <v>0.01788973103217992</v>
+        <v>0.01789082341126246</v>
       </c>
       <c r="G142" t="n">
-        <v>24.44998577774449</v>
+        <v>24.45159218112285</v>
       </c>
       <c r="H142" t="n">
         <v>0</v>
@@ -5038,13 +5038,13 @@
         </is>
       </c>
       <c r="E143" t="n">
-        <v>0.3860963989114594</v>
+        <v>0.3861608202738304</v>
       </c>
       <c r="F143" t="n">
-        <v>0.01541675781855516</v>
+        <v>0.01541770311398974</v>
       </c>
       <c r="G143" t="n">
-        <v>25.04394266489164</v>
+        <v>25.04658556425234</v>
       </c>
       <c r="H143" t="n">
         <v>0</v>
@@ -5070,13 +5070,13 @@
         </is>
       </c>
       <c r="E144" t="n">
-        <v>0.388511220465286</v>
+        <v>0.3885419646505683</v>
       </c>
       <c r="F144" t="n">
-        <v>0.01607750176186945</v>
+        <v>0.01607903963875745</v>
       </c>
       <c r="G144" t="n">
-        <v>24.16489988280033</v>
+        <v>24.16450070126387</v>
       </c>
       <c r="H144" t="n">
         <v>0</v>
@@ -5102,13 +5102,13 @@
         </is>
       </c>
       <c r="E145" t="n">
-        <v>0.6024661962478967</v>
+        <v>0.602458965361732</v>
       </c>
       <c r="F145" t="n">
-        <v>0.02401852701573384</v>
+        <v>0.02401835011198283</v>
       </c>
       <c r="G145" t="n">
-        <v>25.08339482384391</v>
+        <v>25.08327851529153</v>
       </c>
       <c r="H145" t="n">
         <v>0</v>
@@ -5134,13 +5134,13 @@
         </is>
       </c>
       <c r="E146" t="n">
-        <v>0.6706002175398211</v>
+        <v>0.670589668883374</v>
       </c>
       <c r="F146" t="n">
-        <v>0.02706099316857418</v>
+        <v>0.02706068827873644</v>
       </c>
       <c r="G146" t="n">
-        <v>24.78106451369292</v>
+        <v>24.78095390446977</v>
       </c>
       <c r="H146" t="n">
         <v>0</v>
@@ -5166,13 +5166,13 @@
         </is>
       </c>
       <c r="E147" t="n">
-        <v>1.207158257604489</v>
+        <v>1.207280745175909</v>
       </c>
       <c r="F147" t="n">
-        <v>0.04500732607757787</v>
+        <v>0.04501182449999242</v>
       </c>
       <c r="G147" t="n">
-        <v>26.8213724916011</v>
+        <v>26.82141322996785</v>
       </c>
       <c r="H147" t="n">
         <v>0</v>
@@ -5198,13 +5198,13 @@
         </is>
       </c>
       <c r="E148" t="n">
-        <v>0.6219929530068148</v>
+        <v>0.6219822654474819</v>
       </c>
       <c r="F148" t="n">
-        <v>0.02380903080839665</v>
+        <v>0.02380867698242341</v>
       </c>
       <c r="G148" t="n">
-        <v>26.12424495504178</v>
+        <v>26.12418429972114</v>
       </c>
       <c r="H148" t="n">
         <v>0</v>
@@ -5230,13 +5230,13 @@
         </is>
       </c>
       <c r="E149" t="n">
-        <v>0.8439807599152254</v>
+        <v>0.8439884510676571</v>
       </c>
       <c r="F149" t="n">
-        <v>0.03186400210501995</v>
+        <v>0.03186438831960356</v>
       </c>
       <c r="G149" t="n">
-        <v>26.48696661226291</v>
+        <v>26.4868869465143</v>
       </c>
       <c r="H149" t="n">
         <v>0</v>
@@ -5262,13 +5262,13 @@
         </is>
       </c>
       <c r="E150" t="n">
-        <v>0.6819519327279695</v>
+        <v>0.6819480828883202</v>
       </c>
       <c r="F150" t="n">
-        <v>0.02599061009419025</v>
+        <v>0.02599049438418159</v>
       </c>
       <c r="G150" t="n">
-        <v>26.23839649128396</v>
+        <v>26.23836518004563</v>
       </c>
       <c r="H150" t="n">
         <v>0</v>
@@ -5294,13 +5294,13 @@
         </is>
       </c>
       <c r="E151" t="n">
-        <v>0.5883106827624766</v>
+        <v>0.588304239843168</v>
       </c>
       <c r="F151" t="n">
-        <v>0.02275083955325225</v>
+        <v>0.02275070316955462</v>
       </c>
       <c r="G151" t="n">
-        <v>25.8588559494508</v>
+        <v>25.85872776910861</v>
       </c>
       <c r="H151" t="n">
         <v>0</v>
@@ -5326,13 +5326,13 @@
         </is>
       </c>
       <c r="E152" t="n">
-        <v>0.8437745036680143</v>
+        <v>0.8437922782451585</v>
       </c>
       <c r="F152" t="n">
-        <v>0.03227082809134723</v>
+        <v>0.03227147615094197</v>
       </c>
       <c r="G152" t="n">
-        <v>26.14666414054955</v>
+        <v>26.14668985925462</v>
       </c>
       <c r="H152" t="n">
         <v>0</v>
@@ -5358,13 +5358,13 @@
         </is>
       </c>
       <c r="E153" t="n">
-        <v>0.5680732058386033</v>
+        <v>0.568122648428393</v>
       </c>
       <c r="F153" t="n">
-        <v>0.02155887981025</v>
+        <v>0.02156058633121984</v>
       </c>
       <c r="G153" t="n">
-        <v>26.3498479889557</v>
+        <v>26.35005559099283</v>
       </c>
       <c r="H153" t="n">
         <v>0</v>
@@ -5390,13 +5390,13 @@
         </is>
       </c>
       <c r="E154" t="n">
-        <v>0.7298564450047719</v>
+        <v>0.7299057233388319</v>
       </c>
       <c r="F154" t="n">
-        <v>0.02768574508522227</v>
+        <v>0.02768806729615316</v>
       </c>
       <c r="G154" t="n">
-        <v>26.36217456787835</v>
+        <v>26.36174332810436</v>
       </c>
       <c r="H154" t="n">
         <v>0</v>
@@ -5422,13 +5422,13 @@
         </is>
       </c>
       <c r="E155" t="n">
-        <v>0.8230322459809996</v>
+        <v>0.8230882543214093</v>
       </c>
       <c r="F155" t="n">
-        <v>0.0311767198327048</v>
+        <v>0.03117824613131338</v>
       </c>
       <c r="G155" t="n">
-        <v>26.39893646191825</v>
+        <v>26.3994405210739</v>
       </c>
       <c r="H155" t="n">
         <v>0</v>
@@ -5454,13 +5454,13 @@
         </is>
       </c>
       <c r="E156" t="n">
-        <v>2.115041412743845</v>
+        <v>2.115082327396675</v>
       </c>
       <c r="F156" t="n">
-        <v>0.07747398209035748</v>
+        <v>0.07747245003650663</v>
       </c>
       <c r="G156" t="n">
-        <v>27.30002196414512</v>
+        <v>27.3010899535603</v>
       </c>
       <c r="H156" t="n">
         <v>0</v>
@@ -5486,13 +5486,13 @@
         </is>
       </c>
       <c r="E157" t="n">
-        <v>1.157150726052155</v>
+        <v>1.157229426350492</v>
       </c>
       <c r="F157" t="n">
-        <v>0.04211686113123395</v>
+        <v>0.04211917130746829</v>
       </c>
       <c r="G157" t="n">
-        <v>27.47476176866692</v>
+        <v>27.47512333220633</v>
       </c>
       <c r="H157" t="n">
         <v>0</v>
@@ -5518,13 +5518,13 @@
         </is>
       </c>
       <c r="E158" t="n">
-        <v>1.901875839782851</v>
+        <v>1.901872178405749</v>
       </c>
       <c r="F158" t="n">
-        <v>0.06940917873895482</v>
+        <v>0.06940911145467267</v>
       </c>
       <c r="G158" t="n">
-        <v>27.40092699999132</v>
+        <v>27.40090081142095</v>
       </c>
       <c r="H158" t="n">
         <v>0</v>
@@ -5550,13 +5550,13 @@
         </is>
       </c>
       <c r="E159" t="n">
-        <v>0.5827456941782787</v>
+        <v>0.5827642289476045</v>
       </c>
       <c r="F159" t="n">
-        <v>0.02122092702778929</v>
+        <v>0.0212216156313212</v>
       </c>
       <c r="G159" t="n">
-        <v>27.46089713176522</v>
+        <v>27.46087946574793</v>
       </c>
       <c r="H159" t="n">
         <v>0</v>
@@ -5582,13 +5582,13 @@
         </is>
       </c>
       <c r="E160" t="n">
-        <v>0.3344189929444497</v>
+        <v>0.3344311746165434</v>
       </c>
       <c r="F160" t="n">
-        <v>0.01380274111368656</v>
+        <v>0.0138032212255204</v>
       </c>
       <c r="G160" t="n">
-        <v>24.22844782538283</v>
+        <v>24.22848762099053</v>
       </c>
       <c r="H160" t="n">
         <v>0</v>
@@ -5614,13 +5614,13 @@
         </is>
       </c>
       <c r="E161" t="n">
-        <v>0.5391432909317736</v>
+        <v>0.5391664420998231</v>
       </c>
       <c r="F161" t="n">
-        <v>0.02047850000087037</v>
+        <v>0.02047930911966526</v>
       </c>
       <c r="G161" t="n">
-        <v>26.32728426801435</v>
+        <v>26.32737456732665</v>
       </c>
       <c r="H161" t="n">
         <v>0</v>
@@ -5646,13 +5646,13 @@
         </is>
       </c>
       <c r="E162" t="n">
-        <v>0.2212152285581862</v>
+        <v>0.2212195779956147</v>
       </c>
       <c r="F162" t="n">
-        <v>0.01008821542363979</v>
+        <v>0.01008839110959005</v>
       </c>
       <c r="G162" t="n">
-        <v>21.92808333750316</v>
+        <v>21.92813260019178</v>
       </c>
       <c r="H162" t="n">
         <v>0</v>
@@ -5678,13 +5678,13 @@
         </is>
       </c>
       <c r="E163" t="n">
-        <v>1.033838697464558</v>
+        <v>1.033862234922651</v>
       </c>
       <c r="F163" t="n">
-        <v>0.03942775658091074</v>
+        <v>0.03942986685977284</v>
       </c>
       <c r="G163" t="n">
-        <v>26.22108857035195</v>
+        <v>26.22028216765801</v>
       </c>
       <c r="H163" t="n">
         <v>0</v>
@@ -5710,13 +5710,13 @@
         </is>
       </c>
       <c r="E164" t="n">
-        <v>1.495260890803412</v>
+        <v>1.495351971183155</v>
       </c>
       <c r="F164" t="n">
-        <v>0.0554666574341463</v>
+        <v>0.05546987520089493</v>
       </c>
       <c r="G164" t="n">
-        <v>26.9578330468485</v>
+        <v>26.9579112219108</v>
       </c>
       <c r="H164" t="n">
         <v>0</v>
@@ -5742,13 +5742,13 @@
         </is>
       </c>
       <c r="E165" t="n">
-        <v>0.8328405532651444</v>
+        <v>0.8328943412397433</v>
       </c>
       <c r="F165" t="n">
-        <v>0.03278357034677427</v>
+        <v>0.03278488632231547</v>
       </c>
       <c r="G165" t="n">
-        <v>25.40420535134567</v>
+        <v>25.40482626738339</v>
       </c>
       <c r="H165" t="n">
         <v>0</v>
@@ -5774,13 +5774,13 @@
         </is>
       </c>
       <c r="E166" t="n">
-        <v>0.8750718172093689</v>
+        <v>0.8751385943114437</v>
       </c>
       <c r="F166" t="n">
-        <v>0.03411719053478435</v>
+        <v>0.03411783420253711</v>
       </c>
       <c r="G166" t="n">
-        <v>25.64899991667063</v>
+        <v>25.65047327126981</v>
       </c>
       <c r="H166" t="n">
         <v>0</v>
@@ -5806,13 +5806,13 @@
         </is>
       </c>
       <c r="E167" t="n">
-        <v>0.7425063269141935</v>
+        <v>0.7425374164337367</v>
       </c>
       <c r="F167" t="n">
-        <v>0.03056170324874901</v>
+        <v>0.03056239679842891</v>
       </c>
       <c r="G167" t="n">
-        <v>24.29531891094098</v>
+        <v>24.29578482691553</v>
       </c>
       <c r="H167" t="n">
         <v>0</v>
@@ -5838,13 +5838,13 @@
         </is>
       </c>
       <c r="E168" t="n">
-        <v>0.7473253611378311</v>
+        <v>0.7473831133156031</v>
       </c>
       <c r="F168" t="n">
-        <v>0.03037408135536233</v>
+        <v>0.03037602528800283</v>
       </c>
       <c r="G168" t="n">
-        <v>24.60404818074579</v>
+        <v>24.60437487146094</v>
       </c>
       <c r="H168" t="n">
         <v>0</v>
@@ -5870,13 +5870,13 @@
         </is>
       </c>
       <c r="E169" t="n">
-        <v>0.7431880977638249</v>
+        <v>0.7431981792315188</v>
       </c>
       <c r="F169" t="n">
-        <v>0.03006703420020341</v>
+        <v>0.03006762049722465</v>
       </c>
       <c r="G169" t="n">
-        <v>24.7177055372518</v>
+        <v>24.71755885289962</v>
       </c>
       <c r="H169" t="n">
         <v>0</v>
@@ -5902,13 +5902,13 @@
         </is>
       </c>
       <c r="E170" t="n">
-        <v>1.366289140318003</v>
+        <v>1.366456480069261</v>
       </c>
       <c r="F170" t="n">
-        <v>0.05179836754990051</v>
+        <v>0.05180434542135685</v>
       </c>
       <c r="G170" t="n">
-        <v>26.37706948921502</v>
+        <v>26.37725597975704</v>
       </c>
       <c r="H170" t="n">
         <v>0</v>
@@ -5934,13 +5934,13 @@
         </is>
       </c>
       <c r="E171" t="n">
-        <v>0.9718568914384009</v>
+        <v>0.9718512916062787</v>
       </c>
       <c r="F171" t="n">
-        <v>0.03752518844248622</v>
+        <v>0.03752615242564591</v>
       </c>
       <c r="G171" t="n">
-        <v>25.89878776763611</v>
+        <v>25.89797324695093</v>
       </c>
       <c r="H171" t="n">
         <v>0</v>
@@ -5966,13 +5966,13 @@
         </is>
       </c>
       <c r="E172" t="n">
-        <v>0.8478933226839896</v>
+        <v>0.8479036435359056</v>
       </c>
       <c r="F172" t="n">
-        <v>0.03385782273156911</v>
+        <v>0.03385846490363541</v>
       </c>
       <c r="G172" t="n">
-        <v>25.04275981894044</v>
+        <v>25.04258967215678</v>
       </c>
       <c r="H172" t="n">
         <v>0</v>
@@ -5998,13 +5998,13 @@
         </is>
       </c>
       <c r="E173" t="n">
-        <v>1.119813765201637</v>
+        <v>1.119810959028547</v>
       </c>
       <c r="F173" t="n">
-        <v>0.04152157170938502</v>
+        <v>0.04152098405228703</v>
       </c>
       <c r="G173" t="n">
-        <v>26.96944549720788</v>
+        <v>26.96975961820675</v>
       </c>
       <c r="H173" t="n">
         <v>0</v>
@@ -6030,13 +6030,13 @@
         </is>
       </c>
       <c r="E174" t="n">
-        <v>1.515498461901134</v>
+        <v>1.515421726849738</v>
       </c>
       <c r="F174" t="n">
-        <v>0.05579497482917404</v>
+        <v>0.05579329323643694</v>
       </c>
       <c r="G174" t="n">
-        <v>27.16191675888254</v>
+        <v>27.16136006527931</v>
       </c>
       <c r="H174" t="n">
         <v>0</v>
@@ -6062,13 +6062,13 @@
         </is>
       </c>
       <c r="E175" t="n">
-        <v>1.343875751685285</v>
+        <v>1.343900008314496</v>
       </c>
       <c r="F175" t="n">
-        <v>0.04921787584584426</v>
+        <v>0.04922005392216503</v>
       </c>
       <c r="G175" t="n">
-        <v>27.30462720226175</v>
+        <v>27.30391174321732</v>
       </c>
       <c r="H175" t="n">
         <v>0</v>
@@ -6094,13 +6094,13 @@
         </is>
       </c>
       <c r="E176" t="n">
-        <v>1.301542504503784</v>
+        <v>1.301535336052746</v>
       </c>
       <c r="F176" t="n">
-        <v>0.04776266012400215</v>
+        <v>0.04776320712463042</v>
       </c>
       <c r="G176" t="n">
-        <v>27.25020970560369</v>
+        <v>27.24974754373902</v>
       </c>
       <c r="H176" t="n">
         <v>0</v>
@@ -6126,13 +6126,13 @@
         </is>
       </c>
       <c r="E177" t="n">
-        <v>0.7091529492269204</v>
+        <v>0.709141014749191</v>
       </c>
       <c r="F177" t="n">
-        <v>0.02607983984168358</v>
+        <v>0.02607985295578381</v>
       </c>
       <c r="G177" t="n">
-        <v>27.19161442342468</v>
+        <v>27.19114313735928</v>
       </c>
       <c r="H177" t="n">
         <v>0</v>
@@ -6158,13 +6158,13 @@
         </is>
       </c>
       <c r="E178" t="n">
-        <v>1.074048230617214</v>
+        <v>1.074084154481183</v>
       </c>
       <c r="F178" t="n">
-        <v>0.03951772195995498</v>
+        <v>0.03951884611010725</v>
       </c>
       <c r="G178" t="n">
-        <v>27.17890043556698</v>
+        <v>27.17903633778665</v>
       </c>
       <c r="H178" t="n">
         <v>0</v>
@@ -6190,13 +6190,13 @@
         </is>
       </c>
       <c r="E179" t="n">
-        <v>0.7730448957715129</v>
+        <v>0.7730786816968087</v>
       </c>
       <c r="F179" t="n">
-        <v>0.02877115476552315</v>
+        <v>0.02877251330800983</v>
       </c>
       <c r="G179" t="n">
-        <v>26.86874760657831</v>
+        <v>26.8686531966857</v>
       </c>
       <c r="H179" t="n">
         <v>0</v>
@@ -6222,13 +6222,13 @@
         </is>
       </c>
       <c r="E180" t="n">
-        <v>0.2600391472244633</v>
+        <v>0.2600382767879357</v>
       </c>
       <c r="F180" t="n">
-        <v>0.009457537863881697</v>
+        <v>0.009457500306205117</v>
       </c>
       <c r="G180" t="n">
-        <v>27.49543812983889</v>
+        <v>27.49545528323459</v>
       </c>
       <c r="H180" t="n">
         <v>0</v>
@@ -6254,13 +6254,13 @@
         </is>
       </c>
       <c r="E181" t="n">
-        <v>9.657952929075803</v>
+        <v>9.660087808789019</v>
       </c>
       <c r="F181" t="n">
-        <v>0.3522293995669364</v>
+        <v>0.352300139540203</v>
       </c>
       <c r="G181" t="n">
-        <v>27.41949689867674</v>
+        <v>27.42005104332135</v>
       </c>
       <c r="H181" t="n">
         <v>0</v>
@@ -6286,13 +6286,13 @@
         </is>
       </c>
       <c r="E182" t="n">
-        <v>0.1172183401796999</v>
+        <v>0.1172355372066126</v>
       </c>
       <c r="F182" t="n">
-        <v>0.008120105601587385</v>
+        <v>0.008115743263396244</v>
       </c>
       <c r="G182" t="n">
-        <v>14.43556844166527</v>
+        <v>14.44544675543456</v>
       </c>
       <c r="H182" t="n">
         <v>0</v>
@@ -6318,13 +6318,13 @@
         </is>
       </c>
       <c r="E183" t="n">
-        <v>0.02743244679345045</v>
+        <v>0.02743370840845269</v>
       </c>
       <c r="F183" t="n">
-        <v>0.001115277247608761</v>
+        <v>0.001114068944637828</v>
       </c>
       <c r="G183" t="n">
-        <v>24.59697517157346</v>
+        <v>24.62478513189891</v>
       </c>
       <c r="H183" t="n">
         <v>0</v>
@@ -6350,13 +6350,13 @@
         </is>
       </c>
       <c r="E184" t="n">
-        <v>0.8347084576560148</v>
+        <v>0.8347234244909328</v>
       </c>
       <c r="F184" t="n">
-        <v>0.03063233116345429</v>
+        <v>0.03063290477513093</v>
       </c>
       <c r="G184" t="n">
-        <v>27.24926330858584</v>
+        <v>27.24924164362456</v>
       </c>
       <c r="H184" t="n">
         <v>0</v>
@@ -6382,13 +6382,13 @@
         </is>
       </c>
       <c r="E185" t="n">
-        <v>0.6846888099405171</v>
+        <v>0.6846490196384534</v>
       </c>
       <c r="F185" t="n">
-        <v>0.02628202035639561</v>
+        <v>0.02628074316062628</v>
       </c>
       <c r="G185" t="n">
-        <v>26.05160488538506</v>
+        <v>26.05135689762917</v>
       </c>
       <c r="H185" t="n">
         <v>0</v>
@@ -6414,13 +6414,13 @@
         </is>
       </c>
       <c r="E186" t="n">
-        <v>0.562667460011864</v>
+        <v>0.5626281597235694</v>
       </c>
       <c r="F186" t="n">
-        <v>0.02245219980963667</v>
+        <v>0.02245097310898832</v>
       </c>
       <c r="G186" t="n">
-        <v>25.06068290668346</v>
+        <v>25.06030170573137</v>
       </c>
       <c r="H186" t="n">
         <v>0</v>
@@ -6446,13 +6446,13 @@
         </is>
       </c>
       <c r="E187" t="n">
-        <v>0.823011479217434</v>
+        <v>0.8230011622552382</v>
       </c>
       <c r="F187" t="n">
-        <v>0.03108462156973512</v>
+        <v>0.03108445703377321</v>
       </c>
       <c r="G187" t="n">
-        <v>26.47648379262449</v>
+        <v>26.47629203671059</v>
       </c>
       <c r="H187" t="n">
         <v>0</v>
@@ -6478,13 +6478,13 @@
         </is>
       </c>
       <c r="E188" t="n">
-        <v>0.8248770152958443</v>
+        <v>0.8248864248815462</v>
       </c>
       <c r="F188" t="n">
-        <v>0.03010146299004854</v>
+        <v>0.03010180929733386</v>
       </c>
       <c r="G188" t="n">
-        <v>27.40322008738058</v>
+        <v>27.40321741813719</v>
       </c>
       <c r="H188" t="n">
         <v>0</v>
@@ -6510,13 +6510,13 @@
         </is>
       </c>
       <c r="E189" t="n">
-        <v>0.580483748116089</v>
+        <v>0.5804599399957582</v>
       </c>
       <c r="F189" t="n">
-        <v>0.02232119639259212</v>
+        <v>0.02232045994887914</v>
       </c>
       <c r="G189" t="n">
-        <v>26.00594241815515</v>
+        <v>26.00573381100515</v>
       </c>
       <c r="H189" t="n">
         <v>0</v>
@@ -6542,13 +6542,13 @@
         </is>
       </c>
       <c r="E190" t="n">
-        <v>1.033136756750818</v>
+        <v>1.033122122567828</v>
       </c>
       <c r="F190" t="n">
-        <v>0.04190417865187279</v>
+        <v>0.04190962452776305</v>
       </c>
       <c r="G190" t="n">
-        <v>24.65474303432004</v>
+        <v>24.65119013077258</v>
       </c>
       <c r="H190" t="n">
         <v>0</v>
@@ -6574,13 +6574,13 @@
         </is>
       </c>
       <c r="E191" t="n">
-        <v>0.7154305369887292</v>
+        <v>0.7154472484711276</v>
       </c>
       <c r="F191" t="n">
-        <v>0.02601135859695069</v>
+        <v>0.02601196629808324</v>
       </c>
       <c r="G191" t="n">
-        <v>27.50454322847614</v>
+        <v>27.50454311085059</v>
       </c>
       <c r="H191" t="n">
         <v>0</v>
@@ -6606,13 +6606,13 @@
         </is>
       </c>
       <c r="E192" t="n">
-        <v>1.132177935930766</v>
+        <v>1.132211891992571</v>
       </c>
       <c r="F192" t="n">
-        <v>0.04252318810759817</v>
+        <v>0.04252414030939068</v>
       </c>
       <c r="G192" t="n">
-        <v>26.62495420238353</v>
+        <v>26.6251565282301</v>
       </c>
       <c r="H192" t="n">
         <v>0</v>
@@ -6638,13 +6638,13 @@
         </is>
       </c>
       <c r="E193" t="n">
-        <v>1.012732225705554</v>
+        <v>1.012719597143575</v>
       </c>
       <c r="F193" t="n">
-        <v>0.03773726077732631</v>
+        <v>0.03773762210310747</v>
       </c>
       <c r="G193" t="n">
-        <v>26.83640001468252</v>
+        <v>26.83580842348165</v>
       </c>
       <c r="H193" t="n">
         <v>0</v>
@@ -6670,13 +6670,13 @@
         </is>
       </c>
       <c r="E194" t="n">
-        <v>0.8112974926909782</v>
+        <v>0.811306265797717</v>
       </c>
       <c r="F194" t="n">
-        <v>0.03057837934351653</v>
+        <v>0.03057870729192016</v>
       </c>
       <c r="G194" t="n">
-        <v>26.53173615090442</v>
+        <v>26.53173850764965</v>
       </c>
       <c r="H194" t="n">
         <v>0</v>
@@ -6702,13 +6702,13 @@
         </is>
       </c>
       <c r="E195" t="n">
-        <v>1.28617439906152</v>
+        <v>1.286195883140495</v>
       </c>
       <c r="F195" t="n">
-        <v>0.04774535986011903</v>
+        <v>0.0477467792857436</v>
       </c>
       <c r="G195" t="n">
-        <v>26.93820724783988</v>
+        <v>26.93785638223339</v>
       </c>
       <c r="H195" t="n">
         <v>0</v>
@@ -6734,13 +6734,13 @@
         </is>
       </c>
       <c r="E196" t="n">
-        <v>1.827093847680761</v>
+        <v>1.827192363987018</v>
       </c>
       <c r="F196" t="n">
-        <v>0.06701720466772977</v>
+        <v>0.06702075671818039</v>
       </c>
       <c r="G196" t="n">
-        <v>27.26305665406667</v>
+        <v>27.26308166950465</v>
       </c>
       <c r="H196" t="n">
         <v>0</v>
@@ -6766,13 +6766,13 @@
         </is>
       </c>
       <c r="E197" t="n">
-        <v>1.245613221405878</v>
+        <v>1.245751134399016</v>
       </c>
       <c r="F197" t="n">
-        <v>0.04598637226556256</v>
+        <v>0.04599163051731453</v>
       </c>
       <c r="G197" t="n">
-        <v>27.08657282608883</v>
+        <v>27.08647465549063</v>
       </c>
       <c r="H197" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Updated Model based on feedback
</commit_message>
<xml_diff>
--- a/model_coefficients.xlsx
+++ b/model_coefficients.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H149"/>
+  <dimension ref="A1:H147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,13 +490,13 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>-1.843097626707309</v>
+        <v>-1.837012621129299</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2201958456176838</v>
+        <v>0.2190671504213888</v>
       </c>
       <c r="G2" t="n">
-        <v>-8.370265213354784</v>
+        <v>-8.385614262965989</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -522,16 +522,16 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>-0.4412406025198592</v>
+        <v>-0.4404619783841713</v>
       </c>
       <c r="F3" t="n">
-        <v>0.09291291076926529</v>
+        <v>0.09265206501942447</v>
       </c>
       <c r="G3" t="n">
-        <v>-4.748969748788329</v>
+        <v>-4.753935902962063</v>
       </c>
       <c r="H3" t="n">
-        <v>2.044555194036235e-06</v>
+        <v>1.994943075400712e-06</v>
       </c>
     </row>
     <row r="4">
@@ -554,16 +554,16 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.9206513487703433</v>
+        <v>0.918992442107251</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1286379545193733</v>
+        <v>0.1280523449739294</v>
       </c>
       <c r="G4" t="n">
-        <v>7.156918439841431</v>
+        <v>7.176693580169694</v>
       </c>
       <c r="H4" t="n">
-        <v>8.251177519014163e-13</v>
+        <v>7.140954494389007e-13</v>
       </c>
     </row>
     <row r="5">
@@ -586,16 +586,16 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1.322720656771312</v>
+        <v>1.318248673520658</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1893374507664099</v>
+        <v>0.1883850224178371</v>
       </c>
       <c r="G5" t="n">
-        <v>6.986048726282885</v>
+        <v>6.99762994209694</v>
       </c>
       <c r="H5" t="n">
-        <v>2.827293954510424e-12</v>
+        <v>2.603250948141067e-12</v>
       </c>
     </row>
     <row r="6">
@@ -618,16 +618,16 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.08649303368595292</v>
+        <v>0.08608007687616626</v>
       </c>
       <c r="F6" t="n">
-        <v>0.018602118084329</v>
+        <v>0.01861219151155008</v>
       </c>
       <c r="G6" t="n">
-        <v>4.649633621784591</v>
+        <v>4.624929676772508</v>
       </c>
       <c r="H6" t="n">
-        <v>3.325251939134688e-06</v>
+        <v>3.747255153729867e-06</v>
       </c>
     </row>
     <row r="7">
@@ -650,13 +650,13 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>-0.2718111668563498</v>
+        <v>-0.2732438761336686</v>
       </c>
       <c r="F7" t="n">
-        <v>0.02297692548464185</v>
+        <v>0.02304904730883882</v>
       </c>
       <c r="G7" t="n">
-        <v>-11.82974489020313</v>
+        <v>-11.85488807674192</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -678,20 +678,20 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Wellbeing</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>-0.007394993367898142</v>
+        <v>0.1799352843045946</v>
       </c>
       <c r="F8" t="n">
-        <v>0.02566486719600509</v>
+        <v>0.02734523169929034</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.2881368257678374</v>
+        <v>6.580133833815136</v>
       </c>
       <c r="H8" t="n">
-        <v>0.7732420045112998</v>
+        <v>4.700240197053063e-11</v>
       </c>
     </row>
     <row r="9">
@@ -710,20 +710,20 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.1814921712861793</v>
+        <v>-0.008965577920801238</v>
       </c>
       <c r="F9" t="n">
-        <v>0.02926001633167725</v>
+        <v>0.020523369208477</v>
       </c>
       <c r="G9" t="n">
-        <v>6.202736499620162</v>
+        <v>-0.4368472753811414</v>
       </c>
       <c r="H9" t="n">
-        <v>5.548970172242207e-10</v>
+        <v>0.6622221111663067</v>
       </c>
     </row>
     <row r="10">
@@ -784,13 +784,13 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1.144919799796414</v>
+        <v>1.148759180846495</v>
       </c>
       <c r="F11" t="n">
-        <v>0.04383393266926545</v>
+        <v>0.04403787032448508</v>
       </c>
       <c r="G11" t="n">
-        <v>26.11948620738438</v>
+        <v>26.08571151047918</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -816,13 +816,13 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1.082423039622923</v>
+        <v>1.085047069952237</v>
       </c>
       <c r="F12" t="n">
-        <v>0.04671059588389601</v>
+        <v>0.04690493410004076</v>
       </c>
       <c r="G12" t="n">
-        <v>23.17296577183952</v>
+        <v>23.13289829199783</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -848,13 +848,13 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>1.223642647686011</v>
+        <v>1.227578859762203</v>
       </c>
       <c r="F13" t="n">
-        <v>0.05005327128277605</v>
+        <v>0.05027761939719374</v>
       </c>
       <c r="G13" t="n">
-        <v>24.44680669817948</v>
+        <v>24.41601003499989</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -880,13 +880,13 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0.9834448756649364</v>
+        <v>0.9859483790990758</v>
       </c>
       <c r="F14" t="n">
-        <v>0.04790301965298161</v>
+        <v>0.04806842481853964</v>
       </c>
       <c r="G14" t="n">
-        <v>20.52991403816845</v>
+        <v>20.51135194882216</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -912,13 +912,13 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0.8076091531511513</v>
+        <v>0.8102101162743814</v>
       </c>
       <c r="F15" t="n">
-        <v>0.05192610403038012</v>
+        <v>0.05209657990389926</v>
       </c>
       <c r="G15" t="n">
-        <v>15.55304732015125</v>
+        <v>15.55207880734965</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -944,13 +944,13 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.6785081348669154</v>
+        <v>0.6817890830778456</v>
       </c>
       <c r="F16" t="n">
-        <v>0.04846998343518759</v>
+        <v>0.04862785918560658</v>
       </c>
       <c r="G16" t="n">
-        <v>13.99852211132267</v>
+        <v>14.02054489920109</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -976,13 +976,13 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0.7706616293833548</v>
+        <v>0.773113838832875</v>
       </c>
       <c r="F17" t="n">
-        <v>0.04617460888418366</v>
+        <v>0.04633174889234539</v>
       </c>
       <c r="G17" t="n">
-        <v>16.69016041477813</v>
+        <v>16.68648081065459</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1008,13 +1008,13 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>1.157265664463219</v>
+        <v>1.159073445985976</v>
       </c>
       <c r="F18" t="n">
-        <v>0.04593467428607274</v>
+        <v>0.04612580575273752</v>
       </c>
       <c r="G18" t="n">
-        <v>25.19372744935092</v>
+        <v>25.12852463053304</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -1040,13 +1040,13 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>1.218782775136124</v>
+        <v>1.220752617251947</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0448478081006038</v>
+        <v>0.04504764050354982</v>
       </c>
       <c r="G19" t="n">
-        <v>27.17597195329909</v>
+        <v>27.09914667181404</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -1110,16 +1110,16 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0.8232629520355976</v>
+        <v>0.8236204107732202</v>
       </c>
       <c r="F21" t="n">
-        <v>0.1906494003163677</v>
+        <v>0.1903658591924092</v>
       </c>
       <c r="G21" t="n">
-        <v>4.318203732427897</v>
+        <v>4.326513242778647</v>
       </c>
       <c r="H21" t="n">
-        <v>1.573041952673826e-05</v>
+        <v>1.514882162712006e-05</v>
       </c>
     </row>
     <row r="22">
@@ -1142,16 +1142,16 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0.6244738101601359</v>
+        <v>0.6260174631706423</v>
       </c>
       <c r="F22" t="n">
-        <v>0.1794204633580676</v>
+        <v>0.1792841207912715</v>
       </c>
       <c r="G22" t="n">
-        <v>3.48050494614095</v>
+        <v>3.49176190509354</v>
       </c>
       <c r="H22" t="n">
-        <v>0.0005004695833445982</v>
+        <v>0.0004798457741665985</v>
       </c>
     </row>
     <row r="23">
@@ -1174,16 +1174,16 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>0.9915671438008594</v>
+        <v>0.9895205019673853</v>
       </c>
       <c r="F23" t="n">
-        <v>0.1937455352506592</v>
+        <v>0.1932541324750756</v>
       </c>
       <c r="G23" t="n">
-        <v>5.1178838392993</v>
+        <v>5.120307075916659</v>
       </c>
       <c r="H23" t="n">
-        <v>3.08982794017254e-07</v>
+        <v>3.050385382064036e-07</v>
       </c>
     </row>
     <row r="24">
@@ -1206,16 +1206,16 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0.4394509320216015</v>
+        <v>0.4364338115324394</v>
       </c>
       <c r="F24" t="n">
-        <v>0.1138884216840536</v>
+        <v>0.1135170370476783</v>
       </c>
       <c r="G24" t="n">
-        <v>3.858609378544702</v>
+        <v>3.844654713329843</v>
       </c>
       <c r="H24" t="n">
-        <v>0.000114034030519683</v>
+        <v>0.0001207223011916447</v>
       </c>
     </row>
     <row r="25">
@@ -1238,16 +1238,16 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0.2773660274298433</v>
+        <v>0.2752638499425671</v>
       </c>
       <c r="F25" t="n">
-        <v>0.1485750638572205</v>
+        <v>0.1483192285776108</v>
       </c>
       <c r="G25" t="n">
-        <v>1.86684104470265</v>
+        <v>1.855887821022979</v>
       </c>
       <c r="H25" t="n">
-        <v>0.06192378881189198</v>
+        <v>0.06346954928492088</v>
       </c>
     </row>
     <row r="26">
@@ -1270,16 +1270,16 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0.3257706243453888</v>
+        <v>0.3242859954959484</v>
       </c>
       <c r="F26" t="n">
-        <v>0.1051220782061028</v>
+        <v>0.1049012403117977</v>
       </c>
       <c r="G26" t="n">
-        <v>3.098974353452017</v>
+        <v>3.091345674550487</v>
       </c>
       <c r="H26" t="n">
-        <v>0.001941918293187017</v>
+        <v>0.001992515261536099</v>
       </c>
     </row>
     <row r="27">
@@ -1302,16 +1302,16 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>1.264638850741855</v>
+        <v>1.262100634172002</v>
       </c>
       <c r="F27" t="n">
-        <v>0.1912118743265297</v>
+        <v>0.1905520157771525</v>
       </c>
       <c r="G27" t="n">
-        <v>6.613809185174536</v>
+        <v>6.623391670867364</v>
       </c>
       <c r="H27" t="n">
-        <v>3.745537213717398e-11</v>
+        <v>3.510502999404252e-11</v>
       </c>
     </row>
     <row r="28">
@@ -1334,16 +1334,16 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>1.248559305821163</v>
+        <v>1.246841627747155</v>
       </c>
       <c r="F28" t="n">
-        <v>0.1930984044788738</v>
+        <v>0.1925559593951768</v>
       </c>
       <c r="G28" t="n">
-        <v>6.465922435683809</v>
+        <v>6.47521703123103</v>
       </c>
       <c r="H28" t="n">
-        <v>1.006827954341816e-10</v>
+        <v>9.46758227371447e-11</v>
       </c>
     </row>
     <row r="29">
@@ -1366,16 +1366,16 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>-0.6300988806470431</v>
+        <v>-0.6276756617572825</v>
       </c>
       <c r="F29" t="n">
-        <v>0.1409701170569928</v>
+        <v>0.1405764651886387</v>
       </c>
       <c r="G29" t="n">
-        <v>-4.469733683968146</v>
+        <v>-4.465012410936236</v>
       </c>
       <c r="H29" t="n">
-        <v>7.831705096217334e-06</v>
+        <v>8.006411052807749e-06</v>
       </c>
     </row>
     <row r="30">
@@ -1398,16 +1398,16 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>1.05520557210022</v>
+        <v>1.054339609788732</v>
       </c>
       <c r="F30" t="n">
-        <v>0.1661347917150931</v>
+        <v>0.1657191213676402</v>
       </c>
       <c r="G30" t="n">
-        <v>6.351502663592917</v>
+        <v>6.362208543474994</v>
       </c>
       <c r="H30" t="n">
-        <v>2.132216625483352e-10</v>
+        <v>1.988731401780797e-10</v>
       </c>
     </row>
     <row r="31">
@@ -1430,16 +1430,16 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>1.815233189953006</v>
+        <v>1.813060963758237</v>
       </c>
       <c r="F31" t="n">
-        <v>0.2571769966520446</v>
+        <v>0.2564060928076329</v>
       </c>
       <c r="G31" t="n">
-        <v>7.058303089221946</v>
+        <v>7.071052578736511</v>
       </c>
       <c r="H31" t="n">
-        <v>1.685540595985913e-12</v>
+        <v>1.537658889105842e-12</v>
       </c>
     </row>
     <row r="32">
@@ -1462,16 +1462,16 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>1.985317446528774</v>
+        <v>1.982191627376437</v>
       </c>
       <c r="F32" t="n">
-        <v>0.2851953974882085</v>
+        <v>0.2842682279509428</v>
       </c>
       <c r="G32" t="n">
-        <v>6.961253456426822</v>
+        <v>6.972962267564908</v>
       </c>
       <c r="H32" t="n">
-        <v>3.372635504206301e-12</v>
+        <v>3.103295398432238e-12</v>
       </c>
     </row>
     <row r="33">
@@ -1494,16 +1494,16 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>2.263214533917539</v>
+        <v>2.261742973603308</v>
       </c>
       <c r="F33" t="n">
-        <v>0.3186452360041684</v>
+        <v>0.3178308125098762</v>
       </c>
       <c r="G33" t="n">
-        <v>7.10261531693143</v>
+        <v>7.116185355772927</v>
       </c>
       <c r="H33" t="n">
-        <v>1.224131906951698e-12</v>
+        <v>1.109556890810381e-12</v>
       </c>
     </row>
     <row r="34">
@@ -1526,16 +1526,16 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>1.319857154316501</v>
+        <v>1.319113842552651</v>
       </c>
       <c r="F34" t="n">
-        <v>0.1984120486077756</v>
+        <v>0.1979473513618079</v>
       </c>
       <c r="G34" t="n">
-        <v>6.652101843467005</v>
+        <v>6.663963086502289</v>
       </c>
       <c r="H34" t="n">
-        <v>2.88935542158697e-11</v>
+        <v>2.665401233059583e-11</v>
       </c>
     </row>
     <row r="35">
@@ -1558,16 +1558,16 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>2.391630220128873</v>
+        <v>2.389602940744238</v>
       </c>
       <c r="F35" t="n">
-        <v>0.3329598022377586</v>
+        <v>0.3320566079879395</v>
       </c>
       <c r="G35" t="n">
-        <v>7.182939814500145</v>
+        <v>7.196372194538089</v>
       </c>
       <c r="H35" t="n">
-        <v>6.823430709346212e-13</v>
+        <v>6.183942247162122e-13</v>
       </c>
     </row>
     <row r="36">
@@ -1590,16 +1590,16 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>-0.1742226535036641</v>
+        <v>-0.1647941544171725</v>
       </c>
       <c r="F36" t="n">
-        <v>0.1763593278874493</v>
+        <v>0.1759484893116071</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.9878845399879458</v>
+        <v>-0.9366045429602031</v>
       </c>
       <c r="H36" t="n">
-        <v>0.3232091977865901</v>
+        <v>0.3489620142834509</v>
       </c>
     </row>
     <row r="37">
@@ -1622,16 +1622,16 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>0.1106063369853244</v>
+        <v>0.1125273672710314</v>
       </c>
       <c r="F37" t="n">
-        <v>0.1274950055528453</v>
+        <v>0.1273653162286923</v>
       </c>
       <c r="G37" t="n">
-        <v>0.8675346654156719</v>
+        <v>0.8835008666574344</v>
       </c>
       <c r="H37" t="n">
-        <v>0.3856491266132738</v>
+        <v>0.3769657144854486</v>
       </c>
     </row>
     <row r="38">
@@ -1654,16 +1654,16 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>-0.01042026651470534</v>
+        <v>-0.008411345526571076</v>
       </c>
       <c r="F38" t="n">
-        <v>0.1638689710927798</v>
+        <v>0.1636549319629432</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.06358901532824036</v>
+        <v>-0.05139683494796406</v>
       </c>
       <c r="H38" t="n">
-        <v>0.9492974785388337</v>
+        <v>0.9590093067874357</v>
       </c>
     </row>
     <row r="39">
@@ -1686,16 +1686,16 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>2.622743818355956</v>
+        <v>2.618512696900444</v>
       </c>
       <c r="F39" t="n">
-        <v>0.3668323679768929</v>
+        <v>0.3655855530346375</v>
       </c>
       <c r="G39" t="n">
-        <v>7.149706643427972</v>
+        <v>7.162516886013792</v>
       </c>
       <c r="H39" t="n">
-        <v>8.695266728864226e-13</v>
+        <v>7.920331057675867e-13</v>
       </c>
     </row>
     <row r="40">
@@ -1718,16 +1718,16 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>2.717405227837483</v>
+        <v>2.712688299348732</v>
       </c>
       <c r="F40" t="n">
-        <v>0.385109775762487</v>
+        <v>0.3837421741264837</v>
       </c>
       <c r="G40" t="n">
-        <v>7.056183454315535</v>
+        <v>7.069038751126543</v>
       </c>
       <c r="H40" t="n">
-        <v>1.711297770157216e-12</v>
+        <v>1.56008539420327e-12</v>
       </c>
     </row>
     <row r="41">
@@ -1750,16 +1750,16 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>2.253082474786096</v>
+        <v>2.251400285993814</v>
       </c>
       <c r="F41" t="n">
-        <v>0.3252638706868934</v>
+        <v>0.3244279591910594</v>
       </c>
       <c r="G41" t="n">
-        <v>6.926937412449473</v>
+        <v>6.939600062832436</v>
       </c>
       <c r="H41" t="n">
-        <v>4.300559908188006e-12</v>
+        <v>3.932187908617379e-12</v>
       </c>
     </row>
     <row r="42">
@@ -1782,16 +1782,16 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>1.978488828340232</v>
+        <v>1.976699586837923</v>
       </c>
       <c r="F42" t="n">
-        <v>0.2926410656479438</v>
+        <v>0.2918849432918842</v>
       </c>
       <c r="G42" t="n">
-        <v>6.76080379885458</v>
+        <v>6.772187576850978</v>
       </c>
       <c r="H42" t="n">
-        <v>1.372280067357678e-11</v>
+        <v>1.268496419015719e-11</v>
       </c>
     </row>
     <row r="43">
@@ -1814,16 +1814,16 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0.6634636483198882</v>
+        <v>0.6620095515900023</v>
       </c>
       <c r="F43" t="n">
-        <v>0.1677589735171722</v>
+        <v>0.1674045980874758</v>
       </c>
       <c r="G43" t="n">
-        <v>3.954862350466275</v>
+        <v>3.95454819729695</v>
       </c>
       <c r="H43" t="n">
-        <v>7.657872860922232e-05</v>
+        <v>7.667941370192999e-05</v>
       </c>
     </row>
     <row r="44">
@@ -1884,13 +1884,13 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>1.595931183345305</v>
+        <v>1.593644948746522</v>
       </c>
       <c r="F45" t="n">
-        <v>0.1654189623595544</v>
+        <v>0.1652488202713419</v>
       </c>
       <c r="G45" t="n">
-        <v>9.647812805564234</v>
+        <v>9.643911200818746</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
@@ -1940,7 +1940,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>StPunt_beh</t>
+          <t>Stopint2</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1954,16 +1954,16 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0.616046100171495</v>
+        <v>0.2579510567965431</v>
       </c>
       <c r="F47" t="n">
-        <v>0.795506490597451</v>
+        <v>0.05410464237119969</v>
       </c>
       <c r="G47" t="n">
-        <v>0.7744073837889746</v>
+        <v>4.767632600212599</v>
       </c>
       <c r="H47" t="n">
-        <v>0.438689918532849</v>
+        <v>1.864033093212925e-06</v>
       </c>
     </row>
     <row r="48">
@@ -1972,7 +1972,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Stopint2</t>
+          <t>Cantrill_1</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1982,20 +1982,26 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Positive_Outcomes</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>-0.004052986915029768</v>
-      </c>
-      <c r="F48" t="n">
-        <v>0.01008518044237236</v>
-      </c>
-      <c r="G48" t="n">
-        <v>-0.4018754981913343</v>
-      </c>
-      <c r="H48" t="n">
-        <v>0.6877756556501815</v>
+        <v>1</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="49">
@@ -2004,7 +2010,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Cantrill_1</t>
+          <t>Leefst</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2018,22 +2024,16 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>0.3440613827926969</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.1323534160227827</v>
+      </c>
+      <c r="G49" t="n">
+        <v>2.599565565658482</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0.009334184531414769</v>
       </c>
     </row>
     <row r="50">
@@ -2042,7 +2042,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Leefst</t>
+          <t>Q297_1</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2056,16 +2056,16 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0.3481176991927807</v>
+        <v>0.1953532947046138</v>
       </c>
       <c r="F50" t="n">
-        <v>0.1327932217457042</v>
+        <v>0.08719935460308956</v>
       </c>
       <c r="G50" t="n">
-        <v>2.621502021065475</v>
+        <v>2.240306658134966</v>
       </c>
       <c r="H50" t="n">
-        <v>0.00875432432493306</v>
+        <v>0.02507102129927863</v>
       </c>
     </row>
     <row r="51">
@@ -2074,7 +2074,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Q297_1</t>
+          <t>Onnodige_stress_1</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2088,16 +2088,16 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>0.1954180785960611</v>
+        <v>-3.910752595597345</v>
       </c>
       <c r="F51" t="n">
-        <v>0.08741559141689062</v>
+        <v>0.4337874075688778</v>
       </c>
       <c r="G51" t="n">
-        <v>2.23550599414084</v>
+        <v>-9.015366807224277</v>
       </c>
       <c r="H51" t="n">
-        <v>0.02538414854803239</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -2106,7 +2106,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Onnodige_stress_1</t>
+          <t>Onnodige_stress_2</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2120,13 +2120,13 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>-3.934254804307986</v>
+        <v>-4.585840484940034</v>
       </c>
       <c r="F52" t="n">
-        <v>0.437126698982238</v>
+        <v>0.4918203882748596</v>
       </c>
       <c r="G52" t="n">
-        <v>-9.000261968575952</v>
+        <v>-9.32421793455187</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
@@ -2138,7 +2138,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Onnodige_stress_2</t>
+          <t>Onnodige_stress_3</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2152,13 +2152,13 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>-4.610372370040863</v>
+        <v>-4.310834809615412</v>
       </c>
       <c r="F53" t="n">
-        <v>0.4954845272023801</v>
+        <v>0.4671866809701209</v>
       </c>
       <c r="G53" t="n">
-        <v>-9.304775662850227</v>
+        <v>-9.227221119948593</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -2170,7 +2170,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Onnodige_stress_3</t>
+          <t>Onnodige_stress_4</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2184,13 +2184,13 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>-4.319989720460577</v>
+        <v>-5.350415534699463</v>
       </c>
       <c r="F54" t="n">
-        <v>0.4693000078624527</v>
+        <v>0.5644187031660791</v>
       </c>
       <c r="G54" t="n">
-        <v>-9.205177174677395</v>
+        <v>-9.479514949942462</v>
       </c>
       <c r="H54" t="n">
         <v>0</v>
@@ -2202,7 +2202,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Onnodige_stress_4</t>
+          <t>Onnodige_stress_5</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2216,13 +2216,13 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>-5.380123972296032</v>
+        <v>-5.279986857658689</v>
       </c>
       <c r="F55" t="n">
-        <v>0.5688220901093348</v>
+        <v>0.5564848072502685</v>
       </c>
       <c r="G55" t="n">
-        <v>-9.458359768082225</v>
+        <v>-9.488106034267036</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -2234,7 +2234,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Onnodige_stress_5</t>
+          <t>Onnodige_stress_6</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2248,13 +2248,13 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>-5.313100268456053</v>
+        <v>-4.798073004081398</v>
       </c>
       <c r="F56" t="n">
-        <v>0.5612175818008631</v>
+        <v>0.511227510842562</v>
       </c>
       <c r="G56" t="n">
-        <v>-9.467095188639037</v>
+        <v>-9.385396721244977</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -2266,7 +2266,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Onnodige_stress_6</t>
+          <t>Onnodige_stress_7</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2280,13 +2280,13 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>-4.827040265095732</v>
+        <v>-3.713806881656816</v>
       </c>
       <c r="F57" t="n">
-        <v>0.5153985819560014</v>
+        <v>0.429521720184962</v>
       </c>
       <c r="G57" t="n">
-        <v>-9.365645219214906</v>
+        <v>-8.64637737073906</v>
       </c>
       <c r="H57" t="n">
         <v>0</v>
@@ -2298,7 +2298,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Onnodige_stress_7</t>
+          <t>Onnodige_stress_8</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2312,13 +2312,13 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>-3.725751995791548</v>
+        <v>-4.089900667506929</v>
       </c>
       <c r="F58" t="n">
-        <v>0.4317155256752864</v>
+        <v>0.4498022896825676</v>
       </c>
       <c r="G58" t="n">
-        <v>-8.630108889308817</v>
+        <v>-9.092663068443121</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -2330,7 +2330,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Onnodige_stress_8</t>
+          <t>Onnodige_stress_9</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2344,13 +2344,13 @@
         </is>
       </c>
       <c r="E59" t="n">
-        <v>-4.104814044467738</v>
+        <v>-4.701377544154129</v>
       </c>
       <c r="F59" t="n">
-        <v>0.4523926964544253</v>
+        <v>0.5053727818333053</v>
       </c>
       <c r="G59" t="n">
-        <v>-9.073563911684833</v>
+        <v>-9.302791351544439</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Onnodige_stress_9</t>
+          <t>Onnodige_stress_10</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2376,16 +2376,16 @@
         </is>
       </c>
       <c r="E60" t="n">
-        <v>-4.729056133744443</v>
+        <v>-2.777184669439268</v>
       </c>
       <c r="F60" t="n">
-        <v>0.5093782018880741</v>
+        <v>0.3508514895476489</v>
       </c>
       <c r="G60" t="n">
-        <v>-9.283978223265779</v>
+        <v>-7.915556160277281</v>
       </c>
       <c r="H60" t="n">
-        <v>0</v>
+        <v>2.442490654175344e-15</v>
       </c>
     </row>
     <row r="61">
@@ -2394,7 +2394,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Onnodige_stress_10</t>
+          <t>Werk_1</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2408,16 +2408,16 @@
         </is>
       </c>
       <c r="E61" t="n">
-        <v>-2.777047591322549</v>
+        <v>-0.04419552127263621</v>
       </c>
       <c r="F61" t="n">
-        <v>0.3518096386167103</v>
+        <v>0.1408518614963768</v>
       </c>
       <c r="G61" t="n">
-        <v>-7.893608606727782</v>
+        <v>-0.3137730719551712</v>
       </c>
       <c r="H61" t="n">
-        <v>2.886579864025407e-15</v>
+        <v>0.7536933977204967</v>
       </c>
     </row>
     <row r="62">
@@ -2426,7 +2426,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Werk_1</t>
+          <t>Burn1_1</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2436,20 +2436,26 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>-0.05596727543337311</v>
-      </c>
-      <c r="F62" t="n">
-        <v>0.1413186720973291</v>
-      </c>
-      <c r="G62" t="n">
-        <v>-0.3960359561999794</v>
-      </c>
-      <c r="H62" t="n">
-        <v>0.6920785030267727</v>
+        <v>1</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="63">
@@ -2458,7 +2464,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Burn1_1</t>
+          <t>Burn1_2</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2472,22 +2478,16 @@
         </is>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>1.069789612577432</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.04985087771151978</v>
+      </c>
+      <c r="G63" t="n">
+        <v>21.45979492571221</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -2496,7 +2496,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Burn1_2</t>
+          <t>Burn1_3</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2510,13 +2510,13 @@
         </is>
       </c>
       <c r="E64" t="n">
-        <v>1.070246091572693</v>
+        <v>0.9197332176939851</v>
       </c>
       <c r="F64" t="n">
-        <v>0.04981114968677166</v>
+        <v>0.04977018188919372</v>
       </c>
       <c r="G64" t="n">
-        <v>21.48607487041062</v>
+        <v>18.47960330390517</v>
       </c>
       <c r="H64" t="n">
         <v>0</v>
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Burn1_3</t>
+          <t>Burn1_4</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2542,13 +2542,13 @@
         </is>
       </c>
       <c r="E65" t="n">
-        <v>0.9204574102087412</v>
+        <v>0.9599523120152618</v>
       </c>
       <c r="F65" t="n">
-        <v>0.04974979894932188</v>
+        <v>0.04878710881457536</v>
       </c>
       <c r="G65" t="n">
-        <v>18.50173125579608</v>
+        <v>19.67635171094204</v>
       </c>
       <c r="H65" t="n">
         <v>0</v>
@@ -2560,7 +2560,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Burn1_4</t>
+          <t>Depr_1</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2574,13 +2574,13 @@
         </is>
       </c>
       <c r="E66" t="n">
-        <v>0.960318738561553</v>
+        <v>1.260917800217647</v>
       </c>
       <c r="F66" t="n">
-        <v>0.0487281370560762</v>
+        <v>0.05127404859285291</v>
       </c>
       <c r="G66" t="n">
-        <v>19.70768423666009</v>
+        <v>24.59173470395343</v>
       </c>
       <c r="H66" t="n">
         <v>0</v>
@@ -2592,7 +2592,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Depr_1</t>
+          <t>Depr_2</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2606,13 +2606,13 @@
         </is>
       </c>
       <c r="E67" t="n">
-        <v>1.258228310018165</v>
+        <v>1.373370897337855</v>
       </c>
       <c r="F67" t="n">
-        <v>0.05114118312200801</v>
+        <v>0.05575004556618723</v>
       </c>
       <c r="G67" t="n">
-        <v>24.60303483773136</v>
+        <v>24.63443542270715</v>
       </c>
       <c r="H67" t="n">
         <v>0</v>
@@ -2624,7 +2624,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Depr_2</t>
+          <t>Depr_3</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2638,13 +2638,13 @@
         </is>
       </c>
       <c r="E68" t="n">
-        <v>1.371036477629394</v>
+        <v>0.9297598376786836</v>
       </c>
       <c r="F68" t="n">
-        <v>0.0555899459887364</v>
+        <v>0.05558753123890852</v>
       </c>
       <c r="G68" t="n">
-        <v>24.66338927335043</v>
+        <v>16.72605019398976</v>
       </c>
       <c r="H68" t="n">
         <v>0</v>
@@ -2656,7 +2656,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Depr_3</t>
+          <t>Depr_4</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2670,13 +2670,13 @@
         </is>
       </c>
       <c r="E69" t="n">
-        <v>0.9285407433534256</v>
+        <v>-0.9555515713785653</v>
       </c>
       <c r="F69" t="n">
-        <v>0.05546649888379954</v>
+        <v>0.04517746927662268</v>
       </c>
       <c r="G69" t="n">
-        <v>16.74056884826906</v>
+        <v>-21.15106460493725</v>
       </c>
       <c r="H69" t="n">
         <v>0</v>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Depr_4</t>
+          <t>Depr_5</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2702,13 +2702,13 @@
         </is>
       </c>
       <c r="E70" t="n">
-        <v>-0.95112488000929</v>
+        <v>0.9452671184506577</v>
       </c>
       <c r="F70" t="n">
-        <v>0.04501190361834571</v>
+        <v>0.04942540682529834</v>
       </c>
       <c r="G70" t="n">
-        <v>-21.13051889679478</v>
+        <v>19.12512570251012</v>
       </c>
       <c r="H70" t="n">
         <v>0</v>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Depr_5</t>
+          <t>Depr_6</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2734,13 +2734,13 @@
         </is>
       </c>
       <c r="E71" t="n">
-        <v>0.9434622640049224</v>
+        <v>-0.967958485078443</v>
       </c>
       <c r="F71" t="n">
-        <v>0.0493384479937768</v>
+        <v>0.04633891122685135</v>
       </c>
       <c r="G71" t="n">
-        <v>19.12225257074973</v>
+        <v>-20.88867561688988</v>
       </c>
       <c r="H71" t="n">
         <v>0</v>
@@ -2752,7 +2752,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Depr_6</t>
+          <t>Depr_7</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2766,13 +2766,13 @@
         </is>
       </c>
       <c r="E72" t="n">
-        <v>-0.9610240706062971</v>
+        <v>0.9733323288542264</v>
       </c>
       <c r="F72" t="n">
-        <v>0.04632710391505648</v>
+        <v>0.0453917970068945</v>
       </c>
       <c r="G72" t="n">
-        <v>-20.74431573248455</v>
+        <v>21.44291244263684</v>
       </c>
       <c r="H72" t="n">
         <v>0</v>
@@ -2784,7 +2784,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Depr_7</t>
+          <t>Depr_8</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2798,13 +2798,13 @@
         </is>
       </c>
       <c r="E73" t="n">
-        <v>0.9720800334781186</v>
+        <v>1.107495732967219</v>
       </c>
       <c r="F73" t="n">
-        <v>0.04531756266502416</v>
+        <v>0.05241789369231033</v>
       </c>
       <c r="G73" t="n">
-        <v>21.45040413232361</v>
+        <v>21.12819983662487</v>
       </c>
       <c r="H73" t="n">
         <v>0</v>
@@ -2816,7 +2816,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Depr_8</t>
+          <t>Mot_Stress_2</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2830,13 +2830,13 @@
         </is>
       </c>
       <c r="E74" t="n">
-        <v>1.105282318465017</v>
+        <v>0.7450008243818098</v>
       </c>
       <c r="F74" t="n">
-        <v>0.05228294587455884</v>
+        <v>0.04021134718108373</v>
       </c>
       <c r="G74" t="n">
-        <v>21.14039865113479</v>
+        <v>18.52712919585412</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -2848,30 +2848,30 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Mot_Stress_2</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>~~</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Energy_Sources</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>0.7453122122029187</v>
+        <v>0.001392713639713758</v>
       </c>
       <c r="F75" t="n">
-        <v>0.04016453489525221</v>
+        <v>0.001272288785567813</v>
       </c>
       <c r="G75" t="n">
-        <v>18.55647561033912</v>
+        <v>1.094652137484296</v>
       </c>
       <c r="H75" t="n">
-        <v>0</v>
+        <v>0.2736690647205633</v>
       </c>
     </row>
     <row r="76">
@@ -2890,20 +2890,20 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Energy_Sources</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>0.001394706654434728</v>
+        <v>0.02721478098186947</v>
       </c>
       <c r="F76" t="n">
-        <v>0.001265698763745427</v>
+        <v>0.005655304310021612</v>
       </c>
       <c r="G76" t="n">
-        <v>1.101926219162621</v>
+        <v>4.81225757008878</v>
       </c>
       <c r="H76" t="n">
-        <v>0.2704937488387298</v>
+        <v>1.492348465470528e-06</v>
       </c>
     </row>
     <row r="77">
@@ -2912,7 +2912,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2922,20 +2922,20 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Wellbeing</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>0.02703495960735069</v>
+        <v>-0.09985784585730083</v>
       </c>
       <c r="F77" t="n">
-        <v>0.005632003363556634</v>
+        <v>0.009221726053166431</v>
       </c>
       <c r="G77" t="n">
-        <v>4.800238539892802</v>
+        <v>-10.82854177957113</v>
       </c>
       <c r="H77" t="n">
-        <v>1.584767529871911e-06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -2954,17 +2954,17 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>-0.1004301771492345</v>
+        <v>0.2904226677048763</v>
       </c>
       <c r="F78" t="n">
-        <v>0.009251144159482676</v>
+        <v>0.02175764183372733</v>
       </c>
       <c r="G78" t="n">
-        <v>-10.85597364034533</v>
+        <v>13.34807650162406</v>
       </c>
       <c r="H78" t="n">
         <v>0</v>
@@ -2976,7 +2976,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Energy_Sources</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2986,20 +2986,20 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Energy_Sources</t>
         </is>
       </c>
       <c r="E79" t="n">
-        <v>0.2908453601522537</v>
+        <v>0.05966522692244547</v>
       </c>
       <c r="F79" t="n">
-        <v>0.02175908692865865</v>
+        <v>0.016005708421777</v>
       </c>
       <c r="G79" t="n">
-        <v>13.36661603000528</v>
+        <v>3.727746710513519</v>
       </c>
       <c r="H79" t="n">
-        <v>0</v>
+        <v>0.0001931994012216443</v>
       </c>
     </row>
     <row r="80">
@@ -3008,7 +3008,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Energy_Sources</t>
+          <t>Negative_Outcomes</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3018,20 +3018,20 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Energy_Sources</t>
+          <t>Negative_Outcomes</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>0.05946199317940898</v>
+        <v>0.02787955882863766</v>
       </c>
       <c r="F80" t="n">
-        <v>0.01598247565836763</v>
+        <v>0.007234222640435703</v>
       </c>
       <c r="G80" t="n">
-        <v>3.720449475207377</v>
+        <v>3.853843074852433</v>
       </c>
       <c r="H80" t="n">
-        <v>0.0001988685258960121</v>
+        <v>0.0001162781378067912</v>
       </c>
     </row>
     <row r="81">
@@ -3040,7 +3040,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Negative_Outcomes</t>
+          <t>Positive_Outcomes</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3050,20 +3050,20 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Negative_Outcomes</t>
+          <t>Positive_Outcomes</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>0.02789470340597225</v>
+        <v>5.664304343127e-18</v>
       </c>
       <c r="F81" t="n">
-        <v>0.00722281743295863</v>
+        <v>0.008063947695665267</v>
       </c>
       <c r="G81" t="n">
-        <v>3.862025263828927</v>
+        <v>7.024232492814152e-16</v>
       </c>
       <c r="H81" t="n">
-        <v>0.0001124509344483382</v>
+        <v>0.9999999999999993</v>
       </c>
     </row>
     <row r="82">
@@ -3072,7 +3072,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Positive_Outcomes</t>
+          <t>Wellbeing</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3082,20 +3082,20 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Positive_Outcomes</t>
+          <t>Wellbeing</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>0.2362221928574092</v>
+        <v>0.1806703619325559</v>
       </c>
       <c r="F82" t="n">
-        <v>0.3125541315979788</v>
+        <v>0.01416441482679721</v>
       </c>
       <c r="G82" t="n">
-        <v>0.7557801000707713</v>
+        <v>12.75522950499841</v>
       </c>
       <c r="H82" t="n">
-        <v>0.4497810498484465</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -3104,7 +3104,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Bekendgebruik_1</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3114,17 +3114,17 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Bekendgebruik_1</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>0.1816894625962413</v>
+        <v>1.282240733713973</v>
       </c>
       <c r="F83" t="n">
-        <v>0.01421192155879544</v>
+        <v>0.04715791766371915</v>
       </c>
       <c r="G83" t="n">
-        <v>12.78429956370069</v>
+        <v>27.1903594817392</v>
       </c>
       <c r="H83" t="n">
         <v>0</v>
@@ -3136,7 +3136,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Bekendgebruik_1</t>
+          <t>Bekendgebruik_2</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3146,17 +3146,17 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Bekendgebruik_1</t>
+          <t>Bekendgebruik_2</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>1.283580171913479</v>
+        <v>1.762692729941262</v>
       </c>
       <c r="F84" t="n">
-        <v>0.04718981738582204</v>
+        <v>0.06446137473830502</v>
       </c>
       <c r="G84" t="n">
-        <v>27.20036319258832</v>
+        <v>27.34494473737105</v>
       </c>
       <c r="H84" t="n">
         <v>0</v>
@@ -3168,7 +3168,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Bekendgebruik_2</t>
+          <t>Bekendgebruik_3</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3178,17 +3178,17 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Bekendgebruik_2</t>
+          <t>Bekendgebruik_3</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>1.762578156913743</v>
+        <v>1.834770074272736</v>
       </c>
       <c r="F85" t="n">
-        <v>0.06443478774695297</v>
+        <v>0.06693327536866778</v>
       </c>
       <c r="G85" t="n">
-        <v>27.35444964618105</v>
+        <v>27.41192723857349</v>
       </c>
       <c r="H85" t="n">
         <v>0</v>
@@ -3200,7 +3200,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Bekendgebruik_3</t>
+          <t>Bekendgebruik_4</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3210,17 +3210,17 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Bekendgebruik_3</t>
+          <t>Bekendgebruik_4</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>1.833361549858271</v>
+        <v>1.454319022254985</v>
       </c>
       <c r="F86" t="n">
-        <v>0.06685847553631365</v>
+        <v>0.05340461195966033</v>
       </c>
       <c r="G86" t="n">
-        <v>27.42152786351034</v>
+        <v>27.23208668431644</v>
       </c>
       <c r="H86" t="n">
         <v>0</v>
@@ -3232,7 +3232,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Bekendgebruik_4</t>
+          <t>Bekendgebruik_5</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3242,17 +3242,17 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Bekendgebruik_4</t>
+          <t>Bekendgebruik_5</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>1.45352101080358</v>
+        <v>0.6924132191790505</v>
       </c>
       <c r="F87" t="n">
-        <v>0.05335890672168894</v>
+        <v>0.02528174233413066</v>
       </c>
       <c r="G87" t="n">
-        <v>27.24045712476195</v>
+        <v>27.38787580383241</v>
       </c>
       <c r="H87" t="n">
         <v>0</v>
@@ -3264,7 +3264,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Bekendgebruik_5</t>
+          <t>Bekendgebruik_6</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3274,17 +3274,17 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Bekendgebruik_5</t>
+          <t>Bekendgebruik_6</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>0.6920911813736477</v>
+        <v>1.504620800051772</v>
       </c>
       <c r="F88" t="n">
-        <v>0.02526282604186526</v>
+        <v>0.05476174646168028</v>
       </c>
       <c r="G88" t="n">
-        <v>27.39563579305524</v>
+        <v>27.47576359853972</v>
       </c>
       <c r="H88" t="n">
         <v>0</v>
@@ -3296,7 +3296,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Bekendgebruik_6</t>
+          <t>Bekendgebruik_7</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3306,17 +3306,17 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Bekendgebruik_6</t>
+          <t>Bekendgebruik_7</t>
         </is>
       </c>
       <c r="E89" t="n">
-        <v>1.503782903071624</v>
+        <v>0.6656611368155223</v>
       </c>
       <c r="F89" t="n">
-        <v>0.05471369325098353</v>
+        <v>0.02426437826944464</v>
       </c>
       <c r="G89" t="n">
-        <v>27.48458043484585</v>
+        <v>27.43367785468192</v>
       </c>
       <c r="H89" t="n">
         <v>0</v>
@@ -3328,7 +3328,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Bekendgebruik_7</t>
+          <t>Betrok_Ouders</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3338,17 +3338,17 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Bekendgebruik_7</t>
+          <t>Betrok_Ouders</t>
         </is>
       </c>
       <c r="E90" t="n">
-        <v>0.6652649358123868</v>
+        <v>1.474770410409492</v>
       </c>
       <c r="F90" t="n">
-        <v>0.02424232919381178</v>
+        <v>0.05386455152200994</v>
       </c>
       <c r="G90" t="n">
-        <v>27.44228619561703</v>
+        <v>27.37923864045349</v>
       </c>
       <c r="H90" t="n">
         <v>0</v>
@@ -3360,7 +3360,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Betrok_Ouders</t>
+          <t>Bevl_1</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3370,17 +3370,17 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Betrok_Ouders</t>
+          <t>Bevl_1</t>
         </is>
       </c>
       <c r="E91" t="n">
-        <v>1.474270102335801</v>
+        <v>0.4225820871945859</v>
       </c>
       <c r="F91" t="n">
-        <v>0.0538290405586156</v>
+        <v>0.01658222609310502</v>
       </c>
       <c r="G91" t="n">
-        <v>27.38800630680104</v>
+        <v>25.48403843949601</v>
       </c>
       <c r="H91" t="n">
         <v>0</v>
@@ -3392,7 +3392,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Bevl_1</t>
+          <t>Bevl_2</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3402,17 +3402,17 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Bevl_1</t>
+          <t>Bevl_2</t>
         </is>
       </c>
       <c r="E92" t="n">
-        <v>0.4218755574884602</v>
+        <v>0.2522805405174928</v>
       </c>
       <c r="F92" t="n">
-        <v>0.01655993095080236</v>
+        <v>0.01095864797566632</v>
       </c>
       <c r="G92" t="n">
-        <v>25.47568336585026</v>
+        <v>23.02113737521824</v>
       </c>
       <c r="H92" t="n">
         <v>0</v>
@@ -3424,7 +3424,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Bevl_2</t>
+          <t>Bevl_3</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3434,17 +3434,17 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Bevl_2</t>
+          <t>Bevl_3</t>
         </is>
       </c>
       <c r="E93" t="n">
-        <v>0.2530984753426118</v>
+        <v>0.427593290129484</v>
       </c>
       <c r="F93" t="n">
-        <v>0.01098347628096397</v>
+        <v>0.01699981627420381</v>
       </c>
       <c r="G93" t="n">
-        <v>23.04356734108183</v>
+        <v>25.15281831328836</v>
       </c>
       <c r="H93" t="n">
         <v>0</v>
@@ -3456,7 +3456,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Bevl_3</t>
+          <t>Burn1_1</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3466,17 +3466,17 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Bevl_3</t>
+          <t>Burn1_1</t>
         </is>
       </c>
       <c r="E94" t="n">
-        <v>0.4273653059678117</v>
+        <v>0.5254424338178632</v>
       </c>
       <c r="F94" t="n">
-        <v>0.01698877282154548</v>
+        <v>0.02092198204555681</v>
       </c>
       <c r="G94" t="n">
-        <v>25.15574906038318</v>
+        <v>25.11437169999563</v>
       </c>
       <c r="H94" t="n">
         <v>0</v>
@@ -3488,7 +3488,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Burn1_1</t>
+          <t>Burn1_2</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3498,17 +3498,17 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Burn1_1</t>
+          <t>Burn1_2</t>
         </is>
       </c>
       <c r="E95" t="n">
-        <v>0.5243433606819768</v>
+        <v>0.708826173959145</v>
       </c>
       <c r="F95" t="n">
-        <v>0.02088213396077285</v>
+        <v>0.02782264079216287</v>
       </c>
       <c r="G95" t="n">
-        <v>25.10966367909753</v>
+        <v>25.47659581377092</v>
       </c>
       <c r="H95" t="n">
         <v>0</v>
@@ -3520,7 +3520,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Burn1_2</t>
+          <t>Burn1_3</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3530,17 +3530,17 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Burn1_2</t>
+          <t>Burn1_3</t>
         </is>
       </c>
       <c r="E96" t="n">
-        <v>0.7093140294874135</v>
+        <v>0.8685892703731797</v>
       </c>
       <c r="F96" t="n">
-        <v>0.02784034597016098</v>
+        <v>0.03305212754567853</v>
       </c>
       <c r="G96" t="n">
-        <v>25.47791720053234</v>
+        <v>26.27937548487604</v>
       </c>
       <c r="H96" t="n">
         <v>0</v>
@@ -3552,7 +3552,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Burn1_3</t>
+          <t>Burn1_4</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3562,17 +3562,17 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Burn1_3</t>
+          <t>Burn1_4</t>
         </is>
       </c>
       <c r="E97" t="n">
-        <v>0.8696352104509363</v>
+        <v>0.7749630500964432</v>
       </c>
       <c r="F97" t="n">
-        <v>0.03308668387471914</v>
+        <v>0.02979487299750418</v>
       </c>
       <c r="G97" t="n">
-        <v>26.28354094709151</v>
+        <v>26.00994641377895</v>
       </c>
       <c r="H97" t="n">
         <v>0</v>
@@ -3584,7 +3584,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Burn1_4</t>
+          <t>Cantrill_1</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3594,17 +3594,17 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Burn1_4</t>
+          <t>Cantrill_1</t>
         </is>
       </c>
       <c r="E98" t="n">
-        <v>0.7743383500973657</v>
+        <v>0.3767663457941035</v>
       </c>
       <c r="F98" t="n">
-        <v>0.02976939332456589</v>
+        <v>0.01384359691849361</v>
       </c>
       <c r="G98" t="n">
-        <v>26.01122372999001</v>
+        <v>27.21592863366073</v>
       </c>
       <c r="H98" t="n">
         <v>0</v>
@@ -3616,7 +3616,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Cantrill_1</t>
+          <t>Cijfer_huidig_1</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3626,17 +3626,17 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Cantrill_1</t>
+          <t>Cijfer_huidig_1</t>
         </is>
       </c>
       <c r="E99" t="n">
-        <v>0.3766572367110361</v>
+        <v>0.2362708757347188</v>
       </c>
       <c r="F99" t="n">
-        <v>0.01383357465791211</v>
+        <v>0.01178366164126729</v>
       </c>
       <c r="G99" t="n">
-        <v>27.22775898479567</v>
+        <v>20.05071792686488</v>
       </c>
       <c r="H99" t="n">
         <v>0</v>
@@ -3648,7 +3648,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Cijfer_huidig_1</t>
+          <t>Cogn_Eng1_1</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3658,20 +3658,20 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Cijfer_huidig_1</t>
+          <t>Cogn_Eng1_1</t>
         </is>
       </c>
       <c r="E100" t="n">
-        <v>5.45580806151202e-18</v>
+        <v>0.5843785429315377</v>
       </c>
       <c r="F100" t="n">
-        <v>0.3124350479838501</v>
+        <v>0.02211238605659233</v>
       </c>
       <c r="G100" t="n">
-        <v>1.746221525626207e-17</v>
+        <v>26.42765649123109</v>
       </c>
       <c r="H100" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -3680,7 +3680,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_1</t>
+          <t>Cogn_Eng1_2</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3690,17 +3690,17 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_1</t>
+          <t>Cogn_Eng1_2</t>
         </is>
       </c>
       <c r="E101" t="n">
-        <v>0.5844197693019313</v>
+        <v>0.6899679279212954</v>
       </c>
       <c r="F101" t="n">
-        <v>0.0221081292992859</v>
+        <v>0.02592587945804104</v>
       </c>
       <c r="G101" t="n">
-        <v>26.43460970234029</v>
+        <v>26.61309634688921</v>
       </c>
       <c r="H101" t="n">
         <v>0</v>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_2</t>
+          <t>Cogn_Eng1_3</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3722,17 +3722,17 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_2</t>
+          <t>Cogn_Eng1_3</t>
         </is>
       </c>
       <c r="E102" t="n">
-        <v>0.6895471216634583</v>
+        <v>0.9300981099966188</v>
       </c>
       <c r="F102" t="n">
-        <v>0.02590243483268409</v>
+        <v>0.03403239656846933</v>
       </c>
       <c r="G102" t="n">
-        <v>26.62093838247037</v>
+        <v>27.32978584385137</v>
       </c>
       <c r="H102" t="n">
         <v>0</v>
@@ -3744,7 +3744,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_3</t>
+          <t>Cogn_Eng1_4</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3754,17 +3754,17 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_3</t>
+          <t>Cogn_Eng1_4</t>
         </is>
       </c>
       <c r="E103" t="n">
-        <v>0.9294129779987012</v>
+        <v>0.5626417764542803</v>
       </c>
       <c r="F103" t="n">
-        <v>0.03399736152472267</v>
+        <v>0.02105546221266954</v>
       </c>
       <c r="G103" t="n">
-        <v>27.3377972962843</v>
+        <v>26.72189148566895</v>
       </c>
       <c r="H103" t="n">
         <v>0</v>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_4</t>
+          <t>Cogn_Eng1_5</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3786,17 +3786,17 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_4</t>
+          <t>Cogn_Eng1_5</t>
         </is>
       </c>
       <c r="E104" t="n">
-        <v>0.5628941664313842</v>
+        <v>0.4234821106321717</v>
       </c>
       <c r="F104" t="n">
-        <v>0.02105728117580156</v>
+        <v>0.01731194028780949</v>
       </c>
       <c r="G104" t="n">
-        <v>26.73156908079449</v>
+        <v>24.46185139085261</v>
       </c>
       <c r="H104" t="n">
         <v>0</v>
@@ -3808,7 +3808,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_5</t>
+          <t>Cogn_Eng1_6</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3818,17 +3818,17 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_5</t>
+          <t>Cogn_Eng1_6</t>
         </is>
       </c>
       <c r="E105" t="n">
-        <v>0.4239805963995715</v>
+        <v>0.5647175274783313</v>
       </c>
       <c r="F105" t="n">
-        <v>0.0173244342189833</v>
+        <v>0.02169094666675797</v>
       </c>
       <c r="G105" t="n">
-        <v>24.47298370705351</v>
+        <v>26.03471098464058</v>
       </c>
       <c r="H105" t="n">
         <v>0</v>
@@ -3840,7 +3840,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_6</t>
+          <t>Cogn_Eng2_1</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3850,17 +3850,17 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_6</t>
+          <t>Cogn_Eng2_1</t>
         </is>
       </c>
       <c r="E106" t="n">
-        <v>0.5652639724501848</v>
+        <v>0.5344782591744353</v>
       </c>
       <c r="F106" t="n">
-        <v>0.02170539409057005</v>
+        <v>0.0213104217836179</v>
       </c>
       <c r="G106" t="n">
-        <v>26.04255744288569</v>
+        <v>25.08060443741324</v>
       </c>
       <c r="H106" t="n">
         <v>0</v>
@@ -3872,7 +3872,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_1</t>
+          <t>Cogn_Eng2_2</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3882,17 +3882,17 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_1</t>
+          <t>Cogn_Eng2_2</t>
         </is>
       </c>
       <c r="E107" t="n">
-        <v>0.5344789714149311</v>
+        <v>0.8748600560316472</v>
       </c>
       <c r="F107" t="n">
-        <v>0.02130363578722821</v>
+        <v>0.03257075745026131</v>
       </c>
       <c r="G107" t="n">
-        <v>25.08862697090743</v>
+        <v>26.86029200704904</v>
       </c>
       <c r="H107" t="n">
         <v>0</v>
@@ -3904,7 +3904,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_2</t>
+          <t>Cogn_Eng2_3</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3914,17 +3914,17 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_2</t>
+          <t>Cogn_Eng2_3</t>
         </is>
       </c>
       <c r="E108" t="n">
-        <v>0.8749216052357194</v>
+        <v>0.8088402711464276</v>
       </c>
       <c r="F108" t="n">
-        <v>0.03256232415240303</v>
+        <v>0.02994685785259688</v>
       </c>
       <c r="G108" t="n">
-        <v>26.86913873573373</v>
+        <v>27.00918657645676</v>
       </c>
       <c r="H108" t="n">
         <v>0</v>
@@ -3936,7 +3936,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_3</t>
+          <t>Cogn_Eng2_4</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3946,17 +3946,17 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_3</t>
+          <t>Cogn_Eng2_4</t>
         </is>
       </c>
       <c r="E109" t="n">
-        <v>0.8092289669111157</v>
+        <v>0.8020404398643528</v>
       </c>
       <c r="F109" t="n">
-        <v>0.02994941861662247</v>
+        <v>0.03136215829162617</v>
       </c>
       <c r="G109" t="n">
-        <v>27.01985561866497</v>
+        <v>25.57350907998343</v>
       </c>
       <c r="H109" t="n">
         <v>0</v>
@@ -3968,7 +3968,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_4</t>
+          <t>Cogn_Eng2_5</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3978,17 +3978,17 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_4</t>
+          <t>Cogn_Eng2_5</t>
         </is>
       </c>
       <c r="E110" t="n">
-        <v>0.8016718710973612</v>
+        <v>0.7366391703822698</v>
       </c>
       <c r="F110" t="n">
-        <v>0.03134052808123033</v>
+        <v>0.02974212144364219</v>
       </c>
       <c r="G110" t="n">
-        <v>25.57939894930802</v>
+        <v>24.76753959038687</v>
       </c>
       <c r="H110" t="n">
         <v>0</v>
@@ -4000,7 +4000,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_5</t>
+          <t>Cogn_Eng2_6</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -4010,17 +4010,17 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_5</t>
+          <t>Cogn_Eng2_6</t>
         </is>
       </c>
       <c r="E111" t="n">
-        <v>0.7370957153800066</v>
+        <v>0.6032405583597319</v>
       </c>
       <c r="F111" t="n">
-        <v>0.02974545649517122</v>
+        <v>0.0228800493847362</v>
       </c>
       <c r="G111" t="n">
-        <v>24.78011105578037</v>
+        <v>26.36535211046363</v>
       </c>
       <c r="H111" t="n">
         <v>0</v>
@@ -4032,7 +4032,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_6</t>
+          <t>Cogn_Eng2_7</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -4042,17 +4042,17 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_6</t>
+          <t>Cogn_Eng2_7</t>
         </is>
       </c>
       <c r="E112" t="n">
-        <v>0.6033155355028393</v>
+        <v>0.6376100036009857</v>
       </c>
       <c r="F112" t="n">
-        <v>0.02287407401643528</v>
+        <v>0.02659579548646459</v>
       </c>
       <c r="G112" t="n">
-        <v>26.37551732336684</v>
+        <v>23.97409033700499</v>
       </c>
       <c r="H112" t="n">
         <v>0</v>
@@ -4064,7 +4064,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_7</t>
+          <t>Cogn_Eng2_8</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -4074,17 +4074,17 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_7</t>
+          <t>Cogn_Eng2_8</t>
         </is>
       </c>
       <c r="E113" t="n">
-        <v>0.6373164571180598</v>
+        <v>0.6577799779168642</v>
       </c>
       <c r="F113" t="n">
-        <v>0.02657427034220513</v>
+        <v>0.02461202612923326</v>
       </c>
       <c r="G113" t="n">
-        <v>23.98246306999799</v>
+        <v>26.72595805141176</v>
       </c>
       <c r="H113" t="n">
         <v>0</v>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_8</t>
+          <t>Depr_1</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -4106,17 +4106,17 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_8</t>
+          <t>Depr_1</t>
         </is>
       </c>
       <c r="E114" t="n">
-        <v>0.6578543411792062</v>
+        <v>0.5394599439125016</v>
       </c>
       <c r="F114" t="n">
-        <v>0.02460673704787304</v>
+        <v>0.022664215362693</v>
       </c>
       <c r="G114" t="n">
-        <v>26.73472471675537</v>
+        <v>23.80227752233113</v>
       </c>
       <c r="H114" t="n">
         <v>0</v>
@@ -4128,7 +4128,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Depr_1</t>
+          <t>Depr_2</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -4138,17 +4138,17 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Depr_1</t>
+          <t>Depr_2</t>
         </is>
       </c>
       <c r="E115" t="n">
-        <v>0.5395530129995965</v>
+        <v>0.6340915581487429</v>
       </c>
       <c r="F115" t="n">
-        <v>0.02265673152701949</v>
+        <v>0.02667844838815561</v>
       </c>
       <c r="G115" t="n">
-        <v>23.81424753752912</v>
+        <v>23.76793241118519</v>
       </c>
       <c r="H115" t="n">
         <v>0</v>
@@ -4160,7 +4160,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Depr_2</t>
+          <t>Depr_3</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -4170,17 +4170,17 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Depr_2</t>
+          <t>Depr_3</t>
         </is>
       </c>
       <c r="E116" t="n">
-        <v>0.6323617769634136</v>
+        <v>1.188047444149484</v>
       </c>
       <c r="F116" t="n">
-        <v>0.02660804099855945</v>
+        <v>0.04468464934850341</v>
       </c>
       <c r="G116" t="n">
-        <v>23.76581488933678</v>
+        <v>26.58737310115397</v>
       </c>
       <c r="H116" t="n">
         <v>0</v>
@@ -4192,7 +4192,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Depr_3</t>
+          <t>Depr_4</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -4202,17 +4202,17 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Depr_3</t>
+          <t>Depr_4</t>
         </is>
       </c>
       <c r="E117" t="n">
-        <v>1.185441346200605</v>
+        <v>0.5969473810728411</v>
       </c>
       <c r="F117" t="n">
-        <v>0.04457632784686411</v>
+        <v>0.02333356501537052</v>
       </c>
       <c r="G117" t="n">
-        <v>26.59351730915192</v>
+        <v>25.58320516620716</v>
       </c>
       <c r="H117" t="n">
         <v>0</v>
@@ -4224,7 +4224,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Depr_4</t>
+          <t>Depr_5</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -4234,17 +4234,17 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Depr_4</t>
+          <t>Depr_5</t>
         </is>
       </c>
       <c r="E118" t="n">
-        <v>0.5961007352495121</v>
+        <v>0.8240616957500504</v>
       </c>
       <c r="F118" t="n">
-        <v>0.02328487157210939</v>
+        <v>0.0315235088559412</v>
       </c>
       <c r="G118" t="n">
-        <v>25.60034455753328</v>
+        <v>26.14117925418062</v>
       </c>
       <c r="H118" t="n">
         <v>0</v>
@@ -4256,7 +4256,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Depr_5</t>
+          <t>Depr_6</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -4266,17 +4266,17 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Depr_5</t>
+          <t>Depr_6</t>
         </is>
       </c>
       <c r="E119" t="n">
-        <v>0.824187079475788</v>
+        <v>0.6410766413210043</v>
       </c>
       <c r="F119" t="n">
-        <v>0.03151683480967152</v>
+        <v>0.02497517078937802</v>
       </c>
       <c r="G119" t="n">
-        <v>26.15069325415636</v>
+        <v>25.66855885397935</v>
       </c>
       <c r="H119" t="n">
         <v>0</v>
@@ -4288,7 +4288,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Depr_6</t>
+          <t>Depr_7</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -4298,17 +4298,17 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Depr_6</t>
+          <t>Depr_7</t>
         </is>
       </c>
       <c r="E120" t="n">
-        <v>0.6505181552042845</v>
+        <v>0.5885133215907676</v>
       </c>
       <c r="F120" t="n">
-        <v>0.02528887277068355</v>
+        <v>0.02309470513406693</v>
       </c>
       <c r="G120" t="n">
-        <v>25.72349353319862</v>
+        <v>25.48260816273297</v>
       </c>
       <c r="H120" t="n">
         <v>0</v>
@@ -4320,7 +4320,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Depr_7</t>
+          <t>Depr_8</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -4330,17 +4330,17 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Depr_7</t>
+          <t>Depr_8</t>
         </is>
       </c>
       <c r="E121" t="n">
-        <v>0.5888393410357972</v>
+        <v>0.8050840567164395</v>
       </c>
       <c r="F121" t="n">
-        <v>0.02310023661276671</v>
+        <v>0.03145986670671991</v>
       </c>
       <c r="G121" t="n">
-        <v>25.49061946339006</v>
+        <v>25.59082860064631</v>
       </c>
       <c r="H121" t="n">
         <v>0</v>
@@ -4352,7 +4352,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Depr_8</t>
+          <t>Hulp_1</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -4362,17 +4362,17 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Depr_8</t>
+          <t>Hulp_1</t>
         </is>
       </c>
       <c r="E122" t="n">
-        <v>0.8036111409899476</v>
+        <v>2.220184044048251</v>
       </c>
       <c r="F122" t="n">
-        <v>0.03139466015546345</v>
+        <v>0.08076136096005243</v>
       </c>
       <c r="G122" t="n">
-        <v>25.59706450029854</v>
+        <v>27.49067149969087</v>
       </c>
       <c r="H122" t="n">
         <v>0</v>
@@ -4384,7 +4384,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Hulp_1</t>
+          <t>Hulp_2</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -4394,17 +4394,17 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Hulp_1</t>
+          <t>Hulp_2</t>
         </is>
       </c>
       <c r="E123" t="n">
-        <v>2.219837793334615</v>
+        <v>1.165404211770473</v>
       </c>
       <c r="F123" t="n">
-        <v>0.08072369602637006</v>
+        <v>0.04239189132906862</v>
       </c>
       <c r="G123" t="n">
-        <v>27.49920906225553</v>
+        <v>27.4912058699266</v>
       </c>
       <c r="H123" t="n">
         <v>0</v>
@@ -4416,7 +4416,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Hulp_2</t>
+          <t>Hulp_3</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -4426,17 +4426,17 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Hulp_2</t>
+          <t>Hulp_3</t>
         </is>
       </c>
       <c r="E124" t="n">
-        <v>1.164840029438092</v>
+        <v>1.951067778967532</v>
       </c>
       <c r="F124" t="n">
-        <v>0.04235713136138665</v>
+        <v>0.07095968566389844</v>
       </c>
       <c r="G124" t="n">
-        <v>27.50044660655363</v>
+        <v>27.49543999083221</v>
       </c>
       <c r="H124" t="n">
         <v>0</v>
@@ -4448,7 +4448,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Hulp_3</t>
+          <t>Leefst</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -4458,17 +4458,17 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Hulp_3</t>
+          <t>Leefst</t>
         </is>
       </c>
       <c r="E125" t="n">
-        <v>1.950326828680532</v>
+        <v>0.5871154848332156</v>
       </c>
       <c r="F125" t="n">
-        <v>0.07090931202979102</v>
+        <v>0.02136967639111037</v>
       </c>
       <c r="G125" t="n">
-        <v>27.50452335278108</v>
+        <v>27.47423377220524</v>
       </c>
       <c r="H125" t="n">
         <v>0</v>
@@ -4480,7 +4480,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Leefst</t>
+          <t>Mot_Stress_1</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -4490,17 +4490,17 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Leefst</t>
+          <t>Mot_Stress_1</t>
         </is>
       </c>
       <c r="E126" t="n">
-        <v>0.5867886534637434</v>
+        <v>0.3232325320167361</v>
       </c>
       <c r="F126" t="n">
-        <v>0.02135094593699364</v>
+        <v>0.01349760775489848</v>
       </c>
       <c r="G126" t="n">
-        <v>27.48302839452013</v>
+        <v>23.94739407621939</v>
       </c>
       <c r="H126" t="n">
         <v>0</v>
@@ -4512,7 +4512,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Mot_Stress_1</t>
+          <t>Mot_Stress_2</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -4522,17 +4522,17 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Mot_Stress_1</t>
+          <t>Mot_Stress_2</t>
         </is>
       </c>
       <c r="E127" t="n">
-        <v>0.3225388580336419</v>
+        <v>0.5654274144347237</v>
       </c>
       <c r="F127" t="n">
-        <v>0.01347559153299387</v>
+        <v>0.02152392262696794</v>
       </c>
       <c r="G127" t="n">
-        <v>23.93504264506661</v>
+        <v>26.26971970713246</v>
       </c>
       <c r="H127" t="n">
         <v>0</v>
@@ -4544,7 +4544,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Mot_Stress_2</t>
+          <t>Mot_Stress_4</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -4554,17 +4554,17 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Mot_Stress_2</t>
+          <t>Mot_Stress_4</t>
         </is>
       </c>
       <c r="E128" t="n">
-        <v>0.5650212907193957</v>
+        <v>0.2143452128133303</v>
       </c>
       <c r="F128" t="n">
-        <v>0.02150628058780372</v>
+        <v>0.009949030810029388</v>
       </c>
       <c r="G128" t="n">
-        <v>26.27238533349874</v>
+        <v>21.54433098907579</v>
       </c>
       <c r="H128" t="n">
         <v>0</v>
@@ -4576,7 +4576,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Mot_Stress_4</t>
+          <t>Onnodige_stress_1</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -4586,17 +4586,17 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Mot_Stress_4</t>
+          <t>Onnodige_stress_1</t>
         </is>
       </c>
       <c r="E129" t="n">
-        <v>0.2135929773014994</v>
+        <v>0.9949845818475272</v>
       </c>
       <c r="F129" t="n">
-        <v>0.009929907877030932</v>
+        <v>0.03845966088203257</v>
       </c>
       <c r="G129" t="n">
-        <v>21.51006634956357</v>
+        <v>25.8708620669739</v>
       </c>
       <c r="H129" t="n">
         <v>0</v>
@@ -4608,7 +4608,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Onnodige_stress_1</t>
+          <t>Onnodige_stress_10</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -4618,17 +4618,17 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Onnodige_stress_1</t>
+          <t>Onnodige_stress_10</t>
         </is>
       </c>
       <c r="E130" t="n">
-        <v>0.9943947595395821</v>
+        <v>1.519813478578892</v>
       </c>
       <c r="F130" t="n">
-        <v>0.03842931496214422</v>
+        <v>0.05637156251240794</v>
       </c>
       <c r="G130" t="n">
-        <v>25.87594289654292</v>
+        <v>26.9606413378626</v>
       </c>
       <c r="H130" t="n">
         <v>0</v>
@@ -4640,7 +4640,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Onnodige_stress_10</t>
+          <t>Onnodige_stress_2</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -4650,17 +4650,17 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Onnodige_stress_10</t>
+          <t>Onnodige_stress_2</t>
         </is>
       </c>
       <c r="E131" t="n">
-        <v>1.520968195220356</v>
+        <v>0.7575266315114741</v>
       </c>
       <c r="F131" t="n">
-        <v>0.05638314126855246</v>
+        <v>0.03085475730545647</v>
       </c>
       <c r="G131" t="n">
-        <v>26.97558456257378</v>
+        <v>24.55137222398308</v>
       </c>
       <c r="H131" t="n">
         <v>0</v>
@@ -4672,7 +4672,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Onnodige_stress_2</t>
+          <t>Onnodige_stress_3</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -4682,17 +4682,17 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Onnodige_stress_2</t>
+          <t>Onnodige_stress_3</t>
         </is>
       </c>
       <c r="E132" t="n">
-        <v>0.7569492900342515</v>
+        <v>0.833380281528912</v>
       </c>
       <c r="F132" t="n">
-        <v>0.03082475323434567</v>
+        <v>0.03315734393537369</v>
       </c>
       <c r="G132" t="n">
-        <v>24.55654013691452</v>
+        <v>25.13410854404088</v>
       </c>
       <c r="H132" t="n">
         <v>0</v>
@@ -4704,7 +4704,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Onnodige_stress_3</t>
+          <t>Onnodige_stress_4</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -4714,17 +4714,17 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Onnodige_stress_3</t>
+          <t>Onnodige_stress_4</t>
         </is>
       </c>
       <c r="E133" t="n">
-        <v>0.8338953373583715</v>
+        <v>0.639476890978214</v>
       </c>
       <c r="F133" t="n">
-        <v>0.03314557807168964</v>
+        <v>0.02813027999580914</v>
       </c>
       <c r="G133" t="n">
-        <v>25.15856973529332</v>
+        <v>22.73268844287191</v>
       </c>
       <c r="H133" t="n">
         <v>0</v>
@@ -4736,7 +4736,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Onnodige_stress_4</t>
+          <t>Onnodige_stress_5</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -4746,17 +4746,17 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Onnodige_stress_4</t>
+          <t>Onnodige_stress_5</t>
         </is>
       </c>
       <c r="E134" t="n">
-        <v>0.638727027884055</v>
+        <v>0.6019214530159964</v>
       </c>
       <c r="F134" t="n">
-        <v>0.02809882895878991</v>
+        <v>0.026672272171196</v>
       </c>
       <c r="G134" t="n">
-        <v>22.73144652391345</v>
+        <v>22.56731069366704</v>
       </c>
       <c r="H134" t="n">
         <v>0</v>
@@ -4768,7 +4768,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Onnodige_stress_5</t>
+          <t>Onnodige_stress_6</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -4778,17 +4778,17 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>Onnodige_stress_5</t>
+          <t>Onnodige_stress_6</t>
         </is>
       </c>
       <c r="E135" t="n">
-        <v>0.6014375154032539</v>
+        <v>0.7039111710977911</v>
       </c>
       <c r="F135" t="n">
-        <v>0.02665892586449648</v>
+        <v>0.02930165011486789</v>
       </c>
       <c r="G135" t="n">
-        <v>22.56045567768614</v>
+        <v>24.02291912961578</v>
       </c>
       <c r="H135" t="n">
         <v>0</v>
@@ -4800,7 +4800,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Onnodige_stress_6</t>
+          <t>Onnodige_stress_7</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -4810,17 +4810,17 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Onnodige_stress_6</t>
+          <t>Onnodige_stress_7</t>
         </is>
       </c>
       <c r="E136" t="n">
-        <v>0.7034354460637114</v>
+        <v>1.431618821493212</v>
       </c>
       <c r="F136" t="n">
-        <v>0.02928190578195319</v>
+        <v>0.05406647989946418</v>
       </c>
       <c r="G136" t="n">
-        <v>24.02287102751436</v>
+        <v>26.47886128575056</v>
       </c>
       <c r="H136" t="n">
         <v>0</v>
@@ -4832,7 +4832,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Onnodige_stress_7</t>
+          <t>Onnodige_stress_8</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -4842,17 +4842,17 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Onnodige_stress_7</t>
+          <t>Onnodige_stress_8</t>
         </is>
       </c>
       <c r="E137" t="n">
-        <v>1.431166233262962</v>
+        <v>0.9622363299636767</v>
       </c>
       <c r="F137" t="n">
-        <v>0.05402380658836785</v>
+        <v>0.03750371273557868</v>
       </c>
       <c r="G137" t="n">
-        <v>26.49139932217628</v>
+        <v>25.65709525140358</v>
       </c>
       <c r="H137" t="n">
         <v>0</v>
@@ -4864,7 +4864,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Onnodige_stress_8</t>
+          <t>Onnodige_stress_9</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -4874,17 +4874,17 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Onnodige_stress_8</t>
+          <t>Onnodige_stress_9</t>
         </is>
       </c>
       <c r="E138" t="n">
-        <v>0.9621059244475102</v>
+        <v>0.8387957349329741</v>
       </c>
       <c r="F138" t="n">
-        <v>0.03747806128718796</v>
+        <v>0.03395662795514795</v>
       </c>
       <c r="G138" t="n">
-        <v>25.67117645305573</v>
+        <v>24.70197382426213</v>
       </c>
       <c r="H138" t="n">
         <v>0</v>
@@ -4896,7 +4896,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Onnodige_stress_9</t>
+          <t>Partici1_1</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -4906,17 +4906,17 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Onnodige_stress_9</t>
+          <t>Partici1_1</t>
         </is>
       </c>
       <c r="E139" t="n">
-        <v>0.8383056257152561</v>
+        <v>0.8585736842804701</v>
       </c>
       <c r="F139" t="n">
-        <v>0.03393285760227082</v>
+        <v>0.03525010880589092</v>
       </c>
       <c r="G139" t="n">
-        <v>24.7048343383391</v>
+        <v>24.35662508118643</v>
       </c>
       <c r="H139" t="n">
         <v>0</v>
@@ -4928,7 +4928,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Partici1_1</t>
+          <t>Partici1_2</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -4938,17 +4938,17 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Partici1_1</t>
+          <t>Partici1_2</t>
         </is>
       </c>
       <c r="E140" t="n">
-        <v>0.8582168018208364</v>
+        <v>1.202636950171762</v>
       </c>
       <c r="F140" t="n">
-        <v>0.03523002311528514</v>
+        <v>0.04792715781400936</v>
       </c>
       <c r="G140" t="n">
-        <v>24.36038145612581</v>
+        <v>25.09301625633082</v>
       </c>
       <c r="H140" t="n">
         <v>0</v>
@@ -4960,7 +4960,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Partici1_2</t>
+          <t>Partici1_3</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -4970,17 +4970,17 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Partici1_2</t>
+          <t>Partici1_3</t>
         </is>
       </c>
       <c r="E141" t="n">
-        <v>1.204293543736476</v>
+        <v>1.108210185364095</v>
       </c>
       <c r="F141" t="n">
-        <v>0.04797646492562618</v>
+        <v>0.04311866256912878</v>
       </c>
       <c r="G141" t="n">
-        <v>25.10175657123317</v>
+        <v>25.7014044339081</v>
       </c>
       <c r="H141" t="n">
         <v>0</v>
@@ -4992,7 +4992,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Partici1_3</t>
+          <t>Partici1_4</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -5002,17 +5002,17 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>Partici1_3</t>
+          <t>Partici1_4</t>
         </is>
       </c>
       <c r="E142" t="n">
-        <v>1.108410996541822</v>
+        <v>1.150994327245557</v>
       </c>
       <c r="F142" t="n">
-        <v>0.04310929745034911</v>
+        <v>0.04398988200881549</v>
       </c>
       <c r="G142" t="n">
-        <v>25.71164602700186</v>
+        <v>26.16497873280804</v>
       </c>
       <c r="H142" t="n">
         <v>0</v>
@@ -5024,7 +5024,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Partici1_4</t>
+          <t>Q297_1</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -5034,17 +5034,17 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>Partici1_4</t>
+          <t>Q297_1</t>
         </is>
       </c>
       <c r="E143" t="n">
-        <v>1.150362815567634</v>
+        <v>0.2598536619380333</v>
       </c>
       <c r="F143" t="n">
-        <v>0.04395138652124105</v>
+        <v>0.009456102040047256</v>
       </c>
       <c r="G143" t="n">
-        <v>26.17352731262544</v>
+        <v>27.47999765760297</v>
       </c>
       <c r="H143" t="n">
         <v>0</v>
@@ -5056,7 +5056,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Q297_1</t>
+          <t>StopInt</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -5066,17 +5066,17 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Q297_1</t>
+          <t>StopInt</t>
         </is>
       </c>
       <c r="E144" t="n">
-        <v>0.2597003896841297</v>
+        <v>0.1155622167117403</v>
       </c>
       <c r="F144" t="n">
-        <v>0.009447352103327625</v>
+        <v>0.008331955643429997</v>
       </c>
       <c r="G144" t="n">
-        <v>27.48922521530309</v>
+        <v>13.86975899097529</v>
       </c>
       <c r="H144" t="n">
         <v>0</v>
@@ -5088,7 +5088,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>StPunt_beh</t>
+          <t>Stopint2</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -5098,17 +5098,17 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>StPunt_beh</t>
+          <t>Stopint2</t>
         </is>
       </c>
       <c r="E145" t="n">
-        <v>9.602850899705977</v>
+        <v>0.0274988847861541</v>
       </c>
       <c r="F145" t="n">
-        <v>0.3687223031956218</v>
+        <v>0.001134940829490693</v>
       </c>
       <c r="G145" t="n">
-        <v>26.04358569160174</v>
+        <v>24.22935544072806</v>
       </c>
       <c r="H145" t="n">
         <v>0</v>
@@ -5120,7 +5120,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>StopInt</t>
+          <t>Vertr</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -5130,17 +5130,17 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>StopInt</t>
+          <t>Vertr</t>
         </is>
       </c>
       <c r="E146" t="n">
-        <v>0.1155751789757329</v>
+        <v>1.038233502329363</v>
       </c>
       <c r="F146" t="n">
-        <v>0.008321641674167502</v>
+        <v>0.04194838616491448</v>
       </c>
       <c r="G146" t="n">
-        <v>13.888507038295</v>
+        <v>24.750260909274</v>
       </c>
       <c r="H146" t="n">
         <v>0</v>
@@ -5152,7 +5152,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Stopint2</t>
+          <t>Werk_1</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -5162,83 +5162,19 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Stopint2</t>
+          <t>Werk_1</t>
         </is>
       </c>
       <c r="E147" t="n">
-        <v>0.02819181170749526</v>
+        <v>0.7149625503284339</v>
       </c>
       <c r="F147" t="n">
-        <v>0.001025000232952494</v>
+        <v>0.02600320846261175</v>
       </c>
       <c r="G147" t="n">
-        <v>27.5042002661649</v>
+        <v>27.49516665718136</v>
       </c>
       <c r="H147" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" s="1" t="n">
-        <v>146</v>
-      </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>Vertr</t>
-        </is>
-      </c>
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D148" t="inlineStr">
-        <is>
-          <t>Vertr</t>
-        </is>
-      </c>
-      <c r="E148" t="n">
-        <v>1.037428785193426</v>
-      </c>
-      <c r="F148" t="n">
-        <v>0.04192102496031352</v>
-      </c>
-      <c r="G148" t="n">
-        <v>24.74721899454531</v>
-      </c>
-      <c r="H148" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" s="1" t="n">
-        <v>147</v>
-      </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>Werk_1</t>
-        </is>
-      </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D149" t="inlineStr">
-        <is>
-          <t>Werk_1</t>
-        </is>
-      </c>
-      <c r="E149" t="n">
-        <v>0.715319337495336</v>
-      </c>
-      <c r="F149" t="n">
-        <v>0.02600774526631718</v>
-      </c>
-      <c r="G149" t="n">
-        <v>27.50408888363911</v>
-      </c>
-      <c r="H149" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working code with the updated data frame
</commit_message>
<xml_diff>
--- a/model_coefficients.xlsx
+++ b/model_coefficients.xlsx
@@ -490,13 +490,13 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>-1.811461555235611</v>
+        <v>-1.835842957812327</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2136439251191585</v>
+        <v>0.2189416654273608</v>
       </c>
       <c r="G2" t="n">
-        <v>-8.47888164485277</v>
+        <v>-8.385078071916956</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -522,16 +522,16 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>-0.4579472678390026</v>
+        <v>-0.4420866522022651</v>
       </c>
       <c r="F3" t="n">
-        <v>0.09768247683665833</v>
+        <v>0.09297007425655235</v>
       </c>
       <c r="G3" t="n">
-        <v>-4.688120967694952</v>
+        <v>-4.755150038684114</v>
       </c>
       <c r="H3" t="n">
-        <v>2.757250264995292e-06</v>
+        <v>1.98299089659848e-06</v>
       </c>
     </row>
     <row r="4">
@@ -554,16 +554,16 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.9049876664432835</v>
+        <v>0.9185031370564757</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1251008329306027</v>
+        <v>0.1278669578877122</v>
       </c>
       <c r="G4" t="n">
-        <v>7.234065874989608</v>
+        <v>7.183271990062409</v>
       </c>
       <c r="H4" t="n">
-        <v>4.687361609967411e-13</v>
+        <v>6.80566714095221e-13</v>
       </c>
     </row>
     <row r="5">
@@ -586,16 +586,16 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1.368860394810905</v>
+        <v>1.317743844535169</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2019950323433156</v>
+        <v>0.1886409801497791</v>
       </c>
       <c r="G5" t="n">
-        <v>6.776703263066293</v>
+        <v>6.985459063464937</v>
       </c>
       <c r="H5" t="n">
-        <v>1.229483181930391e-11</v>
+        <v>2.839284363176375e-12</v>
       </c>
     </row>
     <row r="6">
@@ -618,16 +618,16 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.08614383127981287</v>
+        <v>0.08420945047963496</v>
       </c>
       <c r="F6" t="n">
-        <v>0.01859125420171105</v>
+        <v>0.01860953746522926</v>
       </c>
       <c r="G6" t="n">
-        <v>4.633567501177573</v>
+        <v>4.525069504411377</v>
       </c>
       <c r="H6" t="n">
-        <v>3.594174915910742e-06</v>
+        <v>6.037566035788089e-06</v>
       </c>
     </row>
     <row r="7">
@@ -650,13 +650,13 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>-0.2732136864066098</v>
+        <v>-0.2780459082178542</v>
       </c>
       <c r="F7" t="n">
-        <v>0.02304331080848166</v>
+        <v>0.02316451192926945</v>
       </c>
       <c r="G7" t="n">
-        <v>-11.85652915353597</v>
+        <v>-12.00309806029313</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -682,16 +682,16 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0.1800263527287751</v>
+        <v>0.187023303780533</v>
       </c>
       <c r="F8" t="n">
-        <v>0.02734843004647206</v>
+        <v>0.02640989962954342</v>
       </c>
       <c r="G8" t="n">
-        <v>6.58269423203749</v>
+        <v>7.081560566183974</v>
       </c>
       <c r="H8" t="n">
-        <v>4.619993276833156e-11</v>
+        <v>1.425304319013776e-12</v>
       </c>
     </row>
     <row r="9">
@@ -714,16 +714,16 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>-0.008943775155867639</v>
+        <v>0.001518006928348461</v>
       </c>
       <c r="F9" t="n">
-        <v>0.02050187103311797</v>
+        <v>0.01566673474574194</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.4362418991410078</v>
+        <v>0.09689363820142206</v>
       </c>
       <c r="H9" t="n">
-        <v>0.6626612313734306</v>
+        <v>0.9228108610158714</v>
       </c>
     </row>
     <row r="10">
@@ -784,13 +784,13 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1.147872229776404</v>
+        <v>1.151872024844843</v>
       </c>
       <c r="F11" t="n">
-        <v>0.04405069793672251</v>
+        <v>0.04425295736751178</v>
       </c>
       <c r="G11" t="n">
-        <v>26.0579805432193</v>
+        <v>26.02926659234888</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -816,13 +816,13 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1.084548967152891</v>
+        <v>1.087437272233255</v>
       </c>
       <c r="F12" t="n">
-        <v>0.04690892649043481</v>
+        <v>0.04710320924457956</v>
       </c>
       <c r="G12" t="n">
-        <v>23.12031095725289</v>
+        <v>23.08626714930908</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -848,13 +848,13 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>1.227802405663815</v>
+        <v>1.232548789002741</v>
       </c>
       <c r="F13" t="n">
-        <v>0.05029107558685367</v>
+        <v>0.0505195846315663</v>
       </c>
       <c r="G13" t="n">
-        <v>24.41392217827918</v>
+        <v>24.39744502982724</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -880,13 +880,13 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0.9868077330619099</v>
+        <v>0.9904602816396002</v>
       </c>
       <c r="F14" t="n">
-        <v>0.048098185145929</v>
+        <v>0.04826654537642128</v>
       </c>
       <c r="G14" t="n">
-        <v>20.51652739178073</v>
+        <v>20.52063751185578</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -912,13 +912,13 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0.8109226327453519</v>
+        <v>0.8130781194260529</v>
       </c>
       <c r="F15" t="n">
-        <v>0.05210020898903077</v>
+        <v>0.052265970317738</v>
       </c>
       <c r="G15" t="n">
-        <v>15.56467139892893</v>
+        <v>15.55654883029225</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -944,13 +944,13 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.6818219743570147</v>
+        <v>0.6842294080193208</v>
       </c>
       <c r="F16" t="n">
-        <v>0.04862768680320669</v>
+        <v>0.04877658216252276</v>
       </c>
       <c r="G16" t="n">
-        <v>14.02127099120067</v>
+        <v>14.02782601137267</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -976,13 +976,13 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0.7736397366488263</v>
+        <v>0.7752830109821204</v>
       </c>
       <c r="F17" t="n">
-        <v>0.04633734765799993</v>
+        <v>0.0464864477719153</v>
       </c>
       <c r="G17" t="n">
-        <v>16.6958139758473</v>
+        <v>16.67761354383005</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1008,13 +1008,13 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>1.159245846515965</v>
+        <v>1.161277886885324</v>
       </c>
       <c r="F18" t="n">
-        <v>0.046144733575259</v>
+        <v>0.04633574472340665</v>
       </c>
       <c r="G18" t="n">
-        <v>25.12195339908487</v>
+        <v>25.06224716560213</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -1040,13 +1040,13 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>1.220908267036182</v>
+        <v>1.222079676271399</v>
       </c>
       <c r="F19" t="n">
-        <v>0.04507010343098306</v>
+        <v>0.04525950843753337</v>
       </c>
       <c r="G19" t="n">
-        <v>27.08909396843741</v>
+        <v>27.00161178133644</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -1110,16 +1110,16 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0.8488922014642085</v>
+        <v>0.81979392161138</v>
       </c>
       <c r="F21" t="n">
-        <v>0.1994644392982965</v>
+        <v>0.1904329602910399</v>
       </c>
       <c r="G21" t="n">
-        <v>4.255857357062255</v>
+        <v>4.304895120856069</v>
       </c>
       <c r="H21" t="n">
-        <v>2.082494505772914e-05</v>
+        <v>1.670648639184869e-05</v>
       </c>
     </row>
     <row r="22">
@@ -1142,16 +1142,16 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0.6442924326005111</v>
+        <v>0.6256053415687026</v>
       </c>
       <c r="F22" t="n">
-        <v>0.1870831246661086</v>
+        <v>0.1795796104594407</v>
       </c>
       <c r="G22" t="n">
-        <v>3.443883213662109</v>
+        <v>3.483721453480468</v>
       </c>
       <c r="H22" t="n">
-        <v>0.0005734233340419781</v>
+        <v>0.0004944938391127085</v>
       </c>
     </row>
     <row r="23">
@@ -1174,16 +1174,16 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>1.021057890471604</v>
+        <v>0.989660567154102</v>
       </c>
       <c r="F23" t="n">
-        <v>0.2034362279811195</v>
+        <v>0.1936126083763608</v>
       </c>
       <c r="G23" t="n">
-        <v>5.019056343107912</v>
+        <v>5.111550200414651</v>
       </c>
       <c r="H23" t="n">
-        <v>5.192591980840433e-07</v>
+        <v>3.19525888636818e-07</v>
       </c>
     </row>
     <row r="24">
@@ -1206,16 +1206,16 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0.4505983932631026</v>
+        <v>0.4359825919630195</v>
       </c>
       <c r="F24" t="n">
-        <v>0.1187281100570792</v>
+        <v>0.1137014106576623</v>
       </c>
       <c r="G24" t="n">
-        <v>3.795212380982731</v>
+        <v>3.834451916096823</v>
       </c>
       <c r="H24" t="n">
-        <v>0.0001475171220917115</v>
+        <v>0.0001258445861644919</v>
       </c>
     </row>
     <row r="25">
@@ -1238,16 +1238,16 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0.2820385011691007</v>
+        <v>0.2730334685656489</v>
       </c>
       <c r="F25" t="n">
-        <v>0.1540061937715988</v>
+        <v>0.1485227500904016</v>
       </c>
       <c r="G25" t="n">
-        <v>1.83134518333432</v>
+        <v>1.838327585488572</v>
       </c>
       <c r="H25" t="n">
-        <v>0.06704903761885173</v>
+        <v>0.06601414861129262</v>
       </c>
     </row>
     <row r="26">
@@ -1270,16 +1270,16 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0.3340913879189776</v>
+        <v>0.3238280528469518</v>
       </c>
       <c r="F26" t="n">
-        <v>0.1093282666873417</v>
+        <v>0.1050712213421764</v>
       </c>
       <c r="G26" t="n">
-        <v>3.055855526104337</v>
+        <v>3.081986187152873</v>
       </c>
       <c r="H26" t="n">
-        <v>0.002244193638919256</v>
+        <v>0.002056243788211898</v>
       </c>
     </row>
     <row r="27">
@@ -1302,16 +1302,16 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>1.310405617336163</v>
+        <v>1.265698078743571</v>
       </c>
       <c r="F27" t="n">
-        <v>0.2035994088530783</v>
+        <v>0.1913243969308348</v>
       </c>
       <c r="G27" t="n">
-        <v>6.436195589719731</v>
+        <v>6.615455734035399</v>
       </c>
       <c r="H27" t="n">
-        <v>1.225051171616087e-10</v>
+        <v>3.704081485977895e-11</v>
       </c>
     </row>
     <row r="28">
@@ -1334,16 +1334,16 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>1.294756778015404</v>
+        <v>1.249505915150312</v>
       </c>
       <c r="F28" t="n">
-        <v>0.2054807860711099</v>
+        <v>0.1932151884747342</v>
       </c>
       <c r="G28" t="n">
-        <v>6.301108744839199</v>
+        <v>6.466913522728762</v>
       </c>
       <c r="H28" t="n">
-        <v>2.955240496760325e-10</v>
+        <v>1.000248772697887e-10</v>
       </c>
     </row>
     <row r="29">
@@ -1366,16 +1366,16 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>-0.6540188788969351</v>
+        <v>-0.6293030590762514</v>
       </c>
       <c r="F29" t="n">
-        <v>0.1479534827168701</v>
+        <v>0.1409602694695458</v>
       </c>
       <c r="G29" t="n">
-        <v>-4.420435848367775</v>
+        <v>-4.464400227382842</v>
       </c>
       <c r="H29" t="n">
-        <v>9.850202548733478e-06</v>
+        <v>8.029335298864737e-06</v>
       </c>
     </row>
     <row r="30">
@@ -1398,16 +1398,16 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>1.095088693329959</v>
+        <v>1.057668469390711</v>
       </c>
       <c r="F30" t="n">
-        <v>0.1767193021320779</v>
+        <v>0.1663979353155412</v>
       </c>
       <c r="G30" t="n">
-        <v>6.196769000962362</v>
+        <v>6.356259573646109</v>
       </c>
       <c r="H30" t="n">
-        <v>5.76339864721831e-10</v>
+        <v>2.067255255866485e-10</v>
       </c>
     </row>
     <row r="31">
@@ -1430,16 +1430,16 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>1.883506657061228</v>
+        <v>1.817881086915973</v>
       </c>
       <c r="F31" t="n">
-        <v>0.2752106453481605</v>
+        <v>0.2574864551324883</v>
       </c>
       <c r="G31" t="n">
-        <v>6.843872825746321</v>
+        <v>7.060103747878824</v>
       </c>
       <c r="H31" t="n">
-        <v>7.708056415367537e-12</v>
+        <v>1.66378022470326e-12</v>
       </c>
     </row>
     <row r="32">
@@ -1462,16 +1462,16 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>2.057069626018855</v>
+        <v>1.986287170057503</v>
       </c>
       <c r="F32" t="n">
-        <v>0.3045539837110131</v>
+        <v>0.2853023601456039</v>
       </c>
       <c r="G32" t="n">
-        <v>6.754367816656192</v>
+        <v>6.962042546850437</v>
       </c>
       <c r="H32" t="n">
-        <v>1.434585783499642e-11</v>
+        <v>3.353761712787673e-12</v>
       </c>
     </row>
     <row r="33">
@@ -1494,16 +1494,16 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>2.346324769447845</v>
+        <v>2.265817457793731</v>
       </c>
       <c r="F33" t="n">
-        <v>0.3408669575365644</v>
+        <v>0.3189386297510006</v>
       </c>
       <c r="G33" t="n">
-        <v>6.883403385290796</v>
+        <v>7.104242780360532</v>
       </c>
       <c r="H33" t="n">
-        <v>5.843991957021899e-12</v>
+        <v>1.209921052236496e-12</v>
       </c>
     </row>
     <row r="34">
@@ -1526,16 +1526,16 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>1.36897591674928</v>
+        <v>1.321431034074632</v>
       </c>
       <c r="F34" t="n">
-        <v>0.2114993544981714</v>
+        <v>0.1985860858518596</v>
       </c>
       <c r="G34" t="n">
-        <v>6.47271912479829</v>
+        <v>6.654197490219597</v>
       </c>
       <c r="H34" t="n">
-        <v>9.62547819227666e-11</v>
+        <v>2.848499214280764e-11</v>
       </c>
     </row>
     <row r="35">
@@ -1558,16 +1558,16 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>2.479295083434804</v>
+        <v>2.393264057014837</v>
       </c>
       <c r="F35" t="n">
-        <v>0.3564191253624828</v>
+        <v>0.3331458231680656</v>
       </c>
       <c r="G35" t="n">
-        <v>6.956122460898734</v>
+        <v>7.183833296328912</v>
       </c>
       <c r="H35" t="n">
-        <v>3.497646616779093e-12</v>
+        <v>6.779021788361206e-13</v>
       </c>
     </row>
     <row r="36">
@@ -1590,16 +1590,16 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>-0.1781857893056666</v>
+        <v>-0.172082474161993</v>
       </c>
       <c r="F36" t="n">
-        <v>0.1826519109425302</v>
+        <v>0.176402837892043</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.97554845380597</v>
+        <v>-0.975508536128713</v>
       </c>
       <c r="H36" t="n">
-        <v>0.3292882790736742</v>
+        <v>0.3293080695334072</v>
       </c>
     </row>
     <row r="37">
@@ -1622,16 +1622,16 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>0.1132071082761124</v>
+        <v>0.1095216620585564</v>
       </c>
       <c r="F37" t="n">
-        <v>0.1320390074703716</v>
+        <v>0.1275516256813871</v>
       </c>
       <c r="G37" t="n">
-        <v>0.857376243915327</v>
+        <v>0.8586457559645178</v>
       </c>
       <c r="H37" t="n">
-        <v>0.391236983924343</v>
+        <v>0.3905359858892541</v>
       </c>
     </row>
     <row r="38">
@@ -1654,16 +1654,16 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>-0.01414351935858683</v>
+        <v>-0.008540598050058636</v>
       </c>
       <c r="F38" t="n">
-        <v>0.1696295405487822</v>
+        <v>0.1639613504258576</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.08337886969891332</v>
+        <v>-0.05208909311751832</v>
       </c>
       <c r="H38" t="n">
-        <v>0.9335502895370742</v>
+        <v>0.9584577036003972</v>
       </c>
     </row>
     <row r="39">
@@ -1686,16 +1686,16 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>2.714997933408478</v>
+        <v>2.623878536756999</v>
       </c>
       <c r="F39" t="n">
-        <v>0.3920651182116728</v>
+        <v>0.3669591560899239</v>
       </c>
       <c r="G39" t="n">
-        <v>6.92486479232194</v>
+        <v>7.150328567103157</v>
       </c>
       <c r="H39" t="n">
-        <v>4.36384262059164e-12</v>
+        <v>8.657519146026971e-13</v>
       </c>
     </row>
     <row r="40">
@@ -1718,16 +1718,16 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>2.81011502881409</v>
+        <v>2.715431609242283</v>
       </c>
       <c r="F40" t="n">
-        <v>0.410915142439047</v>
+        <v>0.3848174434536169</v>
       </c>
       <c r="G40" t="n">
-        <v>6.838674798225742</v>
+        <v>7.056415075327856</v>
       </c>
       <c r="H40" t="n">
-        <v>7.992939643486352e-12</v>
+        <v>1.708633234898116e-12</v>
       </c>
     </row>
     <row r="41">
@@ -1750,16 +1750,16 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>2.330077026712831</v>
+        <v>2.253254211402137</v>
       </c>
       <c r="F41" t="n">
-        <v>0.346707197722038</v>
+        <v>0.3252710722421209</v>
       </c>
       <c r="G41" t="n">
-        <v>6.720590290641093</v>
+        <v>6.927312028897433</v>
       </c>
       <c r="H41" t="n">
-        <v>1.809907779204423e-11</v>
+        <v>4.289013588731905e-12</v>
       </c>
     </row>
     <row r="42">
@@ -1782,16 +1782,16 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>2.047201600442456</v>
+        <v>1.979798384953577</v>
       </c>
       <c r="F42" t="n">
-        <v>0.3116480254286098</v>
+        <v>0.2928123094683205</v>
       </c>
       <c r="G42" t="n">
-        <v>6.568954183554893</v>
+        <v>6.761322256368496</v>
       </c>
       <c r="H42" t="n">
-        <v>5.066991271007737e-11</v>
+        <v>1.367372881588835e-11</v>
       </c>
     </row>
     <row r="43">
@@ -1814,16 +1814,16 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0.6885904533207026</v>
+        <v>0.6637252518124933</v>
       </c>
       <c r="F43" t="n">
-        <v>0.1755536953169581</v>
+        <v>0.1678462213610837</v>
       </c>
       <c r="G43" t="n">
-        <v>3.922392246278532</v>
+        <v>3.954365170846962</v>
       </c>
       <c r="H43" t="n">
-        <v>8.767410684673571e-05</v>
+        <v>7.673813079001057e-05</v>
       </c>
     </row>
     <row r="44">
@@ -1884,13 +1884,13 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>1.596501649134027</v>
+        <v>1.577665941152787</v>
       </c>
       <c r="F45" t="n">
-        <v>0.1652224600377128</v>
+        <v>0.1636824127505529</v>
       </c>
       <c r="G45" t="n">
-        <v>9.662739852438678</v>
+        <v>9.638579457815444</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
@@ -1954,16 +1954,16 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0.258313687932315</v>
+        <v>2.078140084277552</v>
       </c>
       <c r="F47" t="n">
-        <v>0.05410141470960337</v>
+        <v>0.3314136914452223</v>
       </c>
       <c r="G47" t="n">
-        <v>4.774619837837401</v>
+        <v>6.270531779206132</v>
       </c>
       <c r="H47" t="n">
-        <v>1.800470441182256e-06</v>
+        <v>3.598170650320753e-10</v>
       </c>
     </row>
     <row r="48">
@@ -2024,16 +2024,16 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>0.3417343126077159</v>
+        <v>0.3421789656486482</v>
       </c>
       <c r="F49" t="n">
-        <v>0.1303309747733193</v>
+        <v>0.1322890926683966</v>
       </c>
       <c r="G49" t="n">
-        <v>2.622049848084556</v>
+        <v>2.586599989039058</v>
       </c>
       <c r="H49" t="n">
-        <v>0.008740264607713932</v>
+        <v>0.009692804328955251</v>
       </c>
     </row>
     <row r="50">
@@ -2056,16 +2056,16 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0.1910413248175259</v>
+        <v>0.1943546739444523</v>
       </c>
       <c r="F50" t="n">
-        <v>0.08581128249352885</v>
+        <v>0.08716591170450448</v>
       </c>
       <c r="G50" t="n">
-        <v>2.22629611472951</v>
+        <v>2.229709643846689</v>
       </c>
       <c r="H50" t="n">
-        <v>0.02599435355716362</v>
+        <v>0.02576672523708612</v>
       </c>
     </row>
     <row r="51">
@@ -2088,13 +2088,13 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>-3.863051321704191</v>
+        <v>-3.909378600700168</v>
       </c>
       <c r="F51" t="n">
-        <v>0.4229276150364538</v>
+        <v>0.433614547898007</v>
       </c>
       <c r="G51" t="n">
-        <v>-9.134072083143794</v>
+        <v>-9.015792066115596</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -2120,13 +2120,13 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>-4.52952337397024</v>
+        <v>-4.585668229299648</v>
       </c>
       <c r="F52" t="n">
-        <v>0.4791102645256647</v>
+        <v>0.4917540236841477</v>
       </c>
       <c r="G52" t="n">
-        <v>-9.454031168472598</v>
+        <v>-9.325125994771089</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
@@ -2152,13 +2152,13 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>-4.243362961741653</v>
+        <v>-4.310670792199005</v>
       </c>
       <c r="F53" t="n">
-        <v>0.4538684305325283</v>
+        <v>0.4671237129597662</v>
       </c>
       <c r="G53" t="n">
-        <v>-9.349323892727071</v>
+        <v>-9.22811382208948</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -2184,13 +2184,13 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>-5.284940537384883</v>
+        <v>-5.348604531766081</v>
       </c>
       <c r="F54" t="n">
-        <v>0.5496432454403776</v>
+        <v>0.5641856270698578</v>
       </c>
       <c r="G54" t="n">
-        <v>-9.615219656053339</v>
+        <v>-9.480221180987892</v>
       </c>
       <c r="H54" t="n">
         <v>0</v>
@@ -2216,13 +2216,13 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>-5.218823328012321</v>
+        <v>-5.279210853395542</v>
       </c>
       <c r="F55" t="n">
-        <v>0.5422523165823219</v>
+        <v>0.556356152496617</v>
       </c>
       <c r="G55" t="n">
-        <v>-9.624344919161636</v>
+        <v>-9.488905316667914</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -2248,13 +2248,13 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>-4.741357105614218</v>
+        <v>-4.795726264569846</v>
       </c>
       <c r="F56" t="n">
-        <v>0.4981607181334246</v>
+        <v>0.5109479934817797</v>
       </c>
       <c r="G56" t="n">
-        <v>-9.517725772056561</v>
+        <v>-9.385938149753152</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -2280,13 +2280,13 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>-3.659092961567872</v>
+        <v>-3.713378812745065</v>
       </c>
       <c r="F57" t="n">
-        <v>0.4182956783273823</v>
+        <v>0.4294574139893254</v>
       </c>
       <c r="G57" t="n">
-        <v>-8.747623155444861</v>
+        <v>-8.64667529718958</v>
       </c>
       <c r="H57" t="n">
         <v>0</v>
@@ -2312,13 +2312,13 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>-4.030828925160329</v>
+        <v>-4.087692228233797</v>
       </c>
       <c r="F58" t="n">
-        <v>0.4376068117233252</v>
+        <v>0.4495496005275542</v>
       </c>
       <c r="G58" t="n">
-        <v>-9.211074455805297</v>
+        <v>-9.092861440490053</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -2344,13 +2344,13 @@
         </is>
       </c>
       <c r="E59" t="n">
-        <v>-4.645959223301104</v>
+        <v>-4.702869116145844</v>
       </c>
       <c r="F59" t="n">
-        <v>0.4925633140760001</v>
+        <v>0.5054674706758978</v>
       </c>
       <c r="G59" t="n">
-        <v>-9.432207171187791</v>
+        <v>-9.303999542933964</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -2376,16 +2376,16 @@
         </is>
       </c>
       <c r="E60" t="n">
-        <v>-2.726018024982228</v>
+        <v>-2.775145331817605</v>
       </c>
       <c r="F60" t="n">
-        <v>0.341552678595656</v>
+        <v>0.3506702246270046</v>
       </c>
       <c r="G60" t="n">
-        <v>-7.981252075617356</v>
+        <v>-7.9138322472674</v>
       </c>
       <c r="H60" t="n">
-        <v>1.554312234475219e-15</v>
+        <v>2.442490654175344e-15</v>
       </c>
     </row>
     <row r="61">
@@ -2408,16 +2408,16 @@
         </is>
       </c>
       <c r="E61" t="n">
-        <v>-0.05498447280274034</v>
+        <v>-0.04441472492636244</v>
       </c>
       <c r="F61" t="n">
-        <v>0.1388816298095526</v>
+        <v>0.1408263787695885</v>
       </c>
       <c r="G61" t="n">
-        <v>-0.3959088965023253</v>
+        <v>-0.3153864021364613</v>
       </c>
       <c r="H61" t="n">
-        <v>0.6921722377408632</v>
+        <v>0.7524682899421271</v>
       </c>
     </row>
     <row r="62">
@@ -2478,13 +2478,13 @@
         </is>
       </c>
       <c r="E63" t="n">
-        <v>1.069957674100311</v>
+        <v>1.069762331922792</v>
       </c>
       <c r="F63" t="n">
-        <v>0.04981311713831926</v>
+        <v>0.04984925720061331</v>
       </c>
       <c r="G63" t="n">
-        <v>21.47943625185735</v>
+        <v>21.45994528255819</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
@@ -2510,13 +2510,13 @@
         </is>
       </c>
       <c r="E64" t="n">
-        <v>0.920210219611306</v>
+        <v>0.9197509527167139</v>
       </c>
       <c r="F64" t="n">
-        <v>0.04975325852553179</v>
+        <v>0.04976903490294243</v>
       </c>
       <c r="G64" t="n">
-        <v>18.49547641428526</v>
+        <v>18.48038553473852</v>
       </c>
       <c r="H64" t="n">
         <v>0</v>
@@ -2542,13 +2542,13 @@
         </is>
       </c>
       <c r="E65" t="n">
-        <v>0.9598339681269217</v>
+        <v>0.9599488475101852</v>
       </c>
       <c r="F65" t="n">
-        <v>0.04872881036656646</v>
+        <v>0.0487842785977513</v>
       </c>
       <c r="G65" t="n">
-        <v>19.697463592622</v>
+        <v>19.67742221640142</v>
       </c>
       <c r="H65" t="n">
         <v>0</v>
@@ -2574,13 +2574,13 @@
         </is>
       </c>
       <c r="E66" t="n">
-        <v>1.258416611190769</v>
+        <v>1.260945466124432</v>
       </c>
       <c r="F66" t="n">
-        <v>0.05114925750169668</v>
+        <v>0.05127282588344639</v>
       </c>
       <c r="G66" t="n">
-        <v>24.60283242869016</v>
+        <v>24.59286072833641</v>
       </c>
       <c r="H66" t="n">
         <v>0</v>
@@ -2606,13 +2606,13 @@
         </is>
       </c>
       <c r="E67" t="n">
-        <v>1.370663093634589</v>
+        <v>1.373377711715323</v>
       </c>
       <c r="F67" t="n">
-        <v>0.05559089129998246</v>
+        <v>0.05574909455100785</v>
       </c>
       <c r="G67" t="n">
-        <v>24.65625323784592</v>
+        <v>24.63497789070118</v>
       </c>
       <c r="H67" t="n">
         <v>0</v>
@@ -2638,13 +2638,13 @@
         </is>
       </c>
       <c r="E68" t="n">
-        <v>0.9281539469563529</v>
+        <v>0.9300571758592652</v>
       </c>
       <c r="F68" t="n">
-        <v>0.0554688655058953</v>
+        <v>0.05558813737430393</v>
       </c>
       <c r="G68" t="n">
-        <v>16.73288138263752</v>
+        <v>16.73121676266959</v>
       </c>
       <c r="H68" t="n">
         <v>0</v>
@@ -2670,13 +2670,13 @@
         </is>
       </c>
       <c r="E69" t="n">
-        <v>-0.9510700014363189</v>
+        <v>-0.9555890912691544</v>
       </c>
       <c r="F69" t="n">
-        <v>0.04501777403792761</v>
+        <v>0.04517658156498004</v>
       </c>
       <c r="G69" t="n">
-        <v>-21.12654438697731</v>
+        <v>-21.15231073589585</v>
       </c>
       <c r="H69" t="n">
         <v>0</v>
@@ -2702,13 +2702,13 @@
         </is>
       </c>
       <c r="E70" t="n">
-        <v>0.9435146552620745</v>
+        <v>0.9452208234457582</v>
       </c>
       <c r="F70" t="n">
-        <v>0.0493433736107726</v>
+        <v>0.04942334599751207</v>
       </c>
       <c r="G70" t="n">
-        <v>19.12140549378581</v>
+        <v>19.12498646842354</v>
       </c>
       <c r="H70" t="n">
         <v>0</v>
@@ -2734,13 +2734,13 @@
         </is>
       </c>
       <c r="E71" t="n">
-        <v>-0.9610996317125207</v>
+        <v>-0.9680597059645693</v>
       </c>
       <c r="F71" t="n">
-        <v>0.04633259950995575</v>
+        <v>0.04633841516667089</v>
       </c>
       <c r="G71" t="n">
-        <v>-20.74348605208866</v>
+        <v>-20.89108361737756</v>
       </c>
       <c r="H71" t="n">
         <v>0</v>
@@ -2766,13 +2766,13 @@
         </is>
       </c>
       <c r="E72" t="n">
-        <v>0.9722869669455995</v>
+        <v>0.9733665627369689</v>
       </c>
       <c r="F72" t="n">
-        <v>0.04532576349568321</v>
+        <v>0.045390831694753</v>
       </c>
       <c r="G72" t="n">
-        <v>21.45108856283796</v>
+        <v>21.44412266471077</v>
       </c>
       <c r="H72" t="n">
         <v>0</v>
@@ -2798,13 +2798,13 @@
         </is>
       </c>
       <c r="E73" t="n">
-        <v>1.104743867160541</v>
+        <v>1.107409220116947</v>
       </c>
       <c r="F73" t="n">
-        <v>0.05228496291554879</v>
+        <v>0.05241617843436034</v>
       </c>
       <c r="G73" t="n">
-        <v>21.12928470321008</v>
+        <v>21.12724073317562</v>
       </c>
       <c r="H73" t="n">
         <v>0</v>
@@ -2830,13 +2830,13 @@
         </is>
       </c>
       <c r="E74" t="n">
-        <v>0.7452317109842855</v>
+        <v>0.7447978474881367</v>
       </c>
       <c r="F74" t="n">
-        <v>0.04016874324755349</v>
+        <v>0.04020936776825397</v>
       </c>
       <c r="G74" t="n">
-        <v>18.55252743091787</v>
+        <v>18.5229932428245</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -2862,16 +2862,16 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>0.001396915480678074</v>
+        <v>0.001396526346221992</v>
       </c>
       <c r="F75" t="n">
-        <v>0.001245513091245994</v>
+        <v>0.001270445480389538</v>
       </c>
       <c r="G75" t="n">
-        <v>1.121558247259417</v>
+        <v>1.099241460321898</v>
       </c>
       <c r="H75" t="n">
-        <v>0.2620503126326508</v>
+        <v>0.2716627588230394</v>
       </c>
     </row>
     <row r="76">
@@ -2894,16 +2894,16 @@
         </is>
       </c>
       <c r="E76" t="n">
-        <v>0.02799250039075023</v>
+        <v>0.02722193031437132</v>
       </c>
       <c r="F76" t="n">
-        <v>0.005733218837669639</v>
+        <v>0.00565626413963931</v>
       </c>
       <c r="G76" t="n">
-        <v>4.882510362581193</v>
+        <v>4.812704929882307</v>
       </c>
       <c r="H76" t="n">
-        <v>1.047437329759759e-06</v>
+        <v>1.489010573507699e-06</v>
       </c>
     </row>
     <row r="77">
@@ -2926,13 +2926,13 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>-0.09975178367173111</v>
+        <v>-0.09946302907139609</v>
       </c>
       <c r="F77" t="n">
-        <v>0.00921416703741661</v>
+        <v>0.009198361895717063</v>
       </c>
       <c r="G77" t="n">
-        <v>-10.82591440504998</v>
+        <v>-10.8131241397335</v>
       </c>
       <c r="H77" t="n">
         <v>0</v>
@@ -2958,13 +2958,13 @@
         </is>
       </c>
       <c r="E78" t="n">
-        <v>0.290672371502199</v>
+        <v>0.2905030897172218</v>
       </c>
       <c r="F78" t="n">
-        <v>0.02175128343540447</v>
+        <v>0.02176364432465294</v>
       </c>
       <c r="G78" t="n">
-        <v>13.36345840704321</v>
+        <v>13.34809030006083</v>
       </c>
       <c r="H78" t="n">
         <v>0</v>
@@ -2990,16 +2990,16 @@
         </is>
       </c>
       <c r="E79" t="n">
-        <v>0.05546669902243232</v>
+        <v>0.05945031375786577</v>
       </c>
       <c r="F79" t="n">
-        <v>0.01543178052073537</v>
+        <v>0.01597761013601245</v>
       </c>
       <c r="G79" t="n">
-        <v>3.594316219331173</v>
+        <v>3.720851444494063</v>
       </c>
       <c r="H79" t="n">
-        <v>0.0003252446266450715</v>
+        <v>0.0001985522168355125</v>
       </c>
     </row>
     <row r="80">
@@ -3022,16 +3022,16 @@
         </is>
       </c>
       <c r="E80" t="n">
-        <v>0.02783217045113324</v>
+        <v>0.02800158040625777</v>
       </c>
       <c r="F80" t="n">
-        <v>0.007213895165459327</v>
+        <v>0.007294021682337425</v>
       </c>
       <c r="G80" t="n">
-        <v>3.858133478365146</v>
+        <v>3.838976852814273</v>
       </c>
       <c r="H80" t="n">
-        <v>0.0001142562481333265</v>
+        <v>0.0001235480761407892</v>
       </c>
     </row>
     <row r="81">
@@ -3054,16 +3054,16 @@
         </is>
       </c>
       <c r="E81" t="n">
-        <v>0</v>
+        <v>1.444693933957835e-17</v>
       </c>
       <c r="F81" t="n">
-        <v>0.008048853465644207</v>
+        <v>0.004673906041651227</v>
       </c>
       <c r="G81" t="n">
-        <v>0</v>
+        <v>3.090977697827974e-15</v>
       </c>
       <c r="H81" t="n">
-        <v>1</v>
+        <v>0.9999999999999976</v>
       </c>
     </row>
     <row r="82">
@@ -3086,13 +3086,13 @@
         </is>
       </c>
       <c r="E82" t="n">
-        <v>0.180210252742617</v>
+        <v>0.1796333740922703</v>
       </c>
       <c r="F82" t="n">
-        <v>0.01413756754517003</v>
+        <v>0.01411691427379049</v>
       </c>
       <c r="G82" t="n">
-        <v>12.74690657739332</v>
+        <v>12.7246911467794</v>
       </c>
       <c r="H82" t="n">
         <v>0</v>
@@ -3118,13 +3118,13 @@
         </is>
       </c>
       <c r="E83" t="n">
-        <v>1.284946030752931</v>
+        <v>1.282480048871024</v>
       </c>
       <c r="F83" t="n">
-        <v>0.04720361477956644</v>
+        <v>0.04716468637882405</v>
       </c>
       <c r="G83" t="n">
-        <v>27.22134812611721</v>
+        <v>27.19153136189705</v>
       </c>
       <c r="H83" t="n">
         <v>0</v>
@@ -3150,13 +3150,13 @@
         </is>
       </c>
       <c r="E84" t="n">
-        <v>1.762704886407989</v>
+        <v>1.763065197962473</v>
       </c>
       <c r="F84" t="n">
-        <v>0.06443620216680128</v>
+        <v>0.06447034673753474</v>
       </c>
       <c r="G84" t="n">
-        <v>27.35581594051195</v>
+        <v>27.34691663925341</v>
       </c>
       <c r="H84" t="n">
         <v>0</v>
@@ -3182,13 +3182,13 @@
         </is>
       </c>
       <c r="E85" t="n">
-        <v>1.834111053295091</v>
+        <v>1.834645832860533</v>
       </c>
       <c r="F85" t="n">
-        <v>0.06688413310978948</v>
+        <v>0.06692774412438249</v>
       </c>
       <c r="G85" t="n">
-        <v>27.42221462685324</v>
+        <v>27.41233634624686</v>
       </c>
       <c r="H85" t="n">
         <v>0</v>
@@ -3214,13 +3214,13 @@
         </is>
       </c>
       <c r="E86" t="n">
-        <v>1.454092970175563</v>
+        <v>1.45406084015429</v>
       </c>
       <c r="F86" t="n">
-        <v>0.05337364628832652</v>
+        <v>0.05339348105536687</v>
       </c>
       <c r="G86" t="n">
-        <v>27.24365058915505</v>
+        <v>27.2329282786274</v>
       </c>
       <c r="H86" t="n">
         <v>0</v>
@@ -3246,13 +3246,13 @@
         </is>
       </c>
       <c r="E87" t="n">
-        <v>0.6922532645045439</v>
+        <v>0.6925536360403841</v>
       </c>
       <c r="F87" t="n">
-        <v>0.02526670220458729</v>
+        <v>0.02528628180719317</v>
       </c>
       <c r="G87" t="n">
-        <v>27.39784792142222</v>
+        <v>27.3885121305571</v>
       </c>
       <c r="H87" t="n">
         <v>0</v>
@@ -3278,13 +3278,13 @@
         </is>
       </c>
       <c r="E88" t="n">
-        <v>1.504220554087025</v>
+        <v>1.504816267309147</v>
       </c>
       <c r="F88" t="n">
-        <v>0.05472816257970088</v>
+        <v>0.05476808105450573</v>
       </c>
       <c r="G88" t="n">
-        <v>27.48531072770689</v>
+        <v>27.47615469280479</v>
       </c>
       <c r="H88" t="n">
         <v>0</v>
@@ -3310,13 +3310,13 @@
         </is>
       </c>
       <c r="E89" t="n">
-        <v>0.6654035590317982</v>
+        <v>0.6657353765856137</v>
       </c>
       <c r="F89" t="n">
-        <v>0.0242462832021295</v>
+        <v>0.02426672504114468</v>
       </c>
       <c r="G89" t="n">
-        <v>27.44352829079855</v>
+        <v>27.43408413905927</v>
       </c>
       <c r="H89" t="n">
         <v>0</v>
@@ -3342,13 +3342,13 @@
         </is>
       </c>
       <c r="E90" t="n">
-        <v>1.474300547888885</v>
+        <v>1.475154944526797</v>
       </c>
       <c r="F90" t="n">
-        <v>0.05383105689844023</v>
+        <v>0.05387888374888957</v>
       </c>
       <c r="G90" t="n">
-        <v>27.38754601536007</v>
+        <v>27.37909254717661</v>
       </c>
       <c r="H90" t="n">
         <v>0</v>
@@ -3374,13 +3374,13 @@
         </is>
       </c>
       <c r="E91" t="n">
-        <v>0.4230872340472651</v>
+        <v>0.4239115127861293</v>
       </c>
       <c r="F91" t="n">
-        <v>0.01659500836627871</v>
+        <v>0.01661766531996157</v>
       </c>
       <c r="G91" t="n">
-        <v>25.49484909459216</v>
+        <v>25.50969131935797</v>
       </c>
       <c r="H91" t="n">
         <v>0</v>
@@ -3406,13 +3406,13 @@
         </is>
       </c>
       <c r="E92" t="n">
-        <v>0.2530087422950345</v>
+        <v>0.2521084098183359</v>
       </c>
       <c r="F92" t="n">
-        <v>0.01097716886774649</v>
+        <v>0.01094332616176187</v>
       </c>
       <c r="G92" t="n">
-        <v>23.04863351564036</v>
+        <v>23.03764011678775</v>
       </c>
       <c r="H92" t="n">
         <v>0</v>
@@ -3438,13 +3438,13 @@
         </is>
       </c>
       <c r="E93" t="n">
-        <v>0.4276355811250254</v>
+        <v>0.4277772781540122</v>
       </c>
       <c r="F93" t="n">
-        <v>0.01699428179980424</v>
+        <v>0.01699812683571732</v>
       </c>
       <c r="G93" t="n">
-        <v>25.16349829533767</v>
+        <v>25.16614226162726</v>
       </c>
       <c r="H93" t="n">
         <v>0</v>
@@ -3470,13 +3470,13 @@
         </is>
       </c>
       <c r="E94" t="n">
-        <v>0.5245068322902149</v>
+        <v>0.5255060016144718</v>
       </c>
       <c r="F94" t="n">
-        <v>0.0208884733500962</v>
+        <v>0.02092480535633096</v>
       </c>
       <c r="G94" t="n">
-        <v>25.10986913568241</v>
+        <v>25.11402102148406</v>
       </c>
       <c r="H94" t="n">
         <v>0</v>
@@ -3502,13 +3502,13 @@
         </is>
       </c>
       <c r="E95" t="n">
-        <v>0.7093325942228816</v>
+        <v>0.7088152694664491</v>
       </c>
       <c r="F95" t="n">
-        <v>0.02784032108542485</v>
+        <v>0.0278227256905037</v>
       </c>
       <c r="G95" t="n">
-        <v>25.47860680273395</v>
+        <v>25.47612614686784</v>
       </c>
       <c r="H95" t="n">
         <v>0</v>
@@ -3534,13 +3534,13 @@
         </is>
       </c>
       <c r="E96" t="n">
-        <v>0.8696972586299848</v>
+        <v>0.8685758471266943</v>
       </c>
       <c r="F96" t="n">
-        <v>0.03308845481685491</v>
+        <v>0.03305210882144091</v>
       </c>
       <c r="G96" t="n">
-        <v>26.28400943523921</v>
+        <v>26.27898424856238</v>
       </c>
       <c r="H96" t="n">
         <v>0</v>
@@ -3566,13 +3566,13 @@
         </is>
       </c>
       <c r="E97" t="n">
-        <v>0.77450726517105</v>
+        <v>0.7748733202564244</v>
       </c>
       <c r="F97" t="n">
-        <v>0.02977417047553204</v>
+        <v>0.02979206419893625</v>
       </c>
       <c r="G97" t="n">
-        <v>26.01272353772259</v>
+        <v>26.00938676340805</v>
       </c>
       <c r="H97" t="n">
         <v>0</v>
@@ -3598,13 +3598,13 @@
         </is>
       </c>
       <c r="E98" t="n">
-        <v>0.3764977631145509</v>
+        <v>0.3767829052531332</v>
       </c>
       <c r="F98" t="n">
-        <v>0.01383285935122376</v>
+        <v>0.01384426615103997</v>
       </c>
       <c r="G98" t="n">
-        <v>27.21763834416673</v>
+        <v>27.21580913825569</v>
       </c>
       <c r="H98" t="n">
         <v>0</v>
@@ -3630,13 +3630,13 @@
         </is>
       </c>
       <c r="E99" t="n">
-        <v>0.2363270053019035</v>
+        <v>0.2362271185626671</v>
       </c>
       <c r="F99" t="n">
-        <v>0.01177275376817003</v>
+        <v>0.009780019975091713</v>
       </c>
       <c r="G99" t="n">
-        <v>20.07406337850931</v>
+        <v>24.15405276677851</v>
       </c>
       <c r="H99" t="n">
         <v>0</v>
@@ -3662,13 +3662,13 @@
         </is>
       </c>
       <c r="E100" t="n">
-        <v>0.5841966517213202</v>
+        <v>0.584205880175639</v>
       </c>
       <c r="F100" t="n">
-        <v>0.02210067839562414</v>
+        <v>0.02210793932969263</v>
       </c>
       <c r="G100" t="n">
-        <v>26.43342621602763</v>
+        <v>26.42516208485254</v>
       </c>
       <c r="H100" t="n">
         <v>0</v>
@@ -3694,13 +3694,13 @@
         </is>
       </c>
       <c r="E101" t="n">
-        <v>0.6893017229411521</v>
+        <v>0.6898136990164055</v>
       </c>
       <c r="F101" t="n">
-        <v>0.02589549348952946</v>
+        <v>0.02592080177101507</v>
       </c>
       <c r="G101" t="n">
-        <v>26.61859767967908</v>
+        <v>26.61235964395016</v>
       </c>
       <c r="H101" t="n">
         <v>0</v>
@@ -3726,13 +3726,13 @@
         </is>
       </c>
       <c r="E102" t="n">
-        <v>0.9293466955502097</v>
+        <v>0.9300462315004739</v>
       </c>
       <c r="F102" t="n">
-        <v>0.03399581140176428</v>
+        <v>0.03403082352530033</v>
       </c>
       <c r="G102" t="n">
-        <v>27.33709410667699</v>
+        <v>27.32952468169624</v>
       </c>
       <c r="H102" t="n">
         <v>0</v>
@@ -3758,13 +3758,13 @@
         </is>
       </c>
       <c r="E103" t="n">
-        <v>0.5626568545700766</v>
+        <v>0.5625037971774369</v>
       </c>
       <c r="F103" t="n">
-        <v>0.0210509942076249</v>
+        <v>0.02105206520353393</v>
       </c>
       <c r="G103" t="n">
-        <v>26.72827938642195</v>
+        <v>26.71964919889626</v>
       </c>
       <c r="H103" t="n">
         <v>0</v>
@@ -3790,13 +3790,13 @@
         </is>
       </c>
       <c r="E104" t="n">
-        <v>0.4230590428124255</v>
+        <v>0.4220376692614248</v>
       </c>
       <c r="F104" t="n">
-        <v>0.01729190866659757</v>
+        <v>0.01725683254081116</v>
       </c>
       <c r="G104" t="n">
-        <v>24.46572272297357</v>
+        <v>24.45626497440247</v>
       </c>
       <c r="H104" t="n">
         <v>0</v>
@@ -3822,13 +3822,13 @@
         </is>
       </c>
       <c r="E105" t="n">
-        <v>0.5647159974047646</v>
+        <v>0.5634763944085057</v>
       </c>
       <c r="F105" t="n">
-        <v>0.02168587409524698</v>
+        <v>0.02164539703002199</v>
       </c>
       <c r="G105" t="n">
-        <v>26.04073024211167</v>
+        <v>26.03215795029939</v>
       </c>
       <c r="H105" t="n">
         <v>0</v>
@@ -3854,13 +3854,13 @@
         </is>
       </c>
       <c r="E106" t="n">
-        <v>0.5339308349586077</v>
+        <v>0.5342710228737891</v>
       </c>
       <c r="F106" t="n">
-        <v>0.02129106461988382</v>
+        <v>0.02130636298181444</v>
       </c>
       <c r="G106" t="n">
-        <v>25.07769547770241</v>
+        <v>25.07565572335026</v>
       </c>
       <c r="H106" t="n">
         <v>0</v>
@@ -3886,13 +3886,13 @@
         </is>
       </c>
       <c r="E107" t="n">
-        <v>0.8741968661027756</v>
+        <v>0.8744782548370488</v>
       </c>
       <c r="F107" t="n">
-        <v>0.0325372666803531</v>
+        <v>0.03255496220725591</v>
       </c>
       <c r="G107" t="n">
-        <v>26.86755696672494</v>
+        <v>26.86159637486177</v>
       </c>
       <c r="H107" t="n">
         <v>0</v>
@@ -3918,13 +3918,13 @@
         </is>
       </c>
       <c r="E108" t="n">
-        <v>0.8085881715887829</v>
+        <v>0.8085554869582205</v>
       </c>
       <c r="F108" t="n">
-        <v>0.02992785962646203</v>
+        <v>0.02993520803166324</v>
       </c>
       <c r="G108" t="n">
-        <v>27.01790845232435</v>
+        <v>27.01018433130581</v>
       </c>
       <c r="H108" t="n">
         <v>0</v>
@@ -3950,13 +3950,13 @@
         </is>
       </c>
       <c r="E109" t="n">
-        <v>0.8012079814593061</v>
+        <v>0.8018443817644997</v>
       </c>
       <c r="F109" t="n">
-        <v>0.03132526128232607</v>
+        <v>0.03135618008713881</v>
       </c>
       <c r="G109" t="n">
-        <v>25.57705661934179</v>
+        <v>25.5721321765152</v>
       </c>
       <c r="H109" t="n">
         <v>0</v>
@@ -3982,13 +3982,13 @@
         </is>
       </c>
       <c r="E110" t="n">
-        <v>0.7365024175829062</v>
+        <v>0.7365362472222198</v>
       </c>
       <c r="F110" t="n">
-        <v>0.02972993821812725</v>
+        <v>0.02973823317014655</v>
       </c>
       <c r="G110" t="n">
-        <v>24.77308940753416</v>
+        <v>24.76731697486462</v>
       </c>
       <c r="H110" t="n">
         <v>0</v>
@@ -4014,13 +4014,13 @@
         </is>
       </c>
       <c r="E111" t="n">
-        <v>0.6030370610611041</v>
+        <v>0.6031133049333357</v>
       </c>
       <c r="F111" t="n">
-        <v>0.02286662234508012</v>
+        <v>0.02287528366334975</v>
       </c>
       <c r="G111" t="n">
-        <v>26.3719342513425</v>
+        <v>26.36528201279814</v>
       </c>
       <c r="H111" t="n">
         <v>0</v>
@@ -4046,13 +4046,13 @@
         </is>
       </c>
       <c r="E112" t="n">
-        <v>0.6368536883274099</v>
+        <v>0.6375833171259999</v>
       </c>
       <c r="F112" t="n">
-        <v>0.02656422373846348</v>
+        <v>0.02659251262463058</v>
       </c>
       <c r="G112" t="n">
-        <v>23.97411249707658</v>
+        <v>23.97604641960309</v>
       </c>
       <c r="H112" t="n">
         <v>0</v>
@@ -4078,13 +4078,13 @@
         </is>
       </c>
       <c r="E113" t="n">
-        <v>0.6573527529691426</v>
+        <v>0.6576900854277336</v>
       </c>
       <c r="F113" t="n">
-        <v>0.02458935191700811</v>
+        <v>0.02460595459758396</v>
       </c>
       <c r="G113" t="n">
-        <v>26.73322807209603</v>
+        <v>26.72889941305439</v>
       </c>
       <c r="H113" t="n">
         <v>0</v>
@@ -4110,13 +4110,13 @@
         </is>
       </c>
       <c r="E114" t="n">
-        <v>0.5392140556048008</v>
+        <v>0.5393691813976077</v>
       </c>
       <c r="F114" t="n">
-        <v>0.02264656417582112</v>
+        <v>0.0226620978677848</v>
       </c>
       <c r="G114" t="n">
-        <v>23.80997185244945</v>
+        <v>23.80049651716247</v>
       </c>
       <c r="H114" t="n">
         <v>0</v>
@@ -4142,13 +4142,13 @@
         </is>
       </c>
       <c r="E115" t="n">
-        <v>0.6323718642650422</v>
+        <v>0.6340424140319842</v>
       </c>
       <c r="F115" t="n">
-        <v>0.0266070657735241</v>
+        <v>0.02667787491318433</v>
       </c>
       <c r="G115" t="n">
-        <v>23.76706509556306</v>
+        <v>23.76660120311423</v>
       </c>
       <c r="H115" t="n">
         <v>0</v>
@@ -4174,13 +4174,13 @@
         </is>
       </c>
       <c r="E116" t="n">
-        <v>1.18554619897739</v>
+        <v>1.187877016492028</v>
       </c>
       <c r="F116" t="n">
-        <v>0.04457920588769037</v>
+        <v>0.04467984459681882</v>
       </c>
       <c r="G116" t="n">
-        <v>26.59415248305624</v>
+        <v>26.58641781735332</v>
       </c>
       <c r="H116" t="n">
         <v>0</v>
@@ -4206,13 +4206,13 @@
         </is>
       </c>
       <c r="E117" t="n">
-        <v>0.5961002796983804</v>
+        <v>0.5969028429211753</v>
       </c>
       <c r="F117" t="n">
-        <v>0.02328504720247842</v>
+        <v>0.02333256002031888</v>
       </c>
       <c r="G117" t="n">
-        <v>25.60013189963954</v>
+        <v>25.58239826130469</v>
       </c>
       <c r="H117" t="n">
         <v>0</v>
@@ -4238,13 +4238,13 @@
         </is>
       </c>
       <c r="E118" t="n">
-        <v>0.8240182094147381</v>
+        <v>0.8240607134634649</v>
       </c>
       <c r="F118" t="n">
-        <v>0.03151126316189101</v>
+        <v>0.03152375005630224</v>
       </c>
       <c r="G118" t="n">
-        <v>26.14995803738953</v>
+        <v>26.14094807773599</v>
       </c>
       <c r="H118" t="n">
         <v>0</v>
@@ -4270,13 +4270,13 @@
         </is>
       </c>
       <c r="E119" t="n">
-        <v>0.6503559673463103</v>
+        <v>0.640985949893855</v>
       </c>
       <c r="F119" t="n">
-        <v>0.02528367864548572</v>
+        <v>0.02497273966914319</v>
       </c>
       <c r="G119" t="n">
-        <v>25.72236328579924</v>
+        <v>25.66742609583211</v>
       </c>
       <c r="H119" t="n">
         <v>0</v>
@@ -4302,13 +4302,13 @@
         </is>
       </c>
       <c r="E120" t="n">
-        <v>0.588666289074352</v>
+        <v>0.588465954269452</v>
       </c>
       <c r="F120" t="n">
-        <v>0.02309517982966408</v>
+        <v>0.02309361203579888</v>
       </c>
       <c r="G120" t="n">
-        <v>25.48870774726614</v>
+        <v>25.48176323962452</v>
       </c>
       <c r="H120" t="n">
         <v>0</v>
@@ -4334,13 +4334,13 @@
         </is>
       </c>
       <c r="E121" t="n">
-        <v>0.8039163577901308</v>
+        <v>0.8051443023149073</v>
       </c>
       <c r="F121" t="n">
-        <v>0.03140393657840697</v>
+        <v>0.03146230621407725</v>
       </c>
       <c r="G121" t="n">
-        <v>25.59922243370267</v>
+        <v>25.59075920280342</v>
       </c>
       <c r="H121" t="n">
         <v>0</v>
@@ -4366,13 +4366,13 @@
         </is>
       </c>
       <c r="E122" t="n">
-        <v>2.219643583037202</v>
+        <v>2.220522237379774</v>
       </c>
       <c r="F122" t="n">
-        <v>0.08071624216828979</v>
+        <v>0.08077487528280557</v>
       </c>
       <c r="G122" t="n">
-        <v>27.49934242951801</v>
+        <v>27.49025893977409</v>
       </c>
       <c r="H122" t="n">
         <v>0</v>
@@ -4398,13 +4398,13 @@
         </is>
       </c>
       <c r="E123" t="n">
-        <v>1.164841284437451</v>
+        <v>1.165467424005202</v>
       </c>
       <c r="F123" t="n">
-        <v>0.0423570279015206</v>
+        <v>0.04239382237647947</v>
       </c>
       <c r="G123" t="n">
-        <v>27.50054340729919</v>
+        <v>27.49144471163148</v>
       </c>
       <c r="H123" t="n">
         <v>0</v>
@@ -4430,13 +4430,13 @@
         </is>
       </c>
       <c r="E124" t="n">
-        <v>1.949632423105133</v>
+        <v>1.951343187756664</v>
       </c>
       <c r="F124" t="n">
-        <v>0.07088410525503203</v>
+        <v>0.07096970318010774</v>
       </c>
       <c r="G124" t="n">
-        <v>27.50450776042243</v>
+        <v>27.49543960719445</v>
       </c>
       <c r="H124" t="n">
         <v>0</v>
@@ -4462,13 +4462,13 @@
         </is>
       </c>
       <c r="E125" t="n">
-        <v>0.5867557321959612</v>
+        <v>0.5871380959140995</v>
       </c>
       <c r="F125" t="n">
-        <v>0.02134972309048711</v>
+        <v>0.02137032631859922</v>
       </c>
       <c r="G125" t="n">
-        <v>27.48306053814447</v>
+        <v>27.47445626862616</v>
       </c>
       <c r="H125" t="n">
         <v>0</v>
@@ -4494,13 +4494,13 @@
         </is>
       </c>
       <c r="E126" t="n">
-        <v>0.3231258667404248</v>
+        <v>0.3237523884120583</v>
       </c>
       <c r="F126" t="n">
-        <v>0.01348998350194957</v>
+        <v>0.01350421769289169</v>
       </c>
       <c r="G126" t="n">
-        <v>23.95302163785254</v>
+        <v>23.97416834878928</v>
       </c>
       <c r="H126" t="n">
         <v>0</v>
@@ -4526,13 +4526,13 @@
         </is>
       </c>
       <c r="E127" t="n">
-        <v>0.5650257041329596</v>
+        <v>0.5655504568466994</v>
       </c>
       <c r="F127" t="n">
-        <v>0.0215064503376595</v>
+        <v>0.02152810766594596</v>
       </c>
       <c r="G127" t="n">
-        <v>26.27238317972364</v>
+        <v>26.27032833522288</v>
       </c>
       <c r="H127" t="n">
         <v>0</v>
@@ -4558,13 +4558,13 @@
         </is>
       </c>
       <c r="E128" t="n">
-        <v>0.2142859058119277</v>
+        <v>0.2157097302197408</v>
       </c>
       <c r="F128" t="n">
-        <v>0.009944447609382951</v>
+        <v>0.009974171711313366</v>
       </c>
       <c r="G128" t="n">
-        <v>21.54829651756551</v>
+        <v>21.62683142435193</v>
       </c>
       <c r="H128" t="n">
         <v>0</v>
@@ -4590,13 +4590,13 @@
         </is>
       </c>
       <c r="E129" t="n">
-        <v>0.9945205450291195</v>
+        <v>0.9949800977194323</v>
       </c>
       <c r="F129" t="n">
-        <v>0.03843127282631131</v>
+        <v>0.03845893600837709</v>
       </c>
       <c r="G129" t="n">
-        <v>25.87789765636803</v>
+        <v>25.87123308551322</v>
       </c>
       <c r="H129" t="n">
         <v>0</v>
@@ -4622,13 +4622,13 @@
         </is>
       </c>
       <c r="E130" t="n">
-        <v>1.520674631680835</v>
+        <v>1.520428676925219</v>
       </c>
       <c r="F130" t="n">
-        <v>0.05637066820172024</v>
+        <v>0.05639281047993162</v>
       </c>
       <c r="G130" t="n">
-        <v>26.97634568056181</v>
+        <v>26.96139213418577</v>
       </c>
       <c r="H130" t="n">
         <v>0</v>
@@ -4654,13 +4654,13 @@
         </is>
       </c>
       <c r="E131" t="n">
-        <v>0.7569674244806976</v>
+        <v>0.7574570143210273</v>
       </c>
       <c r="F131" t="n">
-        <v>0.03082566794892606</v>
+        <v>0.03085373853647934</v>
       </c>
       <c r="G131" t="n">
-        <v>24.55639974161577</v>
+        <v>24.54992653162314</v>
       </c>
       <c r="H131" t="n">
         <v>0</v>
@@ -4686,13 +4686,13 @@
         </is>
       </c>
       <c r="E132" t="n">
-        <v>0.8339404422518543</v>
+        <v>0.833324036491465</v>
       </c>
       <c r="F132" t="n">
-        <v>0.03314615523734504</v>
+        <v>0.03315655495516684</v>
       </c>
       <c r="G132" t="n">
-        <v>25.15949244354931</v>
+        <v>25.13301027785077</v>
       </c>
       <c r="H132" t="n">
         <v>0</v>
@@ -4718,13 +4718,13 @@
         </is>
       </c>
       <c r="E133" t="n">
-        <v>0.6388897255230963</v>
+        <v>0.6395416274562093</v>
       </c>
       <c r="F133" t="n">
-        <v>0.02810298660002844</v>
+        <v>0.02813130610857694</v>
       </c>
       <c r="G133" t="n">
-        <v>22.73387290088648</v>
+        <v>22.73416047463526</v>
       </c>
       <c r="H133" t="n">
         <v>0</v>
@@ -4750,13 +4750,13 @@
         </is>
       </c>
       <c r="E134" t="n">
-        <v>0.6016755299609584</v>
+        <v>0.6020038327161941</v>
       </c>
       <c r="F134" t="n">
-        <v>0.02666505251120612</v>
+        <v>0.02667615341649269</v>
       </c>
       <c r="G134" t="n">
-        <v>22.56419820233008</v>
+        <v>22.56711540433092</v>
       </c>
       <c r="H134" t="n">
         <v>0</v>
@@ -4782,13 +4782,13 @@
         </is>
       </c>
       <c r="E135" t="n">
-        <v>0.7035670078467765</v>
+        <v>0.7039587527478598</v>
       </c>
       <c r="F135" t="n">
-        <v>0.02928501447782678</v>
+        <v>0.02930117615323052</v>
       </c>
       <c r="G135" t="n">
-        <v>24.02481338554431</v>
+        <v>24.02493159463914</v>
       </c>
       <c r="H135" t="n">
         <v>0</v>
@@ -4814,13 +4814,13 @@
         </is>
       </c>
       <c r="E136" t="n">
-        <v>1.431271433360857</v>
+        <v>1.432160938923689</v>
       </c>
       <c r="F136" t="n">
-        <v>0.05402628707292748</v>
+        <v>0.05408666577884524</v>
       </c>
       <c r="G136" t="n">
-        <v>26.49213023657096</v>
+        <v>26.47900213988356</v>
       </c>
       <c r="H136" t="n">
         <v>0</v>
@@ -4846,13 +4846,13 @@
         </is>
       </c>
       <c r="E137" t="n">
-        <v>0.9620577358329614</v>
+        <v>0.9623097286663731</v>
       </c>
       <c r="F137" t="n">
-        <v>0.03747384990654515</v>
+        <v>0.03750472256259775</v>
       </c>
       <c r="G137" t="n">
-        <v>25.67277550095691</v>
+        <v>25.65836147793279</v>
       </c>
       <c r="H137" t="n">
         <v>0</v>
@@ -4878,13 +4878,13 @@
         </is>
       </c>
       <c r="E138" t="n">
-        <v>0.8382603609460855</v>
+        <v>0.8387136768886635</v>
       </c>
       <c r="F138" t="n">
-        <v>0.03393123436672782</v>
+        <v>0.03395796034877305</v>
       </c>
       <c r="G138" t="n">
-        <v>24.70468217753255</v>
+        <v>24.69858814398047</v>
       </c>
       <c r="H138" t="n">
         <v>0</v>
@@ -4910,13 +4910,13 @@
         </is>
       </c>
       <c r="E139" t="n">
-        <v>0.8586969394304544</v>
+        <v>0.8588914642370777</v>
       </c>
       <c r="F139" t="n">
-        <v>0.0352415867559562</v>
+        <v>0.03526345816057355</v>
       </c>
       <c r="G139" t="n">
-        <v>24.36601238623172</v>
+        <v>24.35641621708584</v>
       </c>
       <c r="H139" t="n">
         <v>0</v>
@@ -4942,13 +4942,13 @@
         </is>
       </c>
       <c r="E140" t="n">
-        <v>1.206011280986018</v>
+        <v>1.203406643769366</v>
       </c>
       <c r="F140" t="n">
-        <v>0.04802325651562785</v>
+        <v>0.04794735298833894</v>
       </c>
       <c r="G140" t="n">
-        <v>25.11306746905932</v>
+        <v>25.09850009940991</v>
       </c>
       <c r="H140" t="n">
         <v>0</v>
@@ -4974,13 +4974,13 @@
         </is>
       </c>
       <c r="E141" t="n">
-        <v>1.109611572378803</v>
+        <v>1.108642139349389</v>
       </c>
       <c r="F141" t="n">
-        <v>0.04314318338996372</v>
+        <v>0.04312822348898525</v>
       </c>
       <c r="G141" t="n">
-        <v>25.7192790416854</v>
+        <v>25.70572237010471</v>
       </c>
       <c r="H141" t="n">
         <v>0</v>
@@ -5006,13 +5006,13 @@
         </is>
       </c>
       <c r="E142" t="n">
-        <v>1.151055379481874</v>
+        <v>1.151430418465126</v>
       </c>
       <c r="F142" t="n">
-        <v>0.04397180711799936</v>
+        <v>0.04400451995167144</v>
       </c>
       <c r="G142" t="n">
-        <v>26.17712245409458</v>
+        <v>26.16618519423764</v>
       </c>
       <c r="H142" t="n">
         <v>0</v>
@@ -5038,13 +5038,13 @@
         </is>
       </c>
       <c r="E143" t="n">
-        <v>0.2597082706783326</v>
+        <v>0.2598549534235534</v>
       </c>
       <c r="F143" t="n">
-        <v>0.009447587082442541</v>
+        <v>0.009456097251513237</v>
       </c>
       <c r="G143" t="n">
-        <v>27.48937568762788</v>
+        <v>27.48014815038934</v>
       </c>
       <c r="H143" t="n">
         <v>0</v>
@@ -5070,13 +5070,13 @@
         </is>
       </c>
       <c r="E144" t="n">
-        <v>0.1155212471587288</v>
+        <v>0.1149140422923449</v>
       </c>
       <c r="F144" t="n">
-        <v>0.008313052888426549</v>
+        <v>0.008371305089670895</v>
       </c>
       <c r="G144" t="n">
-        <v>13.89636860192017</v>
+        <v>13.72713585847048</v>
       </c>
       <c r="H144" t="n">
         <v>0</v>
@@ -5102,13 +5102,13 @@
         </is>
       </c>
       <c r="E145" t="n">
-        <v>0.02748434795394871</v>
+        <v>0.5961933263470798</v>
       </c>
       <c r="F145" t="n">
-        <v>0.001134421521968817</v>
+        <v>0.02962108348061309</v>
       </c>
       <c r="G145" t="n">
-        <v>24.22763267221986</v>
+        <v>20.12733014027522</v>
       </c>
       <c r="H145" t="n">
         <v>0</v>
@@ -5134,13 +5134,13 @@
         </is>
       </c>
       <c r="E146" t="n">
-        <v>1.037562741339259</v>
+        <v>1.039936469507579</v>
       </c>
       <c r="F146" t="n">
-        <v>0.04192132423264421</v>
+        <v>0.04191008813002916</v>
       </c>
       <c r="G146" t="n">
-        <v>24.75023774431621</v>
+        <v>24.81351187466571</v>
       </c>
       <c r="H146" t="n">
         <v>0</v>
@@ -5166,13 +5166,13 @@
         </is>
       </c>
       <c r="E147" t="n">
-        <v>0.7153136837792583</v>
+        <v>0.7148657716873199</v>
       </c>
       <c r="F147" t="n">
-        <v>0.02600753972377753</v>
+        <v>0.02599969149082662</v>
       </c>
       <c r="G147" t="n">
-        <v>27.5040888661135</v>
+        <v>27.49516362192407</v>
       </c>
       <c r="H147" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Table with factor loadings
</commit_message>
<xml_diff>
--- a/model_coefficients.xlsx
+++ b/model_coefficients.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H147"/>
+  <dimension ref="A1:H137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,13 +490,13 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>-1.835842957812327</v>
+        <v>0.4403726426276341</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2189416654273608</v>
+        <v>0.03461160913521575</v>
       </c>
       <c r="G2" t="n">
-        <v>-8.385078071916956</v>
+        <v>12.72326406133056</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -522,16 +522,16 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>-0.4420866522022651</v>
+        <v>-0.4604852796771892</v>
       </c>
       <c r="F3" t="n">
-        <v>0.09297007425655235</v>
+        <v>0.09553185374300691</v>
       </c>
       <c r="G3" t="n">
-        <v>-4.755150038684114</v>
+        <v>-4.820227616551167</v>
       </c>
       <c r="H3" t="n">
-        <v>1.98299089659848e-06</v>
+        <v>1.433945193474173e-06</v>
       </c>
     </row>
     <row r="4">
@@ -554,16 +554,16 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.9185031370564757</v>
+        <v>-0.2251679016470539</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1278669578877122</v>
+        <v>0.02436090984889298</v>
       </c>
       <c r="G4" t="n">
-        <v>7.183271990062409</v>
+        <v>-9.243000488671942</v>
       </c>
       <c r="H4" t="n">
-        <v>6.80566714095221e-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -586,16 +586,16 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1.317743844535169</v>
+        <v>1.329543080928221</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1886409801497791</v>
+        <v>0.1905927296356341</v>
       </c>
       <c r="G5" t="n">
-        <v>6.985459063464937</v>
+        <v>6.975833146746999</v>
       </c>
       <c r="H5" t="n">
-        <v>2.839284363176375e-12</v>
+        <v>3.040678819843379e-12</v>
       </c>
     </row>
     <row r="6">
@@ -618,16 +618,16 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.08420945047963496</v>
+        <v>0.08413017542391608</v>
       </c>
       <c r="F6" t="n">
-        <v>0.01860953746522926</v>
+        <v>0.01862669066675368</v>
       </c>
       <c r="G6" t="n">
-        <v>4.525069504411377</v>
+        <v>4.516646404052939</v>
       </c>
       <c r="H6" t="n">
-        <v>6.037566035788089e-06</v>
+        <v>6.282668494117516e-06</v>
       </c>
     </row>
     <row r="7">
@@ -650,13 +650,13 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>-0.2780459082178542</v>
+        <v>-0.2782810123638836</v>
       </c>
       <c r="F7" t="n">
-        <v>0.02316451192926945</v>
+        <v>0.02316442992978773</v>
       </c>
       <c r="G7" t="n">
-        <v>-12.00309806029313</v>
+        <v>-12.01328991023525</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -682,16 +682,16 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0.187023303780533</v>
+        <v>0.1873009030182755</v>
       </c>
       <c r="F8" t="n">
-        <v>0.02640989962954342</v>
+        <v>0.02642238080547053</v>
       </c>
       <c r="G8" t="n">
-        <v>7.081560566183974</v>
+        <v>7.088721655711195</v>
       </c>
       <c r="H8" t="n">
-        <v>1.425304319013776e-12</v>
+        <v>1.353583911622991e-12</v>
       </c>
     </row>
     <row r="9">
@@ -714,16 +714,16 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.001518006928348461</v>
+        <v>0.001885175454845915</v>
       </c>
       <c r="F9" t="n">
-        <v>0.01566673474574194</v>
+        <v>0.01568677961242423</v>
       </c>
       <c r="G9" t="n">
-        <v>0.09689363820142206</v>
+        <v>0.1201760655343589</v>
       </c>
       <c r="H9" t="n">
-        <v>0.9228108610158714</v>
+        <v>0.9043436772846398</v>
       </c>
     </row>
     <row r="10">
@@ -784,13 +784,13 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1.151872024844843</v>
+        <v>1.151579279695787</v>
       </c>
       <c r="F11" t="n">
-        <v>0.04425295736751178</v>
+        <v>0.04422653294912043</v>
       </c>
       <c r="G11" t="n">
-        <v>26.02926659234888</v>
+        <v>26.03819930887554</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -816,13 +816,13 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1.087437272233255</v>
+        <v>1.087236216102321</v>
       </c>
       <c r="F12" t="n">
-        <v>0.04710320924457956</v>
+        <v>0.04707778165689066</v>
       </c>
       <c r="G12" t="n">
-        <v>23.08626714930908</v>
+        <v>23.09446575038631</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -848,13 +848,13 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>1.232548789002741</v>
+        <v>1.2320839678896</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0505195846315663</v>
+        <v>0.05048884776845797</v>
       </c>
       <c r="G13" t="n">
-        <v>24.39744502982724</v>
+        <v>24.40309142160538</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -880,13 +880,13 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0.9904602816396002</v>
+        <v>0.9899864966097088</v>
       </c>
       <c r="F14" t="n">
-        <v>0.04826654537642128</v>
+        <v>0.04824033073164296</v>
       </c>
       <c r="G14" t="n">
-        <v>20.52063751185578</v>
+        <v>20.52196744040586</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -912,13 +912,13 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0.8130781194260529</v>
+        <v>0.8127986148123081</v>
       </c>
       <c r="F15" t="n">
-        <v>0.052265970317738</v>
+        <v>0.05224202006860408</v>
       </c>
       <c r="G15" t="n">
-        <v>15.55654883029225</v>
+        <v>15.55833051113615</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -944,13 +944,13 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.6842294080193208</v>
+        <v>0.6839555195904967</v>
       </c>
       <c r="F16" t="n">
-        <v>0.04877658216252276</v>
+        <v>0.04875401416842451</v>
       </c>
       <c r="G16" t="n">
-        <v>14.02782601137267</v>
+        <v>14.02870166164556</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -976,13 +976,13 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0.7752830109821204</v>
+        <v>0.7749860599947715</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0464864477719153</v>
+        <v>0.04646479700981244</v>
       </c>
       <c r="G17" t="n">
-        <v>16.67761354383005</v>
+        <v>16.67899377273575</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1008,13 +1008,13 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>1.161277886885324</v>
+        <v>1.161043292234421</v>
       </c>
       <c r="F18" t="n">
-        <v>0.04633574472340665</v>
+        <v>0.04631091734796899</v>
       </c>
       <c r="G18" t="n">
-        <v>25.06224716560213</v>
+        <v>25.07061744179139</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -1040,13 +1040,13 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>1.222079676271399</v>
+        <v>1.221863335055759</v>
       </c>
       <c r="F19" t="n">
-        <v>0.04525950843753337</v>
+        <v>0.04523301210167765</v>
       </c>
       <c r="G19" t="n">
-        <v>27.00161178133644</v>
+        <v>27.01264581456932</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -1110,16 +1110,16 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0.81979392161138</v>
+        <v>0.8209983065336125</v>
       </c>
       <c r="F21" t="n">
-        <v>0.1904329602910399</v>
+        <v>0.1908889424829713</v>
       </c>
       <c r="G21" t="n">
-        <v>4.304895120856069</v>
+        <v>4.300921236454284</v>
       </c>
       <c r="H21" t="n">
-        <v>1.670648639184869e-05</v>
+        <v>1.700895133738278e-05</v>
       </c>
     </row>
     <row r="22">
@@ -1142,16 +1142,16 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0.6256053415687026</v>
+        <v>0.6256821493719346</v>
       </c>
       <c r="F22" t="n">
-        <v>0.1795796104594407</v>
+        <v>0.1799163971738412</v>
       </c>
       <c r="G22" t="n">
-        <v>3.483721453480468</v>
+        <v>3.477627160152068</v>
       </c>
       <c r="H22" t="n">
-        <v>0.0004944938391127085</v>
+        <v>0.0005058730390887778</v>
       </c>
     </row>
     <row r="23">
@@ -1174,16 +1174,16 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>0.989660567154102</v>
+        <v>0.9918695202101342</v>
       </c>
       <c r="F23" t="n">
-        <v>0.1936126083763608</v>
+        <v>0.1941900846374979</v>
       </c>
       <c r="G23" t="n">
-        <v>5.111550200414651</v>
+        <v>5.10772484628444</v>
       </c>
       <c r="H23" t="n">
-        <v>3.19525888636818e-07</v>
+        <v>3.260609893196431e-07</v>
       </c>
     </row>
     <row r="24">
@@ -1206,16 +1206,16 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0.4359825919630195</v>
+        <v>0.43573683512989</v>
       </c>
       <c r="F24" t="n">
-        <v>0.1137014106576623</v>
+        <v>0.1138949189560925</v>
       </c>
       <c r="G24" t="n">
-        <v>3.834451916096823</v>
+        <v>3.825779403680376</v>
       </c>
       <c r="H24" t="n">
-        <v>0.0001258445861644919</v>
+        <v>0.0001303589862762244</v>
       </c>
     </row>
     <row r="25">
@@ -1238,16 +1238,16 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0.2730334685656489</v>
+        <v>0.2747911110050573</v>
       </c>
       <c r="F25" t="n">
-        <v>0.1485227500904016</v>
+        <v>0.1488410342567092</v>
       </c>
       <c r="G25" t="n">
-        <v>1.838327585488572</v>
+        <v>1.846205331583984</v>
       </c>
       <c r="H25" t="n">
-        <v>0.06601414861129262</v>
+        <v>0.06486239711971242</v>
       </c>
     </row>
     <row r="26">
@@ -1270,16 +1270,16 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0.3238280528469518</v>
+        <v>0.3226591439017967</v>
       </c>
       <c r="F26" t="n">
-        <v>0.1050712213421764</v>
+        <v>0.1052006082110049</v>
       </c>
       <c r="G26" t="n">
-        <v>3.081986187152873</v>
+        <v>3.067084396047973</v>
       </c>
       <c r="H26" t="n">
-        <v>0.002056243788211898</v>
+        <v>0.002161578174268097</v>
       </c>
     </row>
     <row r="27">
@@ -1302,16 +1302,16 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>1.265698078743571</v>
+        <v>1.270496544714147</v>
       </c>
       <c r="F27" t="n">
-        <v>0.1913243969308348</v>
+        <v>0.1922450331774532</v>
       </c>
       <c r="G27" t="n">
-        <v>6.615455734035399</v>
+        <v>6.608735340042815</v>
       </c>
       <c r="H27" t="n">
-        <v>3.704081485977895e-11</v>
+        <v>3.876166054794794e-11</v>
       </c>
     </row>
     <row r="28">
@@ -1334,16 +1334,16 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>1.249505915150312</v>
+        <v>1.253561180468181</v>
       </c>
       <c r="F28" t="n">
-        <v>0.1932151884747342</v>
+        <v>0.1940430033904529</v>
       </c>
       <c r="G28" t="n">
-        <v>6.466913522728762</v>
+        <v>6.460223551267697</v>
       </c>
       <c r="H28" t="n">
-        <v>1.000248772697887e-10</v>
+        <v>1.045483699613214e-10</v>
       </c>
     </row>
     <row r="29">
@@ -1366,16 +1366,16 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>-0.6293030590762514</v>
+        <v>-0.6322663402276467</v>
       </c>
       <c r="F29" t="n">
-        <v>0.1409602694695458</v>
+        <v>0.1414513809445739</v>
       </c>
       <c r="G29" t="n">
-        <v>-4.464400227382842</v>
+        <v>-4.469849187763838</v>
       </c>
       <c r="H29" t="n">
-        <v>8.029335298864737e-06</v>
+        <v>7.827477009447747e-06</v>
       </c>
     </row>
     <row r="30">
@@ -1398,16 +1398,16 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>1.057668469390711</v>
+        <v>1.060714738318336</v>
       </c>
       <c r="F30" t="n">
-        <v>0.1663979353155412</v>
+        <v>0.1670517497720977</v>
       </c>
       <c r="G30" t="n">
-        <v>6.356259573646109</v>
+        <v>6.349617646981124</v>
       </c>
       <c r="H30" t="n">
-        <v>2.067255255866485e-10</v>
+        <v>2.158506706706476e-10</v>
       </c>
     </row>
     <row r="31">
@@ -1430,16 +1430,16 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>1.817881086915973</v>
+        <v>1.822840547429641</v>
       </c>
       <c r="F31" t="n">
-        <v>0.2574864551324883</v>
+        <v>0.2585975678177977</v>
       </c>
       <c r="G31" t="n">
-        <v>7.060103747878824</v>
+        <v>7.048946990510472</v>
       </c>
       <c r="H31" t="n">
-        <v>1.66378022470326e-12</v>
+        <v>1.802780147386329e-12</v>
       </c>
     </row>
     <row r="32">
@@ -1462,16 +1462,16 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>1.986287170057503</v>
+        <v>1.990131689630646</v>
       </c>
       <c r="F32" t="n">
-        <v>0.2853023601456039</v>
+        <v>0.2863216824985106</v>
       </c>
       <c r="G32" t="n">
-        <v>6.962042546850437</v>
+        <v>6.950684531668494</v>
       </c>
       <c r="H32" t="n">
-        <v>3.353761712787673e-12</v>
+        <v>3.635092227227688e-12</v>
       </c>
     </row>
     <row r="33">
@@ -1494,16 +1494,16 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>2.265817457793731</v>
+        <v>2.269199588562161</v>
       </c>
       <c r="F33" t="n">
-        <v>0.3189386297510006</v>
+        <v>0.3199775661191219</v>
       </c>
       <c r="G33" t="n">
-        <v>7.104242780360532</v>
+        <v>7.091745887304758</v>
       </c>
       <c r="H33" t="n">
-        <v>1.209921052236496e-12</v>
+        <v>1.324274023772887e-12</v>
       </c>
     </row>
     <row r="34">
@@ -1526,16 +1526,16 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>1.321431034074632</v>
+        <v>1.32563564032576</v>
       </c>
       <c r="F34" t="n">
-        <v>0.1985860858518596</v>
+        <v>0.1994575031783867</v>
       </c>
       <c r="G34" t="n">
-        <v>6.654197490219597</v>
+        <v>6.646205929558431</v>
       </c>
       <c r="H34" t="n">
-        <v>2.848499214280764e-11</v>
+        <v>3.007438742486102e-11</v>
       </c>
     </row>
     <row r="35">
@@ -1558,16 +1558,16 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>2.393264057014837</v>
+        <v>2.398467057485919</v>
       </c>
       <c r="F35" t="n">
-        <v>0.3331458231680656</v>
+        <v>0.3344522558549717</v>
       </c>
       <c r="G35" t="n">
-        <v>7.183833296328912</v>
+        <v>7.171328688896013</v>
       </c>
       <c r="H35" t="n">
-        <v>6.779021788361206e-13</v>
+        <v>7.427392034742297e-13</v>
       </c>
     </row>
     <row r="36">
@@ -1590,16 +1590,16 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>-0.172082474161993</v>
+        <v>-0.1703716453199718</v>
       </c>
       <c r="F36" t="n">
-        <v>0.176402837892043</v>
+        <v>0.1766830315348227</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.975508536128713</v>
+        <v>-0.9642784812950682</v>
       </c>
       <c r="H36" t="n">
-        <v>0.3293080695334072</v>
+        <v>0.3349063264147591</v>
       </c>
     </row>
     <row r="37">
@@ -1622,16 +1622,16 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>0.1095216620585564</v>
+        <v>0.1097374824727145</v>
       </c>
       <c r="F37" t="n">
-        <v>0.1275516256813871</v>
+        <v>0.1277845008792783</v>
       </c>
       <c r="G37" t="n">
-        <v>0.8586457559645178</v>
+        <v>0.8587698955409926</v>
       </c>
       <c r="H37" t="n">
-        <v>0.3905359858892541</v>
+        <v>0.3904674795947591</v>
       </c>
     </row>
     <row r="38">
@@ -1654,16 +1654,16 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>-0.008540598050058636</v>
+        <v>-0.00984839376259249</v>
       </c>
       <c r="F38" t="n">
-        <v>0.1639613504258576</v>
+        <v>0.1642480026443201</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.05208909311751832</v>
+        <v>-0.05996050852356043</v>
       </c>
       <c r="H38" t="n">
-        <v>0.9584577036003972</v>
+        <v>0.9521870877020406</v>
       </c>
     </row>
     <row r="39">
@@ -1686,16 +1686,16 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>2.623878536756999</v>
+        <v>2.627081631813607</v>
       </c>
       <c r="F39" t="n">
-        <v>0.3669591560899239</v>
+        <v>0.3680740846068981</v>
       </c>
       <c r="G39" t="n">
-        <v>7.150328567103157</v>
+        <v>7.137371908734582</v>
       </c>
       <c r="H39" t="n">
-        <v>8.657519146026971e-13</v>
+        <v>9.512390874988341e-13</v>
       </c>
     </row>
     <row r="40">
@@ -1718,16 +1718,16 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>2.715431609242283</v>
+        <v>2.719467206636053</v>
       </c>
       <c r="F40" t="n">
-        <v>0.3848174434536169</v>
+        <v>0.3860729692849083</v>
       </c>
       <c r="G40" t="n">
-        <v>7.056415075327856</v>
+        <v>7.043920250791085</v>
       </c>
       <c r="H40" t="n">
-        <v>1.708633234898116e-12</v>
+        <v>1.868949439653989e-12</v>
       </c>
     </row>
     <row r="41">
@@ -1750,16 +1750,16 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>2.253254211402137</v>
+        <v>2.256167171874979</v>
       </c>
       <c r="F41" t="n">
-        <v>0.3252710722421209</v>
+        <v>0.3262601907419795</v>
       </c>
       <c r="G41" t="n">
-        <v>6.927312028897433</v>
+        <v>6.915238928589782</v>
       </c>
       <c r="H41" t="n">
-        <v>4.289013588731905e-12</v>
+        <v>4.670708264598034e-12</v>
       </c>
     </row>
     <row r="42">
@@ -1782,16 +1782,16 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>1.979798384953577</v>
+        <v>1.979977893918627</v>
       </c>
       <c r="F42" t="n">
-        <v>0.2928123094683205</v>
+        <v>0.2934003003644449</v>
       </c>
       <c r="G42" t="n">
-        <v>6.761322256368496</v>
+        <v>6.748384004557817</v>
       </c>
       <c r="H42" t="n">
-        <v>1.367372881588835e-11</v>
+        <v>1.495004120499743e-11</v>
       </c>
     </row>
     <row r="43">
@@ -1814,16 +1814,16 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0.6637252518124933</v>
+        <v>0.6658911495795273</v>
       </c>
       <c r="F43" t="n">
-        <v>0.1678462213610837</v>
+        <v>0.1682975075377535</v>
       </c>
       <c r="G43" t="n">
-        <v>3.954365170846962</v>
+        <v>3.956631083358106</v>
       </c>
       <c r="H43" t="n">
-        <v>7.673813079001057e-05</v>
+        <v>7.60141845219664e-05</v>
       </c>
     </row>
     <row r="44">
@@ -1884,13 +1884,13 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>1.577665941152787</v>
+        <v>1.574143592817372</v>
       </c>
       <c r="F45" t="n">
-        <v>0.1636824127505529</v>
+        <v>0.1634913993530264</v>
       </c>
       <c r="G45" t="n">
-        <v>9.638579457815444</v>
+        <v>9.628296039039343</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
@@ -1954,16 +1954,16 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>2.078140084277552</v>
+        <v>2.07584177331808</v>
       </c>
       <c r="F47" t="n">
-        <v>0.3314136914452223</v>
+        <v>0.3309873053151422</v>
       </c>
       <c r="G47" t="n">
-        <v>6.270531779206132</v>
+        <v>6.271665831217732</v>
       </c>
       <c r="H47" t="n">
-        <v>3.598170650320753e-10</v>
+        <v>3.57205598433552e-10</v>
       </c>
     </row>
     <row r="48">
@@ -1972,7 +1972,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Cantrill_1</t>
+          <t>Onnodige_stress_1</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2010,7 +2010,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Leefst</t>
+          <t>Onnodige_stress_2</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2024,16 +2024,16 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>0.3421789656486482</v>
+        <v>1.189854152923816</v>
       </c>
       <c r="F49" t="n">
-        <v>0.1322890926683966</v>
+        <v>0.06387495973062768</v>
       </c>
       <c r="G49" t="n">
-        <v>2.586599989039058</v>
+        <v>18.62786540959117</v>
       </c>
       <c r="H49" t="n">
-        <v>0.009692804328955251</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -2042,7 +2042,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Q297_1</t>
+          <t>Onnodige_stress_3</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2056,16 +2056,16 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0.1943546739444523</v>
+        <v>1.097741430111587</v>
       </c>
       <c r="F50" t="n">
-        <v>0.08716591170450448</v>
+        <v>0.0620619692729338</v>
       </c>
       <c r="G50" t="n">
-        <v>2.229709643846689</v>
+        <v>17.68782787517253</v>
       </c>
       <c r="H50" t="n">
-        <v>0.02576672523708612</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -2074,7 +2074,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Onnodige_stress_1</t>
+          <t>Onnodige_stress_4</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2088,13 +2088,13 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>-3.909378600700168</v>
+        <v>1.395488424102209</v>
       </c>
       <c r="F51" t="n">
-        <v>0.433614547898007</v>
+        <v>0.06978431619074034</v>
       </c>
       <c r="G51" t="n">
-        <v>-9.015792066115596</v>
+        <v>19.99716412306664</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -2106,7 +2106,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Onnodige_stress_2</t>
+          <t>Onnodige_stress_5</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2120,13 +2120,13 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>-4.585668229299648</v>
+        <v>1.379602832962423</v>
       </c>
       <c r="F52" t="n">
-        <v>0.4917540236841477</v>
+        <v>0.0686577004385093</v>
       </c>
       <c r="G52" t="n">
-        <v>-9.325125994771089</v>
+        <v>20.0939271797767</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
@@ -2138,7 +2138,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Onnodige_stress_3</t>
+          <t>Onnodige_stress_6</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2152,13 +2152,13 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>-4.310670792199005</v>
+        <v>1.248265783458864</v>
       </c>
       <c r="F53" t="n">
-        <v>0.4671237129597662</v>
+        <v>0.06517528804791024</v>
       </c>
       <c r="G53" t="n">
-        <v>-9.22811382208948</v>
+        <v>19.15243984072788</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -2170,7 +2170,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Onnodige_stress_4</t>
+          <t>Onnodige_stress_7</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2184,13 +2184,13 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>-5.348604531766081</v>
+        <v>0.9382274506534336</v>
       </c>
       <c r="F54" t="n">
-        <v>0.5641856270698578</v>
+        <v>0.06586602129375134</v>
       </c>
       <c r="G54" t="n">
-        <v>-9.480221180987892</v>
+        <v>14.24448345611849</v>
       </c>
       <c r="H54" t="n">
         <v>0</v>
@@ -2202,7 +2202,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Onnodige_stress_5</t>
+          <t>Onnodige_stress_8</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2216,13 +2216,13 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>-5.279210853395542</v>
+        <v>1.040147883001451</v>
       </c>
       <c r="F55" t="n">
-        <v>0.556356152496617</v>
+        <v>0.06207477539197044</v>
       </c>
       <c r="G55" t="n">
-        <v>-9.488905316667914</v>
+        <v>16.75636965928097</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -2234,7 +2234,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Onnodige_stress_6</t>
+          <t>Onnodige_stress_9</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2248,13 +2248,13 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>-4.795726264569846</v>
+        <v>1.205530026629599</v>
       </c>
       <c r="F56" t="n">
-        <v>0.5109479934817797</v>
+        <v>0.06576997836909897</v>
       </c>
       <c r="G56" t="n">
-        <v>-9.385938149753152</v>
+        <v>18.32948795947407</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -2266,7 +2266,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Onnodige_stress_7</t>
+          <t>Burn1_1</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2276,20 +2276,26 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>-3.713378812745065</v>
-      </c>
-      <c r="F57" t="n">
-        <v>0.4294574139893254</v>
-      </c>
-      <c r="G57" t="n">
-        <v>-8.64667529718958</v>
-      </c>
-      <c r="H57" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="58">
@@ -2298,7 +2304,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Onnodige_stress_8</t>
+          <t>Burn1_2</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2308,17 +2314,17 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>-4.087692228233797</v>
+        <v>1.06943846382081</v>
       </c>
       <c r="F58" t="n">
-        <v>0.4495496005275542</v>
+        <v>0.04988569793692187</v>
       </c>
       <c r="G58" t="n">
-        <v>-9.092861440490053</v>
+        <v>21.4377769185795</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -2330,7 +2336,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Onnodige_stress_9</t>
+          <t>Burn1_3</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2340,17 +2346,17 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>-4.702869116145844</v>
+        <v>0.9187936814452946</v>
       </c>
       <c r="F59" t="n">
-        <v>0.5054674706758978</v>
+        <v>0.04979830546892112</v>
       </c>
       <c r="G59" t="n">
-        <v>-9.303999542933964</v>
+        <v>18.45030012116093</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -2362,7 +2368,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Onnodige_stress_10</t>
+          <t>Burn1_4</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2372,20 +2378,20 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>-2.775145331817605</v>
+        <v>0.959549841786135</v>
       </c>
       <c r="F60" t="n">
-        <v>0.3506702246270046</v>
+        <v>0.04881873733158575</v>
       </c>
       <c r="G60" t="n">
-        <v>-7.9138322472674</v>
+        <v>19.65535968800345</v>
       </c>
       <c r="H60" t="n">
-        <v>2.442490654175344e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -2394,7 +2400,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Werk_1</t>
+          <t>Depr_1</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2404,20 +2410,20 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>-0.04441472492636244</v>
+        <v>1.261880386471091</v>
       </c>
       <c r="F61" t="n">
-        <v>0.1408263787695885</v>
+        <v>0.0513238493006214</v>
       </c>
       <c r="G61" t="n">
-        <v>-0.3153864021364613</v>
+        <v>24.58662792526021</v>
       </c>
       <c r="H61" t="n">
-        <v>0.7524682899421271</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -2426,7 +2432,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Burn1_1</t>
+          <t>Depr_2</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2440,22 +2446,16 @@
         </is>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>1.37475705248148</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.05580728065580344</v>
+      </c>
+      <c r="G62" t="n">
+        <v>24.63400897341311</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -2464,7 +2464,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Burn1_2</t>
+          <t>Depr_3</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2478,13 +2478,13 @@
         </is>
       </c>
       <c r="E63" t="n">
-        <v>1.069762331922792</v>
+        <v>0.9298710380081527</v>
       </c>
       <c r="F63" t="n">
-        <v>0.04984925720061331</v>
+        <v>0.05562324181002616</v>
       </c>
       <c r="G63" t="n">
-        <v>21.45994528255819</v>
+        <v>16.71731110472286</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
@@ -2496,7 +2496,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Burn1_3</t>
+          <t>Depr_4</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2510,13 +2510,13 @@
         </is>
       </c>
       <c r="E64" t="n">
-        <v>0.9197509527167139</v>
+        <v>-0.9566943500138969</v>
       </c>
       <c r="F64" t="n">
-        <v>0.04976903490294243</v>
+        <v>0.04521668331846854</v>
       </c>
       <c r="G64" t="n">
-        <v>18.48038553473852</v>
+        <v>-21.15799478821972</v>
       </c>
       <c r="H64" t="n">
         <v>0</v>
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Burn1_4</t>
+          <t>Depr_5</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2542,13 +2542,13 @@
         </is>
       </c>
       <c r="E65" t="n">
-        <v>0.9599488475101852</v>
+        <v>0.9456153501010913</v>
       </c>
       <c r="F65" t="n">
-        <v>0.0487842785977513</v>
+        <v>0.04946008839762814</v>
       </c>
       <c r="G65" t="n">
-        <v>19.67742221640142</v>
+        <v>19.11875576282471</v>
       </c>
       <c r="H65" t="n">
         <v>0</v>
@@ -2560,7 +2560,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Depr_1</t>
+          <t>Depr_6</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2574,13 +2574,13 @@
         </is>
       </c>
       <c r="E66" t="n">
-        <v>1.260945466124432</v>
+        <v>-0.9688908880584808</v>
       </c>
       <c r="F66" t="n">
-        <v>0.05127282588344639</v>
+        <v>0.04637753032073141</v>
       </c>
       <c r="G66" t="n">
-        <v>24.59286072833641</v>
+        <v>-20.89138600820409</v>
       </c>
       <c r="H66" t="n">
         <v>0</v>
@@ -2592,7 +2592,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Depr_2</t>
+          <t>Depr_7</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2606,13 +2606,13 @@
         </is>
       </c>
       <c r="E67" t="n">
-        <v>1.373377711715323</v>
+        <v>0.9736646587534681</v>
       </c>
       <c r="F67" t="n">
-        <v>0.05574909455100785</v>
+        <v>0.04542680030517783</v>
       </c>
       <c r="G67" t="n">
-        <v>24.63497789070118</v>
+        <v>21.43370548202697</v>
       </c>
       <c r="H67" t="n">
         <v>0</v>
@@ -2624,7 +2624,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Depr_3</t>
+          <t>Depr_8</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2638,13 +2638,13 @@
         </is>
       </c>
       <c r="E68" t="n">
-        <v>0.9300571758592652</v>
+        <v>1.108348869541259</v>
       </c>
       <c r="F68" t="n">
-        <v>0.05558813737430393</v>
+        <v>0.05246121169222696</v>
       </c>
       <c r="G68" t="n">
-        <v>16.73121676266959</v>
+        <v>21.12701620432365</v>
       </c>
       <c r="H68" t="n">
         <v>0</v>
@@ -2656,7 +2656,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Depr_4</t>
+          <t>Mot_Stress_2</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2670,13 +2670,13 @@
         </is>
       </c>
       <c r="E69" t="n">
-        <v>-0.9555890912691544</v>
+        <v>0.7440390433598949</v>
       </c>
       <c r="F69" t="n">
-        <v>0.04517658156498004</v>
+        <v>0.04023297734668789</v>
       </c>
       <c r="G69" t="n">
-        <v>-21.15231073589585</v>
+        <v>18.49326329816487</v>
       </c>
       <c r="H69" t="n">
         <v>0</v>
@@ -2688,30 +2688,30 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Depr_5</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>~~</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Energy_Sources</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>0.9452208234457582</v>
+        <v>-0.003548160286332455</v>
       </c>
       <c r="F70" t="n">
-        <v>0.04942334599751207</v>
+        <v>0.0048678120354999</v>
       </c>
       <c r="G70" t="n">
-        <v>19.12498646842354</v>
+        <v>-0.7289024842634816</v>
       </c>
       <c r="H70" t="n">
-        <v>0</v>
+        <v>0.4660613150655566</v>
       </c>
     </row>
     <row r="71">
@@ -2720,27 +2720,27 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Depr_6</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>~~</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>-0.9680597059645693</v>
+        <v>0.4105118788818615</v>
       </c>
       <c r="F71" t="n">
-        <v>0.04633841516667089</v>
+        <v>0.03848399835113004</v>
       </c>
       <c r="G71" t="n">
-        <v>-20.89108361737756</v>
+        <v>10.66707973339106</v>
       </c>
       <c r="H71" t="n">
         <v>0</v>
@@ -2752,27 +2752,27 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Depr_7</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>~~</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Wellbeing</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>0.9733665627369689</v>
+        <v>-0.1045470168792126</v>
       </c>
       <c r="F72" t="n">
-        <v>0.045390831694753</v>
+        <v>0.009461263705098779</v>
       </c>
       <c r="G72" t="n">
-        <v>21.44412266471077</v>
+        <v>-11.05000559405411</v>
       </c>
       <c r="H72" t="n">
         <v>0</v>
@@ -2784,12 +2784,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Depr_8</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>~~</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2798,13 +2798,13 @@
         </is>
       </c>
       <c r="E73" t="n">
-        <v>1.107409220116947</v>
+        <v>0.3023110822641875</v>
       </c>
       <c r="F73" t="n">
-        <v>0.05241617843436034</v>
+        <v>0.02257096121779064</v>
       </c>
       <c r="G73" t="n">
-        <v>21.12724073317562</v>
+        <v>13.39380628648236</v>
       </c>
       <c r="H73" t="n">
         <v>0</v>
@@ -2816,30 +2816,30 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Mot_Stress_2</t>
+          <t>Energy_Sources</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>~~</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Energy_Sources</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>0.7447978474881367</v>
+        <v>0.05923130660622262</v>
       </c>
       <c r="F74" t="n">
-        <v>0.04020936776825397</v>
+        <v>0.01594896362426235</v>
       </c>
       <c r="G74" t="n">
-        <v>18.5229932428245</v>
+        <v>3.713802852519096</v>
       </c>
       <c r="H74" t="n">
-        <v>0</v>
+        <v>0.000204167869259031</v>
       </c>
     </row>
     <row r="75">
@@ -2848,7 +2848,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Negative_Outcomes</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2858,20 +2858,20 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Energy_Sources</t>
+          <t>Negative_Outcomes</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>0.001396526346221992</v>
+        <v>0.02807058658966813</v>
       </c>
       <c r="F75" t="n">
-        <v>0.001270445480389538</v>
+        <v>0.007312186717436477</v>
       </c>
       <c r="G75" t="n">
-        <v>1.099241460321898</v>
+        <v>3.838877160903558</v>
       </c>
       <c r="H75" t="n">
-        <v>0.2716627588230394</v>
+        <v>0.0001235982436800231</v>
       </c>
     </row>
     <row r="76">
@@ -2880,7 +2880,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Positive_Outcomes</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2890,20 +2890,20 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Positive_Outcomes</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>0.02722193031437132</v>
+        <v>1.399499790512308e-17</v>
       </c>
       <c r="F76" t="n">
-        <v>0.00565626413963931</v>
+        <v>0.004679283003150281</v>
       </c>
       <c r="G76" t="n">
-        <v>4.812704929882307</v>
+        <v>2.990842377498912e-15</v>
       </c>
       <c r="H76" t="n">
-        <v>1.489010573507699e-06</v>
+        <v>0.9999999999999976</v>
       </c>
     </row>
     <row r="77">
@@ -2912,7 +2912,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Wellbeing</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2926,13 +2926,13 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>-0.09946302907139609</v>
+        <v>0.1817935537819251</v>
       </c>
       <c r="F77" t="n">
-        <v>0.009198361895717063</v>
+        <v>0.01426766960241574</v>
       </c>
       <c r="G77" t="n">
-        <v>-10.8131241397335</v>
+        <v>12.74164308783846</v>
       </c>
       <c r="H77" t="n">
         <v>0</v>
@@ -2944,7 +2944,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Bekendgebruik_1</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2954,17 +2954,17 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Bekendgebruik_1</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>0.2905030897172218</v>
+        <v>1.282830366555238</v>
       </c>
       <c r="F78" t="n">
-        <v>0.02176364432465294</v>
+        <v>0.04717525107398794</v>
       </c>
       <c r="G78" t="n">
-        <v>13.34809030006083</v>
+        <v>27.19286781359363</v>
       </c>
       <c r="H78" t="n">
         <v>0</v>
@@ -2976,7 +2976,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Energy_Sources</t>
+          <t>Bekendgebruik_2</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2986,20 +2986,20 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Energy_Sources</t>
+          <t>Bekendgebruik_2</t>
         </is>
       </c>
       <c r="E79" t="n">
-        <v>0.05945031375786577</v>
+        <v>1.763407790629023</v>
       </c>
       <c r="F79" t="n">
-        <v>0.01597761013601245</v>
+        <v>0.064482387845873</v>
       </c>
       <c r="G79" t="n">
-        <v>3.720851444494063</v>
+        <v>27.34712298211732</v>
       </c>
       <c r="H79" t="n">
-        <v>0.0001985522168355125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -3008,7 +3008,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Negative_Outcomes</t>
+          <t>Bekendgebruik_3</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3018,20 +3018,20 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Negative_Outcomes</t>
+          <t>Bekendgebruik_3</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>0.02800158040625777</v>
+        <v>1.834735279543154</v>
       </c>
       <c r="F80" t="n">
-        <v>0.007294021682337425</v>
+        <v>0.06693021005228061</v>
       </c>
       <c r="G80" t="n">
-        <v>3.838976852814273</v>
+        <v>27.41266280327807</v>
       </c>
       <c r="H80" t="n">
-        <v>0.0001235480761407892</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -3040,7 +3040,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Positive_Outcomes</t>
+          <t>Bekendgebruik_4</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3050,20 +3050,20 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Positive_Outcomes</t>
+          <t>Bekendgebruik_4</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>1.444693933957835e-17</v>
+        <v>1.45450707144587</v>
       </c>
       <c r="F81" t="n">
-        <v>0.004673906041651227</v>
+        <v>0.05340987743705071</v>
       </c>
       <c r="G81" t="n">
-        <v>3.090977697827974e-15</v>
+        <v>27.23292284527202</v>
       </c>
       <c r="H81" t="n">
-        <v>0.9999999999999976</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -3072,7 +3072,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Bekendgebruik_5</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3082,17 +3082,17 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Bekendgebruik_5</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>0.1796333740922703</v>
+        <v>0.6925815160447715</v>
       </c>
       <c r="F82" t="n">
-        <v>0.01411691427379049</v>
+        <v>0.02528677778789827</v>
       </c>
       <c r="G82" t="n">
-        <v>12.7246911467794</v>
+        <v>27.38907747861958</v>
       </c>
       <c r="H82" t="n">
         <v>0</v>
@@ -3104,7 +3104,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Bekendgebruik_1</t>
+          <t>Bekendgebruik_6</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3114,17 +3114,17 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Bekendgebruik_1</t>
+          <t>Bekendgebruik_6</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>1.282480048871024</v>
+        <v>1.50463022434729</v>
       </c>
       <c r="F83" t="n">
-        <v>0.04716468637882405</v>
+        <v>0.0547616509797847</v>
       </c>
       <c r="G83" t="n">
-        <v>27.19153136189705</v>
+        <v>27.47598360164942</v>
       </c>
       <c r="H83" t="n">
         <v>0</v>
@@ -3136,7 +3136,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Bekendgebruik_2</t>
+          <t>Bekendgebruik_7</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3146,17 +3146,17 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Bekendgebruik_2</t>
+          <t>Bekendgebruik_7</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>1.763065197962473</v>
+        <v>0.6657649916919084</v>
       </c>
       <c r="F84" t="n">
-        <v>0.06447034673753474</v>
+        <v>0.02426718868021428</v>
       </c>
       <c r="G84" t="n">
-        <v>27.34691663925341</v>
+        <v>27.43478037104853</v>
       </c>
       <c r="H84" t="n">
         <v>0</v>
@@ -3168,7 +3168,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Bekendgebruik_3</t>
+          <t>Betrok_Ouders</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3178,17 +3178,17 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Bekendgebruik_3</t>
+          <t>Betrok_Ouders</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>1.834645832860533</v>
+        <v>1.474907848708279</v>
       </c>
       <c r="F85" t="n">
-        <v>0.06692774412438249</v>
+        <v>0.05387044386820244</v>
       </c>
       <c r="G85" t="n">
-        <v>27.41233634624686</v>
+        <v>27.37879517550215</v>
       </c>
       <c r="H85" t="n">
         <v>0</v>
@@ -3200,7 +3200,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Bekendgebruik_4</t>
+          <t>Bevl_1</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3210,17 +3210,17 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Bekendgebruik_4</t>
+          <t>Bevl_1</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>1.45406084015429</v>
+        <v>0.4238465805355996</v>
       </c>
       <c r="F86" t="n">
-        <v>0.05339348105536687</v>
+        <v>0.01661595101600226</v>
       </c>
       <c r="G86" t="n">
-        <v>27.2329282786274</v>
+        <v>25.50841538362137</v>
       </c>
       <c r="H86" t="n">
         <v>0</v>
@@ -3232,7 +3232,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Bekendgebruik_5</t>
+          <t>Bevl_2</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3242,17 +3242,17 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Bekendgebruik_5</t>
+          <t>Bevl_2</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>0.6925536360403841</v>
+        <v>0.2521019290223367</v>
       </c>
       <c r="F87" t="n">
-        <v>0.02528628180719317</v>
+        <v>0.01094305574449421</v>
       </c>
       <c r="G87" t="n">
-        <v>27.3885121305571</v>
+        <v>23.03761717801168</v>
       </c>
       <c r="H87" t="n">
         <v>0</v>
@@ -3264,7 +3264,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Bekendgebruik_6</t>
+          <t>Bevl_3</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3274,17 +3274,17 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Bekendgebruik_6</t>
+          <t>Bevl_3</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>1.504816267309147</v>
+        <v>0.4277152237305323</v>
       </c>
       <c r="F88" t="n">
-        <v>0.05476808105450573</v>
+        <v>0.01699607438194368</v>
       </c>
       <c r="G88" t="n">
-        <v>27.47615469280479</v>
+        <v>25.16553023324985</v>
       </c>
       <c r="H88" t="n">
         <v>0</v>
@@ -3296,7 +3296,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Bekendgebruik_7</t>
+          <t>Burn1_1</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3306,17 +3306,17 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Bekendgebruik_7</t>
+          <t>Burn1_1</t>
         </is>
       </c>
       <c r="E89" t="n">
-        <v>0.6657353765856137</v>
+        <v>0.5256867007511934</v>
       </c>
       <c r="F89" t="n">
-        <v>0.02426672504114468</v>
+        <v>0.02093867197575539</v>
       </c>
       <c r="G89" t="n">
-        <v>27.43408413905927</v>
+        <v>25.10601920383361</v>
       </c>
       <c r="H89" t="n">
         <v>0</v>
@@ -3328,7 +3328,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Betrok_Ouders</t>
+          <t>Burn1_2</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3338,17 +3338,17 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Betrok_Ouders</t>
+          <t>Burn1_2</t>
         </is>
       </c>
       <c r="E90" t="n">
-        <v>1.475154944526797</v>
+        <v>0.7094306849387786</v>
       </c>
       <c r="F90" t="n">
-        <v>0.05387888374888957</v>
+        <v>0.02785178081717521</v>
       </c>
       <c r="G90" t="n">
-        <v>27.37909254717661</v>
+        <v>25.47164540645193</v>
       </c>
       <c r="H90" t="n">
         <v>0</v>
@@ -3360,7 +3360,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Bevl_1</t>
+          <t>Burn1_3</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3370,17 +3370,17 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Bevl_1</t>
+          <t>Burn1_3</t>
         </is>
       </c>
       <c r="E91" t="n">
-        <v>0.4239115127861293</v>
+        <v>0.869507150901301</v>
       </c>
       <c r="F91" t="n">
-        <v>0.01661766531996157</v>
+        <v>0.03308834814442744</v>
       </c>
       <c r="G91" t="n">
-        <v>25.50969131935797</v>
+        <v>26.27834871295805</v>
       </c>
       <c r="H91" t="n">
         <v>0</v>
@@ -3392,7 +3392,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Bevl_2</t>
+          <t>Burn1_4</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3402,17 +3402,17 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Bevl_2</t>
+          <t>Burn1_4</t>
         </is>
       </c>
       <c r="E92" t="n">
-        <v>0.2521084098183359</v>
+        <v>0.7755227875804765</v>
       </c>
       <c r="F92" t="n">
-        <v>0.01094332616176187</v>
+        <v>0.02982046917220859</v>
       </c>
       <c r="G92" t="n">
-        <v>23.03764011678775</v>
+        <v>26.00639121658168</v>
       </c>
       <c r="H92" t="n">
         <v>0</v>
@@ -3424,7 +3424,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Bevl_3</t>
+          <t>Cijfer_huidig_1</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3434,17 +3434,17 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Bevl_3</t>
+          <t>Cijfer_huidig_1</t>
         </is>
       </c>
       <c r="E93" t="n">
-        <v>0.4277772781540122</v>
+        <v>0.2362357040420101</v>
       </c>
       <c r="F93" t="n">
-        <v>0.01699812683571732</v>
+        <v>0.009782862017889419</v>
       </c>
       <c r="G93" t="n">
-        <v>25.16614226162726</v>
+        <v>24.14791331880896</v>
       </c>
       <c r="H93" t="n">
         <v>0</v>
@@ -3456,7 +3456,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Burn1_1</t>
+          <t>Cogn_Eng1_1</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3466,17 +3466,17 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Burn1_1</t>
+          <t>Cogn_Eng1_1</t>
         </is>
       </c>
       <c r="E94" t="n">
-        <v>0.5255060016144718</v>
+        <v>0.5839510629201912</v>
       </c>
       <c r="F94" t="n">
-        <v>0.02092480535633096</v>
+        <v>0.02210177663420681</v>
       </c>
       <c r="G94" t="n">
-        <v>25.11402102148406</v>
+        <v>26.42100101536598</v>
       </c>
       <c r="H94" t="n">
         <v>0</v>
@@ -3488,7 +3488,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Burn1_2</t>
+          <t>Cogn_Eng1_2</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3498,17 +3498,17 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Burn1_2</t>
+          <t>Cogn_Eng1_2</t>
         </is>
       </c>
       <c r="E95" t="n">
-        <v>0.7088152694664491</v>
+        <v>0.6896419207478376</v>
       </c>
       <c r="F95" t="n">
-        <v>0.0278227256905037</v>
+        <v>0.02591658774191148</v>
       </c>
       <c r="G95" t="n">
-        <v>25.47612614686784</v>
+        <v>26.61005868476893</v>
       </c>
       <c r="H95" t="n">
         <v>0</v>
@@ -3520,7 +3520,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Burn1_3</t>
+          <t>Cogn_Eng1_3</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3530,17 +3530,17 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Burn1_3</t>
+          <t>Cogn_Eng1_3</t>
         </is>
       </c>
       <c r="E96" t="n">
-        <v>0.8685758471266943</v>
+        <v>0.9299303613203627</v>
       </c>
       <c r="F96" t="n">
-        <v>0.03305210882144091</v>
+        <v>0.03402770037691703</v>
       </c>
       <c r="G96" t="n">
-        <v>26.27898424856238</v>
+        <v>27.32862788235493</v>
       </c>
       <c r="H96" t="n">
         <v>0</v>
@@ -3552,7 +3552,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Burn1_4</t>
+          <t>Cogn_Eng1_4</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3562,17 +3562,17 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Burn1_4</t>
+          <t>Cogn_Eng1_4</t>
         </is>
       </c>
       <c r="E97" t="n">
-        <v>0.7748733202564244</v>
+        <v>0.56235175374102</v>
       </c>
       <c r="F97" t="n">
-        <v>0.02979206419893625</v>
+        <v>0.02104753314820012</v>
       </c>
       <c r="G97" t="n">
-        <v>26.00938676340805</v>
+        <v>26.71817878868105</v>
       </c>
       <c r="H97" t="n">
         <v>0</v>
@@ -3584,7 +3584,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Cantrill_1</t>
+          <t>Cogn_Eng1_5</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3594,17 +3594,17 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Cantrill_1</t>
+          <t>Cogn_Eng1_5</t>
         </is>
       </c>
       <c r="E98" t="n">
-        <v>0.3767829052531332</v>
+        <v>0.4221095731377473</v>
       </c>
       <c r="F98" t="n">
-        <v>0.01384426615103997</v>
+        <v>0.01725882475123018</v>
       </c>
       <c r="G98" t="n">
-        <v>27.21580913825569</v>
+        <v>24.45760816264169</v>
       </c>
       <c r="H98" t="n">
         <v>0</v>
@@ -3616,7 +3616,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Cijfer_huidig_1</t>
+          <t>Cogn_Eng1_6</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3626,17 +3626,17 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Cijfer_huidig_1</t>
+          <t>Cogn_Eng1_6</t>
         </is>
       </c>
       <c r="E99" t="n">
-        <v>0.2362271185626671</v>
+        <v>0.5635988228919729</v>
       </c>
       <c r="F99" t="n">
-        <v>0.009780019975091713</v>
+        <v>0.02164925796977164</v>
       </c>
       <c r="G99" t="n">
-        <v>24.15405276677851</v>
+        <v>26.03317045105564</v>
       </c>
       <c r="H99" t="n">
         <v>0</v>
@@ -3648,7 +3648,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_1</t>
+          <t>Cogn_Eng2_1</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3658,17 +3658,17 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_1</t>
+          <t>Cogn_Eng2_1</t>
         </is>
       </c>
       <c r="E100" t="n">
-        <v>0.584205880175639</v>
+        <v>0.534059236505266</v>
       </c>
       <c r="F100" t="n">
-        <v>0.02210793932969263</v>
+        <v>0.02130145695725262</v>
       </c>
       <c r="G100" t="n">
-        <v>26.42516208485254</v>
+        <v>25.07148865694656</v>
       </c>
       <c r="H100" t="n">
         <v>0</v>
@@ -3680,7 +3680,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_2</t>
+          <t>Cogn_Eng2_2</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3690,17 +3690,17 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_2</t>
+          <t>Cogn_Eng2_2</t>
         </is>
       </c>
       <c r="E101" t="n">
-        <v>0.6898136990164055</v>
+        <v>0.8745070613203508</v>
       </c>
       <c r="F101" t="n">
-        <v>0.02592080177101507</v>
+        <v>0.0325558528409341</v>
       </c>
       <c r="G101" t="n">
-        <v>26.61235964395016</v>
+        <v>26.86174635222357</v>
       </c>
       <c r="H101" t="n">
         <v>0</v>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_3</t>
+          <t>Cogn_Eng2_3</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3722,17 +3722,17 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_3</t>
+          <t>Cogn_Eng2_3</t>
         </is>
       </c>
       <c r="E102" t="n">
-        <v>0.9300462315004739</v>
+        <v>0.8085558109584936</v>
       </c>
       <c r="F102" t="n">
-        <v>0.03403082352530033</v>
+        <v>0.02993504939967203</v>
       </c>
       <c r="G102" t="n">
-        <v>27.32952468169624</v>
+        <v>27.01033828727678</v>
       </c>
       <c r="H102" t="n">
         <v>0</v>
@@ -3744,7 +3744,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_4</t>
+          <t>Cogn_Eng2_4</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3754,17 +3754,17 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_4</t>
+          <t>Cogn_Eng2_4</t>
         </is>
       </c>
       <c r="E103" t="n">
-        <v>0.5625037971774369</v>
+        <v>0.8017594098532599</v>
       </c>
       <c r="F103" t="n">
-        <v>0.02105206520353393</v>
+        <v>0.03135248340145978</v>
       </c>
       <c r="G103" t="n">
-        <v>26.71964919889626</v>
+        <v>25.57243710366998</v>
       </c>
       <c r="H103" t="n">
         <v>0</v>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_5</t>
+          <t>Cogn_Eng2_5</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3786,17 +3786,17 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_5</t>
+          <t>Cogn_Eng2_5</t>
         </is>
       </c>
       <c r="E104" t="n">
-        <v>0.4220376692614248</v>
+        <v>0.7366029766613043</v>
       </c>
       <c r="F104" t="n">
-        <v>0.01725683254081116</v>
+        <v>0.02973685669374788</v>
       </c>
       <c r="G104" t="n">
-        <v>24.45626497440247</v>
+        <v>24.77070741614069</v>
       </c>
       <c r="H104" t="n">
         <v>0</v>
@@ -3808,7 +3808,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_6</t>
+          <t>Cogn_Eng2_6</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3818,17 +3818,17 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_6</t>
+          <t>Cogn_Eng2_6</t>
         </is>
       </c>
       <c r="E105" t="n">
-        <v>0.5634763944085057</v>
+        <v>0.6029692184563709</v>
       </c>
       <c r="F105" t="n">
-        <v>0.02164539703002199</v>
+        <v>0.02287223949024981</v>
       </c>
       <c r="G105" t="n">
-        <v>26.03215795029939</v>
+        <v>26.36249146862281</v>
       </c>
       <c r="H105" t="n">
         <v>0</v>
@@ -3840,7 +3840,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_1</t>
+          <t>Cogn_Eng2_7</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3850,17 +3850,17 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_1</t>
+          <t>Cogn_Eng2_7</t>
         </is>
       </c>
       <c r="E106" t="n">
-        <v>0.5342710228737891</v>
+        <v>0.6376924576707522</v>
       </c>
       <c r="F106" t="n">
-        <v>0.02130636298181444</v>
+        <v>0.02659722561101119</v>
       </c>
       <c r="G106" t="n">
-        <v>25.07565572335026</v>
+        <v>23.97590135802634</v>
       </c>
       <c r="H106" t="n">
         <v>0</v>
@@ -3872,7 +3872,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_2</t>
+          <t>Cogn_Eng2_8</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3882,17 +3882,17 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_2</t>
+          <t>Cogn_Eng2_8</t>
         </is>
       </c>
       <c r="E107" t="n">
-        <v>0.8744782548370488</v>
+        <v>0.6577478521030644</v>
       </c>
       <c r="F107" t="n">
-        <v>0.03255496220725591</v>
+        <v>0.02460785446994701</v>
       </c>
       <c r="G107" t="n">
-        <v>26.86159637486177</v>
+        <v>26.72918327274843</v>
       </c>
       <c r="H107" t="n">
         <v>0</v>
@@ -3904,7 +3904,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_3</t>
+          <t>Depr_1</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3914,17 +3914,17 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_3</t>
+          <t>Depr_1</t>
         </is>
       </c>
       <c r="E108" t="n">
-        <v>0.8085554869582205</v>
+        <v>0.5388749419206935</v>
       </c>
       <c r="F108" t="n">
-        <v>0.02993520803166324</v>
+        <v>0.02266291379164589</v>
       </c>
       <c r="G108" t="n">
-        <v>27.01018433130581</v>
+        <v>23.77783134380356</v>
       </c>
       <c r="H108" t="n">
         <v>0</v>
@@ -3936,7 +3936,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_4</t>
+          <t>Depr_2</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3946,17 +3946,17 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_4</t>
+          <t>Depr_2</t>
         </is>
       </c>
       <c r="E109" t="n">
-        <v>0.8018443817644997</v>
+        <v>0.6330556595805535</v>
       </c>
       <c r="F109" t="n">
-        <v>0.03135618008713881</v>
+        <v>0.02666694426190306</v>
       </c>
       <c r="G109" t="n">
-        <v>25.5721321765152</v>
+        <v>23.73934011109066</v>
       </c>
       <c r="H109" t="n">
         <v>0</v>
@@ -3968,7 +3968,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_5</t>
+          <t>Depr_3</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3978,17 +3978,17 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_5</t>
+          <t>Depr_3</t>
         </is>
       </c>
       <c r="E110" t="n">
-        <v>0.7365362472222198</v>
+        <v>1.188237281242588</v>
       </c>
       <c r="F110" t="n">
-        <v>0.02973823317014655</v>
+        <v>0.0446979475463557</v>
       </c>
       <c r="G110" t="n">
-        <v>24.76731697486462</v>
+        <v>26.58371013531881</v>
       </c>
       <c r="H110" t="n">
         <v>0</v>
@@ -4000,7 +4000,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_6</t>
+          <t>Depr_4</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -4010,17 +4010,17 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_6</t>
+          <t>Depr_4</t>
         </is>
       </c>
       <c r="E111" t="n">
-        <v>0.6031133049333357</v>
+        <v>0.5962845887310414</v>
       </c>
       <c r="F111" t="n">
-        <v>0.02287528366334975</v>
+        <v>0.02332073526727262</v>
       </c>
       <c r="G111" t="n">
-        <v>26.36528201279814</v>
+        <v>25.56885886622427</v>
       </c>
       <c r="H111" t="n">
         <v>0</v>
@@ -4032,7 +4032,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_7</t>
+          <t>Depr_5</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -4042,17 +4042,17 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_7</t>
+          <t>Depr_5</t>
         </is>
       </c>
       <c r="E112" t="n">
-        <v>0.6375833171259999</v>
+        <v>0.8240026378692793</v>
       </c>
       <c r="F112" t="n">
-        <v>0.02659251262463058</v>
+        <v>0.03152904872984097</v>
       </c>
       <c r="G112" t="n">
-        <v>23.97604641960309</v>
+        <v>26.13471294055439</v>
       </c>
       <c r="H112" t="n">
         <v>0</v>
@@ -4064,7 +4064,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_8</t>
+          <t>Depr_6</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -4074,17 +4074,17 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_8</t>
+          <t>Depr_6</t>
         </is>
       </c>
       <c r="E113" t="n">
-        <v>0.6576900854277336</v>
+        <v>0.6405828386239086</v>
       </c>
       <c r="F113" t="n">
-        <v>0.02460595459758396</v>
+        <v>0.02496781646557808</v>
       </c>
       <c r="G113" t="n">
-        <v>26.72889941305439</v>
+        <v>25.65634201458477</v>
       </c>
       <c r="H113" t="n">
         <v>0</v>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Depr_1</t>
+          <t>Depr_7</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -4106,17 +4106,17 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Depr_1</t>
+          <t>Depr_7</t>
         </is>
       </c>
       <c r="E114" t="n">
-        <v>0.5393691813976077</v>
+        <v>0.5884760936158361</v>
       </c>
       <c r="F114" t="n">
-        <v>0.0226620978677848</v>
+        <v>0.02310186225329814</v>
       </c>
       <c r="G114" t="n">
-        <v>23.80049651716247</v>
+        <v>25.47310200095878</v>
       </c>
       <c r="H114" t="n">
         <v>0</v>
@@ -4128,7 +4128,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Depr_2</t>
+          <t>Depr_8</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -4138,17 +4138,17 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Depr_2</t>
+          <t>Depr_8</t>
         </is>
       </c>
       <c r="E115" t="n">
-        <v>0.6340424140319842</v>
+        <v>0.8046495158083297</v>
       </c>
       <c r="F115" t="n">
-        <v>0.02667787491318433</v>
+        <v>0.03145708945813624</v>
       </c>
       <c r="G115" t="n">
-        <v>23.76660120311423</v>
+        <v>25.57927416818378</v>
       </c>
       <c r="H115" t="n">
         <v>0</v>
@@ -4160,7 +4160,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Depr_3</t>
+          <t>Hulp_1</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -4170,17 +4170,17 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Depr_3</t>
+          <t>Hulp_1</t>
         </is>
       </c>
       <c r="E116" t="n">
-        <v>1.187877016492028</v>
+        <v>2.220296664639501</v>
       </c>
       <c r="F116" t="n">
-        <v>0.04467984459681882</v>
+        <v>0.08076630756456046</v>
       </c>
       <c r="G116" t="n">
-        <v>26.58641781735332</v>
+        <v>27.49038220965121</v>
       </c>
       <c r="H116" t="n">
         <v>0</v>
@@ -4192,7 +4192,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Depr_4</t>
+          <t>Hulp_2</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -4202,17 +4202,17 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Depr_4</t>
+          <t>Hulp_2</t>
         </is>
       </c>
       <c r="E117" t="n">
-        <v>0.5969028429211753</v>
+        <v>1.165452564784034</v>
       </c>
       <c r="F117" t="n">
-        <v>0.02333256002031888</v>
+        <v>0.04239328075045171</v>
       </c>
       <c r="G117" t="n">
-        <v>25.58239826130469</v>
+        <v>27.49144543959656</v>
       </c>
       <c r="H117" t="n">
         <v>0</v>
@@ -4224,7 +4224,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Depr_5</t>
+          <t>Hulp_3</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -4234,17 +4234,17 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Depr_5</t>
+          <t>Hulp_3</t>
         </is>
       </c>
       <c r="E118" t="n">
-        <v>0.8240607134634649</v>
+        <v>1.951092922105484</v>
       </c>
       <c r="F118" t="n">
-        <v>0.03152375005630224</v>
+        <v>0.07096061329281503</v>
       </c>
       <c r="G118" t="n">
-        <v>26.14094807773599</v>
+        <v>27.49543488338963</v>
       </c>
       <c r="H118" t="n">
         <v>0</v>
@@ -4256,7 +4256,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Depr_6</t>
+          <t>Mot_Stress_1</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -4266,17 +4266,17 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Depr_6</t>
+          <t>Mot_Stress_1</t>
         </is>
       </c>
       <c r="E119" t="n">
-        <v>0.640985949893855</v>
+        <v>0.3237655712122806</v>
       </c>
       <c r="F119" t="n">
-        <v>0.02497273966914319</v>
+        <v>0.01350485156137078</v>
       </c>
       <c r="G119" t="n">
-        <v>25.66742609583211</v>
+        <v>23.97401924167788</v>
       </c>
       <c r="H119" t="n">
         <v>0</v>
@@ -4288,7 +4288,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Depr_7</t>
+          <t>Mot_Stress_2</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -4298,17 +4298,17 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Depr_7</t>
+          <t>Mot_Stress_2</t>
         </is>
       </c>
       <c r="E120" t="n">
-        <v>0.588465954269452</v>
+        <v>0.5661452912391401</v>
       </c>
       <c r="F120" t="n">
-        <v>0.02309361203579888</v>
+        <v>0.02155134059542743</v>
       </c>
       <c r="G120" t="n">
-        <v>25.48176323962452</v>
+        <v>26.26960901601593</v>
       </c>
       <c r="H120" t="n">
         <v>0</v>
@@ -4320,7 +4320,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Depr_8</t>
+          <t>Mot_Stress_4</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -4330,17 +4330,17 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Depr_8</t>
+          <t>Mot_Stress_4</t>
         </is>
       </c>
       <c r="E121" t="n">
-        <v>0.8051443023149073</v>
+        <v>0.2156491174349992</v>
       </c>
       <c r="F121" t="n">
-        <v>0.03146230621407725</v>
+        <v>0.009972489461090141</v>
       </c>
       <c r="G121" t="n">
-        <v>25.59075920280342</v>
+        <v>21.62440163559733</v>
       </c>
       <c r="H121" t="n">
         <v>0</v>
@@ -4352,7 +4352,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Hulp_1</t>
+          <t>Onnodige_stress_1</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -4362,17 +4362,17 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Hulp_1</t>
+          <t>Onnodige_stress_1</t>
         </is>
       </c>
       <c r="E122" t="n">
-        <v>2.220522237379774</v>
+        <v>1.000904897128694</v>
       </c>
       <c r="F122" t="n">
-        <v>0.08077487528280557</v>
+        <v>0.03868153819412846</v>
       </c>
       <c r="G122" t="n">
-        <v>27.49025893977409</v>
+        <v>25.87551953284908</v>
       </c>
       <c r="H122" t="n">
         <v>0</v>
@@ -4384,7 +4384,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Hulp_2</t>
+          <t>Onnodige_stress_2</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -4394,17 +4394,17 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Hulp_2</t>
+          <t>Onnodige_stress_2</t>
         </is>
       </c>
       <c r="E123" t="n">
-        <v>1.165467424005202</v>
+        <v>0.7484894114137542</v>
       </c>
       <c r="F123" t="n">
-        <v>0.04239382237647947</v>
+        <v>0.03065637548476587</v>
       </c>
       <c r="G123" t="n">
-        <v>27.49144471163148</v>
+        <v>24.41545680314645</v>
       </c>
       <c r="H123" t="n">
         <v>0</v>
@@ -4416,7 +4416,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Hulp_3</t>
+          <t>Onnodige_stress_3</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -4426,17 +4426,17 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Hulp_3</t>
+          <t>Onnodige_stress_3</t>
         </is>
       </c>
       <c r="E124" t="n">
-        <v>1.951343187756664</v>
+        <v>0.8442890493217505</v>
       </c>
       <c r="F124" t="n">
-        <v>0.07096970318010774</v>
+        <v>0.03353492639094185</v>
       </c>
       <c r="G124" t="n">
-        <v>27.49543960719445</v>
+        <v>25.17640979598589</v>
       </c>
       <c r="H124" t="n">
         <v>0</v>
@@ -4448,7 +4448,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Leefst</t>
+          <t>Onnodige_stress_4</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -4458,17 +4458,17 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Leefst</t>
+          <t>Onnodige_stress_4</t>
         </is>
       </c>
       <c r="E125" t="n">
-        <v>0.5871380959140995</v>
+        <v>0.6189804970117662</v>
       </c>
       <c r="F125" t="n">
-        <v>0.02137032631859922</v>
+        <v>0.02769332106927347</v>
       </c>
       <c r="G125" t="n">
-        <v>27.47445626862616</v>
+        <v>22.35125557678929</v>
       </c>
       <c r="H125" t="n">
         <v>0</v>
@@ -4480,7 +4480,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Mot_Stress_1</t>
+          <t>Onnodige_stress_5</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -4490,17 +4490,17 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Mot_Stress_1</t>
+          <t>Onnodige_stress_5</t>
         </is>
       </c>
       <c r="E126" t="n">
-        <v>0.3237523884120583</v>
+        <v>0.579185509807646</v>
       </c>
       <c r="F126" t="n">
-        <v>0.01350421769289169</v>
+        <v>0.02618191129271775</v>
       </c>
       <c r="G126" t="n">
-        <v>23.97416834878928</v>
+        <v>22.12159010509746</v>
       </c>
       <c r="H126" t="n">
         <v>0</v>
@@ -4512,7 +4512,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Mot_Stress_2</t>
+          <t>Onnodige_stress_6</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -4522,17 +4522,17 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Mot_Stress_2</t>
+          <t>Onnodige_stress_6</t>
         </is>
       </c>
       <c r="E127" t="n">
-        <v>0.5655504568466994</v>
+        <v>0.6904520829840032</v>
       </c>
       <c r="F127" t="n">
-        <v>0.02152810766594596</v>
+        <v>0.02899241448485626</v>
       </c>
       <c r="G127" t="n">
-        <v>26.27032833522288</v>
+        <v>23.81492177275664</v>
       </c>
       <c r="H127" t="n">
         <v>0</v>
@@ -4544,7 +4544,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Mot_Stress_4</t>
+          <t>Onnodige_stress_7</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -4554,17 +4554,17 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Mot_Stress_4</t>
+          <t>Onnodige_stress_7</t>
         </is>
       </c>
       <c r="E128" t="n">
-        <v>0.2157097302197408</v>
+        <v>1.446350998140927</v>
       </c>
       <c r="F128" t="n">
-        <v>0.009974171711313366</v>
+        <v>0.05455760000971599</v>
       </c>
       <c r="G128" t="n">
-        <v>21.62683142435193</v>
+        <v>26.51053194892811</v>
       </c>
       <c r="H128" t="n">
         <v>0</v>
@@ -4576,7 +4576,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Onnodige_stress_1</t>
+          <t>Onnodige_stress_8</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -4586,17 +4586,17 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Onnodige_stress_1</t>
+          <t>Onnodige_stress_8</t>
         </is>
       </c>
       <c r="E129" t="n">
-        <v>0.9949800977194323</v>
+        <v>0.9734085372652544</v>
       </c>
       <c r="F129" t="n">
-        <v>0.03845893600837709</v>
+        <v>0.03788712339250746</v>
       </c>
       <c r="G129" t="n">
-        <v>25.87123308551322</v>
+        <v>25.69233159126731</v>
       </c>
       <c r="H129" t="n">
         <v>0</v>
@@ -4608,7 +4608,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Onnodige_stress_10</t>
+          <t>Onnodige_stress_9</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -4618,17 +4618,17 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Onnodige_stress_10</t>
+          <t>Onnodige_stress_9</t>
         </is>
       </c>
       <c r="E130" t="n">
-        <v>1.520428676925219</v>
+        <v>0.8436355617375196</v>
       </c>
       <c r="F130" t="n">
-        <v>0.05639281047993162</v>
+        <v>0.03416562860521006</v>
       </c>
       <c r="G130" t="n">
-        <v>26.96139213418577</v>
+        <v>24.69252275323796</v>
       </c>
       <c r="H130" t="n">
         <v>0</v>
@@ -4640,7 +4640,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Onnodige_stress_2</t>
+          <t>Partici1_1</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -4650,17 +4650,17 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Onnodige_stress_2</t>
+          <t>Partici1_1</t>
         </is>
       </c>
       <c r="E131" t="n">
-        <v>0.7574570143210273</v>
+        <v>0.8592004597570998</v>
       </c>
       <c r="F131" t="n">
-        <v>0.03085373853647934</v>
+        <v>0.03526679728833845</v>
       </c>
       <c r="G131" t="n">
-        <v>24.54992653162314</v>
+        <v>24.3628717603128</v>
       </c>
       <c r="H131" t="n">
         <v>0</v>
@@ -4672,7 +4672,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Onnodige_stress_3</t>
+          <t>Partici1_2</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -4682,17 +4682,17 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Onnodige_stress_3</t>
+          <t>Partici1_2</t>
         </is>
       </c>
       <c r="E132" t="n">
-        <v>0.833324036491465</v>
+        <v>1.204157666945431</v>
       </c>
       <c r="F132" t="n">
-        <v>0.03315655495516684</v>
+        <v>0.04796907519608008</v>
       </c>
       <c r="G132" t="n">
-        <v>25.13301027785077</v>
+        <v>25.10279095434239</v>
       </c>
       <c r="H132" t="n">
         <v>0</v>
@@ -4704,7 +4704,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Onnodige_stress_4</t>
+          <t>Partici1_3</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -4714,17 +4714,17 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Onnodige_stress_4</t>
+          <t>Partici1_3</t>
         </is>
       </c>
       <c r="E133" t="n">
-        <v>0.6395416274562093</v>
+        <v>1.109106599303096</v>
       </c>
       <c r="F133" t="n">
-        <v>0.02813130610857694</v>
+        <v>0.04314037341224033</v>
       </c>
       <c r="G133" t="n">
-        <v>22.73416047463526</v>
+        <v>25.70924893669781</v>
       </c>
       <c r="H133" t="n">
         <v>0</v>
@@ -4736,7 +4736,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Onnodige_stress_5</t>
+          <t>Partici1_4</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -4746,17 +4746,17 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Onnodige_stress_5</t>
+          <t>Partici1_4</t>
         </is>
       </c>
       <c r="E134" t="n">
-        <v>0.6020038327161941</v>
+        <v>1.151882888797957</v>
       </c>
       <c r="F134" t="n">
-        <v>0.02667615341649269</v>
+        <v>0.04401210006997051</v>
       </c>
       <c r="G134" t="n">
-        <v>22.56711540433092</v>
+        <v>26.17195923258648</v>
       </c>
       <c r="H134" t="n">
         <v>0</v>
@@ -4768,7 +4768,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Onnodige_stress_6</t>
+          <t>StopInt</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -4778,17 +4778,17 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>Onnodige_stress_6</t>
+          <t>StopInt</t>
         </is>
       </c>
       <c r="E135" t="n">
-        <v>0.7039587527478598</v>
+        <v>0.1148350441809471</v>
       </c>
       <c r="F135" t="n">
-        <v>0.02930117615323052</v>
+        <v>0.008385458400948448</v>
       </c>
       <c r="G135" t="n">
-        <v>24.02493159463914</v>
+        <v>13.69454580494538</v>
       </c>
       <c r="H135" t="n">
         <v>0</v>
@@ -4800,7 +4800,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Onnodige_stress_7</t>
+          <t>Stopint2</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -4810,17 +4810,17 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Onnodige_stress_7</t>
+          <t>Stopint2</t>
         </is>
       </c>
       <c r="E136" t="n">
-        <v>1.432160938923689</v>
+        <v>0.5962079965110721</v>
       </c>
       <c r="F136" t="n">
-        <v>0.05408666577884524</v>
+        <v>0.02960685590385007</v>
       </c>
       <c r="G136" t="n">
-        <v>26.47900213988356</v>
+        <v>20.13749782912288</v>
       </c>
       <c r="H136" t="n">
         <v>0</v>
@@ -4832,7 +4832,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Onnodige_stress_8</t>
+          <t>Vertr</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -4842,339 +4842,19 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Onnodige_stress_8</t>
+          <t>Vertr</t>
         </is>
       </c>
       <c r="E137" t="n">
-        <v>0.9623097286663731</v>
+        <v>1.040099187620206</v>
       </c>
       <c r="F137" t="n">
-        <v>0.03750472256259775</v>
+        <v>0.04189994874316431</v>
       </c>
       <c r="G137" t="n">
-        <v>25.65836147793279</v>
+        <v>24.82339999914839</v>
       </c>
       <c r="H137" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" s="1" t="n">
-        <v>136</v>
-      </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>Onnodige_stress_9</t>
-        </is>
-      </c>
-      <c r="C138" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D138" t="inlineStr">
-        <is>
-          <t>Onnodige_stress_9</t>
-        </is>
-      </c>
-      <c r="E138" t="n">
-        <v>0.8387136768886635</v>
-      </c>
-      <c r="F138" t="n">
-        <v>0.03395796034877305</v>
-      </c>
-      <c r="G138" t="n">
-        <v>24.69858814398047</v>
-      </c>
-      <c r="H138" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" s="1" t="n">
-        <v>137</v>
-      </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>Partici1_1</t>
-        </is>
-      </c>
-      <c r="C139" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D139" t="inlineStr">
-        <is>
-          <t>Partici1_1</t>
-        </is>
-      </c>
-      <c r="E139" t="n">
-        <v>0.8588914642370777</v>
-      </c>
-      <c r="F139" t="n">
-        <v>0.03526345816057355</v>
-      </c>
-      <c r="G139" t="n">
-        <v>24.35641621708584</v>
-      </c>
-      <c r="H139" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" s="1" t="n">
-        <v>138</v>
-      </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>Partici1_2</t>
-        </is>
-      </c>
-      <c r="C140" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D140" t="inlineStr">
-        <is>
-          <t>Partici1_2</t>
-        </is>
-      </c>
-      <c r="E140" t="n">
-        <v>1.203406643769366</v>
-      </c>
-      <c r="F140" t="n">
-        <v>0.04794735298833894</v>
-      </c>
-      <c r="G140" t="n">
-        <v>25.09850009940991</v>
-      </c>
-      <c r="H140" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" s="1" t="n">
-        <v>139</v>
-      </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>Partici1_3</t>
-        </is>
-      </c>
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D141" t="inlineStr">
-        <is>
-          <t>Partici1_3</t>
-        </is>
-      </c>
-      <c r="E141" t="n">
-        <v>1.108642139349389</v>
-      </c>
-      <c r="F141" t="n">
-        <v>0.04312822348898525</v>
-      </c>
-      <c r="G141" t="n">
-        <v>25.70572237010471</v>
-      </c>
-      <c r="H141" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" s="1" t="n">
-        <v>140</v>
-      </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>Partici1_4</t>
-        </is>
-      </c>
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D142" t="inlineStr">
-        <is>
-          <t>Partici1_4</t>
-        </is>
-      </c>
-      <c r="E142" t="n">
-        <v>1.151430418465126</v>
-      </c>
-      <c r="F142" t="n">
-        <v>0.04400451995167144</v>
-      </c>
-      <c r="G142" t="n">
-        <v>26.16618519423764</v>
-      </c>
-      <c r="H142" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" s="1" t="n">
-        <v>141</v>
-      </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>Q297_1</t>
-        </is>
-      </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D143" t="inlineStr">
-        <is>
-          <t>Q297_1</t>
-        </is>
-      </c>
-      <c r="E143" t="n">
-        <v>0.2598549534235534</v>
-      </c>
-      <c r="F143" t="n">
-        <v>0.009456097251513237</v>
-      </c>
-      <c r="G143" t="n">
-        <v>27.48014815038934</v>
-      </c>
-      <c r="H143" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" s="1" t="n">
-        <v>142</v>
-      </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>StopInt</t>
-        </is>
-      </c>
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D144" t="inlineStr">
-        <is>
-          <t>StopInt</t>
-        </is>
-      </c>
-      <c r="E144" t="n">
-        <v>0.1149140422923449</v>
-      </c>
-      <c r="F144" t="n">
-        <v>0.008371305089670895</v>
-      </c>
-      <c r="G144" t="n">
-        <v>13.72713585847048</v>
-      </c>
-      <c r="H144" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" s="1" t="n">
-        <v>143</v>
-      </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>Stopint2</t>
-        </is>
-      </c>
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D145" t="inlineStr">
-        <is>
-          <t>Stopint2</t>
-        </is>
-      </c>
-      <c r="E145" t="n">
-        <v>0.5961933263470798</v>
-      </c>
-      <c r="F145" t="n">
-        <v>0.02962108348061309</v>
-      </c>
-      <c r="G145" t="n">
-        <v>20.12733014027522</v>
-      </c>
-      <c r="H145" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" s="1" t="n">
-        <v>144</v>
-      </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>Vertr</t>
-        </is>
-      </c>
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D146" t="inlineStr">
-        <is>
-          <t>Vertr</t>
-        </is>
-      </c>
-      <c r="E146" t="n">
-        <v>1.039936469507579</v>
-      </c>
-      <c r="F146" t="n">
-        <v>0.04191008813002916</v>
-      </c>
-      <c r="G146" t="n">
-        <v>24.81351187466571</v>
-      </c>
-      <c r="H146" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" s="1" t="n">
-        <v>145</v>
-      </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>Werk_1</t>
-        </is>
-      </c>
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D147" t="inlineStr">
-        <is>
-          <t>Werk_1</t>
-        </is>
-      </c>
-      <c r="E147" t="n">
-        <v>0.7148657716873199</v>
-      </c>
-      <c r="F147" t="n">
-        <v>0.02599969149082662</v>
-      </c>
-      <c r="G147" t="n">
-        <v>27.49516362192407</v>
-      </c>
-      <c r="H147" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Model with split up Energy Sources variables
</commit_message>
<xml_diff>
--- a/model_coefficients.xlsx
+++ b/model_coefficients.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H116"/>
+  <dimension ref="A1:H124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,20 +486,20 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Behavior</t>
+          <t>Interventions</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1.514499566704271</v>
+        <v>0.22000606286011</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1536842729542066</v>
+        <v>0.04601361385221889</v>
       </c>
       <c r="G2" t="n">
-        <v>9.854616465184385</v>
+        <v>4.78132544776679</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>1.741431733259802e-06</v>
       </c>
     </row>
     <row r="3">
@@ -508,7 +508,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Participation</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -518,17 +518,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Behavior</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.4602184924030199</v>
+        <v>1.504491051061317</v>
       </c>
       <c r="F3" t="n">
-        <v>0.03550513721240449</v>
+        <v>0.1518252416844932</v>
       </c>
       <c r="G3" t="n">
-        <v>12.96202545667872</v>
+        <v>9.909360488145165</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -550,20 +550,20 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Participation</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>-0.08981114924049034</v>
+        <v>0.4229650206001207</v>
       </c>
       <c r="F4" t="n">
-        <v>0.02489169723174074</v>
+        <v>0.03409781654837914</v>
       </c>
       <c r="G4" t="n">
-        <v>-3.608076556642319</v>
+        <v>12.40446056091595</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0003084754750632968</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -572,7 +572,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -582,20 +582,20 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Participation</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>-0.2885892360037228</v>
+        <v>-0.0881554897120936</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02783988448766571</v>
+        <v>0.02512821280925571</v>
       </c>
       <c r="G5" t="n">
-        <v>-10.36603568241149</v>
+        <v>-3.508227599700773</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>0.0004511029403850841</v>
       </c>
     </row>
     <row r="6">
@@ -614,17 +614,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Participation</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.2975551870387255</v>
+        <v>-0.2558348428210345</v>
       </c>
       <c r="F6" t="n">
-        <v>0.02563012712824544</v>
+        <v>0.02684985439739583</v>
       </c>
       <c r="G6" t="n">
-        <v>11.60958685605574</v>
+        <v>-9.528351216545875</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -636,7 +636,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Negative_Outcomes</t>
+          <t>Wellbeing</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -646,20 +646,20 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Participation</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0.08200615108674134</v>
+        <v>0.2967352896833194</v>
       </c>
       <c r="F7" t="n">
-        <v>0.01858575918955003</v>
+        <v>0.02573431528212479</v>
       </c>
       <c r="G7" t="n">
-        <v>4.412311073546975</v>
+        <v>11.53072410976106</v>
       </c>
       <c r="H7" t="n">
-        <v>1.022730271360572e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -678,20 +678,20 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>-0.2816541540540421</v>
+        <v>0.08205195815105283</v>
       </c>
       <c r="F8" t="n">
-        <v>0.02307623585989477</v>
+        <v>0.01861487005221737</v>
       </c>
       <c r="G8" t="n">
-        <v>-12.20537681066678</v>
+        <v>4.407871659403343</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>1.043913690290665e-05</v>
       </c>
     </row>
     <row r="9">
@@ -700,7 +700,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Positive_Outcomes</t>
+          <t>Negative_Outcomes</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -714,16 +714,16 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.1868296199472279</v>
+        <v>-0.2813538621498325</v>
       </c>
       <c r="F9" t="n">
-        <v>0.02629527693798333</v>
+        <v>0.02304703269200632</v>
       </c>
       <c r="G9" t="n">
-        <v>7.105063786958974</v>
+        <v>-12.20781286239986</v>
       </c>
       <c r="H9" t="n">
-        <v>1.20259358027397e-12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -742,20 +742,20 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Wellbeing</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0.001247157208958832</v>
+        <v>0.186688753059603</v>
       </c>
       <c r="F10" t="n">
-        <v>0.01578784848974785</v>
+        <v>0.02626709562129757</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0789947540787273</v>
+        <v>7.107323769024808</v>
       </c>
       <c r="H10" t="n">
-        <v>0.937036795664274</v>
+        <v>1.183053655040567e-12</v>
       </c>
     </row>
     <row r="11">
@@ -764,7 +764,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Bevl_1</t>
+          <t>Positive_Outcomes</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -774,26 +774,20 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>0.001193803198630036</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0158202612865855</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.07546039707743891</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.9398484062141881</v>
       </c>
     </row>
     <row r="12">
@@ -802,7 +796,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Bevl_2</t>
+          <t>Bevl_1</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -816,16 +810,22 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1.158443906224244</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.04392512887182232</v>
-      </c>
-      <c r="G12" t="n">
-        <v>26.37314757979013</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -834,7 +834,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Bevl_3</t>
+          <t>Bevl_2</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -848,13 +848,13 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>1.085684741454036</v>
+        <v>1.157228755222232</v>
       </c>
       <c r="F13" t="n">
-        <v>0.04672439958765086</v>
+        <v>0.04383595579127213</v>
       </c>
       <c r="G13" t="n">
-        <v>23.23592707476425</v>
+        <v>26.3990766097597</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -866,7 +866,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_5</t>
+          <t>Bevl_3</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -880,13 +880,13 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>1.21149388708344</v>
+        <v>1.085003590900024</v>
       </c>
       <c r="F14" t="n">
-        <v>0.04995572958897787</v>
+        <v>0.04664425713781688</v>
       </c>
       <c r="G14" t="n">
-        <v>24.25135008590666</v>
+        <v>23.26124709567076</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -898,7 +898,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_6</t>
+          <t>Cogn_Eng1_5</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -912,13 +912,13 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0.9663225135987087</v>
+        <v>1.209691211324009</v>
       </c>
       <c r="F15" t="n">
-        <v>0.04778593743167492</v>
+        <v>0.04985715088071573</v>
       </c>
       <c r="G15" t="n">
-        <v>20.22190136920825</v>
+        <v>24.26314359988113</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -930,7 +930,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_2</t>
+          <t>Cogn_Eng1_6</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -944,13 +944,13 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.7704670120872801</v>
+        <v>0.9645820987828628</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0517733472784784</v>
+        <v>0.04769888057479481</v>
       </c>
       <c r="G16" t="n">
-        <v>14.88153755885653</v>
+        <v>20.22232151234903</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -962,7 +962,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_3</t>
+          <t>Cogn_Eng2_2</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -976,13 +976,13 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0.6461929164955096</v>
+        <v>0.769213818840775</v>
       </c>
       <c r="F17" t="n">
-        <v>0.04835559920765859</v>
+        <v>0.05169998405195595</v>
       </c>
       <c r="G17" t="n">
-        <v>13.36335247769615</v>
+        <v>14.87841501175077</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -994,7 +994,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_8</t>
+          <t>Cogn_Eng2_3</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1008,13 +1008,13 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0.743591741068354</v>
+        <v>0.645232430084827</v>
       </c>
       <c r="F18" t="n">
-        <v>0.04605162689738987</v>
+        <v>0.04829110357116322</v>
       </c>
       <c r="G18" t="n">
-        <v>16.14691578017524</v>
+        <v>13.36131051800528</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -1026,7 +1026,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Mot_Stress_1</t>
+          <t>Cogn_Eng2_8</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1040,13 +1040,13 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>1.165624869670636</v>
+        <v>0.7420155188042223</v>
       </c>
       <c r="F19" t="n">
-        <v>0.04598041674764562</v>
+        <v>0.04598415648044851</v>
       </c>
       <c r="G19" t="n">
-        <v>25.35046335144343</v>
+        <v>16.13632989230922</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Mot_Stress_4</t>
+          <t>Mot_Stress_1</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1072,13 +1072,13 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>1.232159566032149</v>
+        <v>1.164872911068902</v>
       </c>
       <c r="F20" t="n">
-        <v>0.04495477981887783</v>
+        <v>0.04589416102893826</v>
       </c>
       <c r="G20" t="n">
-        <v>27.40886666488176</v>
+        <v>25.38172362076774</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>StopInt</t>
+          <t>Mot_Stress_4</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1100,26 +1100,20 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Negative_Outcomes</t>
+          <t>Wellbeing</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>1.23117918955364</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.04486338066553105</v>
+      </c>
+      <c r="G21" t="n">
+        <v>27.44285364281796</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1128,7 +1122,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Vertr</t>
+          <t>Bekendgebruik_4</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1138,20 +1132,26 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Negative_Outcomes</t>
+          <t>Interventions</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>1.567771621546356</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0.1621536837308032</v>
-      </c>
-      <c r="G22" t="n">
-        <v>9.668430500409709</v>
-      </c>
-      <c r="H22" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -1160,7 +1160,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Cijfer_huidig_1</t>
+          <t>Bekendgebruik_5</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1170,26 +1170,20 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Positive_Outcomes</t>
+          <t>Interventions</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>1.123949235679905</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.08155909850398647</v>
+      </c>
+      <c r="G23" t="n">
+        <v>13.78079523048171</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1198,7 +1192,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Stopint2</t>
+          <t>Bekendgebruik_6</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1208,20 +1202,20 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Positive_Outcomes</t>
+          <t>Interventions</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>2.053800532997672</v>
+        <v>1.256380751396518</v>
       </c>
       <c r="F24" t="n">
-        <v>0.3276011088173964</v>
+        <v>0.1002520074604448</v>
       </c>
       <c r="G24" t="n">
-        <v>6.269211176987143</v>
+        <v>12.53222537094532</v>
       </c>
       <c r="H24" t="n">
-        <v>3.628817246692506e-10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1230,7 +1224,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Onnodige_stress_1</t>
+          <t>Bekendgebruik_7</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1240,26 +1234,20 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Interventions</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>1.220124379180625</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.08850153647619852</v>
+      </c>
+      <c r="G25" t="n">
+        <v>13.7864767974393</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1268,7 +1256,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Onnodige_stress_2</t>
+          <t>StopInt</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1278,20 +1266,26 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Negative_Outcomes</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>1.186263139436734</v>
-      </c>
-      <c r="F26" t="n">
-        <v>0.06343012110820431</v>
-      </c>
-      <c r="G26" t="n">
-        <v>18.70188987018339</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -1300,7 +1294,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Onnodige_stress_3</t>
+          <t>Vertr</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1310,17 +1304,17 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Negative_Outcomes</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>1.098958121858965</v>
+        <v>1.566811553098113</v>
       </c>
       <c r="F27" t="n">
-        <v>0.0617416679848754</v>
+        <v>0.162183044944133</v>
       </c>
       <c r="G27" t="n">
-        <v>17.79929434543901</v>
+        <v>9.660760492122778</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
@@ -1332,7 +1326,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Onnodige_stress_4</t>
+          <t>Cijfer_huidig_1</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1342,20 +1336,26 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Positive_Outcomes</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>1.387130870343167</v>
-      </c>
-      <c r="F28" t="n">
-        <v>0.06916525507485427</v>
-      </c>
-      <c r="G28" t="n">
-        <v>20.05531344924392</v>
-      </c>
-      <c r="H28" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Onnodige_stress_5</t>
+          <t>Stopint2</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1374,20 +1374,20 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Positive_Outcomes</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>1.368393003181974</v>
+        <v>2.05137106211305</v>
       </c>
       <c r="F29" t="n">
-        <v>0.06797587516620979</v>
+        <v>0.3272179265340076</v>
       </c>
       <c r="G29" t="n">
-        <v>20.13056837908958</v>
+        <v>6.269127990130404</v>
       </c>
       <c r="H29" t="n">
-        <v>0</v>
+        <v>3.630755696093502e-10</v>
       </c>
     </row>
     <row r="30">
@@ -1396,7 +1396,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Onnodige_stress_6</t>
+          <t>Onnodige_stress_1</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1410,16 +1410,22 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>1.240447948378192</v>
-      </c>
-      <c r="F30" t="n">
-        <v>0.06461984208187529</v>
-      </c>
-      <c r="G30" t="n">
-        <v>19.19608449038471</v>
-      </c>
-      <c r="H30" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -1428,7 +1434,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Onnodige_stress_7</t>
+          <t>Onnodige_stress_2</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1442,13 +1448,13 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>0.9327799432160967</v>
+        <v>1.15679760286918</v>
       </c>
       <c r="F31" t="n">
-        <v>0.06544301353520708</v>
+        <v>0.06176121428058527</v>
       </c>
       <c r="G31" t="n">
-        <v>14.25331586694164</v>
+        <v>18.7301628752803</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -1460,7 +1466,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Onnodige_stress_8</t>
+          <t>Onnodige_stress_3</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1474,13 +1480,13 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>1.038127335403254</v>
+        <v>1.087715978140208</v>
       </c>
       <c r="F32" t="n">
-        <v>0.06170210309318733</v>
+        <v>0.06051066811429799</v>
       </c>
       <c r="G32" t="n">
-        <v>16.82482903084467</v>
+        <v>17.97560681477945</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -1492,7 +1498,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Onnodige_stress_9</t>
+          <t>Onnodige_stress_4</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1506,13 +1512,13 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>1.202113978193233</v>
+        <v>1.401729893948441</v>
       </c>
       <c r="F33" t="n">
-        <v>0.06532406453892665</v>
+        <v>0.06841753818756773</v>
       </c>
       <c r="G33" t="n">
-        <v>18.40231447108577</v>
+        <v>20.48787388527616</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -1524,7 +1530,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Burn1_1</t>
+          <t>Onnodige_stress_5</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1534,26 +1540,20 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>1.373019924155111</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.06701383024964125</v>
+      </c>
+      <c r="G34" t="n">
+        <v>20.48860539712208</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1562,7 +1562,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Burn1_2</t>
+          <t>Onnodige_stress_6</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1572,17 +1572,17 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>1.069345207552132</v>
+        <v>1.165588661317256</v>
       </c>
       <c r="F35" t="n">
-        <v>0.04991257262746914</v>
+        <v>0.06194955456184417</v>
       </c>
       <c r="G35" t="n">
-        <v>21.42436567058855</v>
+        <v>18.81512578326669</v>
       </c>
       <c r="H35" t="n">
         <v>0</v>
@@ -1594,7 +1594,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Burn1_3</t>
+          <t>Onnodige_stress_7</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1604,17 +1604,17 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>0.9191037245884878</v>
+        <v>0.8961662258467628</v>
       </c>
       <c r="F36" t="n">
-        <v>0.04982414698323703</v>
+        <v>0.06393555290928846</v>
       </c>
       <c r="G36" t="n">
-        <v>18.44695354000273</v>
+        <v>14.01671190838411</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Burn1_4</t>
+          <t>Burn1_1</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1640,16 +1640,22 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>0.9604633822967859</v>
-      </c>
-      <c r="F37" t="n">
-        <v>0.04884805917972399</v>
-      </c>
-      <c r="G37" t="n">
-        <v>19.66226291086291</v>
-      </c>
-      <c r="H37" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="38">
@@ -1658,7 +1664,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Depr_1</t>
+          <t>Burn1_2</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1672,13 +1678,13 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>1.261896608911247</v>
+        <v>1.068551792631324</v>
       </c>
       <c r="F38" t="n">
-        <v>0.05135797817448639</v>
+        <v>0.05003518666571394</v>
       </c>
       <c r="G38" t="n">
-        <v>24.57060526408264</v>
+        <v>21.35600691867072</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
@@ -1690,7 +1696,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Depr_2</t>
+          <t>Burn1_3</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1704,13 +1710,13 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>1.37505840110441</v>
+        <v>0.9182068875946553</v>
       </c>
       <c r="F39" t="n">
-        <v>0.05584196940703116</v>
+        <v>0.04993430079524552</v>
       </c>
       <c r="G39" t="n">
-        <v>24.62410290469895</v>
+        <v>18.38829968484697</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
@@ -1722,7 +1728,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Depr_3</t>
+          <t>Burn1_4</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1736,13 +1742,13 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>0.9301966499697882</v>
+        <v>0.9609920543902299</v>
       </c>
       <c r="F40" t="n">
-        <v>0.05565054295854031</v>
+        <v>0.04896786737777525</v>
       </c>
       <c r="G40" t="n">
-        <v>16.71496090606107</v>
+        <v>19.62495215396627</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -1754,7 +1760,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Depr_4</t>
+          <t>Depr_1</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1768,13 +1774,13 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>-0.9577429898122831</v>
+        <v>1.265034784381275</v>
       </c>
       <c r="F41" t="n">
-        <v>0.04524782708433089</v>
+        <v>0.05152901239782343</v>
       </c>
       <c r="G41" t="n">
-        <v>-21.16660736008643</v>
+        <v>24.54995206564757</v>
       </c>
       <c r="H41" t="n">
         <v>0</v>
@@ -1786,7 +1792,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Depr_5</t>
+          <t>Depr_2</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1800,13 +1806,13 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>0.9460796442808924</v>
+        <v>1.376928305929334</v>
       </c>
       <c r="F42" t="n">
-        <v>0.04948739562456238</v>
+        <v>0.05601807590154022</v>
       </c>
       <c r="G42" t="n">
-        <v>19.11758807109666</v>
+        <v>24.58007140989459</v>
       </c>
       <c r="H42" t="n">
         <v>0</v>
@@ -1818,7 +1824,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Depr_6</t>
+          <t>Depr_3</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1832,13 +1838,13 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>-0.9699714295729585</v>
+        <v>0.9311663453595262</v>
       </c>
       <c r="F43" t="n">
-        <v>0.04640849373196924</v>
+        <v>0.05577829981285603</v>
       </c>
       <c r="G43" t="n">
-        <v>-20.90073069714558</v>
+        <v>16.69406110381681</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
@@ -1850,7 +1856,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Depr_7</t>
+          <t>Depr_4</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1864,13 +1870,13 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>0.9736982458141215</v>
+        <v>-0.9614359760669733</v>
       </c>
       <c r="F44" t="n">
-        <v>0.04545300941122162</v>
+        <v>0.04538715776386744</v>
       </c>
       <c r="G44" t="n">
-        <v>21.42208532296453</v>
+        <v>-21.18299588283949</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
@@ -1882,7 +1888,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Depr_8</t>
+          <t>Depr_5</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1896,13 +1902,13 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>1.108521046212654</v>
+        <v>0.9488829343049381</v>
       </c>
       <c r="F45" t="n">
-        <v>0.05249039947056976</v>
+        <v>0.0496188872813919</v>
       </c>
       <c r="G45" t="n">
-        <v>21.11854848452925</v>
+        <v>19.12342227476079</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
@@ -1914,7 +1920,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Mot_Stress_2</t>
+          <t>Depr_6</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1928,13 +1934,13 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>0.7434108515533393</v>
+        <v>-0.97309366980914</v>
       </c>
       <c r="F46" t="n">
-        <v>0.04024907595522928</v>
+        <v>0.0465444272310099</v>
       </c>
       <c r="G46" t="n">
-        <v>18.47025885418577</v>
+        <v>-20.90677074955853</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
@@ -1946,7 +1952,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Partici1_1</t>
+          <t>Depr_7</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1956,26 +1962,20 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Participation</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>0.9760086291275456</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.04558639770482466</v>
+      </c>
+      <c r="G47" t="n">
+        <v>21.41008454815545</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1984,7 +1984,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Partici1_2</t>
+          <t>Depr_8</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1994,17 +1994,17 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Participation</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>1.193654499633509</v>
+        <v>1.109433385814482</v>
       </c>
       <c r="F48" t="n">
-        <v>0.06010062546226148</v>
+        <v>0.05262915055738412</v>
       </c>
       <c r="G48" t="n">
-        <v>19.86093306737997</v>
+        <v>21.08020695838008</v>
       </c>
       <c r="H48" t="n">
         <v>0</v>
@@ -2016,7 +2016,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Partici1_3</t>
+          <t>Mot_Stress_2</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2026,17 +2026,17 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Participation</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>1.066261809301718</v>
+        <v>0.7418807573426818</v>
       </c>
       <c r="F49" t="n">
-        <v>0.05485699083048486</v>
+        <v>0.04033706894254549</v>
       </c>
       <c r="G49" t="n">
-        <v>19.4371180981685</v>
+        <v>18.39203434391812</v>
       </c>
       <c r="H49" t="n">
         <v>0</v>
@@ -2048,7 +2048,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Partici1_4</t>
+          <t>Partici1_1</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2062,16 +2062,22 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0.8731324878915472</v>
-      </c>
-      <c r="F50" t="n">
-        <v>0.05157652977533776</v>
-      </c>
-      <c r="G50" t="n">
-        <v>16.9288723316186</v>
-      </c>
-      <c r="H50" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="51">
@@ -2080,7 +2086,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_1</t>
+          <t>Partici1_2</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2090,26 +2096,20 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Behavior</t>
+          <t>Participation</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>1.192456436487136</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0.05988644846329608</v>
+      </c>
+      <c r="G51" t="n">
+        <v>19.91195783129585</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -2118,7 +2118,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_2</t>
+          <t>Partici1_3</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2128,17 +2128,17 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Behavior</t>
+          <t>Participation</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>1.175584106510044</v>
+        <v>1.06413912386902</v>
       </c>
       <c r="F52" t="n">
-        <v>0.128437114248326</v>
+        <v>0.0546577058472339</v>
       </c>
       <c r="G52" t="n">
-        <v>9.152993769604358</v>
+        <v>19.46915091576982</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
@@ -2150,7 +2150,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_4</t>
+          <t>Partici1_4</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2160,17 +2160,17 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Behavior</t>
+          <t>Participation</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>1.054520891708222</v>
+        <v>0.8738021107985809</v>
       </c>
       <c r="F53" t="n">
-        <v>0.1151750111965659</v>
+        <v>0.05146613905084955</v>
       </c>
       <c r="G53" t="n">
-        <v>9.15581323364793</v>
+        <v>16.97819434090965</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -2182,7 +2182,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_1</t>
+          <t>Cogn_Eng1_1</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2196,16 +2196,22 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>1.68151117531203</v>
-      </c>
-      <c r="F54" t="n">
-        <v>0.1565149866049773</v>
-      </c>
-      <c r="G54" t="n">
-        <v>10.74345154911711</v>
-      </c>
-      <c r="H54" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="55">
@@ -2214,7 +2220,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_4</t>
+          <t>Cogn_Eng1_2</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2228,13 +2234,13 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>1.780644332624391</v>
+        <v>1.171616474678231</v>
       </c>
       <c r="F55" t="n">
-        <v>0.1724808618195509</v>
+        <v>0.1274908376443077</v>
       </c>
       <c r="G55" t="n">
-        <v>10.3237212165427</v>
+        <v>9.18980921544955</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -2246,7 +2252,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_5</t>
+          <t>Cogn_Eng1_4</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2260,13 +2266,13 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>2.150009530507127</v>
+        <v>1.053419257090001</v>
       </c>
       <c r="F56" t="n">
-        <v>0.1961699835385357</v>
+        <v>0.1144569148012657</v>
       </c>
       <c r="G56" t="n">
-        <v>10.95993123776666</v>
+        <v>9.203631418074428</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -2278,7 +2284,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_6</t>
+          <t>Cogn_Eng2_1</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2292,13 +2298,13 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>1.294874045266537</v>
+        <v>1.670728615287617</v>
       </c>
       <c r="F57" t="n">
-        <v>0.1319851185959613</v>
+        <v>0.1549076009968827</v>
       </c>
       <c r="G57" t="n">
-        <v>9.81075790234088</v>
+        <v>10.78532366730314</v>
       </c>
       <c r="H57" t="n">
         <v>0</v>
@@ -2310,7 +2316,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_7</t>
+          <t>Cogn_Eng2_4</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2324,13 +2330,13 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>2.216888341717609</v>
+        <v>1.762720243536617</v>
       </c>
       <c r="F58" t="n">
-        <v>0.1990782264887325</v>
+        <v>0.1703716393529171</v>
       </c>
       <c r="G58" t="n">
-        <v>11.13576497443805</v>
+        <v>10.34632436608112</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -2342,27 +2348,27 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Cogn_Eng2_5</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>~~</t>
+          <t>~</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Behavior</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>-0.1242130239619878</v>
+        <v>2.137147993868972</v>
       </c>
       <c r="F59" t="n">
-        <v>0.01059797337742206</v>
+        <v>0.1941815656176792</v>
       </c>
       <c r="G59" t="n">
-        <v>-11.72045064907324</v>
+        <v>11.00592626833466</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -2374,27 +2380,27 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Cogn_Eng2_6</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>~~</t>
+          <t>~</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Behavior</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>0.308513463810027</v>
+        <v>1.293885388754712</v>
       </c>
       <c r="F60" t="n">
-        <v>0.02299129205513257</v>
+        <v>0.1311670482526958</v>
       </c>
       <c r="G60" t="n">
-        <v>13.41870926857005</v>
+        <v>9.86440882813916</v>
       </c>
       <c r="H60" t="n">
         <v>0</v>
@@ -2406,30 +2412,30 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Cogn_Eng2_7</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>~~</t>
+          <t>~</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Participation</t>
+          <t>Behavior</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>0.09945677754046607</v>
+        <v>2.203379179676104</v>
       </c>
       <c r="F61" t="n">
-        <v>0.01490664329593976</v>
+        <v>0.1970104957479858</v>
       </c>
       <c r="G61" t="n">
-        <v>6.67197675286722</v>
+        <v>11.18407002276399</v>
       </c>
       <c r="H61" t="n">
-        <v>2.523803388498891e-11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -2438,7 +2444,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2448,17 +2454,17 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Wellbeing</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>0.4134523404958916</v>
+        <v>-0.1318399782036039</v>
       </c>
       <c r="F62" t="n">
-        <v>0.03858232249544154</v>
+        <v>0.0109748778776175</v>
       </c>
       <c r="G62" t="n">
-        <v>10.71610814859641</v>
+        <v>-12.01288794843627</v>
       </c>
       <c r="H62" t="n">
         <v>0</v>
@@ -2470,7 +2476,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Behavior</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2480,20 +2486,20 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Behavior</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>0.08104626907798274</v>
+        <v>0.3175937039066615</v>
       </c>
       <c r="F63" t="n">
-        <v>0.01343802458455764</v>
+        <v>0.02367677078860072</v>
       </c>
       <c r="G63" t="n">
-        <v>6.031114808726146</v>
+        <v>13.41372549191356</v>
       </c>
       <c r="H63" t="n">
-        <v>1.62832458627804e-09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -2502,7 +2508,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Behavior</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2512,20 +2518,20 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Participation</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>-0.02748957598042596</v>
+        <v>0.09779719199797181</v>
       </c>
       <c r="F64" t="n">
-        <v>0.006418237712339084</v>
+        <v>0.01515116592171223</v>
       </c>
       <c r="G64" t="n">
-        <v>-4.283041110068909</v>
+        <v>6.454763448360747</v>
       </c>
       <c r="H64" t="n">
-        <v>1.843560929581933e-05</v>
+        <v>1.083879652696851e-10</v>
       </c>
     </row>
     <row r="65">
@@ -2534,7 +2540,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Negative_Outcomes</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2544,20 +2550,20 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Negative_Outcomes</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>0.02781051128598262</v>
+        <v>0.4306448700094357</v>
       </c>
       <c r="F65" t="n">
-        <v>0.007310628666012839</v>
+        <v>0.03962538222070087</v>
       </c>
       <c r="G65" t="n">
-        <v>3.804120350342748</v>
+        <v>10.86790450625843</v>
       </c>
       <c r="H65" t="n">
-        <v>0.0001423089840042469</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -2566,7 +2572,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Participation</t>
+          <t>Behavior</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2576,20 +2582,20 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Participation</t>
+          <t>Behavior</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>0.3578102782547822</v>
+        <v>0.08189928305034826</v>
       </c>
       <c r="F66" t="n">
-        <v>0.03188432216572128</v>
+        <v>0.01350683155309406</v>
       </c>
       <c r="G66" t="n">
-        <v>11.22213846616569</v>
+        <v>6.063545156563661</v>
       </c>
       <c r="H66" t="n">
-        <v>0</v>
+        <v>1.331533772130911e-09</v>
       </c>
     </row>
     <row r="67">
@@ -2598,7 +2604,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Positive_Outcomes</t>
+          <t>Behavior</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2608,20 +2614,20 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Positive_Outcomes</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>0</v>
+        <v>-0.02754746787894086</v>
       </c>
       <c r="F67" t="n">
-        <v>0.004730973868449785</v>
+        <v>0.006608368768989561</v>
       </c>
       <c r="G67" t="n">
-        <v>0</v>
+        <v>-4.168573037879116</v>
       </c>
       <c r="H67" t="n">
-        <v>1</v>
+        <v>3.065125442192063e-05</v>
       </c>
     </row>
     <row r="68">
@@ -2630,7 +2636,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Interventions</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2640,20 +2646,20 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Interventions</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>0.239575395115194</v>
+        <v>0.2755614833870266</v>
       </c>
       <c r="F68" t="n">
-        <v>0.01799192483406218</v>
+        <v>0.03645911250017031</v>
       </c>
       <c r="G68" t="n">
-        <v>13.31571787407182</v>
+        <v>7.55809630248628</v>
       </c>
       <c r="H68" t="n">
-        <v>0</v>
+        <v>4.085620730620576e-14</v>
       </c>
     </row>
     <row r="69">
@@ -2662,7 +2668,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Bevl_1</t>
+          <t>Interventions</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2672,20 +2678,20 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Bevl_1</t>
+          <t>Behavior</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>0.4208894290188266</v>
+        <v>0.001377811005985378</v>
       </c>
       <c r="F69" t="n">
-        <v>0.01653719630935653</v>
+        <v>0.005178330792355976</v>
       </c>
       <c r="G69" t="n">
-        <v>25.45107532860584</v>
+        <v>0.2660724200456968</v>
       </c>
       <c r="H69" t="n">
-        <v>0</v>
+        <v>0.7901834352268187</v>
       </c>
     </row>
     <row r="70">
@@ -2694,7 +2700,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Bevl_2</t>
+          <t>Interventions</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2704,20 +2710,20 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Bevl_2</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>0.2433518688035599</v>
+        <v>0.006680671795616268</v>
       </c>
       <c r="F70" t="n">
-        <v>0.01071418506417035</v>
+        <v>0.0109840663079175</v>
       </c>
       <c r="G70" t="n">
-        <v>22.71305445289046</v>
+        <v>0.6082148093181585</v>
       </c>
       <c r="H70" t="n">
-        <v>0</v>
+        <v>0.5430450137781837</v>
       </c>
     </row>
     <row r="71">
@@ -2726,7 +2732,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Bevl_3</t>
+          <t>Negative_Outcomes</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2736,20 +2742,20 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Bevl_3</t>
+          <t>Negative_Outcomes</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>0.4253883273941809</v>
+        <v>0.02782218713595457</v>
       </c>
       <c r="F71" t="n">
-        <v>0.01694200175934998</v>
+        <v>0.007316276641060098</v>
       </c>
       <c r="G71" t="n">
-        <v>25.108504497369</v>
+        <v>3.802779541715152</v>
       </c>
       <c r="H71" t="n">
-        <v>0</v>
+        <v>0.0001430816735561447</v>
       </c>
     </row>
     <row r="72">
@@ -2758,7 +2764,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Burn1_1</t>
+          <t>Participation</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2768,17 +2774,17 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Burn1_1</t>
+          <t>Participation</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>0.5259987188958628</v>
+        <v>0.3445860761129239</v>
       </c>
       <c r="F72" t="n">
-        <v>0.02094993159685618</v>
+        <v>0.03102268292844378</v>
       </c>
       <c r="G72" t="n">
-        <v>25.10741939365991</v>
+        <v>11.1075523963105</v>
       </c>
       <c r="H72" t="n">
         <v>0</v>
@@ -2790,7 +2796,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Burn1_2</t>
+          <t>Positive_Outcomes</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2800,20 +2806,20 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Burn1_2</t>
+          <t>Positive_Outcomes</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>0.7097499919590958</v>
+        <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>0.02786295089238025</v>
+        <v>0.004736342253182931</v>
       </c>
       <c r="G73" t="n">
-        <v>25.47289390398775</v>
+        <v>0</v>
       </c>
       <c r="H73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -2822,7 +2828,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Burn1_3</t>
+          <t>Wellbeing</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2832,17 +2838,17 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Burn1_3</t>
+          <t>Wellbeing</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>0.869445235597983</v>
+        <v>0.2455245207041751</v>
       </c>
       <c r="F74" t="n">
-        <v>0.03308715247329973</v>
+        <v>0.01838211024347821</v>
       </c>
       <c r="G74" t="n">
-        <v>26.27742705490659</v>
+        <v>13.35671027095097</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -2854,7 +2860,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Burn1_4</t>
+          <t>Bekendgebruik_4</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2864,17 +2870,17 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Burn1_4</t>
+          <t>Bekendgebruik_4</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>0.7749733732147754</v>
+        <v>1.237204570514979</v>
       </c>
       <c r="F75" t="n">
-        <v>0.02980383373631819</v>
+        <v>0.04849337118965018</v>
       </c>
       <c r="G75" t="n">
-        <v>26.00247270351701</v>
+        <v>25.51285959581873</v>
       </c>
       <c r="H75" t="n">
         <v>0</v>
@@ -2886,7 +2892,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Cijfer_huidig_1</t>
+          <t>Bekendgebruik_5</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2896,17 +2902,17 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Cijfer_huidig_1</t>
+          <t>Bekendgebruik_5</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>0.2361266063074851</v>
+        <v>0.3559100163682629</v>
       </c>
       <c r="F76" t="n">
-        <v>0.00980418643907289</v>
+        <v>0.02059544659333671</v>
       </c>
       <c r="G76" t="n">
-        <v>24.08426316153669</v>
+        <v>17.28100503856665</v>
       </c>
       <c r="H76" t="n">
         <v>0</v>
@@ -2918,7 +2924,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_1</t>
+          <t>Bekendgebruik_6</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2928,17 +2934,17 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_1</t>
+          <t>Bekendgebruik_6</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>0.5985654482232138</v>
+        <v>1.074460413756551</v>
       </c>
       <c r="F77" t="n">
-        <v>0.0227479857501244</v>
+        <v>0.04518739569957283</v>
       </c>
       <c r="G77" t="n">
-        <v>26.31289885495148</v>
+        <v>23.77787870042996</v>
       </c>
       <c r="H77" t="n">
         <v>0</v>
@@ -2950,7 +2956,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_2</t>
+          <t>Bekendgebruik_7</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2960,17 +2966,17 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_2</t>
+          <t>Bekendgebruik_7</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>0.6707017520883463</v>
+        <v>0.2618294745230861</v>
       </c>
       <c r="F78" t="n">
-        <v>0.02576098255535592</v>
+        <v>0.02082877955884647</v>
       </c>
       <c r="G78" t="n">
-        <v>26.0355656319043</v>
+        <v>12.57056246482336</v>
       </c>
       <c r="H78" t="n">
         <v>0</v>
@@ -2982,7 +2988,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_4</t>
+          <t>Bevl_1</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2992,17 +2998,17 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_4</t>
+          <t>Bevl_1</t>
         </is>
       </c>
       <c r="E79" t="n">
-        <v>0.5389117162577276</v>
+        <v>0.4204571984461671</v>
       </c>
       <c r="F79" t="n">
-        <v>0.02070071178671597</v>
+        <v>0.01652468187574982</v>
       </c>
       <c r="G79" t="n">
-        <v>26.03348724354124</v>
+        <v>25.44419321244236</v>
       </c>
       <c r="H79" t="n">
         <v>0</v>
@@ -3014,7 +3020,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_5</t>
+          <t>Bevl_2</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3024,17 +3030,17 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_5</t>
+          <t>Bevl_2</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>0.4335287486552395</v>
+        <v>0.2433924122424365</v>
       </c>
       <c r="F80" t="n">
-        <v>0.01764175635740445</v>
+        <v>0.01071612248598125</v>
       </c>
       <c r="G80" t="n">
-        <v>24.57401291843079</v>
+        <v>22.71273145096352</v>
       </c>
       <c r="H80" t="n">
         <v>0</v>
@@ -3046,7 +3052,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_6</t>
+          <t>Bevl_3</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3056,17 +3062,17 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_6</t>
+          <t>Bevl_3</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>0.575340647206382</v>
+        <v>0.425150152123728</v>
       </c>
       <c r="F81" t="n">
-        <v>0.02204205208698793</v>
+        <v>0.01693514287443493</v>
       </c>
       <c r="G81" t="n">
-        <v>26.10195479575699</v>
+        <v>25.10460970131078</v>
       </c>
       <c r="H81" t="n">
         <v>0</v>
@@ -3078,7 +3084,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_1</t>
+          <t>Burn1_1</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3088,17 +3094,17 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_1</t>
+          <t>Burn1_1</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>0.501503491790547</v>
+        <v>0.5272961099190492</v>
       </c>
       <c r="F82" t="n">
-        <v>0.0213698978731892</v>
+        <v>0.02099622915663872</v>
       </c>
       <c r="G82" t="n">
-        <v>23.46775332025656</v>
+        <v>25.11384810863581</v>
       </c>
       <c r="H82" t="n">
         <v>0</v>
@@ -3110,7 +3116,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_2</t>
+          <t>Burn1_2</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3120,17 +3126,17 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_2</t>
+          <t>Burn1_2</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>0.8935618376827826</v>
+        <v>0.7115174579380774</v>
       </c>
       <c r="F83" t="n">
-        <v>0.03318508139038573</v>
+        <v>0.02792302095603875</v>
       </c>
       <c r="G83" t="n">
-        <v>26.92661280965656</v>
+        <v>25.4813925410431</v>
       </c>
       <c r="H83" t="n">
         <v>0</v>
@@ -3142,7 +3148,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_3</t>
+          <t>Burn1_3</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3152,17 +3158,17 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_3</t>
+          <t>Burn1_3</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>0.8229577080835823</v>
+        <v>0.8709176359110185</v>
       </c>
       <c r="F84" t="n">
-        <v>0.03041100760206704</v>
+        <v>0.03313723144332283</v>
       </c>
       <c r="G84" t="n">
-        <v>27.06117859773198</v>
+        <v>26.28214844605634</v>
       </c>
       <c r="H84" t="n">
         <v>0</v>
@@ -3174,7 +3180,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_4</t>
+          <t>Burn1_4</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3184,17 +3190,17 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_4</t>
+          <t>Burn1_4</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>0.7795809558575126</v>
+        <v>0.7754282241543875</v>
       </c>
       <c r="F85" t="n">
-        <v>0.03169043261470903</v>
+        <v>0.02982181550191983</v>
       </c>
       <c r="G85" t="n">
-        <v>24.59988367186481</v>
+        <v>26.00204618925585</v>
       </c>
       <c r="H85" t="n">
         <v>0</v>
@@ -3206,7 +3212,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_5</t>
+          <t>Cijfer_huidig_1</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3216,17 +3222,17 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_5</t>
+          <t>Cijfer_huidig_1</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>0.6671425956049469</v>
+        <v>0.2361717262883765</v>
       </c>
       <c r="F86" t="n">
-        <v>0.02960464228581058</v>
+        <v>0.009808217786270869</v>
       </c>
       <c r="G86" t="n">
-        <v>22.53506693786911</v>
+        <v>24.07896433487446</v>
       </c>
       <c r="H86" t="n">
         <v>0</v>
@@ -3238,7 +3244,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_6</t>
+          <t>Cogn_Eng1_1</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3248,17 +3254,17 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_6</t>
+          <t>Cogn_Eng1_1</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>0.5710867245372515</v>
+        <v>0.5979152457722768</v>
       </c>
       <c r="F87" t="n">
-        <v>0.02247410392376013</v>
+        <v>0.0227354805577168</v>
       </c>
       <c r="G87" t="n">
-        <v>25.4108785137402</v>
+        <v>26.29877315450171</v>
       </c>
       <c r="H87" t="n">
         <v>0</v>
@@ -3270,7 +3276,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_7</t>
+          <t>Cogn_Eng1_2</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3280,17 +3286,17 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_7</t>
+          <t>Cogn_Eng1_2</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>0.5798542682816514</v>
+        <v>0.6702546129917241</v>
       </c>
       <c r="F88" t="n">
-        <v>0.02706645155461012</v>
+        <v>0.02575055971051178</v>
       </c>
       <c r="G88" t="n">
-        <v>21.42335751290841</v>
+        <v>26.02873958860346</v>
       </c>
       <c r="H88" t="n">
         <v>0</v>
@@ -3302,7 +3308,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_8</t>
+          <t>Cogn_Eng1_4</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3312,17 +3318,17 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_8</t>
+          <t>Cogn_Eng1_4</t>
         </is>
       </c>
       <c r="E89" t="n">
-        <v>0.6708527318138986</v>
+        <v>0.5381182172269497</v>
       </c>
       <c r="F89" t="n">
-        <v>0.02504173150562117</v>
+        <v>0.02068210397262114</v>
       </c>
       <c r="G89" t="n">
-        <v>26.78939080696243</v>
+        <v>26.01854327360937</v>
       </c>
       <c r="H89" t="n">
         <v>0</v>
@@ -3334,7 +3340,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Depr_1</t>
+          <t>Cogn_Eng1_5</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3344,17 +3350,17 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Depr_1</t>
+          <t>Cogn_Eng1_5</t>
         </is>
       </c>
       <c r="E90" t="n">
-        <v>0.539311145863299</v>
+        <v>0.4339185286706527</v>
       </c>
       <c r="F90" t="n">
-        <v>0.02267850784535689</v>
+        <v>0.01765431487224644</v>
       </c>
       <c r="G90" t="n">
-        <v>23.78071562366634</v>
+        <v>24.57861048622273</v>
       </c>
       <c r="H90" t="n">
         <v>0</v>
@@ -3366,7 +3372,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Depr_2</t>
+          <t>Cogn_Eng1_6</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3376,17 +3382,17 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Depr_2</t>
+          <t>Cogn_Eng1_6</t>
         </is>
       </c>
       <c r="E91" t="n">
-        <v>0.6329835154741625</v>
+        <v>0.5755551922691445</v>
       </c>
       <c r="F91" t="n">
-        <v>0.02666628204789356</v>
+        <v>0.02204829579532264</v>
       </c>
       <c r="G91" t="n">
-        <v>23.73722419621773</v>
+        <v>26.10429384592797</v>
       </c>
       <c r="H91" t="n">
         <v>0</v>
@@ -3398,7 +3404,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Depr_3</t>
+          <t>Cogn_Eng2_1</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3408,17 +3414,17 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Depr_3</t>
+          <t>Cogn_Eng2_1</t>
         </is>
       </c>
       <c r="E92" t="n">
-        <v>1.18818572542012</v>
+        <v>0.5018784764259465</v>
       </c>
       <c r="F92" t="n">
-        <v>0.04469716474244075</v>
+        <v>0.02137508082902266</v>
       </c>
       <c r="G92" t="n">
-        <v>26.58302226193183</v>
+        <v>23.47960601491744</v>
       </c>
       <c r="H92" t="n">
         <v>0</v>
@@ -3430,7 +3436,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Depr_4</t>
+          <t>Cogn_Eng2_2</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3440,17 +3446,17 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Depr_4</t>
+          <t>Cogn_Eng2_2</t>
         </is>
       </c>
       <c r="E93" t="n">
-        <v>0.5956873177849643</v>
+        <v>0.8936722794788061</v>
       </c>
       <c r="F93" t="n">
-        <v>0.02330302645249285</v>
+        <v>0.03318842593172655</v>
       </c>
       <c r="G93" t="n">
-        <v>25.56265895220996</v>
+        <v>26.92722701854838</v>
       </c>
       <c r="H93" t="n">
         <v>0</v>
@@ -3462,7 +3468,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Depr_5</t>
+          <t>Cogn_Eng2_3</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3472,17 +3478,17 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Depr_5</t>
+          <t>Cogn_Eng2_3</t>
         </is>
       </c>
       <c r="E94" t="n">
-        <v>0.8238349885201204</v>
+        <v>0.8229896717314351</v>
       </c>
       <c r="F94" t="n">
-        <v>0.03152460054834962</v>
+        <v>0.03041184011150728</v>
       </c>
       <c r="G94" t="n">
-        <v>26.13308255025984</v>
+        <v>27.06148883746662</v>
       </c>
       <c r="H94" t="n">
         <v>0</v>
@@ -3494,7 +3500,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Depr_6</t>
+          <t>Cogn_Eng2_4</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3504,17 +3510,17 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Depr_6</t>
+          <t>Cogn_Eng2_4</t>
         </is>
       </c>
       <c r="E95" t="n">
-        <v>0.6399233133818231</v>
+        <v>0.7814914604204354</v>
       </c>
       <c r="F95" t="n">
-        <v>0.02494798372669663</v>
+        <v>0.03172326659383327</v>
       </c>
       <c r="G95" t="n">
-        <v>25.65030185871879</v>
+        <v>24.63464656403688</v>
       </c>
       <c r="H95" t="n">
         <v>0</v>
@@ -3526,7 +3532,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Depr_7</t>
+          <t>Cogn_Eng2_5</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3536,17 +3542,17 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Depr_7</t>
+          <t>Cogn_Eng2_5</t>
         </is>
       </c>
       <c r="E96" t="n">
-        <v>0.5886985609519824</v>
+        <v>0.6677195095991738</v>
       </c>
       <c r="F96" t="n">
-        <v>0.02311004419986894</v>
+        <v>0.02961589954841889</v>
       </c>
       <c r="G96" t="n">
-        <v>25.47370986550719</v>
+        <v>22.54598103579385</v>
       </c>
       <c r="H96" t="n">
         <v>0</v>
@@ -3558,7 +3564,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Depr_8</t>
+          <t>Cogn_Eng2_6</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3568,17 +3574,17 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Depr_8</t>
+          <t>Cogn_Eng2_6</t>
         </is>
       </c>
       <c r="E97" t="n">
-        <v>0.8047344118676152</v>
+        <v>0.5698941437347723</v>
       </c>
       <c r="F97" t="n">
-        <v>0.03146091567527443</v>
+        <v>0.02244823245553536</v>
       </c>
       <c r="G97" t="n">
-        <v>25.57886172634474</v>
+        <v>25.38703859371605</v>
       </c>
       <c r="H97" t="n">
         <v>0</v>
@@ -3590,7 +3596,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Mot_Stress_1</t>
+          <t>Cogn_Eng2_7</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3600,17 +3606,17 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Mot_Stress_1</t>
+          <t>Cogn_Eng2_7</t>
         </is>
       </c>
       <c r="E98" t="n">
-        <v>0.316480088993965</v>
+        <v>0.5805729566394868</v>
       </c>
       <c r="F98" t="n">
-        <v>0.01330757400282351</v>
+        <v>0.02707855007984639</v>
       </c>
       <c r="G98" t="n">
-        <v>23.78195221030028</v>
+        <v>21.44032656497906</v>
       </c>
       <c r="H98" t="n">
         <v>0</v>
@@ -3622,7 +3628,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Mot_Stress_2</t>
+          <t>Cogn_Eng2_8</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3632,17 +3638,17 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Mot_Stress_2</t>
+          <t>Cogn_Eng2_8</t>
         </is>
       </c>
       <c r="E99" t="n">
-        <v>0.5666148783269894</v>
+        <v>0.6712387818801341</v>
       </c>
       <c r="F99" t="n">
-        <v>0.02156668890002201</v>
+        <v>0.02505447793309664</v>
       </c>
       <c r="G99" t="n">
-        <v>26.27268751950785</v>
+        <v>26.79117017108727</v>
       </c>
       <c r="H99" t="n">
         <v>0</v>
@@ -3654,7 +3660,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Mot_Stress_4</t>
+          <t>Depr_1</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3664,17 +3670,17 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Mot_Stress_4</t>
+          <t>Depr_1</t>
         </is>
       </c>
       <c r="E100" t="n">
-        <v>0.2035194657337798</v>
+        <v>0.5377144289783268</v>
       </c>
       <c r="F100" t="n">
-        <v>0.00968003601269677</v>
+        <v>0.02263885250846431</v>
       </c>
       <c r="G100" t="n">
-        <v>21.02465997500524</v>
+        <v>23.75184116569212</v>
       </c>
       <c r="H100" t="n">
         <v>0</v>
@@ -3686,7 +3692,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Onnodige_stress_1</t>
+          <t>Depr_2</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3696,17 +3702,17 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Onnodige_stress_1</t>
+          <t>Depr_2</t>
         </is>
       </c>
       <c r="E101" t="n">
-        <v>0.9977536130348553</v>
+        <v>0.6328672361584818</v>
       </c>
       <c r="F101" t="n">
-        <v>0.03857413294740872</v>
+        <v>0.02667279422783044</v>
       </c>
       <c r="G101" t="n">
-        <v>25.86587271758794</v>
+        <v>23.72706926499737</v>
       </c>
       <c r="H101" t="n">
         <v>0</v>
@@ -3718,7 +3724,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Onnodige_stress_2</t>
+          <t>Depr_3</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3728,17 +3734,17 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Onnodige_stress_2</t>
+          <t>Depr_3</t>
         </is>
       </c>
       <c r="E102" t="n">
-        <v>0.7478648525179342</v>
+        <v>1.18843279881116</v>
       </c>
       <c r="F102" t="n">
-        <v>0.03062066579356252</v>
+        <v>0.04470898655756116</v>
       </c>
       <c r="G102" t="n">
-        <v>24.42353335931502</v>
+        <v>26.58151951743562</v>
       </c>
       <c r="H102" t="n">
         <v>0</v>
@@ -3750,7 +3756,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Onnodige_stress_3</t>
+          <t>Depr_4</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3760,17 +3766,17 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Onnodige_stress_3</t>
+          <t>Depr_4</t>
         </is>
       </c>
       <c r="E103" t="n">
-        <v>0.8396974583269216</v>
+        <v>0.5938508323709645</v>
       </c>
       <c r="F103" t="n">
-        <v>0.03338477612997924</v>
+        <v>0.02324990567833644</v>
       </c>
       <c r="G103" t="n">
-        <v>25.15210690742744</v>
+        <v>25.54207490393196</v>
       </c>
       <c r="H103" t="n">
         <v>0</v>
@@ -3782,7 +3788,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Onnodige_stress_4</t>
+          <t>Depr_5</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3792,17 +3798,17 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Onnodige_stress_4</t>
+          <t>Depr_5</t>
         </is>
       </c>
       <c r="E104" t="n">
-        <v>0.6228727864026194</v>
+        <v>0.8225564479041247</v>
       </c>
       <c r="F104" t="n">
-        <v>0.02776596918467102</v>
+        <v>0.03148763398921845</v>
       </c>
       <c r="G104" t="n">
-        <v>22.43295676939888</v>
+        <v>26.12315832176053</v>
       </c>
       <c r="H104" t="n">
         <v>0</v>
@@ -3814,7 +3820,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Onnodige_stress_5</t>
+          <t>Depr_6</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3824,17 +3830,17 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Onnodige_stress_5</t>
+          <t>Depr_6</t>
         </is>
       </c>
       <c r="E105" t="n">
-        <v>0.5864636925449173</v>
+        <v>0.6384454242521397</v>
       </c>
       <c r="F105" t="n">
-        <v>0.02634321121283908</v>
+        <v>0.02490573275891</v>
       </c>
       <c r="G105" t="n">
-        <v>22.26242229105409</v>
+        <v>25.63447662458764</v>
       </c>
       <c r="H105" t="n">
         <v>0</v>
@@ -3846,7 +3852,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Onnodige_stress_6</t>
+          <t>Depr_7</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3856,17 +3862,17 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Onnodige_stress_6</t>
+          <t>Depr_7</t>
         </is>
       </c>
       <c r="E106" t="n">
-        <v>0.6939536300359488</v>
+        <v>0.5879565150437984</v>
       </c>
       <c r="F106" t="n">
-        <v>0.02907158952067893</v>
+        <v>0.02309156685348047</v>
       </c>
       <c r="G106" t="n">
-        <v>23.87050868059559</v>
+        <v>25.46195841750413</v>
       </c>
       <c r="H106" t="n">
         <v>0</v>
@@ -3878,7 +3884,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Onnodige_stress_7</t>
+          <t>Depr_8</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3888,17 +3894,17 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Onnodige_stress_7</t>
+          <t>Depr_8</t>
         </is>
       </c>
       <c r="E107" t="n">
-        <v>1.447381353537493</v>
+        <v>0.8051338445835351</v>
       </c>
       <c r="F107" t="n">
-        <v>0.0545771519599996</v>
+        <v>0.03147871728143838</v>
       </c>
       <c r="G107" t="n">
-        <v>26.51991358163541</v>
+        <v>25.57708553876527</v>
       </c>
       <c r="H107" t="n">
         <v>0</v>
@@ -3910,7 +3916,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Onnodige_stress_8</t>
+          <t>Mot_Stress_1</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3920,17 +3926,17 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Onnodige_stress_8</t>
+          <t>Mot_Stress_1</t>
         </is>
       </c>
       <c r="E108" t="n">
-        <v>0.9720225769293808</v>
+        <v>0.3161762287455623</v>
       </c>
       <c r="F108" t="n">
-        <v>0.03783391082378913</v>
+        <v>0.01329898338204736</v>
       </c>
       <c r="G108" t="n">
-        <v>25.69183454047004</v>
+        <v>23.77446603539652</v>
       </c>
       <c r="H108" t="n">
         <v>0</v>
@@ -3942,7 +3948,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Onnodige_stress_9</t>
+          <t>Mot_Stress_2</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3952,17 +3958,17 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Onnodige_stress_9</t>
+          <t>Mot_Stress_2</t>
         </is>
       </c>
       <c r="E109" t="n">
-        <v>0.8428300667304646</v>
+        <v>0.5681902447569463</v>
       </c>
       <c r="F109" t="n">
-        <v>0.03412488234578931</v>
+        <v>0.02161948899056125</v>
       </c>
       <c r="G109" t="n">
-        <v>24.6984021267919</v>
+        <v>26.28139106242189</v>
       </c>
       <c r="H109" t="n">
         <v>0</v>
@@ -3974,7 +3980,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Partici1_1</t>
+          <t>Mot_Stress_4</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3984,17 +3990,17 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Partici1_1</t>
+          <t>Mot_Stress_4</t>
         </is>
       </c>
       <c r="E110" t="n">
-        <v>0.72418667081259</v>
+        <v>0.2033504204272714</v>
       </c>
       <c r="F110" t="n">
-        <v>0.03406277043198094</v>
+        <v>0.009676672532630366</v>
       </c>
       <c r="G110" t="n">
-        <v>21.26035732288538</v>
+        <v>21.01449849837804</v>
       </c>
       <c r="H110" t="n">
         <v>0</v>
@@ -4006,7 +4012,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Partici1_2</t>
+          <t>Onnodige_stress_1</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -4016,17 +4022,17 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Partici1_2</t>
+          <t>Onnodige_stress_1</t>
         </is>
       </c>
       <c r="E111" t="n">
-        <v>0.867218941111824</v>
+        <v>0.9800434942016013</v>
       </c>
       <c r="F111" t="n">
-        <v>0.0432181612341215</v>
+        <v>0.03845525904293287</v>
       </c>
       <c r="G111" t="n">
-        <v>20.06607676790917</v>
+        <v>25.48529170176592</v>
       </c>
       <c r="H111" t="n">
         <v>0</v>
@@ -4038,7 +4044,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Partici1_3</t>
+          <t>Onnodige_stress_2</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -4048,17 +4054,17 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Partici1_3</t>
+          <t>Onnodige_stress_2</t>
         </is>
       </c>
       <c r="E112" t="n">
-        <v>0.7923880924972636</v>
+        <v>0.7533026009153689</v>
       </c>
       <c r="F112" t="n">
-        <v>0.03771024173495044</v>
+        <v>0.03142416818561204</v>
       </c>
       <c r="G112" t="n">
-        <v>21.01254343702213</v>
+        <v>23.97207768370799</v>
       </c>
       <c r="H112" t="n">
         <v>0</v>
@@ -4070,7 +4076,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Partici1_4</t>
+          <t>Onnodige_stress_3</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -4080,17 +4086,17 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Partici1_4</t>
+          <t>Onnodige_stress_3</t>
         </is>
       </c>
       <c r="E113" t="n">
-        <v>0.9696494944529384</v>
+        <v>0.8294833043162358</v>
       </c>
       <c r="F113" t="n">
-        <v>0.04042109679612595</v>
+        <v>0.03361604875914392</v>
       </c>
       <c r="G113" t="n">
-        <v>23.98869826119818</v>
+        <v>24.67521719267891</v>
       </c>
       <c r="H113" t="n">
         <v>0</v>
@@ -4102,7 +4108,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>StopInt</t>
+          <t>Onnodige_stress_4</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -4112,17 +4118,17 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>StopInt</t>
+          <t>Onnodige_stress_4</t>
         </is>
       </c>
       <c r="E114" t="n">
-        <v>0.1144998219306582</v>
+        <v>0.5721058775648915</v>
       </c>
       <c r="F114" t="n">
-        <v>0.008378832876477491</v>
+        <v>0.02774347526839094</v>
       </c>
       <c r="G114" t="n">
-        <v>13.66536647824026</v>
+        <v>20.62127660683121</v>
       </c>
       <c r="H114" t="n">
         <v>0</v>
@@ -4134,7 +4140,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Stopint2</t>
+          <t>Onnodige_stress_5</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -4144,17 +4150,17 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Stopint2</t>
+          <t>Onnodige_stress_5</t>
         </is>
       </c>
       <c r="E115" t="n">
-        <v>0.596832230540301</v>
+        <v>0.548713417108797</v>
       </c>
       <c r="F115" t="n">
-        <v>0.02948234745855595</v>
+        <v>0.02661225383317656</v>
       </c>
       <c r="G115" t="n">
-        <v>20.24371469602408</v>
+        <v>20.61882546769174</v>
       </c>
       <c r="H115" t="n">
         <v>0</v>
@@ -4166,29 +4172,285 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
+          <t>Onnodige_stress_6</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>~~</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Onnodige_stress_6</t>
+        </is>
+      </c>
+      <c r="E116" t="n">
+        <v>0.7449814165031058</v>
+      </c>
+      <c r="F116" t="n">
+        <v>0.03120095793242363</v>
+      </c>
+      <c r="G116" t="n">
+        <v>23.87687641170318</v>
+      </c>
+      <c r="H116" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Onnodige_stress_7</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>~~</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Onnodige_stress_7</t>
+        </is>
+      </c>
+      <c r="E117" t="n">
+        <v>1.461391374689254</v>
+      </c>
+      <c r="F117" t="n">
+        <v>0.05531947254858133</v>
+      </c>
+      <c r="G117" t="n">
+        <v>26.41730492602671</v>
+      </c>
+      <c r="H117" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Partici1_1</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>~~</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Partici1_1</t>
+        </is>
+      </c>
+      <c r="E118" t="n">
+        <v>0.7239515254346804</v>
+      </c>
+      <c r="F118" t="n">
+        <v>0.03398144147455329</v>
+      </c>
+      <c r="G118" t="n">
+        <v>21.30432065265686</v>
+      </c>
+      <c r="H118" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Partici1_2</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>~~</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Partici1_2</t>
+        </is>
+      </c>
+      <c r="E119" t="n">
+        <v>0.8681667499490331</v>
+      </c>
+      <c r="F119" t="n">
+        <v>0.04309848720495597</v>
+      </c>
+      <c r="G119" t="n">
+        <v>20.14378708469047</v>
+      </c>
+      <c r="H119" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Partici1_3</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>~~</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Partici1_3</t>
+        </is>
+      </c>
+      <c r="E120" t="n">
+        <v>0.79435104936144</v>
+      </c>
+      <c r="F120" t="n">
+        <v>0.03764238683608348</v>
+      </c>
+      <c r="G120" t="n">
+        <v>21.10256856982521</v>
+      </c>
+      <c r="H120" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Partici1_4</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>~~</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Partici1_4</t>
+        </is>
+      </c>
+      <c r="E121" t="n">
+        <v>0.9686471100017132</v>
+      </c>
+      <c r="F121" t="n">
+        <v>0.04035286947334166</v>
+      </c>
+      <c r="G121" t="n">
+        <v>24.00441709895319</v>
+      </c>
+      <c r="H121" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>StopInt</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>~~</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>StopInt</t>
+        </is>
+      </c>
+      <c r="E122" t="n">
+        <v>0.1145100545020604</v>
+      </c>
+      <c r="F122" t="n">
+        <v>0.008383970513512674</v>
+      </c>
+      <c r="G122" t="n">
+        <v>13.65821293190895</v>
+      </c>
+      <c r="H122" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Stopint2</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>~~</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Stopint2</t>
+        </is>
+      </c>
+      <c r="E123" t="n">
+        <v>0.5966656361882181</v>
+      </c>
+      <c r="F123" t="n">
+        <v>0.02946127502615425</v>
+      </c>
+      <c r="G123" t="n">
+        <v>20.25253949933516</v>
+      </c>
+      <c r="H123" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
           <t>Vertr</t>
         </is>
       </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr">
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>~~</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
         <is>
           <t>Vertr</t>
         </is>
       </c>
-      <c r="E116" t="n">
-        <v>1.040930196915984</v>
-      </c>
-      <c r="F116" t="n">
-        <v>0.04186420723283895</v>
-      </c>
-      <c r="G116" t="n">
-        <v>24.86444305756727</v>
-      </c>
-      <c r="H116" t="n">
+      <c r="E124" t="n">
+        <v>1.040919503277965</v>
+      </c>
+      <c r="F124" t="n">
+        <v>0.04186049646654874</v>
+      </c>
+      <c r="G124" t="n">
+        <v>24.86639173247528</v>
+      </c>
+      <c r="H124" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Model with Energy Sources back
</commit_message>
<xml_diff>
--- a/model_coefficients.xlsx
+++ b/model_coefficients.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H124"/>
+  <dimension ref="A1:H98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Participation</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -486,20 +486,20 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Interventions</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.22000606286011</v>
+        <v>0.4003229797458346</v>
       </c>
       <c r="F2" t="n">
-        <v>0.04601361385221889</v>
+        <v>0.03575645574775392</v>
       </c>
       <c r="G2" t="n">
-        <v>4.78132544776679</v>
+        <v>11.19582384111953</v>
       </c>
       <c r="H2" t="n">
-        <v>1.741431733259802e-06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -508,7 +508,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Participation</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -518,20 +518,20 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Behavior</t>
+          <t>Energy_Sources</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1.504491051061317</v>
+        <v>-0.2652338752111249</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1518252416844932</v>
+        <v>0.05608406810843652</v>
       </c>
       <c r="G3" t="n">
-        <v>9.909360488145165</v>
+        <v>-4.729219618904527</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>2.253844765043311e-06</v>
       </c>
     </row>
     <row r="4">
@@ -540,7 +540,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Wellbeing</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -554,16 +554,16 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.4229650206001207</v>
+        <v>-0.1910539616163615</v>
       </c>
       <c r="F4" t="n">
-        <v>0.03409781654837914</v>
+        <v>0.02674199160375509</v>
       </c>
       <c r="G4" t="n">
-        <v>12.40446056091595</v>
+        <v>-7.144343040717637</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>9.041656312547275e-13</v>
       </c>
     </row>
     <row r="5">
@@ -572,7 +572,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Wellbeing</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -582,20 +582,20 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Participation</t>
+          <t>Energy_Sources</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>-0.0881554897120936</v>
+        <v>0.675651908784292</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02512821280925571</v>
+        <v>0.06720875436759929</v>
       </c>
       <c r="G5" t="n">
-        <v>-3.508227599700773</v>
+        <v>10.05303423834863</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0004511029403850841</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -604,7 +604,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Negative_Outcomes</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -614,20 +614,20 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>-0.2558348428210345</v>
+        <v>0.09985673288449368</v>
       </c>
       <c r="F6" t="n">
-        <v>0.02684985439739583</v>
+        <v>0.01915109558626071</v>
       </c>
       <c r="G6" t="n">
-        <v>-9.528351216545875</v>
+        <v>5.214152497412121</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>1.846595141241636e-07</v>
       </c>
     </row>
     <row r="7">
@@ -636,27 +636,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>Negative_Outcomes</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>~</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>Wellbeing</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Participation</t>
-        </is>
-      </c>
       <c r="E7" t="n">
-        <v>0.2967352896833194</v>
+        <v>-0.2225058250189574</v>
       </c>
       <c r="F7" t="n">
-        <v>0.02573431528212479</v>
+        <v>0.02349159242224503</v>
       </c>
       <c r="G7" t="n">
-        <v>11.53072410976106</v>
+        <v>-9.471721670038297</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -668,7 +668,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Negative_Outcomes</t>
+          <t>Positive_Outcomes</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -678,20 +678,20 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Wellbeing</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0.08205195815105283</v>
+        <v>0.1426344029495041</v>
       </c>
       <c r="F8" t="n">
-        <v>0.01861487005221737</v>
+        <v>0.0307425077739059</v>
       </c>
       <c r="G8" t="n">
-        <v>4.407871659403343</v>
+        <v>4.639647617359698</v>
       </c>
       <c r="H8" t="n">
-        <v>1.043913690290665e-05</v>
+        <v>3.490037664422019e-06</v>
       </c>
     </row>
     <row r="9">
@@ -700,7 +700,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Negative_Outcomes</t>
+          <t>Positive_Outcomes</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -710,20 +710,20 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>-0.2813538621498325</v>
+        <v>-0.02433195844800822</v>
       </c>
       <c r="F9" t="n">
-        <v>0.02304703269200632</v>
+        <v>0.02659848361382834</v>
       </c>
       <c r="G9" t="n">
-        <v>-12.20781286239986</v>
+        <v>-0.9147874292519231</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>0.3603032353954521</v>
       </c>
     </row>
     <row r="10">
@@ -732,7 +732,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Positive_Outcomes</t>
+          <t>Bevl_1</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -746,16 +746,22 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0.186688753059603</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.02626709562129757</v>
-      </c>
-      <c r="G10" t="n">
-        <v>7.107323769024808</v>
-      </c>
-      <c r="H10" t="n">
-        <v>1.183053655040567e-12</v>
+        <v>1</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -764,7 +770,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Positive_Outcomes</t>
+          <t>Bevl_2</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -774,20 +780,20 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Wellbeing</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0.001193803198630036</v>
+        <v>1.145957816451314</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0158202612865855</v>
+        <v>0.04771744293913333</v>
       </c>
       <c r="G11" t="n">
-        <v>0.07546039707743891</v>
+        <v>24.0154908947875</v>
       </c>
       <c r="H11" t="n">
-        <v>0.9398484062141881</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -796,7 +802,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Bevl_1</t>
+          <t>Bevl_3</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -810,22 +816,16 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>1.106807498358706</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.05132774612077631</v>
+      </c>
+      <c r="G12" t="n">
+        <v>21.56353204624996</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -834,7 +834,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Bevl_2</t>
+          <t>Cogn_Eng1_5</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -848,13 +848,13 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>1.157228755222232</v>
+        <v>1.163423790317772</v>
       </c>
       <c r="F13" t="n">
-        <v>0.04383595579127213</v>
+        <v>0.05447694099769282</v>
       </c>
       <c r="G13" t="n">
-        <v>26.3990766097597</v>
+        <v>21.35626136470637</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -866,7 +866,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Bevl_3</t>
+          <t>Cogn_Eng1_6</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -880,13 +880,13 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>1.085003590900024</v>
+        <v>0.9090230797653056</v>
       </c>
       <c r="F14" t="n">
-        <v>0.04664425713781688</v>
+        <v>0.05214404823388956</v>
       </c>
       <c r="G14" t="n">
-        <v>23.26124709567076</v>
+        <v>17.43292112017261</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -898,7 +898,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_5</t>
+          <t>Cogn_Eng2_8</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -912,13 +912,13 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>1.209691211324009</v>
+        <v>0.6837507240529963</v>
       </c>
       <c r="F15" t="n">
-        <v>0.04985715088071573</v>
+        <v>0.04952497562223639</v>
       </c>
       <c r="G15" t="n">
-        <v>24.26314359988113</v>
+        <v>13.80617992131208</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -930,7 +930,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_6</t>
+          <t>Mot_Stress_1</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -944,13 +944,13 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.9645820987828628</v>
+        <v>1.163158542831544</v>
       </c>
       <c r="F16" t="n">
-        <v>0.04769888057479481</v>
+        <v>0.04990210556138797</v>
       </c>
       <c r="G16" t="n">
-        <v>20.22232151234903</v>
+        <v>23.30880690750322</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -962,7 +962,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_2</t>
+          <t>Mot_Stress_4</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -976,13 +976,13 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0.769213818840775</v>
+        <v>1.23377526117264</v>
       </c>
       <c r="F17" t="n">
-        <v>0.05169998405195595</v>
+        <v>0.04884461440004392</v>
       </c>
       <c r="G17" t="n">
-        <v>14.87841501175077</v>
+        <v>25.25918724718752</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -994,7 +994,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_3</t>
+          <t>StopInt</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1004,20 +1004,26 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Negative_Outcomes</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0.645232430084827</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.04829110357116322</v>
-      </c>
-      <c r="G18" t="n">
-        <v>13.36131051800528</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -1026,7 +1032,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_8</t>
+          <t>Vertr</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1036,17 +1042,17 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Negative_Outcomes</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>0.7420155188042223</v>
+        <v>2.154547755055875</v>
       </c>
       <c r="F19" t="n">
-        <v>0.04598415648044851</v>
+        <v>0.2020842941016271</v>
       </c>
       <c r="G19" t="n">
-        <v>16.13632989230922</v>
+        <v>10.66162892382771</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -1058,7 +1064,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Mot_Stress_1</t>
+          <t>Cijfer_huidig_1</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1068,20 +1074,26 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Positive_Outcomes</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>1.164872911068902</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0.04589416102893826</v>
-      </c>
-      <c r="G20" t="n">
-        <v>25.38172362076774</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -1090,7 +1102,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Mot_Stress_4</t>
+          <t>StPunt_beh</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1100,20 +1112,20 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Positive_Outcomes</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>1.23117918955364</v>
+        <v>1.245585553585299</v>
       </c>
       <c r="F21" t="n">
-        <v>0.04486338066553105</v>
+        <v>0.1807533874639266</v>
       </c>
       <c r="G21" t="n">
-        <v>27.44285364281796</v>
+        <v>6.891077235423828</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>5.537126313015506e-12</v>
       </c>
     </row>
     <row r="22">
@@ -1122,7 +1134,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Bekendgebruik_4</t>
+          <t>Onnodige_stress_1</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1132,7 +1144,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Interventions</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1160,7 +1172,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Bekendgebruik_5</t>
+          <t>Onnodige_stress_2</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1170,17 +1182,17 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Interventions</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>1.123949235679905</v>
+        <v>1.140321678766409</v>
       </c>
       <c r="F23" t="n">
-        <v>0.08155909850398647</v>
+        <v>0.06551549289654568</v>
       </c>
       <c r="G23" t="n">
-        <v>13.78079523048171</v>
+        <v>17.40537433717647</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -1192,7 +1204,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Bekendgebruik_6</t>
+          <t>Onnodige_stress_3</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1202,17 +1214,17 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Interventions</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>1.256380751396518</v>
+        <v>1.055251326480455</v>
       </c>
       <c r="F24" t="n">
-        <v>0.1002520074604448</v>
+        <v>0.0634661510640471</v>
       </c>
       <c r="G24" t="n">
-        <v>12.53222537094532</v>
+        <v>16.6269942130084</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -1224,7 +1236,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Bekendgebruik_7</t>
+          <t>Onnodige_stress_4</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1234,17 +1246,17 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Interventions</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>1.220124379180625</v>
+        <v>1.380995269259073</v>
       </c>
       <c r="F25" t="n">
-        <v>0.08850153647619852</v>
+        <v>0.07260718127243863</v>
       </c>
       <c r="G25" t="n">
-        <v>13.7864767974393</v>
+        <v>19.02009202172778</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -1256,7 +1268,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>StopInt</t>
+          <t>Onnodige_stress_5</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1266,26 +1278,20 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Negative_Outcomes</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>1.349527238403467</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.07085523133450973</v>
+      </c>
+      <c r="G26" t="n">
+        <v>19.04626112944662</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1294,7 +1300,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Vertr</t>
+          <t>Onnodige_stress_6</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1304,17 +1310,17 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Negative_Outcomes</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>1.566811553098113</v>
+        <v>1.130419389954186</v>
       </c>
       <c r="F27" t="n">
-        <v>0.162183044944133</v>
+        <v>0.06511175820675494</v>
       </c>
       <c r="G27" t="n">
-        <v>9.660760492122778</v>
+        <v>17.36121740634475</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
@@ -1326,7 +1332,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Cijfer_huidig_1</t>
+          <t>Onnodige_stress_7</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1336,26 +1342,20 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Positive_Outcomes</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>0.885344748386345</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.06838186160655282</v>
+      </c>
+      <c r="G28" t="n">
+        <v>12.94706999156276</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Stopint2</t>
+          <t>Burn1_1</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1374,20 +1374,26 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Positive_Outcomes</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>2.05137106211305</v>
-      </c>
-      <c r="F29" t="n">
-        <v>0.3272179265340076</v>
-      </c>
-      <c r="G29" t="n">
-        <v>6.269127990130404</v>
-      </c>
-      <c r="H29" t="n">
-        <v>3.630755696093502e-10</v>
+        <v>1</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -1396,7 +1402,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Onnodige_stress_1</t>
+          <t>Burn1_2</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1406,26 +1412,20 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>1.074621077802647</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.05512059701644244</v>
+      </c>
+      <c r="G30" t="n">
+        <v>19.49581709832701</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1434,7 +1434,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Onnodige_stress_2</t>
+          <t>Burn1_3</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1444,17 +1444,17 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>1.15679760286918</v>
+        <v>0.9223528875473581</v>
       </c>
       <c r="F31" t="n">
-        <v>0.06176121428058527</v>
+        <v>0.05477318099516192</v>
       </c>
       <c r="G31" t="n">
-        <v>18.7301628752803</v>
+        <v>16.83949828679823</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Onnodige_stress_3</t>
+          <t>Burn1_4</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1476,17 +1476,17 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>1.087715978140208</v>
+        <v>0.9267827084638389</v>
       </c>
       <c r="F32" t="n">
-        <v>0.06051066811429799</v>
+        <v>0.0534540716342362</v>
       </c>
       <c r="G32" t="n">
-        <v>17.97560681477945</v>
+        <v>17.3379254397698</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -1498,7 +1498,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Onnodige_stress_4</t>
+          <t>Depr_1</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1508,17 +1508,17 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>1.401729893948441</v>
+        <v>1.233028292696302</v>
       </c>
       <c r="F33" t="n">
-        <v>0.06841753818756773</v>
+        <v>0.05559774929913315</v>
       </c>
       <c r="G33" t="n">
-        <v>20.48787388527616</v>
+        <v>22.17766561088741</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -1530,7 +1530,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Onnodige_stress_5</t>
+          <t>Depr_2</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1540,17 +1540,17 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>1.373019924155111</v>
+        <v>1.360927501766553</v>
       </c>
       <c r="F34" t="n">
-        <v>0.06701383024964125</v>
+        <v>0.06113101071949898</v>
       </c>
       <c r="G34" t="n">
-        <v>20.48860539712208</v>
+        <v>22.26247342758549</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
@@ -1562,7 +1562,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Onnodige_stress_6</t>
+          <t>Depr_3</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1572,17 +1572,17 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>1.165588661317256</v>
+        <v>0.9079292701681343</v>
       </c>
       <c r="F35" t="n">
-        <v>0.06194955456184417</v>
+        <v>0.061302089911182</v>
       </c>
       <c r="G35" t="n">
-        <v>18.81512578326669</v>
+        <v>14.81073926629229</v>
       </c>
       <c r="H35" t="n">
         <v>0</v>
@@ -1594,7 +1594,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Onnodige_stress_7</t>
+          <t>Depr_4</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1604,17 +1604,17 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>0.8961662258467628</v>
+        <v>0.9489318949112598</v>
       </c>
       <c r="F36" t="n">
-        <v>0.06393555290928846</v>
+        <v>0.04940507366488211</v>
       </c>
       <c r="G36" t="n">
-        <v>14.01671190838411</v>
+        <v>19.20717498224414</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Burn1_1</t>
+          <t>Depr_5</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1640,22 +1640,16 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>0.9388208827189463</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.05406170649867979</v>
+      </c>
+      <c r="G37" t="n">
+        <v>17.36572785996881</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1664,7 +1658,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Burn1_2</t>
+          <t>Depr_6</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1678,13 +1672,13 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>1.068551792631324</v>
+        <v>0.9492381281131602</v>
       </c>
       <c r="F38" t="n">
-        <v>0.05003518666571394</v>
+        <v>0.05114525830492474</v>
       </c>
       <c r="G38" t="n">
-        <v>21.35600691867072</v>
+        <v>18.55965068032904</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
@@ -1696,7 +1690,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Burn1_3</t>
+          <t>Depr_7</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1710,13 +1704,13 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>0.9182068875946553</v>
+        <v>0.9385179543725224</v>
       </c>
       <c r="F39" t="n">
-        <v>0.04993430079524552</v>
+        <v>0.04866590968140395</v>
       </c>
       <c r="G39" t="n">
-        <v>18.38829968484697</v>
+        <v>19.28491546746655</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
@@ -1728,7 +1722,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Burn1_4</t>
+          <t>Depr_8</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1742,13 +1736,13 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>0.9609920543902299</v>
+        <v>1.106714044412322</v>
       </c>
       <c r="F40" t="n">
-        <v>0.04896786737777525</v>
+        <v>0.05768309997323096</v>
       </c>
       <c r="G40" t="n">
-        <v>19.62495215396627</v>
+        <v>19.18610554749536</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -1760,7 +1754,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Depr_1</t>
+          <t>Mot_Stress_2</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1774,13 +1768,13 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>1.265034784381275</v>
+        <v>0.7301212169335763</v>
       </c>
       <c r="F41" t="n">
-        <v>0.05152901239782343</v>
+        <v>0.04418591529332094</v>
       </c>
       <c r="G41" t="n">
-        <v>24.54995206564757</v>
+        <v>16.52384503229734</v>
       </c>
       <c r="H41" t="n">
         <v>0</v>
@@ -1792,7 +1786,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Depr_2</t>
+          <t>Cogn_Eng2_1</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1802,20 +1796,26 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Energy_Sources</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>1.376928305929334</v>
-      </c>
-      <c r="F42" t="n">
-        <v>0.05601807590154022</v>
-      </c>
-      <c r="G42" t="n">
-        <v>24.58007140989459</v>
-      </c>
-      <c r="H42" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="43">
@@ -1824,7 +1824,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Depr_3</t>
+          <t>Cogn_Eng2_4</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1834,17 +1834,17 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Energy_Sources</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0.9311663453595262</v>
+        <v>1.217760426522173</v>
       </c>
       <c r="F43" t="n">
-        <v>0.05577829981285603</v>
+        <v>0.1127678209366678</v>
       </c>
       <c r="G43" t="n">
-        <v>16.69406110381681</v>
+        <v>10.79882910210074</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Depr_4</t>
+          <t>Cogn_Eng2_5</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1866,17 +1866,17 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Energy_Sources</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>-0.9614359760669733</v>
+        <v>1.416396881139643</v>
       </c>
       <c r="F44" t="n">
-        <v>0.04538715776386744</v>
+        <v>0.1210508704493564</v>
       </c>
       <c r="G44" t="n">
-        <v>-21.18299588283949</v>
+        <v>11.70084011680457</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
@@ -1888,7 +1888,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Depr_5</t>
+          <t>Cogn_Eng2_7</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1898,17 +1898,17 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Energy_Sources</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>0.9488829343049381</v>
+        <v>1.504709002043763</v>
       </c>
       <c r="F45" t="n">
-        <v>0.0496188872813919</v>
+        <v>0.1228194985865323</v>
       </c>
       <c r="G45" t="n">
-        <v>19.12342227476079</v>
+        <v>12.25138532031517</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
@@ -1920,7 +1920,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Depr_6</t>
+          <t>Partici1_1</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1930,17 +1930,17 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Energy_Sources</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>-0.97309366980914</v>
+        <v>1.953352778306596</v>
       </c>
       <c r="F46" t="n">
-        <v>0.0465444272310099</v>
+        <v>0.1515189481812861</v>
       </c>
       <c r="G46" t="n">
-        <v>-20.90677074955853</v>
+        <v>12.89180529392666</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
@@ -1952,7 +1952,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Depr_7</t>
+          <t>Partici1_2</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1962,17 +1962,17 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Energy_Sources</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0.9760086291275456</v>
+        <v>2.121717968063729</v>
       </c>
       <c r="F47" t="n">
-        <v>0.04558639770482466</v>
+        <v>0.1669230871744594</v>
       </c>
       <c r="G47" t="n">
-        <v>21.41008454815545</v>
+        <v>12.71075202337654</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
@@ -1984,7 +1984,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Depr_8</t>
+          <t>Partici1_3</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1994,17 +1994,17 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Energy_Sources</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>1.109433385814482</v>
+        <v>1.764918813676792</v>
       </c>
       <c r="F48" t="n">
-        <v>0.05262915055738412</v>
+        <v>0.1458429052741661</v>
       </c>
       <c r="G48" t="n">
-        <v>21.08020695838008</v>
+        <v>12.10150614009552</v>
       </c>
       <c r="H48" t="n">
         <v>0</v>
@@ -2016,7 +2016,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Mot_Stress_2</t>
+          <t>Partici1_4</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2026,17 +2026,17 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Energy_Sources</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>0.7418807573426818</v>
+        <v>1.510532471745356</v>
       </c>
       <c r="F49" t="n">
-        <v>0.04033706894254549</v>
+        <v>0.1340960194888896</v>
       </c>
       <c r="G49" t="n">
-        <v>18.39203434391812</v>
+        <v>11.26455861621787</v>
       </c>
       <c r="H49" t="n">
         <v>0</v>
@@ -2048,36 +2048,30 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Partici1_1</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>~~</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Participation</t>
+          <t>Wellbeing</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>-0.1245528900240659</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.01150811312639142</v>
+      </c>
+      <c r="G50" t="n">
+        <v>-10.82305054228283</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -2086,27 +2080,27 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Partici1_2</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>~~</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Participation</t>
+          <t>Response_to_Stress</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>1.192456436487136</v>
+        <v>0.3100557965274285</v>
       </c>
       <c r="F51" t="n">
-        <v>0.05988644846329608</v>
+        <v>0.02536323563181863</v>
       </c>
       <c r="G51" t="n">
-        <v>19.91195783129585</v>
+        <v>12.22461522717683</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -2118,30 +2112,30 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Partici1_3</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>~~</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Participation</t>
+          <t>Energy_Sources</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>1.06413912386902</v>
+        <v>0.01674407356307667</v>
       </c>
       <c r="F52" t="n">
-        <v>0.0546577058472339</v>
+        <v>0.008552245081751678</v>
       </c>
       <c r="G52" t="n">
-        <v>19.46915091576982</v>
+        <v>1.957857077417767</v>
       </c>
       <c r="H52" t="n">
-        <v>0</v>
+        <v>0.05024678568063856</v>
       </c>
     </row>
     <row r="53">
@@ -2150,27 +2144,27 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Partici1_4</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>~~</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Participation</t>
+          <t>Stressors</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>0.8738021107985809</v>
+        <v>0.4348190032963086</v>
       </c>
       <c r="F53" t="n">
-        <v>0.05146613905084955</v>
+        <v>0.04281480019653033</v>
       </c>
       <c r="G53" t="n">
-        <v>16.97819434090965</v>
+        <v>10.15581063768201</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -2182,36 +2176,30 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_1</t>
+          <t>Negative_Outcomes</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>~~</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Behavior</t>
+          <t>Positive_Outcomes</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>-0.03203284506601356</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.00458820366008066</v>
+      </c>
+      <c r="G54" t="n">
+        <v>-6.981565647953137</v>
+      </c>
+      <c r="H54" t="n">
+        <v>2.918998376344462e-12</v>
       </c>
     </row>
     <row r="55">
@@ -2220,30 +2208,30 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_2</t>
+          <t>Negative_Outcomes</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>~~</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Behavior</t>
+          <t>Negative_Outcomes</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>1.171616474678231</v>
+        <v>0.01931791669535863</v>
       </c>
       <c r="F55" t="n">
-        <v>0.1274908376443077</v>
+        <v>0.005539724023818518</v>
       </c>
       <c r="G55" t="n">
-        <v>9.18980921544955</v>
+        <v>3.487162286210004</v>
       </c>
       <c r="H55" t="n">
-        <v>0</v>
+        <v>0.0004881750321006351</v>
       </c>
     </row>
     <row r="56">
@@ -2252,30 +2240,30 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_4</t>
+          <t>Energy_Sources</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>~~</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Behavior</t>
+          <t>Energy_Sources</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>1.053419257090001</v>
+        <v>0.1376409973676975</v>
       </c>
       <c r="F56" t="n">
-        <v>0.1144569148012657</v>
+        <v>0.01897083944005765</v>
       </c>
       <c r="G56" t="n">
-        <v>9.203631418074428</v>
+        <v>7.255398359959124</v>
       </c>
       <c r="H56" t="n">
-        <v>0</v>
+        <v>4.005684672847565e-13</v>
       </c>
     </row>
     <row r="57">
@@ -2284,30 +2272,30 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_1</t>
+          <t>Positive_Outcomes</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>~~</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Behavior</t>
+          <t>Positive_Outcomes</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>1.670728615287617</v>
+        <v>0.1101238567414543</v>
       </c>
       <c r="F57" t="n">
-        <v>0.1549076009968827</v>
+        <v>0.01828293011183185</v>
       </c>
       <c r="G57" t="n">
-        <v>10.78532366730314</v>
+        <v>6.023315522284035</v>
       </c>
       <c r="H57" t="n">
-        <v>0</v>
+        <v>1.708798658128785e-09</v>
       </c>
     </row>
     <row r="58">
@@ -2316,27 +2304,27 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_4</t>
+          <t>Wellbeing</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>~~</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Behavior</t>
+          <t>Wellbeing</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>1.762720243536617</v>
+        <v>0.2295021337029828</v>
       </c>
       <c r="F58" t="n">
-        <v>0.1703716393529171</v>
+        <v>0.018975216776572</v>
       </c>
       <c r="G58" t="n">
-        <v>10.34632436608112</v>
+        <v>12.0948359322169</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -2348,27 +2336,27 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_5</t>
+          <t>Bevl_1</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>~~</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Behavior</t>
+          <t>Bevl_1</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>2.137147993868972</v>
+        <v>0.4176792784369274</v>
       </c>
       <c r="F59" t="n">
-        <v>0.1941815656176792</v>
+        <v>0.01786622166849094</v>
       </c>
       <c r="G59" t="n">
-        <v>11.00592626833466</v>
+        <v>23.3781538236578</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -2380,27 +2368,27 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_6</t>
+          <t>Bevl_2</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>~~</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Behavior</t>
+          <t>Bevl_2</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>1.293885388754712</v>
+        <v>0.2333344811744716</v>
       </c>
       <c r="F60" t="n">
-        <v>0.1311670482526958</v>
+        <v>0.01126138224096891</v>
       </c>
       <c r="G60" t="n">
-        <v>9.86440882813916</v>
+        <v>20.71987933283011</v>
       </c>
       <c r="H60" t="n">
         <v>0</v>
@@ -2412,27 +2400,27 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_7</t>
+          <t>Bevl_3</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>~~</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Behavior</t>
+          <t>Bevl_3</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>2.203379179676104</v>
+        <v>0.3997601760546594</v>
       </c>
       <c r="F61" t="n">
-        <v>0.1970104957479858</v>
+        <v>0.01750902316006345</v>
       </c>
       <c r="G61" t="n">
-        <v>11.18407002276399</v>
+        <v>22.83166641435746</v>
       </c>
       <c r="H61" t="n">
         <v>0</v>
@@ -2444,7 +2432,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Burn1_1</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2454,17 +2442,17 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Burn1_1</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>-0.1318399782036039</v>
+        <v>0.5248616217124623</v>
       </c>
       <c r="F62" t="n">
-        <v>0.0109748778776175</v>
+        <v>0.02275587383157974</v>
       </c>
       <c r="G62" t="n">
-        <v>-12.01288794843627</v>
+        <v>23.06488538185751</v>
       </c>
       <c r="H62" t="n">
         <v>0</v>
@@ -2476,7 +2464,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Burn1_2</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2486,17 +2474,17 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Response_to_Stress</t>
+          <t>Burn1_2</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>0.3175937039066615</v>
+        <v>0.7072732459553226</v>
       </c>
       <c r="F63" t="n">
-        <v>0.02367677078860072</v>
+        <v>0.03024242631402247</v>
       </c>
       <c r="G63" t="n">
-        <v>13.41372549191356</v>
+        <v>23.38678909515918</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
@@ -2508,7 +2496,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Burn1_3</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2518,20 +2506,20 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Participation</t>
+          <t>Burn1_3</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>0.09779719199797181</v>
+        <v>0.857920083366933</v>
       </c>
       <c r="F64" t="n">
-        <v>0.01515116592171223</v>
+        <v>0.03553512412991204</v>
       </c>
       <c r="G64" t="n">
-        <v>6.454763448360747</v>
+        <v>24.14287565751395</v>
       </c>
       <c r="H64" t="n">
-        <v>1.083879652696851e-10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -2540,7 +2528,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Burn1_4</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2550,17 +2538,17 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Burn1_4</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>0.4306448700094357</v>
+        <v>0.7903328660967985</v>
       </c>
       <c r="F65" t="n">
-        <v>0.03962538222070087</v>
+        <v>0.03288836241389375</v>
       </c>
       <c r="G65" t="n">
-        <v>10.86790450625843</v>
+        <v>24.03077587526493</v>
       </c>
       <c r="H65" t="n">
         <v>0</v>
@@ -2572,7 +2560,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Behavior</t>
+          <t>Cijfer_huidig_1</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2582,20 +2570,20 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Behavior</t>
+          <t>Cijfer_huidig_1</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>0.08189928305034826</v>
+        <v>0.1429782425184556</v>
       </c>
       <c r="F66" t="n">
-        <v>0.01350683155309406</v>
+        <v>0.01781644028194609</v>
       </c>
       <c r="G66" t="n">
-        <v>6.063545156563661</v>
+        <v>8.025073485376002</v>
       </c>
       <c r="H66" t="n">
-        <v>1.331533772130911e-09</v>
+        <v>1.110223024625157e-15</v>
       </c>
     </row>
     <row r="67">
@@ -2604,7 +2592,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Behavior</t>
+          <t>Cogn_Eng1_5</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2614,20 +2602,20 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Cogn_Eng1_5</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>-0.02754746787894086</v>
+        <v>0.4618268332486154</v>
       </c>
       <c r="F67" t="n">
-        <v>0.006608368768989561</v>
+        <v>0.02013128099538665</v>
       </c>
       <c r="G67" t="n">
-        <v>-4.168573037879116</v>
+        <v>22.94075738804244</v>
       </c>
       <c r="H67" t="n">
-        <v>3.065125442192063e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -2636,7 +2624,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Interventions</t>
+          <t>Cogn_Eng1_6</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2646,20 +2634,20 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Interventions</t>
+          <t>Cogn_Eng1_6</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>0.2755614833870266</v>
+        <v>0.602518899508121</v>
       </c>
       <c r="F68" t="n">
-        <v>0.03645911250017031</v>
+        <v>0.02489050463062121</v>
       </c>
       <c r="G68" t="n">
-        <v>7.55809630248628</v>
+        <v>24.20677717970706</v>
       </c>
       <c r="H68" t="n">
-        <v>4.085620730620576e-14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -2668,7 +2656,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Interventions</t>
+          <t>Cogn_Eng2_1</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2678,20 +2666,20 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Behavior</t>
+          <t>Cogn_Eng2_1</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>0.001377811005985378</v>
+        <v>0.5871443425384891</v>
       </c>
       <c r="F69" t="n">
-        <v>0.005178330792355976</v>
+        <v>0.0248233249702054</v>
       </c>
       <c r="G69" t="n">
-        <v>0.2660724200456968</v>
+        <v>23.65292897786923</v>
       </c>
       <c r="H69" t="n">
-        <v>0.7901834352268187</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -2700,7 +2688,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Interventions</t>
+          <t>Cogn_Eng2_4</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2710,20 +2698,20 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Stressors</t>
+          <t>Cogn_Eng2_4</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>0.006680671795616268</v>
+        <v>0.8275913504681069</v>
       </c>
       <c r="F70" t="n">
-        <v>0.0109840663079175</v>
+        <v>0.03511768842897255</v>
       </c>
       <c r="G70" t="n">
-        <v>0.6082148093181585</v>
+        <v>23.56622509816925</v>
       </c>
       <c r="H70" t="n">
-        <v>0.5430450137781837</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -2732,7 +2720,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Negative_Outcomes</t>
+          <t>Cogn_Eng2_5</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2742,20 +2730,20 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Negative_Outcomes</t>
+          <t>Cogn_Eng2_5</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>0.02782218713595457</v>
+        <v>0.7646375060447067</v>
       </c>
       <c r="F71" t="n">
-        <v>0.007316276641060098</v>
+        <v>0.0336088983898275</v>
       </c>
       <c r="G71" t="n">
-        <v>3.802779541715152</v>
+        <v>22.75104340383232</v>
       </c>
       <c r="H71" t="n">
-        <v>0.0001430816735561447</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -2764,7 +2752,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Participation</t>
+          <t>Cogn_Eng2_7</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2774,17 +2762,17 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Participation</t>
+          <t>Cogn_Eng2_7</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>0.3445860761129239</v>
+        <v>0.6587315017606573</v>
       </c>
       <c r="F72" t="n">
-        <v>0.03102268292844378</v>
+        <v>0.03000975544712032</v>
       </c>
       <c r="G72" t="n">
-        <v>11.1075523963105</v>
+        <v>21.9505788009318</v>
       </c>
       <c r="H72" t="n">
         <v>0</v>
@@ -2796,7 +2784,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Positive_Outcomes</t>
+          <t>Cogn_Eng2_8</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2806,20 +2794,20 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Positive_Outcomes</t>
+          <t>Cogn_Eng2_8</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>0</v>
+        <v>0.6634711691749394</v>
       </c>
       <c r="F73" t="n">
-        <v>0.004736342253182931</v>
+        <v>0.02681384464054593</v>
       </c>
       <c r="G73" t="n">
-        <v>0</v>
+        <v>24.74360458354202</v>
       </c>
       <c r="H73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -2828,7 +2816,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Depr_1</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2838,17 +2826,17 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Wellbeing</t>
+          <t>Depr_1</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>0.2455245207041751</v>
+        <v>0.5272996527774788</v>
       </c>
       <c r="F74" t="n">
-        <v>0.01838211024347821</v>
+        <v>0.02406856217963475</v>
       </c>
       <c r="G74" t="n">
-        <v>13.35671027095097</v>
+        <v>21.90823235804826</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -2860,7 +2848,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Bekendgebruik_4</t>
+          <t>Depr_2</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2870,17 +2858,17 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Bekendgebruik_4</t>
+          <t>Depr_2</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>1.237204570514979</v>
+        <v>0.6295527640196724</v>
       </c>
       <c r="F75" t="n">
-        <v>0.04849337118965018</v>
+        <v>0.02882718488994694</v>
       </c>
       <c r="G75" t="n">
-        <v>25.51285959581873</v>
+        <v>21.83885684298576</v>
       </c>
       <c r="H75" t="n">
         <v>0</v>
@@ -2892,7 +2880,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Bekendgebruik_5</t>
+          <t>Depr_3</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2902,17 +2890,17 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Bekendgebruik_5</t>
+          <t>Depr_3</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>0.3559100163682629</v>
+        <v>1.207119295091454</v>
       </c>
       <c r="F76" t="n">
-        <v>0.02059544659333671</v>
+        <v>0.04925767902163156</v>
       </c>
       <c r="G76" t="n">
-        <v>17.28100503856665</v>
+        <v>24.50621545803732</v>
       </c>
       <c r="H76" t="n">
         <v>0</v>
@@ -2924,7 +2912,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Bekendgebruik_6</t>
+          <t>Depr_4</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2934,17 +2922,17 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Bekendgebruik_6</t>
+          <t>Depr_4</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>1.074460413756551</v>
+        <v>0.5832644909734961</v>
       </c>
       <c r="F77" t="n">
-        <v>0.04518739569957283</v>
+        <v>0.02482846989890094</v>
       </c>
       <c r="G77" t="n">
-        <v>23.77787870042996</v>
+        <v>23.4917614063613</v>
       </c>
       <c r="H77" t="n">
         <v>0</v>
@@ -2956,7 +2944,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Bekendgebruik_7</t>
+          <t>Depr_5</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2966,17 +2954,17 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Bekendgebruik_7</t>
+          <t>Depr_5</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>0.2618294745230861</v>
+        <v>0.806852064317106</v>
       </c>
       <c r="F78" t="n">
-        <v>0.02082877955884647</v>
+        <v>0.03358497584758088</v>
       </c>
       <c r="G78" t="n">
-        <v>12.57056246482336</v>
+        <v>24.02419665134877</v>
       </c>
       <c r="H78" t="n">
         <v>0</v>
@@ -2988,7 +2976,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Bevl_1</t>
+          <t>Depr_6</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2998,17 +2986,17 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Bevl_1</t>
+          <t>Depr_6</t>
         </is>
       </c>
       <c r="E79" t="n">
-        <v>0.4204571984461671</v>
+        <v>0.6603685167157289</v>
       </c>
       <c r="F79" t="n">
-        <v>0.01652468187574982</v>
+        <v>0.02785962591750434</v>
       </c>
       <c r="G79" t="n">
-        <v>25.44419321244236</v>
+        <v>23.70342368011168</v>
       </c>
       <c r="H79" t="n">
         <v>0</v>
@@ -3020,7 +3008,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Bevl_2</t>
+          <t>Depr_7</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3030,17 +3018,17 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Bevl_2</t>
+          <t>Depr_7</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>0.2433924122424365</v>
+        <v>0.5620285553659282</v>
       </c>
       <c r="F80" t="n">
-        <v>0.01071612248598125</v>
+        <v>0.02395261266144106</v>
       </c>
       <c r="G80" t="n">
-        <v>22.71273145096352</v>
+        <v>23.46418586091104</v>
       </c>
       <c r="H80" t="n">
         <v>0</v>
@@ -3052,7 +3040,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Bevl_3</t>
+          <t>Depr_8</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3062,17 +3050,17 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Bevl_3</t>
+          <t>Depr_8</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>0.425150152123728</v>
+        <v>0.7965822429374761</v>
       </c>
       <c r="F81" t="n">
-        <v>0.01693514287443493</v>
+        <v>0.03389834345776725</v>
       </c>
       <c r="G81" t="n">
-        <v>25.10460970131078</v>
+        <v>23.49914956482787</v>
       </c>
       <c r="H81" t="n">
         <v>0</v>
@@ -3084,7 +3072,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Burn1_1</t>
+          <t>Mot_Stress_1</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3094,17 +3082,17 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Burn1_1</t>
+          <t>Mot_Stress_1</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>0.5272961099190492</v>
+        <v>0.2922920964481741</v>
       </c>
       <c r="F82" t="n">
-        <v>0.02099622915663872</v>
+        <v>0.01356580403055483</v>
       </c>
       <c r="G82" t="n">
-        <v>25.11384810863581</v>
+        <v>21.54624198965914</v>
       </c>
       <c r="H82" t="n">
         <v>0</v>
@@ -3116,7 +3104,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Burn1_2</t>
+          <t>Mot_Stress_2</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3126,17 +3114,17 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Burn1_2</t>
+          <t>Mot_Stress_2</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>0.7115174579380774</v>
+        <v>0.5696128675202559</v>
       </c>
       <c r="F83" t="n">
-        <v>0.02792302095603875</v>
+        <v>0.02352941499039245</v>
       </c>
       <c r="G83" t="n">
-        <v>25.4813925410431</v>
+        <v>24.20854354979213</v>
       </c>
       <c r="H83" t="n">
         <v>0</v>
@@ -3148,7 +3136,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Burn1_3</t>
+          <t>Mot_Stress_4</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3158,17 +3146,17 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Burn1_3</t>
+          <t>Mot_Stress_4</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>0.8709176359110185</v>
+        <v>0.1768546313112034</v>
       </c>
       <c r="F84" t="n">
-        <v>0.03313723144332283</v>
+        <v>0.009666249935599404</v>
       </c>
       <c r="G84" t="n">
-        <v>26.28214844605634</v>
+        <v>18.29609543216726</v>
       </c>
       <c r="H84" t="n">
         <v>0</v>
@@ -3180,7 +3168,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Burn1_4</t>
+          <t>Onnodige_stress_1</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3190,17 +3178,17 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Burn1_4</t>
+          <t>Onnodige_stress_1</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>0.7754282241543875</v>
+        <v>0.9489918465552518</v>
       </c>
       <c r="F85" t="n">
-        <v>0.02982181550191983</v>
+        <v>0.04068775810927716</v>
       </c>
       <c r="G85" t="n">
-        <v>26.00204618925585</v>
+        <v>23.32376839203509</v>
       </c>
       <c r="H85" t="n">
         <v>0</v>
@@ -3212,7 +3200,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Cijfer_huidig_1</t>
+          <t>Onnodige_stress_2</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3222,17 +3210,17 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Cijfer_huidig_1</t>
+          <t>Onnodige_stress_2</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>0.2361717262883765</v>
+        <v>0.7400791349502707</v>
       </c>
       <c r="F86" t="n">
-        <v>0.009808217786270869</v>
+        <v>0.03367435496929501</v>
       </c>
       <c r="G86" t="n">
-        <v>24.07896433487446</v>
+        <v>21.97752965433526</v>
       </c>
       <c r="H86" t="n">
         <v>0</v>
@@ -3244,7 +3232,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_1</t>
+          <t>Onnodige_stress_3</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3254,17 +3242,17 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_1</t>
+          <t>Onnodige_stress_3</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>0.5979152457722768</v>
+        <v>0.803631718256845</v>
       </c>
       <c r="F87" t="n">
-        <v>0.0227354805577168</v>
+        <v>0.03541700662306269</v>
       </c>
       <c r="G87" t="n">
-        <v>26.29877315450171</v>
+        <v>22.69056012517018</v>
       </c>
       <c r="H87" t="n">
         <v>0</v>
@@ -3276,7 +3264,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_2</t>
+          <t>Onnodige_stress_4</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3286,17 +3274,17 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_2</t>
+          <t>Onnodige_stress_4</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>0.6702546129917241</v>
+        <v>0.5779652826769897</v>
       </c>
       <c r="F88" t="n">
-        <v>0.02575055971051178</v>
+        <v>0.03042460110897269</v>
       </c>
       <c r="G88" t="n">
-        <v>26.02873958860346</v>
+        <v>18.99664290052243</v>
       </c>
       <c r="H88" t="n">
         <v>0</v>
@@ -3308,7 +3296,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_4</t>
+          <t>Onnodige_stress_5</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3318,17 +3306,17 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_4</t>
+          <t>Onnodige_stress_5</t>
         </is>
       </c>
       <c r="E89" t="n">
-        <v>0.5381182172269497</v>
+        <v>0.5446609455453296</v>
       </c>
       <c r="F89" t="n">
-        <v>0.02068210397262114</v>
+        <v>0.02879823816368834</v>
       </c>
       <c r="G89" t="n">
-        <v>26.01854327360937</v>
+        <v>18.91299538640454</v>
       </c>
       <c r="H89" t="n">
         <v>0</v>
@@ -3340,7 +3328,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_5</t>
+          <t>Onnodige_stress_6</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3350,17 +3338,17 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_5</t>
+          <t>Onnodige_stress_6</t>
         </is>
       </c>
       <c r="E90" t="n">
-        <v>0.4339185286706527</v>
+        <v>0.7376832697310085</v>
       </c>
       <c r="F90" t="n">
-        <v>0.01765431487224644</v>
+        <v>0.03349263593116809</v>
       </c>
       <c r="G90" t="n">
-        <v>24.57861048622273</v>
+        <v>22.02523776346008</v>
       </c>
       <c r="H90" t="n">
         <v>0</v>
@@ -3372,7 +3360,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_6</t>
+          <t>Onnodige_stress_7</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3382,17 +3370,17 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Cogn_Eng1_6</t>
+          <t>Onnodige_stress_7</t>
         </is>
       </c>
       <c r="E91" t="n">
-        <v>0.5755551922691445</v>
+        <v>1.445260338769903</v>
       </c>
       <c r="F91" t="n">
-        <v>0.02204829579532264</v>
+        <v>0.05949619837587566</v>
       </c>
       <c r="G91" t="n">
-        <v>26.10429384592797</v>
+        <v>24.29164178885808</v>
       </c>
       <c r="H91" t="n">
         <v>0</v>
@@ -3404,7 +3392,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_1</t>
+          <t>Partici1_1</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3414,17 +3402,17 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_1</t>
+          <t>Partici1_1</t>
         </is>
       </c>
       <c r="E92" t="n">
-        <v>0.5018784764259465</v>
+        <v>0.7554419314991707</v>
       </c>
       <c r="F92" t="n">
-        <v>0.02137508082902266</v>
+        <v>0.03710211028142579</v>
       </c>
       <c r="G92" t="n">
-        <v>23.47960601491744</v>
+        <v>20.36115805135219</v>
       </c>
       <c r="H92" t="n">
         <v>0</v>
@@ -3436,7 +3424,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_2</t>
+          <t>Partici1_2</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3446,17 +3434,17 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_2</t>
+          <t>Partici1_2</t>
         </is>
       </c>
       <c r="E93" t="n">
-        <v>0.8936722794788061</v>
+        <v>1.005173585199297</v>
       </c>
       <c r="F93" t="n">
-        <v>0.03318842593172655</v>
+        <v>0.04803961820914168</v>
       </c>
       <c r="G93" t="n">
-        <v>26.92722701854838</v>
+        <v>20.92384624711888</v>
       </c>
       <c r="H93" t="n">
         <v>0</v>
@@ -3468,7 +3456,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_3</t>
+          <t>Partici1_3</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3478,17 +3466,17 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_3</t>
+          <t>Partici1_3</t>
         </is>
       </c>
       <c r="E94" t="n">
-        <v>0.8229896717314351</v>
+        <v>0.9793168618043058</v>
       </c>
       <c r="F94" t="n">
-        <v>0.03041184011150728</v>
+        <v>0.04410705847437994</v>
       </c>
       <c r="G94" t="n">
-        <v>27.06148883746662</v>
+        <v>22.20317780545146</v>
       </c>
       <c r="H94" t="n">
         <v>0</v>
@@ -3500,7 +3488,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_4</t>
+          <t>Partici1_4</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3510,17 +3498,17 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_4</t>
+          <t>Partici1_4</t>
         </is>
       </c>
       <c r="E95" t="n">
-        <v>0.7814914604204354</v>
+        <v>1.053194409922732</v>
       </c>
       <c r="F95" t="n">
-        <v>0.03172326659383327</v>
+        <v>0.04539706128055195</v>
       </c>
       <c r="G95" t="n">
-        <v>24.63464656403688</v>
+        <v>23.19961645514529</v>
       </c>
       <c r="H95" t="n">
         <v>0</v>
@@ -3532,7 +3520,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_5</t>
+          <t>StPunt_beh</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3542,17 +3530,17 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_5</t>
+          <t>StPunt_beh</t>
         </is>
       </c>
       <c r="E96" t="n">
-        <v>0.6677195095991738</v>
+        <v>0.5207959911284874</v>
       </c>
       <c r="F96" t="n">
-        <v>0.02961589954841889</v>
+        <v>0.03332734126250635</v>
       </c>
       <c r="G96" t="n">
-        <v>22.54598103579385</v>
+        <v>15.62668882017187</v>
       </c>
       <c r="H96" t="n">
         <v>0</v>
@@ -3564,7 +3552,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_6</t>
+          <t>StopInt</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3574,17 +3562,17 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_6</t>
+          <t>StopInt</t>
         </is>
       </c>
       <c r="E97" t="n">
-        <v>0.5698941437347723</v>
+        <v>0.1336662169257126</v>
       </c>
       <c r="F97" t="n">
-        <v>0.02244823245553536</v>
+        <v>0.007465393073639377</v>
       </c>
       <c r="G97" t="n">
-        <v>25.38703859371605</v>
+        <v>17.90477950582254</v>
       </c>
       <c r="H97" t="n">
         <v>0</v>
@@ -3596,7 +3584,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_7</t>
+          <t>Vertr</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3606,851 +3594,19 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Cogn_Eng2_7</t>
+          <t>Vertr</t>
         </is>
       </c>
       <c r="E98" t="n">
-        <v>0.5805729566394868</v>
+        <v>0.9481449780119635</v>
       </c>
       <c r="F98" t="n">
-        <v>0.02707855007984639</v>
+        <v>0.04475956810742612</v>
       </c>
       <c r="G98" t="n">
-        <v>21.44032656497906</v>
+        <v>21.18306806971787</v>
       </c>
       <c r="H98" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="1" t="n">
-        <v>97</v>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>Cogn_Eng2_8</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>Cogn_Eng2_8</t>
-        </is>
-      </c>
-      <c r="E99" t="n">
-        <v>0.6712387818801341</v>
-      </c>
-      <c r="F99" t="n">
-        <v>0.02505447793309664</v>
-      </c>
-      <c r="G99" t="n">
-        <v>26.79117017108727</v>
-      </c>
-      <c r="H99" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="1" t="n">
-        <v>98</v>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>Depr_1</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>Depr_1</t>
-        </is>
-      </c>
-      <c r="E100" t="n">
-        <v>0.5377144289783268</v>
-      </c>
-      <c r="F100" t="n">
-        <v>0.02263885250846431</v>
-      </c>
-      <c r="G100" t="n">
-        <v>23.75184116569212</v>
-      </c>
-      <c r="H100" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="1" t="n">
-        <v>99</v>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>Depr_2</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>Depr_2</t>
-        </is>
-      </c>
-      <c r="E101" t="n">
-        <v>0.6328672361584818</v>
-      </c>
-      <c r="F101" t="n">
-        <v>0.02667279422783044</v>
-      </c>
-      <c r="G101" t="n">
-        <v>23.72706926499737</v>
-      </c>
-      <c r="H101" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>Depr_3</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>Depr_3</t>
-        </is>
-      </c>
-      <c r="E102" t="n">
-        <v>1.18843279881116</v>
-      </c>
-      <c r="F102" t="n">
-        <v>0.04470898655756116</v>
-      </c>
-      <c r="G102" t="n">
-        <v>26.58151951743562</v>
-      </c>
-      <c r="H102" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="1" t="n">
-        <v>101</v>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>Depr_4</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>Depr_4</t>
-        </is>
-      </c>
-      <c r="E103" t="n">
-        <v>0.5938508323709645</v>
-      </c>
-      <c r="F103" t="n">
-        <v>0.02324990567833644</v>
-      </c>
-      <c r="G103" t="n">
-        <v>25.54207490393196</v>
-      </c>
-      <c r="H103" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="1" t="n">
-        <v>102</v>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>Depr_5</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>Depr_5</t>
-        </is>
-      </c>
-      <c r="E104" t="n">
-        <v>0.8225564479041247</v>
-      </c>
-      <c r="F104" t="n">
-        <v>0.03148763398921845</v>
-      </c>
-      <c r="G104" t="n">
-        <v>26.12315832176053</v>
-      </c>
-      <c r="H104" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="1" t="n">
-        <v>103</v>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>Depr_6</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>Depr_6</t>
-        </is>
-      </c>
-      <c r="E105" t="n">
-        <v>0.6384454242521397</v>
-      </c>
-      <c r="F105" t="n">
-        <v>0.02490573275891</v>
-      </c>
-      <c r="G105" t="n">
-        <v>25.63447662458764</v>
-      </c>
-      <c r="H105" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="1" t="n">
-        <v>104</v>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>Depr_7</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>Depr_7</t>
-        </is>
-      </c>
-      <c r="E106" t="n">
-        <v>0.5879565150437984</v>
-      </c>
-      <c r="F106" t="n">
-        <v>0.02309156685348047</v>
-      </c>
-      <c r="G106" t="n">
-        <v>25.46195841750413</v>
-      </c>
-      <c r="H106" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="1" t="n">
-        <v>105</v>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>Depr_8</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>Depr_8</t>
-        </is>
-      </c>
-      <c r="E107" t="n">
-        <v>0.8051338445835351</v>
-      </c>
-      <c r="F107" t="n">
-        <v>0.03147871728143838</v>
-      </c>
-      <c r="G107" t="n">
-        <v>25.57708553876527</v>
-      </c>
-      <c r="H107" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="1" t="n">
-        <v>106</v>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>Mot_Stress_1</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>Mot_Stress_1</t>
-        </is>
-      </c>
-      <c r="E108" t="n">
-        <v>0.3161762287455623</v>
-      </c>
-      <c r="F108" t="n">
-        <v>0.01329898338204736</v>
-      </c>
-      <c r="G108" t="n">
-        <v>23.77446603539652</v>
-      </c>
-      <c r="H108" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="1" t="n">
-        <v>107</v>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>Mot_Stress_2</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>Mot_Stress_2</t>
-        </is>
-      </c>
-      <c r="E109" t="n">
-        <v>0.5681902447569463</v>
-      </c>
-      <c r="F109" t="n">
-        <v>0.02161948899056125</v>
-      </c>
-      <c r="G109" t="n">
-        <v>26.28139106242189</v>
-      </c>
-      <c r="H109" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="1" t="n">
-        <v>108</v>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>Mot_Stress_4</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>Mot_Stress_4</t>
-        </is>
-      </c>
-      <c r="E110" t="n">
-        <v>0.2033504204272714</v>
-      </c>
-      <c r="F110" t="n">
-        <v>0.009676672532630366</v>
-      </c>
-      <c r="G110" t="n">
-        <v>21.01449849837804</v>
-      </c>
-      <c r="H110" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="1" t="n">
-        <v>109</v>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>Onnodige_stress_1</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>Onnodige_stress_1</t>
-        </is>
-      </c>
-      <c r="E111" t="n">
-        <v>0.9800434942016013</v>
-      </c>
-      <c r="F111" t="n">
-        <v>0.03845525904293287</v>
-      </c>
-      <c r="G111" t="n">
-        <v>25.48529170176592</v>
-      </c>
-      <c r="H111" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="1" t="n">
-        <v>110</v>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>Onnodige_stress_2</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>Onnodige_stress_2</t>
-        </is>
-      </c>
-      <c r="E112" t="n">
-        <v>0.7533026009153689</v>
-      </c>
-      <c r="F112" t="n">
-        <v>0.03142416818561204</v>
-      </c>
-      <c r="G112" t="n">
-        <v>23.97207768370799</v>
-      </c>
-      <c r="H112" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="1" t="n">
-        <v>111</v>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>Onnodige_stress_3</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>Onnodige_stress_3</t>
-        </is>
-      </c>
-      <c r="E113" t="n">
-        <v>0.8294833043162358</v>
-      </c>
-      <c r="F113" t="n">
-        <v>0.03361604875914392</v>
-      </c>
-      <c r="G113" t="n">
-        <v>24.67521719267891</v>
-      </c>
-      <c r="H113" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="1" t="n">
-        <v>112</v>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>Onnodige_stress_4</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>Onnodige_stress_4</t>
-        </is>
-      </c>
-      <c r="E114" t="n">
-        <v>0.5721058775648915</v>
-      </c>
-      <c r="F114" t="n">
-        <v>0.02774347526839094</v>
-      </c>
-      <c r="G114" t="n">
-        <v>20.62127660683121</v>
-      </c>
-      <c r="H114" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="1" t="n">
-        <v>113</v>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>Onnodige_stress_5</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>Onnodige_stress_5</t>
-        </is>
-      </c>
-      <c r="E115" t="n">
-        <v>0.548713417108797</v>
-      </c>
-      <c r="F115" t="n">
-        <v>0.02661225383317656</v>
-      </c>
-      <c r="G115" t="n">
-        <v>20.61882546769174</v>
-      </c>
-      <c r="H115" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="1" t="n">
-        <v>114</v>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>Onnodige_stress_6</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>Onnodige_stress_6</t>
-        </is>
-      </c>
-      <c r="E116" t="n">
-        <v>0.7449814165031058</v>
-      </c>
-      <c r="F116" t="n">
-        <v>0.03120095793242363</v>
-      </c>
-      <c r="G116" t="n">
-        <v>23.87687641170318</v>
-      </c>
-      <c r="H116" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="1" t="n">
-        <v>115</v>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>Onnodige_stress_7</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>Onnodige_stress_7</t>
-        </is>
-      </c>
-      <c r="E117" t="n">
-        <v>1.461391374689254</v>
-      </c>
-      <c r="F117" t="n">
-        <v>0.05531947254858133</v>
-      </c>
-      <c r="G117" t="n">
-        <v>26.41730492602671</v>
-      </c>
-      <c r="H117" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="1" t="n">
-        <v>116</v>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>Partici1_1</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>Partici1_1</t>
-        </is>
-      </c>
-      <c r="E118" t="n">
-        <v>0.7239515254346804</v>
-      </c>
-      <c r="F118" t="n">
-        <v>0.03398144147455329</v>
-      </c>
-      <c r="G118" t="n">
-        <v>21.30432065265686</v>
-      </c>
-      <c r="H118" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" s="1" t="n">
-        <v>117</v>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>Partici1_2</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t>Partici1_2</t>
-        </is>
-      </c>
-      <c r="E119" t="n">
-        <v>0.8681667499490331</v>
-      </c>
-      <c r="F119" t="n">
-        <v>0.04309848720495597</v>
-      </c>
-      <c r="G119" t="n">
-        <v>20.14378708469047</v>
-      </c>
-      <c r="H119" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="1" t="n">
-        <v>118</v>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>Partici1_3</t>
-        </is>
-      </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>Partici1_3</t>
-        </is>
-      </c>
-      <c r="E120" t="n">
-        <v>0.79435104936144</v>
-      </c>
-      <c r="F120" t="n">
-        <v>0.03764238683608348</v>
-      </c>
-      <c r="G120" t="n">
-        <v>21.10256856982521</v>
-      </c>
-      <c r="H120" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" s="1" t="n">
-        <v>119</v>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>Partici1_4</t>
-        </is>
-      </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D121" t="inlineStr">
-        <is>
-          <t>Partici1_4</t>
-        </is>
-      </c>
-      <c r="E121" t="n">
-        <v>0.9686471100017132</v>
-      </c>
-      <c r="F121" t="n">
-        <v>0.04035286947334166</v>
-      </c>
-      <c r="G121" t="n">
-        <v>24.00441709895319</v>
-      </c>
-      <c r="H121" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" s="1" t="n">
-        <v>120</v>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>StopInt</t>
-        </is>
-      </c>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D122" t="inlineStr">
-        <is>
-          <t>StopInt</t>
-        </is>
-      </c>
-      <c r="E122" t="n">
-        <v>0.1145100545020604</v>
-      </c>
-      <c r="F122" t="n">
-        <v>0.008383970513512674</v>
-      </c>
-      <c r="G122" t="n">
-        <v>13.65821293190895</v>
-      </c>
-      <c r="H122" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" s="1" t="n">
-        <v>121</v>
-      </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>Stopint2</t>
-        </is>
-      </c>
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D123" t="inlineStr">
-        <is>
-          <t>Stopint2</t>
-        </is>
-      </c>
-      <c r="E123" t="n">
-        <v>0.5966656361882181</v>
-      </c>
-      <c r="F123" t="n">
-        <v>0.02946127502615425</v>
-      </c>
-      <c r="G123" t="n">
-        <v>20.25253949933516</v>
-      </c>
-      <c r="H123" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" s="1" t="n">
-        <v>122</v>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>Vertr</t>
-        </is>
-      </c>
-      <c r="C124" t="inlineStr">
-        <is>
-          <t>~~</t>
-        </is>
-      </c>
-      <c r="D124" t="inlineStr">
-        <is>
-          <t>Vertr</t>
-        </is>
-      </c>
-      <c r="E124" t="n">
-        <v>1.040919503277965</v>
-      </c>
-      <c r="F124" t="n">
-        <v>0.04186049646654874</v>
-      </c>
-      <c r="G124" t="n">
-        <v>24.86639173247528</v>
-      </c>
-      <c r="H124" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>